<commit_message>
Add FY22 results to £SDRY model, update Fashion Retailers Overview file
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2608807C-04C5-409F-AE2B-0679614CEF51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC14D2A-2808-4354-B5D6-DC47CE2CAD38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="32295" windowHeight="18855" firstSheet="1" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="537">
   <si>
     <t>Ticker</t>
   </si>
@@ -1646,7 +1646,13 @@
     <t>InvQ/H</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>FY22 E</t>
+  </si>
+  <si>
+    <t>22 RevG</t>
+  </si>
+  <si>
+    <t>Released</t>
   </si>
 </sst>
 </file>
@@ -1946,7 +1952,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2197,6 +2203,9 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2709,27 +2718,28 @@
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
       <sheetName val="Trustpilot Reviews"/>
+      <sheetName val="Historical Projections"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>1.022</v>
+            <v>1.1299999999999999</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>83.94708</v>
+            <v>92.523351359999978</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-2.1999999999999957</v>
+            <v>8.3000000000000007</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>86.147079999999988</v>
+            <v>84.223351359999981</v>
           </cell>
         </row>
         <row r="24">
@@ -2744,37 +2754,40 @@
         </row>
         <row r="26">
           <cell r="C26">
-            <v>226</v>
+            <v>220</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>159.4</v>
+            <v>132.69999999999999</v>
           </cell>
         </row>
         <row r="29">
           <cell r="C29" t="str">
-            <v>H122</v>
+            <v>FY22</v>
+          </cell>
+          <cell r="D29">
+            <v>44841</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>34.458832000000143</v>
+            <v>3.7102797955947073</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>-4.6059933708871261</v>
+            <v>4.0759185621145306</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>0.91152134454347877</v>
+            <v>0.89050386294513961</v>
           </cell>
         </row>
         <row r="39">
           <cell r="C39">
-            <v>-2.3222384525207773</v>
+            <v>-2.5676413418282564</v>
           </cell>
         </row>
       </sheetData>
@@ -2789,6 +2802,9 @@
           <cell r="S17">
             <v>-36.099999999999973</v>
           </cell>
+          <cell r="T17">
+            <v>22.700000000000035</v>
+          </cell>
         </row>
         <row r="21">
           <cell r="Q21">
@@ -2800,6 +2816,9 @@
           <cell r="S21">
             <v>-0.21053378762066999</v>
           </cell>
+          <cell r="T21">
+            <v>9.6205718395971918E-2</v>
+          </cell>
         </row>
         <row r="33">
           <cell r="J33">
@@ -2807,27 +2826,33 @@
           </cell>
         </row>
         <row r="34">
-          <cell r="J34">
-            <v>2.7056277056277018E-2</v>
+          <cell r="T34">
+            <v>4.2486876640420002E-2</v>
           </cell>
         </row>
         <row r="35">
-          <cell r="J35">
-            <v>9.0187590187589799E-3</v>
+          <cell r="T35">
+            <v>3.7237532808399004E-2</v>
           </cell>
         </row>
         <row r="36">
-          <cell r="J36">
-            <v>0.375000000000001</v>
+          <cell r="T36">
+            <v>-0.26815642458100508</v>
           </cell>
         </row>
         <row r="79">
-          <cell r="J79">
-            <v>-4.2642642642642614E-2</v>
+          <cell r="T79">
+            <v>-0.10519217801753222</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="T82">
+            <v>0.2176837270341207</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7732,13 +7757,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AH29"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE9" sqref="AE9"/>
+      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7750,17 +7775,17 @@
     <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="6"/>
     <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="18" width="9.140625" style="1"/>
-    <col min="19" max="21" width="9.140625" style="4"/>
-    <col min="22" max="27" width="9.140625" style="1"/>
-    <col min="28" max="28" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="9.140625" style="4"/>
-    <col min="32" max="33" width="9.140625" style="1"/>
-    <col min="34" max="34" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="23" width="9.140625" style="4"/>
+    <col min="24" max="29" width="9.140625" style="1"/>
+    <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="9.140625" style="4"/>
+    <col min="34" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="89" t="s">
         <v>499</v>
@@ -7788,8 +7813,10 @@
       <c r="AA1" s="89"/>
       <c r="AB1" s="89"/>
       <c r="AC1" s="89"/>
-    </row>
-    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD1" s="89"/>
+      <c r="AE1" s="89"/>
+    </row>
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -7819,7 +7846,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>514</v>
@@ -7828,67 +7855,73 @@
         <v>501</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -7929,84 +7962,85 @@
         <f>[1]Main!$C$33</f>
         <v>24.304770592127053</v>
       </c>
-      <c r="N3" s="56">
+      <c r="O3" s="56">
         <f>'[1]Financial Model'!$AD$21*1000*E28</f>
         <v>5622.7799999999934</v>
       </c>
-      <c r="O3" s="56">
+      <c r="P3" s="56">
         <f>'[1]Financial Model'!$AC$21*1000*E28</f>
         <v>5326.1099999999988</v>
       </c>
-      <c r="P3" s="56">
+      <c r="Q3" s="56">
         <f>'[1]Financial Model'!$AB$21*1000*E28</f>
         <v>2361.27</v>
       </c>
-      <c r="Q3" s="51">
+      <c r="R3" s="51">
         <f>[1]Main!$C$34</f>
         <v>24.880641209063874</v>
       </c>
-      <c r="R3" s="51">
+      <c r="S3" s="51">
         <f>[1]Main!$C$38</f>
         <v>37.504159682207103</v>
       </c>
-      <c r="S3" s="51">
+      <c r="T3" s="51">
         <f>[1]Main!$C$36</f>
         <v>9.4420201618000252</v>
       </c>
-      <c r="T3" s="53">
+      <c r="U3" s="53"/>
+      <c r="V3" s="53">
         <f>'[1]Financial Model'!$AD$25</f>
         <v>4.8767344739323759E-2</v>
       </c>
-      <c r="U3" s="53">
+      <c r="W3" s="53">
         <f>'[1]Financial Model'!$AC$25</f>
         <v>0.19076009945726247</v>
       </c>
-      <c r="V3" s="53">
+      <c r="X3" s="53">
         <f>'[1]Financial Model'!$AB$25</f>
         <v>-4.3817266150267264E-2</v>
       </c>
-      <c r="W3" s="53">
+      <c r="Y3" s="53">
         <f>'[1]Financial Model'!$W$34</f>
         <v>0.44257901789233084</v>
       </c>
-      <c r="X3" s="53">
+      <c r="Z3" s="53">
         <f>'[1]Financial Model'!$W$35</f>
         <v>0.13360132419011606</v>
       </c>
-      <c r="Y3" s="53">
+      <c r="AA3" s="53">
         <f>'[1]Financial Model'!$W$36</f>
         <v>0.11570899345787047</v>
       </c>
-      <c r="Z3" s="53">
+      <c r="AB3" s="53">
         <f>'[1]Financial Model'!$W$37</f>
         <v>0.19693654266958391</v>
       </c>
-      <c r="AB3" s="56">
+      <c r="AD3" s="56">
         <f>[1]Main!$C$26*E28</f>
         <v>8985.66</v>
       </c>
-      <c r="AC3" s="53">
+      <c r="AE3" s="53">
         <f>'[1]Financial Model'!$W$72</f>
         <v>0.44230482161516638</v>
       </c>
-      <c r="AD3" s="53">
+      <c r="AF3" s="53">
         <f>'[1]Financial Model'!$W$73</f>
         <v>0.14750593824228031</v>
       </c>
-      <c r="AE3" s="53">
+      <c r="AG3" s="53">
         <f>'[1]Financial Model'!$AD$85</f>
         <v>0.18026118604153288</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AI3" s="4">
         <f>[1]Main!$C$24</f>
         <v>1964</v>
       </c>
-      <c r="AH3" s="4" t="str">
+      <c r="AJ3" s="4" t="str">
         <f>[1]Main!$C$23</f>
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8043,69 +8077,70 @@
         <f>[2]Main!$C$33</f>
         <v>13.471618843205112</v>
       </c>
-      <c r="N4" s="56">
+      <c r="O4" s="56">
         <f>'[2]Financial Model'!$AA$22*E28</f>
         <v>1289.817929999999</v>
       </c>
-      <c r="O4" s="56">
+      <c r="P4" s="56">
         <f>'[2]Financial Model'!$Z$22*$E$28</f>
         <v>379.29957000000132</v>
       </c>
-      <c r="P4" s="56">
+      <c r="Q4" s="56">
         <f>'[2]Financial Model'!$Y$22*$E$28</f>
         <v>631.88757000000021</v>
       </c>
-      <c r="Q4" s="51">
+      <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
         <v>10.068932086717085</v>
       </c>
-      <c r="S4" s="51">
+      <c r="T4" s="51">
         <f>[2]Main!$C$36</f>
         <v>4.1363260534772177</v>
       </c>
-      <c r="T4" s="53">
+      <c r="U4" s="53"/>
+      <c r="V4" s="53">
         <f>'[2]Financial Model'!$AA$26</f>
         <v>0.28174654717062797</v>
       </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="53">
+      <c r="X4" s="4"/>
+      <c r="Y4" s="53">
         <f>'[2]Financial Model'!$AA$35</f>
         <v>0.54513731020621858</v>
       </c>
-      <c r="X4" s="53">
+      <c r="Z4" s="53">
         <f>'[2]Financial Model'!$AA$36</f>
         <v>0.13783073519228486</v>
       </c>
-      <c r="Y4" s="53">
+      <c r="AA4" s="53">
         <f>'[2]Financial Model'!$AA$37</f>
         <v>0.1171191035146683</v>
       </c>
-      <c r="Z4" s="53">
+      <c r="AB4" s="53">
         <f>'[2]Financial Model'!$AA$38</f>
         <v>0.20153557290196375</v>
       </c>
-      <c r="AB4" s="56">
+      <c r="AD4" s="56">
         <f>[2]Main!$C$26*E28</f>
         <v>2177.4973500000001</v>
       </c>
-      <c r="AC4" s="53">
+      <c r="AE4" s="53">
         <f>'[2]Financial Model'!$T$76</f>
         <v>0.9241949083593437</v>
       </c>
-      <c r="AF4" s="57">
+      <c r="AH4" s="57">
         <f>[2]Main!$C$25</f>
         <v>1297</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AI4" s="4">
         <f>[2]Main!$C$24</f>
         <v>1899</v>
       </c>
-      <c r="AH4" s="4" t="str">
+      <c r="AJ4" s="4" t="str">
         <f>[2]Main!$C$23</f>
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8142,84 +8177,85 @@
         <f>[3]Main!$C$33</f>
         <v>11.170021490774916</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <f>'[3]Financial Model'!$O$17</f>
         <v>677.49999999999943</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <f>'[3]Financial Model'!$N$17</f>
         <v>286.70000000000039</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <f>'[3]Financial Model'!$M$17</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="51">
+      <c r="R5" s="51">
         <f>[3]Main!$C$34</f>
         <v>9.8614553505535145</v>
       </c>
-      <c r="R5" s="51">
+      <c r="S5" s="51">
         <f>[3]Main!$C$38</f>
         <v>23.595786536449214</v>
       </c>
-      <c r="S5" s="51">
+      <c r="T5" s="51">
         <f>[3]Main!$C$36</f>
         <v>6.6149861386138609</v>
       </c>
-      <c r="T5" s="53">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53">
         <f>'[3]Financial Model'!$O$21</f>
         <v>0.3088218650973289</v>
       </c>
-      <c r="U5" s="53">
+      <c r="W5" s="53">
         <f>'[3]Financial Model'!$N$21</f>
         <v>0</v>
       </c>
-      <c r="V5" s="53">
+      <c r="X5" s="53">
         <f>'[3]Financial Model'!$M$21</f>
         <v>0</v>
       </c>
-      <c r="W5" s="53">
+      <c r="Y5" s="53">
         <f>'[3]Financial Model'!$O$24</f>
         <v>0.42629542359324668</v>
       </c>
-      <c r="X5" s="53">
+      <c r="Z5" s="53">
         <f>'[3]Financial Model'!$O$25</f>
         <v>0.19572407531507371</v>
       </c>
-      <c r="Y5" s="53">
+      <c r="AA5" s="53">
         <f>'[3]Financial Model'!$O$26</f>
         <v>0.14645798655396777</v>
       </c>
-      <c r="Z5" s="53">
+      <c r="AB5" s="53">
         <f>'[3]Financial Model'!$O$27</f>
         <v>0.1768922366662618</v>
       </c>
-      <c r="AB5" s="56">
+      <c r="AD5" s="56">
         <f>[3]Main!$C$26</f>
         <v>633</v>
       </c>
-      <c r="AC5" s="53">
+      <c r="AE5" s="53">
         <f>'[3]Financial Model'!$O$66</f>
         <v>0.17899050102439928</v>
       </c>
-      <c r="AE5" s="53">
+      <c r="AG5" s="53">
         <f>'[3]Financial Model'!$O$68</f>
         <v>0.13683823688363347</v>
       </c>
-      <c r="AF5" s="57">
+      <c r="AH5" s="57">
         <f>[3]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AI5" s="4">
         <f>[3]Main!$C$24</f>
         <v>1864</v>
       </c>
-      <c r="AH5" s="4" t="str">
+      <c r="AJ5" s="4" t="str">
         <f>[3]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8260,84 +8296,85 @@
         <f>[4]Main!$C$33</f>
         <v>19.696809986130337</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <f>'[4]Financial Model'!$T$18</f>
         <v>459.60000000000014</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <f>'[4]Financial Model'!$S$18</f>
         <v>229.20000000000027</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <f>'[4]Financial Model'!$R$18</f>
         <v>250.70000000000005</v>
       </c>
-      <c r="Q6" s="52">
+      <c r="R6" s="52">
         <f>[4]Main!$C$34</f>
         <v>13.208756530668998</v>
       </c>
-      <c r="R6" s="52">
+      <c r="S6" s="52">
         <f>[4]Main!$C$38</f>
         <v>21.698173855148315</v>
       </c>
-      <c r="S6" s="52">
+      <c r="T6" s="52">
         <f>[4]Main!$C$36</f>
         <v>1.9809164028971902</v>
       </c>
-      <c r="T6" s="53">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53">
         <f>'[4]Financial Model'!$T$22</f>
         <v>0.38845199682194798</v>
       </c>
-      <c r="U6" s="53">
+      <c r="W6" s="53">
         <f>'[4]Financial Model'!$S$22</f>
         <v>9.245925247103548E-3</v>
       </c>
-      <c r="V6" s="53">
+      <c r="X6" s="53">
         <f>'[4]Financial Model'!$R$22</f>
         <v>0.29526474204078168</v>
       </c>
-      <c r="W6" s="53">
+      <c r="Y6" s="53">
         <f>'[4]Financial Model'!$L$27</f>
         <v>0.48450691473710422</v>
       </c>
-      <c r="X6" s="53">
+      <c r="Z6" s="53">
         <f>'[4]Financial Model'!$L$28</f>
         <v>7.5349131979810399E-2</v>
       </c>
-      <c r="Y6" s="53">
+      <c r="AA6" s="53">
         <f>'[4]Financial Model'!$L$29</f>
         <v>4.8957696747470719E-2</v>
       </c>
-      <c r="Z6" s="53">
+      <c r="AB6" s="53">
         <f>'[4]Financial Model'!$L$30</f>
         <v>0.27489104927924868</v>
       </c>
-      <c r="AB6" s="56">
+      <c r="AD6" s="56">
         <f>[4]Main!$C$26</f>
         <v>1428.5</v>
       </c>
-      <c r="AC6" s="53">
+      <c r="AE6" s="53">
         <f>'[4]Financial Model'!$L$72</f>
         <v>0.43322965787097423</v>
       </c>
-      <c r="AE6" s="53">
+      <c r="AG6" s="53">
         <f>'[4]Financial Model'!$L$75</f>
         <v>0.32332903284217196</v>
       </c>
-      <c r="AF6" s="57">
+      <c r="AH6" s="57">
         <f>[4]Main!$C$25</f>
         <v>3402</v>
       </c>
-      <c r="AG6" s="4">
+      <c r="AI6" s="4">
         <f>[4]Main!$C$24</f>
         <v>1981</v>
       </c>
-      <c r="AH6" s="4" t="str">
+      <c r="AJ6" s="4" t="str">
         <f>[4]Main!$C$23</f>
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>526</v>
       </c>
@@ -8367,27 +8404,28 @@
         <v>3461.73</v>
       </c>
       <c r="J7" s="59"/>
-      <c r="P7" s="4"/>
-      <c r="S7" s="1"/>
-      <c r="V7" s="4"/>
-      <c r="AB7" s="49">
+      <c r="Q7" s="4"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="53"/>
+      <c r="X7" s="4"/>
+      <c r="AD7" s="49">
         <f>[5]Main!$C$26</f>
         <v>0</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="AH7" s="4">
         <f>[5]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="4">
+      <c r="AI7" s="4">
         <f>[5]Main!$C$24</f>
         <v>1982</v>
       </c>
-      <c r="AH7" s="4" t="str">
+      <c r="AJ7" s="4" t="str">
         <f>[5]Main!$C$23</f>
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8424,85 +8462,86 @@
         <f>[6]Main!$C$34</f>
         <v>15.715778773521555</v>
       </c>
-      <c r="N8" s="56">
+      <c r="O8" s="56">
         <f>'[6]Financial Model'!$AA$20*$E$28</f>
         <v>334.85580000000039</v>
       </c>
-      <c r="O8" s="56">
+      <c r="P8" s="56">
         <f>'[6]Financial Model'!$Z$20*$E$28</f>
         <v>-510.73461000000003</v>
       </c>
-      <c r="P8" s="56">
+      <c r="Q8" s="56">
         <f>'[6]Financial Model'!$Y$20*$E$28</f>
         <v>85.692059999999287</v>
       </c>
-      <c r="Q8" s="52">
+      <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
         <v>18.4823862349457</v>
       </c>
-      <c r="R8" s="52">
+      <c r="S8" s="52">
         <f>[6]Main!$C$41</f>
         <v>8.6491744709215048</v>
       </c>
-      <c r="S8" s="52">
+      <c r="T8" s="52">
         <f>[6]Main!$C$37</f>
         <v>1.7736424834957014</v>
       </c>
-      <c r="T8" s="53">
+      <c r="U8" s="53"/>
+      <c r="V8" s="53">
         <f>'[6]Financial Model'!$AA$24</f>
         <v>0.27014278380938728</v>
       </c>
-      <c r="U8" s="53">
+      <c r="W8" s="53">
         <f>'[6]Financial Model'!$Z$24</f>
         <v>-0.15045474463142361</v>
       </c>
-      <c r="V8" s="53" t="str">
+      <c r="X8" s="53" t="str">
         <f>'[6]Financial Model'!$Y$24</f>
         <v>-</v>
       </c>
-      <c r="W8" s="53">
+      <c r="Y8" s="53">
         <f>'[6]Financial Model'!$Q$30</f>
         <v>0.46713889776340067</v>
       </c>
-      <c r="X8" s="53">
+      <c r="Z8" s="53">
         <f>'[6]Financial Model'!$Q$31</f>
         <v>2.5560817667452114E-2</v>
       </c>
-      <c r="Y8" s="53">
+      <c r="AA8" s="53">
         <f>'[6]Financial Model'!$Q$32</f>
         <v>5.6943479778837729E-3</v>
       </c>
-      <c r="Z8" s="53">
+      <c r="AB8" s="53">
         <f>'[6]Financial Model'!$Q$33</f>
         <v>0.39734494626677114</v>
       </c>
-      <c r="AB8" s="56">
+      <c r="AD8" s="56">
         <f>[6]Main!$C$27*E28</f>
         <v>887.58642000000009</v>
       </c>
-      <c r="AC8" s="53"/>
-      <c r="AD8" s="53">
+      <c r="AE8" s="53"/>
+      <c r="AF8" s="53">
         <f>'[6]Financial Model'!$Q$80</f>
         <v>0.15760593361675279</v>
       </c>
-      <c r="AE8" s="53">
+      <c r="AG8" s="53">
         <f>'[6]Financial Model'!$AA$94</f>
         <v>0.14276675535667846</v>
       </c>
-      <c r="AF8" s="57">
+      <c r="AH8" s="57">
         <f>[6]Main!$C$26</f>
         <v>422</v>
       </c>
-      <c r="AG8" s="4">
+      <c r="AI8" s="4">
         <f>[6]Main!$C$24</f>
         <v>1996</v>
       </c>
-      <c r="AH8" s="4" t="str">
+      <c r="AJ8" s="4" t="str">
         <f>[6]Main!$C$23</f>
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8529,9 +8568,11 @@
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
       <c r="M9" s="56"/>
-      <c r="AB9" s="56"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="N9" s="56"/>
+      <c r="U9" s="53"/>
+      <c r="AD9" s="56"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8568,66 +8609,67 @@
         <f>[8]Main!$C$33</f>
         <v>59.925343415248761</v>
       </c>
-      <c r="N10" s="56">
+      <c r="O10" s="56">
         <f>'[8]Financial Model'!$Z$16*E28</f>
         <v>390.2521799999999</v>
       </c>
-      <c r="O10" s="56">
+      <c r="P10" s="56">
         <f>'[8]Financial Model'!$Y$16*F28</f>
         <v>-225.093548387097</v>
       </c>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="52">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="52">
         <f>[8]Main!$C$34</f>
         <v>4.0901579978361697</v>
       </c>
-      <c r="S10" s="52">
+      <c r="T10" s="52">
         <f>[8]Main!$C$36</f>
         <v>1.2473050731522497</v>
       </c>
-      <c r="T10" s="53">
+      <c r="U10" s="53"/>
+      <c r="V10" s="53">
         <f>'[8]Financial Model'!$Z$20</f>
         <v>0.33299379683036578</v>
       </c>
-      <c r="V10" s="4"/>
-      <c r="W10" s="53">
+      <c r="X10" s="4"/>
+      <c r="Y10" s="53">
         <f>'[8]Financial Model'!$O$23</f>
         <v>0.36778425780328089</v>
       </c>
-      <c r="X10" s="53">
+      <c r="Z10" s="53">
         <f>'[8]Financial Model'!$O$24</f>
         <v>3.9716142656608319E-2</v>
       </c>
-      <c r="Y10" s="53">
+      <c r="AA10" s="53">
         <f>'[8]Financial Model'!$O$25</f>
         <v>3.0084252969327211E-2</v>
       </c>
-      <c r="Z10" s="53">
+      <c r="AB10" s="53">
         <f>'[8]Financial Model'!$O$26</f>
         <v>0.23990612577230669</v>
       </c>
-      <c r="AB10" s="56">
+      <c r="AD10" s="56">
         <f>[8]Main!$C$26*E28</f>
         <v>634.35300000000007</v>
       </c>
-      <c r="AC10" s="53">
+      <c r="AE10" s="53">
         <f>'[8]Financial Model'!$O$71</f>
         <v>0.4615447248541884</v>
       </c>
-      <c r="AF10" s="57">
+      <c r="AH10" s="57">
         <f>[8]Main!$C$25</f>
         <v>1141</v>
       </c>
-      <c r="AG10" s="4">
+      <c r="AI10" s="4">
         <f>[8]Main!$C$24</f>
         <v>1977</v>
       </c>
-      <c r="AH10" s="4" t="str">
+      <c r="AJ10" s="4" t="str">
         <f>[8]Main!$C$23</f>
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -8662,76 +8704,77 @@
       </c>
       <c r="K11" s="85"/>
       <c r="L11" s="56"/>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <f>'[9]Financial Model'!$S$13</f>
         <v>128.40000000000015</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <f>'[9]Financial Model'!$R$13</f>
         <v>113.30000000000014</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q11" s="1">
         <f>'[9]Financial Model'!$Q$13</f>
         <v>24.599999999999909</v>
       </c>
-      <c r="S11" s="52">
+      <c r="T11" s="52">
         <f>[9]Main!$C$36</f>
         <v>0.57205092846638639</v>
       </c>
-      <c r="T11" s="53">
+      <c r="U11" s="53"/>
+      <c r="V11" s="53">
         <f>'[9]Financial Model'!$S$17</f>
         <v>0.19825340891680709</v>
       </c>
-      <c r="U11" s="53">
+      <c r="W11" s="53">
         <f>'[9]Financial Model'!$R$17</f>
         <v>0.19389061642582761</v>
       </c>
-      <c r="V11" s="53">
+      <c r="X11" s="53">
         <f>'[9]Financial Model'!$Q$17</f>
         <v>0.13080709882927222</v>
       </c>
-      <c r="W11" s="53">
+      <c r="Y11" s="53">
         <f>'[9]Financial Model'!$K$20</f>
         <v>0.43071703008831885</v>
       </c>
-      <c r="X11" s="53">
+      <c r="Z11" s="53">
         <f>'[9]Financial Model'!$K$21</f>
         <v>-2.1954992265856019E-3</v>
       </c>
-      <c r="Y11" s="53">
+      <c r="AA11" s="53">
         <f>'[9]Financial Model'!$K$22</f>
         <v>-6.7361908088419773E-3</v>
       </c>
-      <c r="Z11" s="53">
+      <c r="AB11" s="53">
         <f>'[9]Financial Model'!$K$23</f>
         <v>0.14556962025316267</v>
       </c>
-      <c r="AB11" s="56">
+      <c r="AD11" s="56">
         <f>[9]Main!$C$26</f>
         <v>986.4</v>
       </c>
-      <c r="AC11" s="53">
+      <c r="AE11" s="53">
         <f>'[9]Financial Model'!$S$57</f>
         <v>0</v>
       </c>
-      <c r="AE11" s="53">
+      <c r="AG11" s="53">
         <f>'[9]Financial Model'!$S$71</f>
         <v>0.20639304436772793</v>
       </c>
-      <c r="AF11" s="53" t="str">
+      <c r="AH11" s="53" t="str">
         <f>'[6]Financial Model'!$Y$24</f>
         <v>-</v>
       </c>
-      <c r="AG11" s="4">
+      <c r="AI11" s="4">
         <f>[9]Main!$C$24</f>
         <v>2000</v>
       </c>
-      <c r="AH11" s="85" t="str">
+      <c r="AJ11" s="85" t="str">
         <f>[9]Main!$C$23</f>
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -8772,80 +8815,82 @@
         <f>[10]Main!$C$38</f>
         <v>2.420425719782521</v>
       </c>
-      <c r="N12" s="56">
+      <c r="N12" s="50"/>
+      <c r="O12" s="56">
         <f>'[10]Financial Model'!$X$18*E28</f>
         <v>244.59929999999974</v>
       </c>
-      <c r="O12" s="56">
+      <c r="P12" s="56">
         <f>'[10]Financial Model'!$W$18*$E$28</f>
         <v>-106.03953000000016</v>
       </c>
-      <c r="P12" s="56">
+      <c r="Q12" s="56">
         <f>'[10]Financial Model'!$V$18*$E$28</f>
         <v>36.602940000000572</v>
       </c>
-      <c r="Q12" s="52">
+      <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
         <v>-50.21450968486225</v>
       </c>
-      <c r="R12" s="52">
+      <c r="S12" s="52">
         <f>[10]Main!$C$37</f>
         <v>3.5983436371240685</v>
       </c>
-      <c r="S12" s="52">
+      <c r="T12" s="52">
         <f>[10]Main!$C$35</f>
         <v>1.1733497350330941</v>
       </c>
-      <c r="T12" s="53">
+      <c r="U12" s="53"/>
+      <c r="V12" s="53">
         <f>'[10]Financial Model'!$X$22</f>
         <v>0.18793978595910144</v>
       </c>
-      <c r="U12" s="53">
+      <c r="W12" s="53">
         <f>'[10]Financial Model'!$W$22</f>
         <v>-0.137366539399013</v>
       </c>
-      <c r="V12" s="53">
+      <c r="X12" s="53">
         <f>'[10]Financial Model'!$V$22</f>
         <v>0</v>
       </c>
-      <c r="W12" s="53">
+      <c r="Y12" s="53">
         <f>'[10]Financial Model'!$O$27</f>
         <v>0.55310902822720542</v>
       </c>
-      <c r="X12" s="53">
+      <c r="Z12" s="53">
         <f>'[10]Financial Model'!$O$28</f>
         <v>-1.1966602769322474E-2</v>
       </c>
-      <c r="Y12" s="53">
+      <c r="AA12" s="53">
         <f>'[10]Financial Model'!$O$30</f>
         <v>-2.0263004421958795E-2</v>
       </c>
-      <c r="Z12" s="53">
+      <c r="AB12" s="53">
         <f>'[10]Financial Model'!$O$31</f>
         <v>0.12839781600422653</v>
       </c>
-      <c r="AB12" s="56">
+      <c r="AD12" s="56">
         <f>'[10]Financial Model'!$O$41*E28</f>
         <v>523.13430000000005</v>
       </c>
-      <c r="AC12" s="53">
+      <c r="AE12" s="53">
         <f>'[10]Financial Model'!$X$69</f>
         <v>-0.25498478543021663</v>
       </c>
-      <c r="AF12" s="57">
+      <c r="AH12" s="57">
         <f>[10]Main!$C$25</f>
         <v>728</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AI12" s="4">
         <f>[10]Main!$C$24</f>
         <v>1892</v>
       </c>
-      <c r="AH12" s="4" t="str">
+      <c r="AJ12" s="4" t="str">
         <f>[10]Main!$C$23</f>
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -8886,80 +8931,81 @@
         <v>44832</v>
       </c>
       <c r="L13" s="56"/>
-      <c r="N13" s="55">
+      <c r="O13" s="55">
         <f>'[11]Financial Model'!$T$14</f>
         <v>-4.0000000000000462</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <f>'[11]Financial Model'!$S$14</f>
         <v>93.39999999999992</v>
       </c>
-      <c r="P13" s="55">
+      <c r="Q13" s="55">
         <f>'[11]Financial Model'!$R$14</f>
         <v>72.882999999999953</v>
       </c>
-      <c r="S13" s="52">
+      <c r="T13" s="52">
         <f>[11]Main!$C$35</f>
         <v>1.1237883419689116</v>
       </c>
-      <c r="T13" s="53">
+      <c r="U13" s="53"/>
+      <c r="V13" s="53">
         <f>'[11]Financial Model'!$T$18</f>
         <v>0.13607975706182329</v>
       </c>
-      <c r="U13" s="53">
+      <c r="W13" s="53">
         <f>'[11]Financial Model'!$S$18</f>
         <v>0.4133402867980267</v>
       </c>
-      <c r="V13" s="53">
+      <c r="X13" s="53">
         <f>'[11]Financial Model'!$R$18</f>
         <v>0.44106334313588214</v>
       </c>
-      <c r="W13" s="53">
+      <c r="Y13" s="53">
         <f>'[11]Financial Model'!$M$21</f>
         <v>0.52527198549410703</v>
       </c>
-      <c r="X13" s="53">
+      <c r="Z13" s="53">
         <f>'[11]Financial Model'!$M$22</f>
         <v>-1.3372620126926577E-2</v>
       </c>
-      <c r="Y13" s="53">
+      <c r="AA13" s="53">
         <f>'[11]Financial Model'!$M$23</f>
         <v>-1.6659111514052596E-2</v>
       </c>
-      <c r="Z13" s="53">
+      <c r="AB13" s="53">
         <f>'[11]Financial Model'!$M$24</f>
         <v>3.2894736842105241E-2</v>
       </c>
-      <c r="AB13" s="56">
+      <c r="AD13" s="56">
         <f>[11]Main!$C$25</f>
         <v>269.7</v>
       </c>
-      <c r="AC13" s="53">
+      <c r="AE13" s="53">
         <f>'[11]Financial Model'!$M$60</f>
         <v>5.6818181818181879E-2</v>
       </c>
-      <c r="AD13" s="53">
+      <c r="AF13" s="53">
         <f>'[11]Financial Model'!$M$61</f>
         <v>-3.4717251252684322E-2</v>
       </c>
-      <c r="AE13" s="53">
+      <c r="AG13" s="53">
         <f>'[11]Financial Model'!$M$75</f>
         <v>0.30564369900271987</v>
       </c>
-      <c r="AF13" s="53" t="str">
+      <c r="AH13" s="53" t="str">
         <f>'[6]Financial Model'!$Y$24</f>
         <v>-</v>
       </c>
-      <c r="AG13" s="4">
+      <c r="AI13" s="4">
         <f>[11]Main!$C$24</f>
         <v>2006</v>
       </c>
-      <c r="AH13" s="4" t="str">
+      <c r="AJ13" s="4" t="str">
         <f>[11]Main!$C$23</f>
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>391</v>
       </c>
@@ -8992,55 +9038,56 @@
         <f>[12]Main!$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="53">
+      <c r="Q14" s="4"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53">
         <f>'[12]Financial Model'!$T$23</f>
         <v>0.20588400900900905</v>
       </c>
-      <c r="V14" s="4"/>
-      <c r="W14" s="53">
+      <c r="X14" s="4"/>
+      <c r="Y14" s="53">
         <f>'[12]Financial Model'!$T$26</f>
         <v>0.55486890948567691</v>
       </c>
-      <c r="X14" s="53">
+      <c r="Z14" s="53">
         <f>'[12]Financial Model'!$T$27</f>
         <v>-8.0487007680993719E-2</v>
       </c>
-      <c r="Y14" s="53">
+      <c r="AA14" s="53">
         <f>'[12]Financial Model'!$T$28</f>
         <v>-8.2866014521513875E-2</v>
       </c>
-      <c r="Z14" s="53">
+      <c r="AB14" s="53">
         <f>'[12]Financial Model'!$T$29</f>
         <v>0.19258416742493159</v>
       </c>
-      <c r="AB14" s="56">
+      <c r="AD14" s="56">
         <f>[12]Main!$C$26</f>
         <v>103.071</v>
       </c>
-      <c r="AC14" s="53">
+      <c r="AE14" s="53">
         <f>'[12]Financial Model'!$T$74</f>
         <v>0.17328795191694746</v>
       </c>
-      <c r="AE14" s="53">
+      <c r="AG14" s="53">
         <f>'[12]Financial Model'!$T$76</f>
         <v>0.24063455746737328</v>
       </c>
-      <c r="AF14" s="4">
+      <c r="AH14" s="4">
         <f>[12]Main!$C$25</f>
         <v>85</v>
       </c>
-      <c r="AG14" s="4">
+      <c r="AI14" s="4">
         <f>[12]Main!$C$24</f>
         <v>1987</v>
       </c>
-      <c r="AH14" s="4" t="str">
+      <c r="AJ14" s="4" t="str">
         <f>[12]Main!$C$23</f>
         <v>London, UK</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9055,125 +9102,142 @@
       </c>
       <c r="F15" s="7">
         <f>[13]Main!$C$6</f>
-        <v>1.022</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G15" s="49">
         <f>[13]Main!$C$8</f>
-        <v>83.94708</v>
+        <v>92.523351359999978</v>
       </c>
       <c r="H15" s="49">
         <f>[13]Main!$C$11</f>
-        <v>-2.1999999999999957</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I15" s="49">
         <f>[13]Main!$C$12</f>
-        <v>86.147079999999988</v>
+        <v>84.223351359999981</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>[13]Main!$C$29</f>
-        <v>H122</v>
+        <v>FY22</v>
+      </c>
+      <c r="K15" s="90">
+        <f>[13]Main!$D$29</f>
+        <v>44841</v>
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>34.458832000000143</v>
+        <v>3.7102797955947073</v>
       </c>
       <c r="N15" s="1">
+        <f xml:space="preserve"> '[13]Financial Model'!$T$17</f>
+        <v>22.700000000000035</v>
+      </c>
+      <c r="O15" s="1">
         <f>'[13]Financial Model'!$S$17</f>
         <v>-36.099999999999973</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <f>'[13]Financial Model'!$R$17</f>
         <v>-143.40000000000003</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <f>'[13]Financial Model'!$Q$17</f>
         <v>-98.499999999999972</v>
       </c>
-      <c r="Q15" s="51">
+      <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>-4.6059933708871261</v>
-      </c>
-      <c r="R15" s="51">
+        <v>4.0759185621145306</v>
+      </c>
+      <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
-        <v>-2.3222384525207773</v>
-      </c>
-      <c r="S15" s="51">
+        <v>-2.5676413418282564</v>
+      </c>
+      <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>0.91152134454347877</v>
-      </c>
-      <c r="T15" s="53">
+        <v>0.89050386294513961</v>
+      </c>
+      <c r="U15" s="53">
+        <f xml:space="preserve"> '[13]Financial Model'!$T$21</f>
+        <v>9.6205718395971918E-2</v>
+      </c>
+      <c r="V15" s="53">
         <f>'[13]Financial Model'!$S$21</f>
         <v>-0.21053378762066999</v>
       </c>
-      <c r="U15" s="53">
+      <c r="W15" s="53">
         <f>'[13]Financial Model'!$R$21</f>
         <v>-0.19192382700470356</v>
       </c>
-      <c r="V15" s="53">
+      <c r="X15" s="53">
         <f>'[13]Financial Model'!$Q$21</f>
         <v>-3.4403669724769603E-4</v>
       </c>
-      <c r="W15" s="53">
+      <c r="Y15" s="53">
         <f>'[13]Financial Model'!$J$33</f>
         <v>0.5523088023088023</v>
       </c>
-      <c r="X15" s="53">
-        <f>'[13]Financial Model'!$J$34</f>
-        <v>2.7056277056277018E-2</v>
-      </c>
-      <c r="Y15" s="53">
-        <f>'[13]Financial Model'!$J$35</f>
-        <v>9.0187590187589799E-3</v>
-      </c>
       <c r="Z15" s="53">
-        <f>'[13]Financial Model'!$J$36</f>
-        <v>0.375000000000001</v>
-      </c>
-      <c r="AB15" s="56">
+        <f>'[13]Financial Model'!T34</f>
+        <v>4.2486876640420002E-2</v>
+      </c>
+      <c r="AA15" s="53">
+        <f>'[13]Financial Model'!T35</f>
+        <v>3.7237532808399004E-2</v>
+      </c>
+      <c r="AB15" s="53">
+        <f>'[13]Financial Model'!T36</f>
+        <v>-0.26815642458100508</v>
+      </c>
+      <c r="AD15" s="56">
         <f>[13]Main!$C$27</f>
-        <v>159.4</v>
-      </c>
-      <c r="AC15" s="53">
-        <f>'[13]Financial Model'!$J$79</f>
-        <v>-4.2642642642642614E-2</v>
-      </c>
-      <c r="AF15" s="57">
+        <v>132.69999999999999</v>
+      </c>
+      <c r="AE15" s="53">
+        <f>'[13]Financial Model'!T79</f>
+        <v>-0.10519217801753222</v>
+      </c>
+      <c r="AG15" s="53">
+        <f>'[13]Financial Model'!$T$82</f>
+        <v>0.2176837270341207</v>
+      </c>
+      <c r="AH15" s="57">
         <f>[13]Main!$C$26</f>
-        <v>226</v>
-      </c>
-      <c r="AG15" s="4">
+        <v>220</v>
+      </c>
+      <c r="AI15" s="4">
         <f>[13]Main!$C$25</f>
         <v>1985</v>
       </c>
-      <c r="AH15" s="4" t="str">
+      <c r="AJ15" s="4" t="str">
         <f>[13]Main!$C$24</f>
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="F16" s="7"/>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
       <c r="L16" s="50"/>
-      <c r="Q16" s="51"/>
       <c r="R16" s="51"/>
       <c r="S16" s="51"/>
-      <c r="T16" s="53"/>
-      <c r="U16" s="53"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
       <c r="V16" s="53"/>
       <c r="W16" s="53"/>
       <c r="X16" s="53"/>
       <c r="Y16" s="53"/>
       <c r="Z16" s="53"/>
-      <c r="AB16" s="55"/>
-      <c r="AC16" s="53"/>
-      <c r="AF16" s="57"/>
-      <c r="AG16" s="4"/>
-      <c r="AH16" s="4"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="AA16" s="53"/>
+      <c r="AB16" s="53"/>
+      <c r="AD16" s="55"/>
+      <c r="AE16" s="53"/>
+      <c r="AH16" s="57"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -9188,8 +9252,9 @@
       <c r="I17" s="49"/>
       <c r="L17" s="56"/>
       <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
@@ -9206,8 +9271,9 @@
       <c r="K18" s="1"/>
       <c r="L18" s="56"/>
       <c r="M18" s="56"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="56"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>445</v>
       </c>
@@ -9224,8 +9290,9 @@
       <c r="K19" s="1"/>
       <c r="L19" s="56"/>
       <c r="M19" s="56"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9242,8 +9309,9 @@
       <c r="K20" s="1"/>
       <c r="L20" s="56"/>
       <c r="M20" s="56"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="56"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9251,8 +9319,9 @@
       <c r="K21" s="1"/>
       <c r="L21" s="56"/>
       <c r="M21" s="56"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="56"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>492</v>
       </c>
@@ -9272,8 +9341,9 @@
       <c r="K22" s="1"/>
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="56"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>511</v>
       </c>
@@ -9293,26 +9363,30 @@
       <c r="K23" s="1"/>
       <c r="L23" s="56"/>
       <c r="M23" s="56"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="56"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="56"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="M25" s="56"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="56"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="56"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="56"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D27" s="87" t="s">
         <v>495</v>
       </c>
@@ -9324,7 +9398,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D28" s="43" t="s">
         <v>497</v>
       </c>
@@ -9339,7 +9413,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D29" s="46" t="s">
         <v>498</v>
       </c>
@@ -9357,7 +9431,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F1:AC1"/>
+    <mergeCell ref="F1:AE1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{B8F2A7D5-5402-48EE-B9EB-3A9CE47578C7}"/>
@@ -9377,7 +9451,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId14"/>
   <ignoredErrors>
-    <ignoredError sqref="AF12 G12" formula="1"/>
+    <ignoredError sqref="AH12 G12" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small updates to £SDRY model & fashion retailers overview
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC14D2A-2808-4354-B5D6-DC47CE2CAD38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA5C2A8-46C6-4BA6-B818-CC334E4EBA12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="32295" windowHeight="18855" firstSheet="1" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -2194,6 +2194,9 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2201,9 +2204,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2843,6 +2843,11 @@
         <row r="79">
           <cell r="T79">
             <v>-0.10519217801753222</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="K80">
+            <v>-0.16750313676286088</v>
           </cell>
         </row>
         <row r="82">
@@ -7763,7 +7768,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
+      <selection pane="bottomRight" activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7787,34 +7792,34 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="90" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -9120,7 +9125,7 @@
         <f>[13]Main!$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="K15" s="90">
+      <c r="K15" s="87">
         <f>[13]Main!$D$29</f>
         <v>44841</v>
       </c>
@@ -9195,6 +9200,10 @@
       <c r="AE15" s="53">
         <f>'[13]Financial Model'!T79</f>
         <v>-0.10519217801753222</v>
+      </c>
+      <c r="AF15" s="53">
+        <f>'[13]Financial Model'!$K$80</f>
+        <v>-0.16750313676286088</v>
       </c>
       <c r="AG15" s="53">
         <f>'[13]Financial Model'!$T$82</f>
@@ -9387,10 +9396,10 @@
       <c r="N26" s="56"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="88" t="s">
         <v>495</v>
       </c>
-      <c r="E27" s="88"/>
+      <c r="E27" s="89"/>
       <c r="F27" s="42" t="s">
         <v>496</v>
       </c>

</xml_diff>

<commit_message>
Update £ASC in Overview, Add some averages to header for comparison, cleanup
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27463E2-3553-F549-A208-3A90F8FA5F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA651E6C-7F39-4A7B-8F89-888E4D99DA3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32300" windowHeight="18860" firstSheet="1" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="32295" windowHeight="18855" firstSheet="1" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -37,22 +37,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="538">
   <si>
     <t>Ticker</t>
   </si>
@@ -1663,6 +1653,9 @@
   </si>
   <si>
     <t>Released</t>
+  </si>
+  <si>
+    <t>(GBP)</t>
   </si>
 </sst>
 </file>
@@ -1670,13 +1663,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1762,7 +1755,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1826,6 +1819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1962,7 +1961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2054,7 +2053,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2063,13 +2062,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2098,16 +2097,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2116,12 +2115,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2159,7 +2158,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2177,7 +2176,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2198,7 +2197,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2212,6 +2211,16 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2863,8 +2872,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2876,17 +2885,18 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Price History"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>35.78</v>
+            <v>27.84</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>13914.901645259999</v>
+            <v>10827.02240928</v>
           </cell>
         </row>
         <row r="11">
@@ -2896,7 +2906,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>18683.801645259999</v>
+            <v>15595.92240928</v>
           </cell>
         </row>
         <row r="23">
@@ -2926,17 +2936,17 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>13.471618843205112</v>
+            <v>11.245159106006854</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>10.068932086717085</v>
+            <v>7.8345184263332488</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>4.1363260534772177</v>
+            <v>3.2184269795641627</v>
           </cell>
         </row>
       </sheetData>
@@ -2983,6 +2993,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3391,8 +3402,8 @@
           </cell>
         </row>
         <row r="24">
-          <cell r="Y24" t="str">
-            <v>-</v>
+          <cell r="Y24">
+            <v>1.4239238540510346E-2</v>
           </cell>
           <cell r="Z24">
             <v>-0.15045474463142361</v>
@@ -3596,22 +3607,22 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>6.01</v>
+            <v>5.1749999999999998</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>600.63939999999991</v>
+            <v>515.92694489999997</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-15.399999999999977</v>
+            <v>-117.10000000000002</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>616.03939999999989</v>
+            <v>633.02694489999999</v>
           </cell>
         </row>
         <row r="23">
@@ -3626,66 +3637,95 @@
         </row>
         <row r="26">
           <cell r="C26">
-            <v>986.4</v>
+            <v>1078.4000000000001</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28" t="str">
-            <v>H122</v>
+            <v>FY22</v>
+          </cell>
+          <cell r="D28">
+            <v>44853</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>0.52410295093457915</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>0.57205092846638639</v>
+            <v>-16.750874834415534</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="C41">
+            <v>4.0138826705607427</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="13">
-          <cell r="Q13">
-            <v>24.599999999999909</v>
-          </cell>
-          <cell r="R13">
-            <v>113.30000000000014</v>
-          </cell>
-          <cell r="S13">
-            <v>128.40000000000015</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="Q17">
+        <row r="4">
+          <cell r="Q4">
+            <v>2733.5</v>
+          </cell>
+          <cell r="R4">
+            <v>3263.5</v>
+          </cell>
+          <cell r="S4">
+            <v>3910.5</v>
+          </cell>
+          <cell r="T4">
+            <v>3936.5</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="Q19">
             <v>0.13080709882927222</v>
           </cell>
-          <cell r="R17">
+          <cell r="R19">
             <v>0.19389061642582761</v>
           </cell>
-          <cell r="S17">
+          <cell r="S19">
             <v>0.19825340891680709</v>
           </cell>
-        </row>
-        <row r="20">
-          <cell r="K20">
-            <v>0.43071703008831885</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="K21">
-            <v>-2.1954992265856019E-3</v>
+          <cell r="T19">
+            <v>6.6487661424370348E-3</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="K22">
-            <v>-6.7361908088419773E-3</v>
+          <cell r="T22">
+            <v>0.43630128286548964</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="K23">
-            <v>0.14556962025316267</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="S71">
-            <v>0.20639304436772793</v>
+          <cell r="T23">
+            <v>-2.4895211482281444E-3</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="T24">
+            <v>-7.8242093230026909E-3</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="T25">
+            <v>3.4482758620689558E-2</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="T60">
+            <v>0.33614174203940039</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="L61">
+            <v>9.3268450932684654E-2</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="T76">
+            <v>0.27394893941318432</v>
           </cell>
         </row>
       </sheetData>
@@ -4001,25 +4041,25 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4061,7 +4101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>241</v>
       </c>
@@ -4105,7 +4145,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4149,7 +4189,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4193,7 +4233,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>259</v>
       </c>
@@ -4237,7 +4277,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4281,7 +4321,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4325,7 +4365,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4369,7 +4409,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4413,7 +4453,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4457,7 +4497,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4501,7 +4541,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>301</v>
       </c>
@@ -4545,7 +4585,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -4589,7 +4629,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>312</v>
       </c>
@@ -4633,7 +4673,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -4677,7 +4717,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -4721,7 +4761,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -4765,7 +4805,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -4809,7 +4849,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -4853,7 +4893,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -4897,7 +4937,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -4941,7 +4981,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -4985,7 +5025,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5029,7 +5069,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5073,7 +5113,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5117,7 +5157,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5161,7 +5201,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5205,7 +5245,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="61" t="s">
         <v>391</v>
       </c>
@@ -5249,7 +5289,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5293,7 +5333,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5337,7 +5377,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>10</v>
       </c>
@@ -5381,7 +5421,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5425,7 +5465,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5469,7 +5509,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5513,7 +5553,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -5557,7 +5597,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -5601,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -5645,7 +5685,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>445</v>
       </c>
@@ -5689,7 +5729,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -5733,7 +5773,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -5777,7 +5817,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -5821,7 +5861,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -5865,7 +5905,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -5909,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6027,25 +6067,25 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6087,7 +6127,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6131,7 +6171,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6175,7 +6215,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6219,7 +6259,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6263,7 +6303,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>56</v>
       </c>
@@ -6307,7 +6347,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6351,7 +6391,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6395,7 +6435,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6439,7 +6479,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6483,7 +6523,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73" t="s">
         <v>86</v>
       </c>
@@ -6527,7 +6567,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
@@ -6571,7 +6611,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -6615,7 +6655,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -6659,7 +6699,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -6703,7 +6743,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -6747,7 +6787,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>121</v>
       </c>
@@ -6791,7 +6831,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -6835,7 +6875,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -6879,7 +6919,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -6923,7 +6963,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -6967,7 +7007,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7011,7 +7051,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7055,7 +7095,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7099,7 +7139,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7143,7 +7183,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7187,7 +7227,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7231,7 +7271,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7275,7 +7315,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7319,7 +7359,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7363,7 +7403,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7407,7 +7447,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7451,7 +7491,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7495,7 +7535,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -7539,7 +7579,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -7583,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -7627,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -7671,7 +7711,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -7780,29 +7820,29 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q35" sqref="Q35"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="23" width="9.1640625" style="4"/>
-    <col min="24" max="29" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="23" width="9.140625" style="4"/>
+    <col min="24" max="29" width="9.140625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.1640625" style="4"/>
-    <col min="34" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1640625" style="1"/>
+    <col min="31" max="33" width="9.140625" style="4"/>
+    <col min="34" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="89" t="s">
         <v>499</v>
@@ -7818,22 +7858,47 @@
       <c r="O1" s="89"/>
       <c r="P1" s="89"/>
       <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-    </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="92">
+        <f>AVERAGE(Y3:Y15)</f>
+        <v>0.48684562094335121</v>
+      </c>
+      <c r="Z1" s="92">
+        <f>AVERAGE(Z3:Z15)</f>
+        <v>4.926848653784497E-2</v>
+      </c>
+      <c r="AA1" s="92">
+        <f>AVERAGE(AA3:AA15)</f>
+        <v>3.3967961295369026E-2</v>
+      </c>
+      <c r="AB1" s="92">
+        <f>AVERAGE(AB3:AB15)</f>
+        <v>0.14615541162428036</v>
+      </c>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="93" t="s">
+        <v>537</v>
+      </c>
+      <c r="AE1" s="92">
+        <f>AVERAGE(AE3:AE15)</f>
+        <v>0.23199575663598668</v>
+      </c>
+      <c r="AF1" s="92">
+        <f>AVERAGE(AF3:AF15)</f>
+        <v>3.9231986955234513E-2</v>
+      </c>
+      <c r="AG1" s="92">
+        <f>AVERAGE(AG3:AG15)</f>
+        <v>0.22763826675517687</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -7938,7 +8003,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -7953,19 +8018,19 @@
       </c>
       <c r="F3" s="7">
         <f>[1]Main!$C$6*$E$28</f>
-        <v>88.656900000000007</v>
+        <v>84.843699999999998</v>
       </c>
       <c r="G3" s="49">
         <f>[1]Main!$C$8*$E$28</f>
-        <v>138934.22798999998</v>
+        <v>132958.56226999999</v>
       </c>
       <c r="H3" s="49">
         <f>[1]Main!$C$11*$E$28</f>
-        <v>2273.85</v>
+        <v>2176.0500000000002</v>
       </c>
       <c r="I3" s="49">
         <f>[1]Main!$C$12*$E$28</f>
-        <v>136660.37798999998</v>
+        <v>130782.51226999999</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>[1]Main!$C$28</f>
@@ -7981,15 +8046,15 @@
       </c>
       <c r="O3" s="56">
         <f>'[1]Financial Model'!$AD$21*1000*E28</f>
-        <v>5622.7799999999934</v>
+        <v>5380.9399999999932</v>
       </c>
       <c r="P3" s="56">
         <f>'[1]Financial Model'!$AC$21*1000*E28</f>
-        <v>5326.1099999999988</v>
+        <v>5097.0299999999988</v>
       </c>
       <c r="Q3" s="56">
         <f>'[1]Financial Model'!$AB$21*1000*E28</f>
-        <v>2361.27</v>
+        <v>2259.71</v>
       </c>
       <c r="R3" s="51">
         <f>[1]Main!$C$34</f>
@@ -8034,7 +8099,7 @@
       </c>
       <c r="AD3" s="56">
         <f>[1]Main!$C$26*E28</f>
-        <v>8985.66</v>
+        <v>8599.18</v>
       </c>
       <c r="AE3" s="53">
         <f>'[1]Financial Model'!$W$72</f>
@@ -8057,7 +8122,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8072,19 +8137,19 @@
       </c>
       <c r="F4" s="7">
         <f>[2]Main!$C$6*$E$28</f>
-        <v>33.275400000000005</v>
+        <v>24.7776</v>
       </c>
       <c r="G4" s="49">
         <f>[2]Main!$C$8*$E$28</f>
-        <v>12940.8585300918</v>
+        <v>9636.0499442592009</v>
       </c>
       <c r="H4" s="49">
         <f>[2]Main!$C$11*$E$28</f>
-        <v>-4435.0770000000002</v>
+        <v>-4244.3209999999999</v>
       </c>
       <c r="I4" s="49">
         <f>[2]Main!$C$12*$E$28</f>
-        <v>17375.9355300918</v>
+        <v>13880.370944259199</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>[2]Main!$C$28</f>
@@ -8092,27 +8157,27 @@
       </c>
       <c r="L4" s="50">
         <f>[2]Main!$C$33</f>
-        <v>13.471618843205112</v>
+        <v>11.245159106006854</v>
       </c>
       <c r="O4" s="56">
         <f>'[2]Financial Model'!$AA$22*E28</f>
-        <v>1289.817929999999</v>
+        <v>1234.341889999999</v>
       </c>
       <c r="P4" s="56">
         <f>'[2]Financial Model'!$Z$22*$E$28</f>
-        <v>379.29957000000132</v>
+        <v>362.98561000000126</v>
       </c>
       <c r="Q4" s="56">
         <f>'[2]Financial Model'!$Y$22*$E$28</f>
-        <v>631.88757000000021</v>
+        <v>604.70961000000023</v>
       </c>
       <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
-        <v>10.068932086717085</v>
+        <v>7.8345184263332488</v>
       </c>
       <c r="T4" s="51">
         <f>[2]Main!$C$36</f>
-        <v>4.1363260534772177</v>
+        <v>3.2184269795641627</v>
       </c>
       <c r="U4" s="53"/>
       <c r="V4" s="53">
@@ -8138,7 +8203,7 @@
       </c>
       <c r="AD4" s="56">
         <f>[2]Main!$C$26*E28</f>
-        <v>2177.4973500000001</v>
+        <v>2083.8415500000001</v>
       </c>
       <c r="AE4" s="53">
         <f>'[2]Financial Model'!$T$76</f>
@@ -8157,7 +8222,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8272,7 +8337,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8391,7 +8456,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>526</v>
       </c>
@@ -8442,7 +8507,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8457,19 +8522,19 @@
       </c>
       <c r="F8" s="7">
         <f>[6]Main!$C$6*E28</f>
-        <v>6.2217000000000011</v>
+        <v>5.9541000000000004</v>
       </c>
       <c r="G8" s="49">
         <f>[6]Main!$C$8*E28</f>
-        <v>2852.0272800000002</v>
+        <v>2729.3594400000002</v>
       </c>
       <c r="H8" s="49">
         <f>[6]Main!$C$11*$E$28</f>
-        <v>350.21847000000008</v>
+        <v>335.15531000000004</v>
       </c>
       <c r="I8" s="49">
         <f>[6]Main!$C$12*$E$28</f>
-        <v>2501.80881</v>
+        <v>2394.2041299999996</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
@@ -8481,15 +8546,15 @@
       </c>
       <c r="O8" s="56">
         <f>'[6]Financial Model'!$AA$20*$E$28</f>
-        <v>334.85580000000039</v>
+        <v>320.45340000000039</v>
       </c>
       <c r="P8" s="56">
         <f>'[6]Financial Model'!$Z$20*$E$28</f>
-        <v>-510.73461000000003</v>
+        <v>-488.76753000000002</v>
       </c>
       <c r="Q8" s="56">
         <f>'[6]Financial Model'!$Y$20*$E$28</f>
-        <v>85.692059999999287</v>
+        <v>82.006379999999311</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
@@ -8512,9 +8577,9 @@
         <f>'[6]Financial Model'!$Z$24</f>
         <v>-0.15045474463142361</v>
       </c>
-      <c r="X8" s="53" t="str">
+      <c r="X8" s="53">
         <f>'[6]Financial Model'!$Y$24</f>
-        <v>-</v>
+        <v>1.4239238540510346E-2</v>
       </c>
       <c r="Y8" s="53">
         <f>'[6]Financial Model'!$Q$30</f>
@@ -8534,7 +8599,7 @@
       </c>
       <c r="AD8" s="56">
         <f>[6]Main!$C$27*E28</f>
-        <v>887.58642000000009</v>
+        <v>849.41066000000001</v>
       </c>
       <c r="AE8" s="53">
         <f>'[6]Financial Model'!$AA$79</f>
@@ -8561,7 +8626,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8576,15 +8641,15 @@
       </c>
       <c r="F9" s="7">
         <f>[7]Main!$C$6*E28</f>
-        <v>19.53</v>
+        <v>18.690000000000001</v>
       </c>
       <c r="G9" s="49">
         <f>[7]Main!$C$8*$E$28</f>
-        <v>1809.6497999999999</v>
+        <v>1731.8154</v>
       </c>
       <c r="H9" s="49"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="56"/>
+      <c r="J9" s="59"/>
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
       <c r="M9" s="56"/>
@@ -8592,7 +8657,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8607,19 +8672,19 @@
       </c>
       <c r="F10" s="7">
         <f>[8]Main!$C$6*E28</f>
-        <v>9.523200000000001</v>
+        <v>9.1135999999999999</v>
       </c>
       <c r="G10" s="49">
         <f>[8]Main!$C$8*E28</f>
-        <v>1604.2782720000002</v>
+        <v>1535.2770560000001</v>
       </c>
       <c r="H10" s="49">
         <f>[8]Main!$C$11*$E$28</f>
-        <v>-164.61</v>
+        <v>-157.53</v>
       </c>
       <c r="I10" s="49">
         <f>[8]Main!$C$12*$E$28</f>
-        <v>1768.8882720000001</v>
+        <v>1692.8070560000001</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>[8]Main!$C$28</f>
@@ -8631,11 +8696,11 @@
       </c>
       <c r="O10" s="56">
         <f>'[8]Financial Model'!$Z$16*E28</f>
-        <v>390.2521799999999</v>
+        <v>373.46713999999986</v>
       </c>
       <c r="P10" s="56">
         <f>'[8]Financial Model'!$Y$16*F28</f>
-        <v>-225.093548387097</v>
+        <v>-235.21011235955083</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="52">
@@ -8670,7 +8735,7 @@
       </c>
       <c r="AD10" s="56">
         <f>[8]Main!$C$26*E28</f>
-        <v>634.35300000000007</v>
+        <v>607.06900000000007</v>
       </c>
       <c r="AE10" s="53">
         <f>'[8]Financial Model'!$O$71</f>
@@ -8689,7 +8754,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -8704,86 +8769,107 @@
       </c>
       <c r="F11" s="6">
         <f>[9]Main!$C$6</f>
-        <v>6.01</v>
+        <v>5.1749999999999998</v>
       </c>
       <c r="G11" s="49">
         <f>[9]Main!$C$8</f>
-        <v>600.63939999999991</v>
+        <v>515.92694489999997</v>
       </c>
       <c r="H11" s="49">
         <f>[9]Main!$C$11</f>
-        <v>-15.399999999999977</v>
+        <v>-117.10000000000002</v>
       </c>
       <c r="I11" s="49">
         <f>[9]Main!$C$12</f>
-        <v>616.03939999999989</v>
+        <v>633.02694489999999</v>
       </c>
       <c r="J11" s="85" t="str">
         <f>[9]Main!$C$28</f>
-        <v>H122</v>
-      </c>
-      <c r="K11" s="85"/>
+        <v>FY22</v>
+      </c>
+      <c r="K11" s="86">
+        <f>[9]Main!$D$28</f>
+        <v>44853</v>
+      </c>
       <c r="L11" s="56"/>
-      <c r="O11" s="1">
-        <f>'[9]Financial Model'!$S$13</f>
-        <v>128.40000000000015</v>
-      </c>
-      <c r="P11" s="1">
-        <f>'[9]Financial Model'!$R$13</f>
-        <v>113.30000000000014</v>
-      </c>
-      <c r="Q11" s="1">
-        <f>'[9]Financial Model'!$Q$13</f>
-        <v>24.599999999999909</v>
+      <c r="N11" s="56">
+        <f>'[9]Financial Model'!$T$4</f>
+        <v>3936.5</v>
+      </c>
+      <c r="O11" s="56">
+        <f>'[9]Financial Model'!$S$4</f>
+        <v>3910.5</v>
+      </c>
+      <c r="P11" s="56">
+        <f>'[9]Financial Model'!$R$4</f>
+        <v>3263.5</v>
+      </c>
+      <c r="Q11" s="56">
+        <f>'[9]Financial Model'!$Q$4</f>
+        <v>2733.5</v>
+      </c>
+      <c r="R11" s="52">
+        <f>[9]Main!$C$36</f>
+        <v>-16.750874834415534</v>
+      </c>
+      <c r="S11" s="52">
+        <f>[9]Main!$C$41</f>
+        <v>4.0138826705607427</v>
       </c>
       <c r="T11" s="52">
-        <f>[9]Main!$C$36</f>
-        <v>0.57205092846638639</v>
-      </c>
-      <c r="U11" s="53"/>
-      <c r="V11" s="53">
-        <f>'[9]Financial Model'!$S$17</f>
+        <f>[9]Main!$C$33</f>
+        <v>0.52410295093457915</v>
+      </c>
+      <c r="U11" s="90">
+        <f>'[9]Financial Model'!$T$19</f>
+        <v>6.6487661424370348E-3</v>
+      </c>
+      <c r="V11" s="90">
+        <f>'[9]Financial Model'!$S$19</f>
         <v>0.19825340891680709</v>
       </c>
       <c r="W11" s="53">
-        <f>'[9]Financial Model'!$R$17</f>
+        <f>'[9]Financial Model'!$R$19</f>
         <v>0.19389061642582761</v>
       </c>
       <c r="X11" s="53">
-        <f>'[9]Financial Model'!$Q$17</f>
+        <f>'[9]Financial Model'!$Q$19</f>
         <v>0.13080709882927222</v>
       </c>
       <c r="Y11" s="53">
-        <f>'[9]Financial Model'!$K$20</f>
-        <v>0.43071703008831885</v>
+        <f>'[9]Financial Model'!$T$22</f>
+        <v>0.43630128286548964</v>
       </c>
       <c r="Z11" s="53">
-        <f>'[9]Financial Model'!$K$21</f>
-        <v>-2.1954992265856019E-3</v>
+        <f>'[9]Financial Model'!$T$23</f>
+        <v>-2.4895211482281444E-3</v>
       </c>
       <c r="AA11" s="53">
-        <f>'[9]Financial Model'!$K$22</f>
-        <v>-6.7361908088419773E-3</v>
+        <f>'[9]Financial Model'!$T$24</f>
+        <v>-7.8242093230026909E-3</v>
       </c>
       <c r="AB11" s="53">
-        <f>'[9]Financial Model'!$K$23</f>
-        <v>0.14556962025316267</v>
+        <f>'[9]Financial Model'!$T$25</f>
+        <v>3.4482758620689558E-2</v>
       </c>
       <c r="AD11" s="56">
         <f>[9]Main!$C$26</f>
-        <v>986.4</v>
+        <v>1078.4000000000001</v>
       </c>
       <c r="AE11" s="53">
-        <f>'[9]Financial Model'!$S$57</f>
+        <f>'[9]Financial Model'!$T$60</f>
+        <v>0.33614174203940039</v>
+      </c>
+      <c r="AF11" s="53">
+        <f>'[9]Financial Model'!$L$61</f>
+        <v>9.3268450932684654E-2</v>
+      </c>
+      <c r="AG11" s="53">
+        <f>'[9]Financial Model'!$T$76</f>
+        <v>0.27394893941318432</v>
+      </c>
+      <c r="AH11" s="57">
         <v>0</v>
-      </c>
-      <c r="AG11" s="53">
-        <f>'[9]Financial Model'!$S$71</f>
-        <v>0.20639304436772793</v>
-      </c>
-      <c r="AH11" s="53" t="str">
-        <f>'[6]Financial Model'!$Y$24</f>
-        <v>-</v>
       </c>
       <c r="AI11" s="4">
         <f>[9]Main!$C$24</f>
@@ -8794,7 +8880,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -8809,19 +8895,19 @@
       </c>
       <c r="F12" s="54">
         <f>[10]Main!$C$6*E28</f>
-        <v>14.768400000000002</v>
+        <v>14.1332</v>
       </c>
       <c r="G12" s="49">
         <f>[10]Main!$C$8*E28</f>
-        <v>745.0194367608002</v>
+        <v>712.97559001840011</v>
       </c>
       <c r="H12" s="49">
         <f>[10]Main!$C$11*E28</f>
-        <v>152.98500000000001</v>
+        <v>146.405</v>
       </c>
       <c r="I12" s="49">
         <f>[10]Main!$C$12*E28</f>
-        <v>592.03443676080019</v>
+        <v>566.57059001840014</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>[10]Main!$C$27</f>
@@ -8838,15 +8924,15 @@
       <c r="N12" s="50"/>
       <c r="O12" s="56">
         <f>'[10]Financial Model'!$X$18*E28</f>
-        <v>244.59929999999974</v>
+        <v>234.07889999999975</v>
       </c>
       <c r="P12" s="56">
         <f>'[10]Financial Model'!$W$18*$E$28</f>
-        <v>-106.03953000000016</v>
+        <v>-101.47869000000014</v>
       </c>
       <c r="Q12" s="56">
         <f>'[10]Financial Model'!$V$18*$E$28</f>
-        <v>36.602940000000572</v>
+        <v>35.028620000000551</v>
       </c>
       <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
@@ -8891,7 +8977,7 @@
       </c>
       <c r="AD12" s="56">
         <f>'[10]Financial Model'!$O$41*E28</f>
-        <v>523.13430000000005</v>
+        <v>500.63389999999998</v>
       </c>
       <c r="AE12" s="53">
         <f>'[10]Financial Model'!$X$69</f>
@@ -8910,7 +8996,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9012,9 +9098,9 @@
         <f>'[11]Financial Model'!$M$75</f>
         <v>0.30564369900271987</v>
       </c>
-      <c r="AH13" s="53" t="str">
+      <c r="AH13" s="53">
         <f>'[6]Financial Model'!$Y$24</f>
-        <v>-</v>
+        <v>1.4239238540510346E-2</v>
       </c>
       <c r="AI13" s="4">
         <f>[11]Main!$C$24</f>
@@ -9025,7 +9111,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>391</v>
       </c>
@@ -9107,7 +9193,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9237,7 +9323,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="F16" s="7"/>
       <c r="G16" s="49"/>
@@ -9261,7 +9347,7 @@
       <c r="AI16" s="4"/>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -9278,7 +9364,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
@@ -9297,7 +9383,7 @@
       <c r="M18" s="56"/>
       <c r="N18" s="56"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>445</v>
       </c>
@@ -9316,7 +9402,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9335,7 +9421,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9345,7 +9431,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>492</v>
       </c>
@@ -9367,7 +9453,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>511</v>
       </c>
@@ -9389,28 +9475,28 @@
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D27" s="87" t="s">
         <v>495</v>
       </c>
@@ -9422,31 +9508,31 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D28" s="43" t="s">
         <v>497</v>
       </c>
       <c r="E28" s="44">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="F28" s="45">
         <f>1/E28</f>
-        <v>1.075268817204301</v>
+        <v>1.1235955056179776</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D29" s="46" t="s">
         <v>498</v>
       </c>
       <c r="E29" s="48">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="F29" s="47">
         <f>1/E29</f>
-        <v>1.1235955056179776</v>
+        <v>1.1363636363636365</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
@@ -9455,7 +9541,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F1:AE1"/>
+    <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{B8F2A7D5-5402-48EE-B9EB-3A9CE47578C7}"/>

</xml_diff>

<commit_message>
Updating misc fashion models
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF71F06-B30C-4524-859C-E30733C6D265}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822D6924-0785-5348-8A44-5A350D5B0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="32295" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="9800" yWindow="500" windowWidth="22500" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -37,6 +37,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1663,13 +1673,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1961,7 +1971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2053,7 +2063,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2062,13 +2072,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2097,16 +2107,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2115,12 +2125,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2158,7 +2168,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2176,7 +2186,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2197,7 +2207,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2220,6 +2230,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2388,22 +2401,22 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>15.88</v>
+            <v>17.739999999999998</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>801.09616856000014</v>
+            <v>894.82333999999992</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>164.5</v>
+            <v>65.737000000000023</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>636.59616856000014</v>
+            <v>829.08633999999984</v>
           </cell>
         </row>
         <row r="23">
@@ -2418,37 +2431,40 @@
         </row>
         <row r="25">
           <cell r="C25">
-            <v>728</v>
+            <v>734</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27" t="str">
-            <v>Q122</v>
+            <v>Q222</v>
+          </cell>
+          <cell r="D27">
+            <v>44798</v>
           </cell>
         </row>
         <row r="32">
           <cell r="C32">
-            <v>-0.96423583702713767</v>
+            <v>-1.077175299046689</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>-50.21450968486225</v>
+            <v>-56.096058048454417</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>1.1733497350330941</v>
+            <v>1.3298883267742285</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>3.5983436371240685</v>
+            <v>4.0198120983993046</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>2.420425719782521</v>
+            <v>3.1522996844226485</v>
           </cell>
         </row>
       </sheetData>
@@ -2473,28 +2489,33 @@
           </cell>
         </row>
         <row r="27">
-          <cell r="O27">
-            <v>0.55310902822720542</v>
+          <cell r="P27">
+            <v>0.57868116771892864</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="O28">
-            <v>-1.1966602769322474E-2</v>
+          <cell r="P28">
+            <v>-2.721431490353244E-3</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="O30">
-            <v>-2.0263004421958795E-2</v>
+          <cell r="P30">
+            <v>-2.0909437566684987E-2</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="O31">
-            <v>0.12839781600422653</v>
+          <cell r="P31">
+            <v>-0.61857707509881543</v>
           </cell>
         </row>
         <row r="41">
-          <cell r="O41">
-            <v>562.51</v>
+          <cell r="P41">
+            <v>708.024</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="P67">
+            <v>0.25868695667632569</v>
           </cell>
         </row>
         <row r="69">
@@ -3610,12 +3631,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>5.1749999999999998</v>
+            <v>6.17</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>515.92694489999997</v>
+            <v>615.12449275999995</v>
           </cell>
         </row>
         <row r="11">
@@ -3625,7 +3646,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>633.02694489999999</v>
+            <v>732.22449275999998</v>
           </cell>
         </row>
         <row r="23">
@@ -3653,17 +3674,17 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>0.52410295093457915</v>
+            <v>0.62487250381958526</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>-16.750874834415534</v>
+            <v>-19.971574440259683</v>
           </cell>
         </row>
         <row r="41">
           <cell r="C41">
-            <v>4.0138826705607427</v>
+            <v>4.7856340246105864</v>
           </cell>
         </row>
       </sheetData>
@@ -3732,7 +3753,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4044,25 +4065,25 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4104,7 +4125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>241</v>
       </c>
@@ -4148,7 +4169,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4192,7 +4213,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4236,7 +4257,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>259</v>
       </c>
@@ -4280,7 +4301,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4324,7 +4345,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4368,7 +4389,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4412,7 +4433,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4456,7 +4477,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4500,7 +4521,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4544,7 +4565,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>301</v>
       </c>
@@ -4588,7 +4609,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -4632,7 +4653,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>312</v>
       </c>
@@ -4676,7 +4697,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -4720,7 +4741,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -4764,7 +4785,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -4808,7 +4829,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -4852,7 +4873,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -4896,7 +4917,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -4940,7 +4961,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -4984,7 +5005,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5028,7 +5049,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5072,7 +5093,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5116,7 +5137,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5160,7 +5181,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5204,7 +5225,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5248,7 +5269,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61" t="s">
         <v>391</v>
       </c>
@@ -5292,7 +5313,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5336,7 +5357,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5380,7 +5401,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="73" t="s">
         <v>10</v>
       </c>
@@ -5424,7 +5445,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5468,7 +5489,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5512,7 +5533,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5556,7 +5577,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -5600,7 +5621,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -5644,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -5688,7 +5709,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>445</v>
       </c>
@@ -5732,7 +5753,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -5776,7 +5797,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -5820,7 +5841,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -5864,7 +5885,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -5908,7 +5929,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -5952,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6070,25 +6091,25 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6130,7 +6151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6174,7 +6195,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6218,7 +6239,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6262,7 +6283,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6306,7 +6327,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>56</v>
       </c>
@@ -6350,7 +6371,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6394,7 +6415,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6438,7 +6459,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6482,7 +6503,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6526,7 +6547,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="73" t="s">
         <v>86</v>
       </c>
@@ -6570,7 +6591,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
@@ -6614,7 +6635,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -6658,7 +6679,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -6702,7 +6723,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -6746,7 +6767,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -6790,7 +6811,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>121</v>
       </c>
@@ -6834,7 +6855,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -6878,7 +6899,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -6922,7 +6943,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -6966,7 +6987,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7010,7 +7031,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7054,7 +7075,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7098,7 +7119,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7142,7 +7163,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7186,7 +7207,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7230,7 +7251,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7274,7 +7295,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7318,7 +7339,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7362,7 +7383,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7406,7 +7427,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7450,7 +7471,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7494,7 +7515,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7538,7 +7559,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -7582,7 +7603,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -7626,7 +7647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -7670,7 +7691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -7714,7 +7735,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -7823,29 +7844,29 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="23" width="9.140625" style="4"/>
-    <col min="24" max="29" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="23" width="9.1640625" style="4"/>
+    <col min="24" max="29" width="9.1640625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.140625" style="4"/>
-    <col min="34" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="33" width="9.1640625" style="4"/>
+    <col min="34" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="93" t="s">
         <v>499</v>
@@ -7870,19 +7891,19 @@
       <c r="X1" s="88"/>
       <c r="Y1" s="89">
         <f>AVERAGE(Y3:Y15)</f>
-        <v>0.48684562094335121</v>
+        <v>0.48917036089714422</v>
       </c>
       <c r="Z1" s="89">
         <f>AVERAGE(Z3:Z15)</f>
-        <v>4.926848653784497E-2</v>
+        <v>5.0108956654114897E-2</v>
       </c>
       <c r="AA1" s="89">
         <f>AVERAGE(AA3:AA15)</f>
-        <v>3.3967961295369026E-2</v>
+        <v>3.3909194645848455E-2</v>
       </c>
       <c r="AB1" s="89">
         <f>AVERAGE(AB3:AB15)</f>
-        <v>0.14615541162428036</v>
+        <v>7.8248603342185627E-2</v>
       </c>
       <c r="AC1" s="88"/>
       <c r="AD1" s="90" t="s">
@@ -7894,14 +7915,18 @@
       </c>
       <c r="AF1" s="89">
         <f>AVERAGE(AF3:AF15)</f>
-        <v>3.9231986955234513E-2</v>
+        <v>7.5807815242083035E-2</v>
       </c>
       <c r="AG1" s="89">
         <f>AVERAGE(AG3:AG15)</f>
         <v>0.22763826675517687</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AH1" s="94">
+        <f>AVERAGE(AH3:AH15)</f>
+        <v>663.72856720350364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8006,7 +8031,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8125,7 +8150,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8229,7 +8254,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8344,7 +8369,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8463,7 +8488,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>526</v>
       </c>
@@ -8514,7 +8539,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8633,7 +8658,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8664,7 +8689,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8761,7 +8786,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -8776,11 +8801,11 @@
       </c>
       <c r="F11" s="6">
         <f>[9]Main!$C$6</f>
-        <v>5.1749999999999998</v>
+        <v>6.17</v>
       </c>
       <c r="G11" s="49">
         <f>[9]Main!$C$8</f>
-        <v>515.92694489999997</v>
+        <v>615.12449275999995</v>
       </c>
       <c r="H11" s="49">
         <f>[9]Main!$C$11</f>
@@ -8788,7 +8813,7 @@
       </c>
       <c r="I11" s="49">
         <f>[9]Main!$C$12</f>
-        <v>633.02694489999999</v>
+        <v>732.22449275999998</v>
       </c>
       <c r="J11" s="85" t="str">
         <f>[9]Main!$C$28</f>
@@ -8817,15 +8842,15 @@
       </c>
       <c r="R11" s="52">
         <f>[9]Main!$C$36</f>
-        <v>-16.750874834415534</v>
+        <v>-19.971574440259683</v>
       </c>
       <c r="S11" s="52">
         <f>[9]Main!$C$41</f>
-        <v>4.0138826705607427</v>
+        <v>4.7856340246105864</v>
       </c>
       <c r="T11" s="52">
         <f>[9]Main!$C$33</f>
-        <v>0.52410295093457915</v>
+        <v>0.62487250381958526</v>
       </c>
       <c r="U11" s="87">
         <f>'[9]Financial Model'!$T$19</f>
@@ -8887,7 +8912,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -8902,31 +8927,35 @@
       </c>
       <c r="F12" s="54">
         <f>[10]Main!$C$6*E28</f>
-        <v>14.1332</v>
+        <v>15.788599999999999</v>
       </c>
       <c r="G12" s="49">
         <f>[10]Main!$C$8*E28</f>
-        <v>712.97559001840011</v>
+        <v>796.39277259999994</v>
       </c>
       <c r="H12" s="49">
         <f>[10]Main!$C$11*E28</f>
-        <v>146.405</v>
+        <v>58.505930000000021</v>
       </c>
       <c r="I12" s="49">
         <f>[10]Main!$C$12*E28</f>
-        <v>566.57059001840014</v>
+        <v>737.88684259999991</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>[10]Main!$C$27</f>
-        <v>Q122</v>
+        <v>Q222</v>
+      </c>
+      <c r="K12" s="86">
+        <f>[10]Main!$D$27</f>
+        <v>44798</v>
       </c>
       <c r="L12" s="50">
         <f>[10]Main!$C$32</f>
-        <v>-0.96423583702713767</v>
+        <v>-1.077175299046689</v>
       </c>
       <c r="M12" s="50">
         <f>[10]Main!$C$38</f>
-        <v>2.420425719782521</v>
+        <v>3.1522996844226485</v>
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
@@ -8943,15 +8972,15 @@
       </c>
       <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
-        <v>-50.21450968486225</v>
+        <v>-56.096058048454417</v>
       </c>
       <c r="S12" s="52">
         <f>[10]Main!$C$37</f>
-        <v>3.5983436371240685</v>
+        <v>4.0198120983993046</v>
       </c>
       <c r="T12" s="52">
         <f>[10]Main!$C$35</f>
-        <v>1.1733497350330941</v>
+        <v>1.3298883267742285</v>
       </c>
       <c r="U12" s="53"/>
       <c r="V12" s="53">
@@ -8967,32 +8996,36 @@
         <v>0</v>
       </c>
       <c r="Y12" s="53">
-        <f>'[10]Financial Model'!$O$27</f>
-        <v>0.55310902822720542</v>
+        <f>'[10]Financial Model'!$P$27</f>
+        <v>0.57868116771892864</v>
       </c>
       <c r="Z12" s="53">
-        <f>'[10]Financial Model'!$O$28</f>
-        <v>-1.1966602769322474E-2</v>
+        <f>'[10]Financial Model'!$P$28</f>
+        <v>-2.721431490353244E-3</v>
       </c>
       <c r="AA12" s="53">
-        <f>'[10]Financial Model'!$O$30</f>
-        <v>-2.0263004421958795E-2</v>
+        <f>'[10]Financial Model'!$P$30</f>
+        <v>-2.0909437566684987E-2</v>
       </c>
       <c r="AB12" s="53">
-        <f>'[10]Financial Model'!$O$31</f>
-        <v>0.12839781600422653</v>
+        <f>'[10]Financial Model'!$P$31</f>
+        <v>-0.61857707509881543</v>
       </c>
       <c r="AD12" s="56">
-        <f>'[10]Financial Model'!$O$41*E28</f>
-        <v>500.63389999999998</v>
+        <f>'[10]Financial Model'!$P$41*E28</f>
+        <v>630.14135999999996</v>
       </c>
       <c r="AE12" s="53">
         <f>'[10]Financial Model'!$X$69</f>
         <v>-0.25498478543021663</v>
       </c>
+      <c r="AF12" s="53">
+        <f>'[10]Financial Model'!$P$67</f>
+        <v>0.25868695667632569</v>
+      </c>
       <c r="AH12" s="57">
         <f>[10]Main!$C$25</f>
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="AI12" s="4">
         <f>[10]Main!$C$24</f>
@@ -9003,7 +9036,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9118,7 +9151,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
         <v>391</v>
       </c>
@@ -9200,7 +9233,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9330,7 +9363,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B16" s="3"/>
       <c r="F16" s="7"/>
       <c r="G16" s="49"/>
@@ -9354,7 +9387,7 @@
       <c r="AI16" s="4"/>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -9371,7 +9404,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
@@ -9390,7 +9423,7 @@
       <c r="M18" s="56"/>
       <c r="N18" s="56"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>445</v>
       </c>
@@ -9409,7 +9442,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9428,7 +9461,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9438,7 +9471,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>492</v>
       </c>
@@ -9460,7 +9493,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>511</v>
       </c>
@@ -9482,28 +9515,28 @@
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D27" s="91" t="s">
         <v>495</v>
       </c>
@@ -9515,7 +9548,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D28" s="43" t="s">
         <v>497</v>
       </c>
@@ -9530,7 +9563,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D29" s="46" t="s">
         <v>498</v>
       </c>

</xml_diff>

<commit_message>
Input $UA FQ223 results
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822D6924-0785-5348-8A44-5A350D5B0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914C75B-D185-483A-AB85-DFB796E6891A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="500" windowWidth="22500" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="9795" yWindow="495" windowWidth="22500" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -37,16 +37,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1673,13 +1663,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2063,7 +2053,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2072,13 +2062,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2107,16 +2097,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2125,12 +2115,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2168,7 +2158,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2186,7 +2176,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2207,7 +2197,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2223,6 +2213,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2230,9 +2223,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3349,22 +3339,22 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>6.48</v>
+            <v>7.12</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>2970.4320000000002</v>
+            <v>3234.7726400000001</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>376.57900000000006</v>
+            <v>180.2700000000001</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>2593.8530000000001</v>
+            <v>3054.5026400000002</v>
           </cell>
         </row>
         <row r="23">
@@ -3379,96 +3369,94 @@
         </row>
         <row r="26">
           <cell r="C26">
-            <v>422</v>
+            <v>437</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>954.39400000000001</v>
+            <v>1080.42</v>
           </cell>
         </row>
         <row r="29">
           <cell r="C29" t="str">
-            <v>FQ123</v>
+            <v>FQ223</v>
+          </cell>
+          <cell r="D29">
+            <v>44868</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>15.153400361038278</v>
+            <v>21.115922407952812</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>17.902221644611082</v>
+            <v>22.825917900868863</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1.7179676073321593</v>
+            <v>1.8876434204020021</v>
           </cell>
         </row>
         <row r="41">
           <cell r="C41">
-            <v>8.3776757207132064</v>
+            <v>9.2051004832527816</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="20">
           <cell r="Y20">
+            <v>-46.302000000000398</v>
+          </cell>
+          <cell r="Z20">
             <v>92.141999999999229</v>
           </cell>
-          <cell r="Z20">
+          <cell r="AA20">
             <v>-549.17700000000002</v>
-          </cell>
-          <cell r="AA20">
-            <v>360.0600000000004</v>
           </cell>
         </row>
         <row r="24">
           <cell r="Y24">
+            <v>4.0876132736743287E-2</v>
+          </cell>
+          <cell r="Z24">
             <v>1.4239238540510346E-2</v>
           </cell>
-          <cell r="Z24">
+          <cell r="AA24">
             <v>-0.15045474463142361</v>
           </cell>
-          <cell r="AA24">
-            <v>0.27014278380938728</v>
-          </cell>
         </row>
         <row r="30">
-          <cell r="Q30">
-            <v>0.46713889776340067</v>
+          <cell r="R30">
+            <v>0.45354902041762896</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="Q31">
-            <v>2.5560817667452114E-2</v>
+          <cell r="R31">
+            <v>7.5869583864132367E-2</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="Q32">
-            <v>5.6943479778837729E-3</v>
+          <cell r="R32">
+            <v>5.5229575223094414E-2</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="Q33">
-            <v>0.39734494626677114</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="AA79">
-            <v>-9.4382203054999447E-2</v>
+          <cell r="R33">
+            <v>0.20212746629846307</v>
           </cell>
         </row>
         <row r="80">
-          <cell r="Q80">
-            <v>0.15760593361675279</v>
+          <cell r="R80">
+            <v>0.13204818974134369</v>
           </cell>
         </row>
         <row r="95">
           <cell r="AA95">
-            <v>0.14276675535667846</v>
+            <v>0.20023255361795636</v>
           </cell>
         </row>
       </sheetData>
@@ -3753,7 +3741,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4065,25 +4053,25 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4125,7 +4113,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>241</v>
       </c>
@@ -4169,7 +4157,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4213,7 +4201,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4257,7 +4245,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>259</v>
       </c>
@@ -4301,7 +4289,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4345,7 +4333,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4389,7 +4377,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4433,7 +4421,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4477,7 +4465,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4521,7 +4509,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4565,7 +4553,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>301</v>
       </c>
@@ -4609,7 +4597,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -4653,7 +4641,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>312</v>
       </c>
@@ -4697,7 +4685,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -4741,7 +4729,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -4785,7 +4773,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -4829,7 +4817,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -4873,7 +4861,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -4917,7 +4905,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -4961,7 +4949,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -5005,7 +4993,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5049,7 +5037,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5093,7 +5081,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5137,7 +5125,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5181,7 +5169,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5225,7 +5213,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5269,7 +5257,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="61" t="s">
         <v>391</v>
       </c>
@@ -5313,7 +5301,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5357,7 +5345,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5401,7 +5389,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>10</v>
       </c>
@@ -5445,7 +5433,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5489,7 +5477,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5533,7 +5521,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5577,7 +5565,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -5621,7 +5609,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -5665,7 +5653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -5709,7 +5697,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>445</v>
       </c>
@@ -5753,7 +5741,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -5797,7 +5785,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -5841,7 +5829,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -5885,7 +5873,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -5929,7 +5917,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -5973,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6091,25 +6079,25 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6151,7 +6139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6195,7 +6183,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6239,7 +6227,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6283,7 +6271,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6327,7 +6315,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>56</v>
       </c>
@@ -6371,7 +6359,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6415,7 +6403,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6459,7 +6447,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6503,7 +6491,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6547,7 +6535,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73" t="s">
         <v>86</v>
       </c>
@@ -6591,7 +6579,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
@@ -6635,7 +6623,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -6679,7 +6667,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -6723,7 +6711,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -6767,7 +6755,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -6811,7 +6799,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>121</v>
       </c>
@@ -6855,7 +6843,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -6899,7 +6887,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -6943,7 +6931,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -6987,7 +6975,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7031,7 +7019,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7075,7 +7063,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7119,7 +7107,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7163,7 +7151,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7207,7 +7195,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7251,7 +7239,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7295,7 +7283,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7339,7 +7327,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7383,7 +7371,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7427,7 +7415,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7471,7 +7459,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7515,7 +7503,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7559,7 +7547,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -7603,7 +7591,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -7647,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -7691,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -7735,7 +7723,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -7844,44 +7832,44 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="23" width="9.1640625" style="4"/>
-    <col min="24" max="29" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="23" width="9.140625" style="4"/>
+    <col min="24" max="29" width="9.140625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.1640625" style="4"/>
-    <col min="34" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1640625" style="1"/>
+    <col min="31" max="33" width="9.140625" style="4"/>
+    <col min="34" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="94" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
       <c r="R1" s="88"/>
       <c r="S1" s="88"/>
       <c r="T1" s="88"/>
@@ -7891,19 +7879,19 @@
       <c r="X1" s="88"/>
       <c r="Y1" s="89">
         <f>AVERAGE(Y3:Y15)</f>
-        <v>0.48917036089714422</v>
+        <v>0.48793491750207407</v>
       </c>
       <c r="Z1" s="89">
         <f>AVERAGE(Z3:Z15)</f>
-        <v>5.0108956654114897E-2</v>
+        <v>5.4682480853813109E-2</v>
       </c>
       <c r="AA1" s="89">
         <f>AVERAGE(AA3:AA15)</f>
-        <v>3.3909194645848455E-2</v>
+        <v>3.84123971226858E-2</v>
       </c>
       <c r="AB1" s="89">
         <f>AVERAGE(AB3:AB15)</f>
-        <v>7.8248603342185627E-2</v>
+        <v>6.0501559708703058E-2</v>
       </c>
       <c r="AC1" s="88"/>
       <c r="AD1" s="90" t="s">
@@ -7911,22 +7899,22 @@
       </c>
       <c r="AE1" s="89">
         <f>AVERAGE(AE3:AE15)</f>
-        <v>0.23199575663598668</v>
+        <v>0.24057595691371392</v>
       </c>
       <c r="AF1" s="89">
         <f>AVERAGE(AF3:AF15)</f>
-        <v>7.5807815242083035E-2</v>
+        <v>7.1548191262848185E-2</v>
       </c>
       <c r="AG1" s="89">
         <f>AVERAGE(AG3:AG15)</f>
-        <v>0.22763826675517687</v>
-      </c>
-      <c r="AH1" s="94">
+        <v>0.23482149153783663</v>
+      </c>
+      <c r="AH1" s="91">
         <f>AVERAGE(AH3:AH15)</f>
-        <v>663.72856720350364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>665.09462510297612</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8031,7 +8019,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8150,7 +8138,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8254,7 +8242,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8369,7 +8357,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8488,7 +8476,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>526</v>
       </c>
@@ -8539,7 +8527,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8554,100 +8542,104 @@
       </c>
       <c r="F8" s="7">
         <f>[6]Main!$C$6*E28</f>
-        <v>5.7672000000000008</v>
+        <v>6.3368000000000002</v>
       </c>
       <c r="G8" s="49">
         <f>[6]Main!$C$8*E28</f>
-        <v>2643.6844800000003</v>
+        <v>2878.9476496000002</v>
       </c>
       <c r="H8" s="49">
         <f>[6]Main!$C$11*$E$28</f>
-        <v>335.15531000000004</v>
+        <v>160.44030000000009</v>
       </c>
       <c r="I8" s="49">
         <f>[6]Main!$C$12*$E$28</f>
-        <v>2308.5291700000002</v>
+        <v>2718.5073496</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
-        <v>FQ123</v>
+        <v>FQ223</v>
+      </c>
+      <c r="K8" s="86">
+        <f>[6]Main!$D$29</f>
+        <v>44868</v>
       </c>
       <c r="L8" s="50">
         <f>[6]Main!$C$34</f>
-        <v>15.153400361038278</v>
+        <v>21.115922407952812</v>
       </c>
       <c r="O8" s="56">
         <f>'[6]Financial Model'!$AA$20*$E$28</f>
-        <v>320.45340000000039</v>
+        <v>-488.76753000000002</v>
       </c>
       <c r="P8" s="56">
         <f>'[6]Financial Model'!$Z$20*$E$28</f>
-        <v>-488.76753000000002</v>
+        <v>82.006379999999311</v>
       </c>
       <c r="Q8" s="56">
         <f>'[6]Financial Model'!$Y$20*$E$28</f>
-        <v>82.006379999999311</v>
+        <v>-41.208780000000353</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
-        <v>17.902221644611082</v>
+        <v>22.825917900868863</v>
       </c>
       <c r="S8" s="52">
         <f>[6]Main!$C$41</f>
-        <v>8.3776757207132064</v>
+        <v>9.2051004832527816</v>
       </c>
       <c r="T8" s="52">
         <f>[6]Main!$C$37</f>
-        <v>1.7179676073321593</v>
+        <v>1.8876434204020021</v>
       </c>
       <c r="U8" s="53"/>
       <c r="V8" s="53">
         <f>'[6]Financial Model'!$AA$24</f>
-        <v>0.27014278380938728</v>
+        <v>-0.15045474463142361</v>
       </c>
       <c r="W8" s="53">
         <f>'[6]Financial Model'!$Z$24</f>
-        <v>-0.15045474463142361</v>
+        <v>1.4239238540510346E-2</v>
       </c>
       <c r="X8" s="53">
         <f>'[6]Financial Model'!$Y$24</f>
-        <v>1.4239238540510346E-2</v>
+        <v>4.0876132736743287E-2</v>
       </c>
       <c r="Y8" s="53">
-        <f>'[6]Financial Model'!$Q$30</f>
-        <v>0.46713889776340067</v>
+        <f>'[6]Financial Model'!$R$30</f>
+        <v>0.45354902041762896</v>
       </c>
       <c r="Z8" s="53">
-        <f>'[6]Financial Model'!$Q$31</f>
-        <v>2.5560817667452114E-2</v>
+        <f>'[6]Financial Model'!$R$31</f>
+        <v>7.5869583864132367E-2</v>
       </c>
       <c r="AA8" s="53">
-        <f>'[6]Financial Model'!$Q$32</f>
-        <v>5.6943479778837729E-3</v>
+        <f>'[6]Financial Model'!$R$32</f>
+        <v>5.5229575223094414E-2</v>
       </c>
       <c r="AB8" s="53">
-        <f>'[6]Financial Model'!$Q$33</f>
-        <v>0.39734494626677114</v>
+        <f>'[6]Financial Model'!$R$33</f>
+        <v>0.20212746629846307</v>
       </c>
       <c r="AD8" s="56">
         <f>[6]Main!$C$27*E28</f>
-        <v>849.41066000000001</v>
+        <v>961.57380000000012</v>
       </c>
       <c r="AE8" s="53">
         <f>'[6]Financial Model'!$AA$79</f>
-        <v>-9.4382203054999447E-2</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="53">
-        <f>'[6]Financial Model'!$Q$80</f>
-        <v>0.15760593361675279</v>
+        <f>'[6]Financial Model'!$R$80</f>
+        <v>0.13204818974134369</v>
       </c>
       <c r="AG8" s="53">
         <f>'[6]Financial Model'!$AA$95</f>
-        <v>0.14276675535667846</v>
+        <v>0.20023255361795636</v>
       </c>
       <c r="AH8" s="57">
         <f>[6]Main!$C$26</f>
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="AI8" s="4">
         <f>[6]Main!$C$24</f>
@@ -8658,7 +8650,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8689,7 +8681,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8786,7 +8778,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -8912,7 +8904,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9036,7 +9028,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9140,7 +9132,7 @@
       </c>
       <c r="AH13" s="53">
         <f>'[6]Financial Model'!$Y$24</f>
-        <v>1.4239238540510346E-2</v>
+        <v>4.0876132736743287E-2</v>
       </c>
       <c r="AI13" s="4">
         <f>[11]Main!$C$24</f>
@@ -9151,7 +9143,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>391</v>
       </c>
@@ -9233,7 +9225,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9363,7 +9355,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="F16" s="7"/>
       <c r="G16" s="49"/>
@@ -9387,7 +9379,7 @@
       <c r="AI16" s="4"/>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -9404,7 +9396,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
@@ -9423,7 +9415,7 @@
       <c r="M18" s="56"/>
       <c r="N18" s="56"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>445</v>
       </c>
@@ -9442,7 +9434,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9461,7 +9453,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9471,7 +9463,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>492</v>
       </c>
@@ -9493,7 +9485,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>511</v>
       </c>
@@ -9515,32 +9507,32 @@
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="D27" s="91" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D27" s="92" t="s">
         <v>495</v>
       </c>
-      <c r="E27" s="92"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="42" t="s">
         <v>496</v>
       </c>
@@ -9548,7 +9540,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D28" s="43" t="s">
         <v>497</v>
       </c>
@@ -9563,7 +9555,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D29" s="46" t="s">
         <v>498</v>
       </c>

</xml_diff>

<commit_message>
Update $UA historical balance sheet data to compare with latest results
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914C75B-D185-483A-AB85-DFB796E6891A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7617977A-A47A-E54F-B6F0-96692CAE7DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="495" windowWidth="22500" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="4660" yWindow="500" windowWidth="27640" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -37,6 +37,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1663,13 +1673,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2053,7 +2063,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2062,13 +2072,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2097,16 +2107,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2115,12 +2125,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2158,7 +2168,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2176,7 +2186,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2197,7 +2207,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3447,6 +3457,11 @@
         <row r="33">
           <cell r="R33">
             <v>0.20212746629846307</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="R79">
+            <v>0.28968415021367022</v>
           </cell>
         </row>
         <row r="80">
@@ -4053,25 +4068,25 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4113,7 +4128,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>241</v>
       </c>
@@ -4157,7 +4172,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4201,7 +4216,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4245,7 +4260,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>259</v>
       </c>
@@ -4289,7 +4304,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4333,7 +4348,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4377,7 +4392,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4421,7 +4436,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4465,7 +4480,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4509,7 +4524,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4553,7 +4568,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>301</v>
       </c>
@@ -4597,7 +4612,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -4641,7 +4656,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>312</v>
       </c>
@@ -4685,7 +4700,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -4729,7 +4744,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -4773,7 +4788,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -4817,7 +4832,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -4861,7 +4876,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -4905,7 +4920,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -4949,7 +4964,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -4993,7 +5008,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5037,7 +5052,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5081,7 +5096,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5125,7 +5140,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5169,7 +5184,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5213,7 +5228,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5257,7 +5272,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61" t="s">
         <v>391</v>
       </c>
@@ -5301,7 +5316,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5345,7 +5360,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5389,7 +5404,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="73" t="s">
         <v>10</v>
       </c>
@@ -5433,7 +5448,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5477,7 +5492,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5521,7 +5536,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5565,7 +5580,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -5609,7 +5624,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -5653,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -5697,7 +5712,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>445</v>
       </c>
@@ -5741,7 +5756,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -5785,7 +5800,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -5829,7 +5844,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -5873,7 +5888,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -5917,7 +5932,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -5961,7 +5976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6079,25 +6094,25 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6139,7 +6154,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6183,7 +6198,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6227,7 +6242,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6271,7 +6286,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6315,7 +6330,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>56</v>
       </c>
@@ -6359,7 +6374,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6403,7 +6418,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6447,7 +6462,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6491,7 +6506,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6535,7 +6550,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="73" t="s">
         <v>86</v>
       </c>
@@ -6579,7 +6594,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
@@ -6623,7 +6638,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -6667,7 +6682,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -6711,7 +6726,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -6755,7 +6770,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -6799,7 +6814,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>121</v>
       </c>
@@ -6843,7 +6858,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -6887,7 +6902,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -6931,7 +6946,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -6975,7 +6990,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7019,7 +7034,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7063,7 +7078,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7107,7 +7122,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7151,7 +7166,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7195,7 +7210,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7239,7 +7254,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7283,7 +7298,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7327,7 +7342,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7371,7 +7386,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7415,7 +7430,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7459,7 +7474,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7503,7 +7518,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7547,7 +7562,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -7591,7 +7606,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -7635,7 +7650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -7679,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -7723,7 +7738,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -7826,35 +7841,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="23" width="9.140625" style="4"/>
-    <col min="24" max="29" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="23" width="9.1640625" style="4"/>
+    <col min="24" max="29" width="9.1640625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.140625" style="4"/>
-    <col min="34" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="33" width="9.1640625" style="4"/>
+    <col min="34" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="94" t="s">
         <v>499</v>
@@ -7899,7 +7914,7 @@
       </c>
       <c r="AE1" s="89">
         <f>AVERAGE(AE3:AE15)</f>
-        <v>0.24057595691371392</v>
+        <v>0.26691087966041116</v>
       </c>
       <c r="AF1" s="89">
         <f>AVERAGE(AF3:AF15)</f>
@@ -7914,7 +7929,7 @@
         <v>665.09462510297612</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8019,7 +8034,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8138,7 +8153,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8242,7 +8257,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8357,7 +8372,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8476,7 +8491,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>526</v>
       </c>
@@ -8527,7 +8542,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8626,8 +8641,8 @@
         <v>961.57380000000012</v>
       </c>
       <c r="AE8" s="53">
-        <f>'[6]Financial Model'!$AA$79</f>
-        <v>0</v>
+        <f>'[6]Financial Model'!$R$79</f>
+        <v>0.28968415021367022</v>
       </c>
       <c r="AF8" s="53">
         <f>'[6]Financial Model'!$R$80</f>
@@ -8650,7 +8665,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8681,7 +8696,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8778,7 +8793,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -8904,7 +8919,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9028,7 +9043,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9143,7 +9158,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
         <v>391</v>
       </c>
@@ -9225,7 +9240,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9355,7 +9370,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B16" s="3"/>
       <c r="F16" s="7"/>
       <c r="G16" s="49"/>
@@ -9379,7 +9394,7 @@
       <c r="AI16" s="4"/>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -9396,7 +9411,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
@@ -9415,7 +9430,7 @@
       <c r="M18" s="56"/>
       <c r="N18" s="56"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>445</v>
       </c>
@@ -9434,7 +9449,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9453,7 +9468,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9463,7 +9478,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>492</v>
       </c>
@@ -9485,7 +9500,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>511</v>
       </c>
@@ -9507,28 +9522,31 @@
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G24" s="49"/>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G26" s="49"/>
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D27" s="92" t="s">
         <v>495</v>
       </c>
@@ -9536,11 +9554,12 @@
       <c r="F27" s="42" t="s">
         <v>496</v>
       </c>
+      <c r="G27" s="49"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D28" s="43" t="s">
         <v>497</v>
       </c>
@@ -9551,11 +9570,12 @@
         <f>1/E28</f>
         <v>1.1235955056179776</v>
       </c>
+      <c r="G28" s="49"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
       <c r="D29" s="46" t="s">
         <v>498</v>
       </c>
@@ -9566,9 +9586,25 @@
         <f>1/E29</f>
         <v>1.1363636363636365</v>
       </c>
+      <c r="G29" s="49"/>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G30" s="49"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G31" s="49"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G32" s="49"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G33" s="49"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G34" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add £JOUL to compare. Colour-code acquisitions & administrations
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7617977A-A47A-E54F-B6F0-96692CAE7DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DA6752-794E-D44F-AEEF-BDBCC1204AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="500" windowWidth="27640" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -31,6 +31,7 @@
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="538">
   <si>
     <t>Ticker</t>
   </si>
@@ -1672,7 +1673,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -1680,6 +1681,7 @@
     <numFmt numFmtId="168" formatCode="0.0\x"/>
     <numFmt numFmtId="169" formatCode="0.#\x"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1765,7 +1767,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1835,6 +1837,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1971,7 +1979,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2226,6 +2234,35 @@
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2235,6 +2272,36 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="171" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2761,12 +2828,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>1.1299999999999999</v>
+            <v>1.1519999999999999</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>92.523351359999978</v>
+            <v>94.324690943999983</v>
           </cell>
         </row>
         <row r="11">
@@ -2776,7 +2843,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>84.223351359999981</v>
+            <v>86.024690943999985</v>
           </cell>
         </row>
         <row r="24">
@@ -2809,22 +2876,22 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>3.7102797955947073</v>
+            <v>3.7896339622907425</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>4.0759185621145306</v>
+            <v>4.1552727288105658</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>0.89050386294513961</v>
+            <v>0.90784110629451398</v>
           </cell>
         </row>
         <row r="39">
           <cell r="C39">
-            <v>-2.5676413418282564</v>
+            <v>-2.6176308192797801</v>
           </cell>
         </row>
       </sheetData>
@@ -2895,6 +2962,91 @@
       </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>9.2200000000000004E-2</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>10.16966</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-6.5050000000000026</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>16.674660000000003</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Market Harborough</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1989</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26">
+            <v>61.878</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D28">
+            <v>44600</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>0.20742534761796225</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="21">
+          <cell r="K21">
+            <v>0.50353090223741115</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="K22">
+            <v>2.5932384981739429E-2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="K23">
+            <v>1.7767906718489747E-2</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="K65">
+            <v>0.44899775196702874</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7841,13 +7993,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AJ34"/>
+  <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20:G32"/>
+      <selection pane="bottomRight" activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7871,61 +8023,79 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="107" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="104">
+        <f>AVERAGE(R3:R16)</f>
+        <v>1.1609166178244328</v>
+      </c>
+      <c r="S1" s="104">
+        <f>AVERAGE(S3:S16)</f>
+        <v>14.027290837255359</v>
+      </c>
+      <c r="T1" s="104">
+        <f>AVERAGE(T3:T16)</f>
+        <v>2.6126027375685812</v>
+      </c>
       <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
+      <c r="V1" s="89">
+        <f>AVERAGE(V3:V16)</f>
+        <v>0.15708636175947649</v>
+      </c>
+      <c r="W1" s="89">
+        <f>AVERAGE(W3:W16)</f>
+        <v>6.1523225008126764E-2</v>
+      </c>
+      <c r="X1" s="89">
+        <f>AVERAGE(X3:X16)</f>
+        <v>0.10798125173689554</v>
+      </c>
       <c r="Y1" s="89">
-        <f>AVERAGE(Y3:Y15)</f>
-        <v>0.48793491750207407</v>
+        <f>AVERAGE(Y3:Y16)</f>
+        <v>0.48923458289668553</v>
       </c>
       <c r="Z1" s="89">
-        <f>AVERAGE(Z3:Z15)</f>
-        <v>5.4682480853813109E-2</v>
+        <f>AVERAGE(Z3:Z16)</f>
+        <v>5.2286639531140301E-2</v>
       </c>
       <c r="AA1" s="89">
-        <f>AVERAGE(AA3:AA15)</f>
-        <v>3.84123971226858E-2</v>
+        <f>AVERAGE(AA3:AA16)</f>
+        <v>3.6692022922336129E-2</v>
       </c>
       <c r="AB1" s="89">
-        <f>AVERAGE(AB3:AB15)</f>
-        <v>6.0501559708703058E-2</v>
+        <f>AVERAGE(AB3:AB16)</f>
+        <v>5.6940421959518615E-2</v>
       </c>
       <c r="AC1" s="88"/>
       <c r="AD1" s="90" t="s">
         <v>537</v>
       </c>
       <c r="AE1" s="89">
-        <f>AVERAGE(AE3:AE15)</f>
-        <v>0.26691087966041116</v>
+        <f>AVERAGE(AE3:AE16)</f>
+        <v>0.28208478568596257</v>
       </c>
       <c r="AF1" s="89">
-        <f>AVERAGE(AF3:AF15)</f>
+        <f>AVERAGE(AF3:AF16)</f>
         <v>7.1548191262848185E-2</v>
       </c>
       <c r="AG1" s="89">
-        <f>AVERAGE(AG3:AG15)</f>
+        <f>AVERAGE(AG3:AG16)</f>
         <v>0.23482149153783663</v>
       </c>
       <c r="AH1" s="91">
-        <f>AVERAGE(AH3:AH15)</f>
+        <f>AVERAGE(AH3:AH16)</f>
         <v>665.09462510297612</v>
       </c>
     </row>
@@ -8048,20 +8218,20 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$28</f>
-        <v>83.508700000000005</v>
+        <f>[1]Main!$C$6*$E$27</f>
+        <v>79.755499999999998</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$28</f>
-        <v>130866.48376999999</v>
+        <f>[1]Main!$C$8*$E$27</f>
+        <v>124984.84404999999</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$28</f>
-        <v>2176.0500000000002</v>
+        <f>[1]Main!$C$11*$E$27</f>
+        <v>2078.25</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$28</f>
-        <v>128690.43376999999</v>
+        <f>[1]Main!$C$12*$E$27</f>
+        <v>122906.59404999999</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>[1]Main!$C$28</f>
@@ -8076,16 +8246,16 @@
         <v>23.915976347998704</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E28</f>
-        <v>5380.9399999999932</v>
+        <f>'[1]Financial Model'!$AD$21*1000*E27</f>
+        <v>5139.099999999994</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AC$21*1000*E28</f>
-        <v>5097.0299999999988</v>
+        <f>'[1]Financial Model'!$AC$21*1000*E27</f>
+        <v>4867.949999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AB$21*1000*E28</f>
-        <v>2259.71</v>
+        <f>'[1]Financial Model'!$AB$21*1000*E27</f>
+        <v>2158.15</v>
       </c>
       <c r="R3" s="51">
         <f>[1]Main!$C$34</f>
@@ -8129,8 +8299,8 @@
         <v>0.19693654266958391</v>
       </c>
       <c r="AD3" s="56">
-        <f>[1]Main!$C$26*E28</f>
-        <v>8599.18</v>
+        <f>[1]Main!$C$26*E27</f>
+        <v>8212.6999999999989</v>
       </c>
       <c r="AE3" s="53">
         <f>'[1]Financial Model'!$W$72</f>
@@ -8167,20 +8337,20 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$28</f>
-        <v>24.937799999999999</v>
+        <f>[2]Main!$C$6*$E$27</f>
+        <v>23.817</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$28</f>
-        <v>9668.0858063999985</v>
+        <f>[2]Main!$C$8*$E$27</f>
+        <v>9233.5650959999984</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$28</f>
-        <v>-4152.7711499999996</v>
+        <f>[2]Main!$C$11*$E$27</f>
+        <v>-3966.1297499999996</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$28</f>
-        <v>13820.856956399999</v>
+        <f>[2]Main!$C$12*$E$27</f>
+        <v>13199.694845999999</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>[2]Main!$C$28</f>
@@ -8195,16 +8365,16 @@
         <v>11.196943949135527</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E28</f>
-        <v>1234.341889999999</v>
+        <f>'[2]Financial Model'!$AA$22*E27</f>
+        <v>1178.865849999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$28</f>
-        <v>362.98561000000126</v>
+        <f>'[2]Financial Model'!$Z$22*$E$27</f>
+        <v>346.67165000000119</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$28</f>
-        <v>604.70961000000023</v>
+        <f>'[2]Financial Model'!$Y$22*$E$27</f>
+        <v>577.53165000000013</v>
       </c>
       <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
@@ -8237,8 +8407,8 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AD4" s="56">
-        <f>[2]Main!$C$26*E28</f>
-        <v>2083.8415500000001</v>
+        <f>[2]Main!$C$26*E27</f>
+        <v>1990.1857499999999</v>
       </c>
       <c r="AE4" s="53">
         <f>'[2]Financial Model'!$T$76</f>
@@ -8491,53 +8661,57 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:36" s="97" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="98" t="s">
         <v>526</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="97" t="s">
         <v>527</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="100">
         <f>[5]Main!$C$6</f>
         <v>7.25</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="101">
         <f>[5]Main!$C$8</f>
         <v>3461.73</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="101">
         <f>[5]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I7" s="49">
+      <c r="I7" s="101">
         <f>[5]Main!$C$12</f>
         <v>3461.73</v>
       </c>
-      <c r="J7" s="59"/>
-      <c r="Q7" s="4"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="53"/>
-      <c r="X7" s="4"/>
-      <c r="AD7" s="49">
+      <c r="K7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="U7" s="102"/>
+      <c r="V7" s="99"/>
+      <c r="W7" s="99"/>
+      <c r="X7" s="99"/>
+      <c r="AD7" s="101">
         <f>[5]Main!$C$26</f>
         <v>0</v>
       </c>
-      <c r="AH7" s="4">
+      <c r="AE7" s="99"/>
+      <c r="AF7" s="99"/>
+      <c r="AG7" s="99"/>
+      <c r="AH7" s="99">
         <f>[5]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="AI7" s="4">
+      <c r="AI7" s="99">
         <f>[5]Main!$C$24</f>
         <v>1982</v>
       </c>
-      <c r="AJ7" s="4" t="str">
+      <c r="AJ7" s="99" t="str">
         <f>[5]Main!$C$23</f>
         <v>Mansfiled, UK</v>
       </c>
@@ -8556,20 +8730,20 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E28</f>
-        <v>6.3368000000000002</v>
+        <f>[6]Main!$C$6*E27</f>
+        <v>6.0519999999999996</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E28</f>
-        <v>2878.9476496000002</v>
+        <f>[6]Main!$C$8*E27</f>
+        <v>2749.556744</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$28</f>
-        <v>160.44030000000009</v>
+        <f>[6]Main!$C$11*$E$27</f>
+        <v>153.22950000000009</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$28</f>
-        <v>2718.5073496</v>
+        <f>[6]Main!$C$12*$E$27</f>
+        <v>2596.3272440000001</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
@@ -8584,16 +8758,16 @@
         <v>21.115922407952812</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$28</f>
-        <v>-488.76753000000002</v>
+        <f>'[6]Financial Model'!$AA$20*$E$27</f>
+        <v>-466.80045000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$28</f>
-        <v>82.006379999999311</v>
+        <f>'[6]Financial Model'!$Z$20*$E$27</f>
+        <v>78.320699999999349</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$28</f>
-        <v>-41.208780000000353</v>
+        <f>'[6]Financial Model'!$Y$20*$E$27</f>
+        <v>-39.356700000000338</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
@@ -8637,8 +8811,8 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AD8" s="56">
-        <f>[6]Main!$C$27*E28</f>
-        <v>961.57380000000012</v>
+        <f>[6]Main!$C$27*E27</f>
+        <v>918.35700000000008</v>
       </c>
       <c r="AE8" s="53">
         <f>'[6]Financial Model'!$R$79</f>
@@ -8679,12 +8853,12 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E28</f>
-        <v>18.690000000000001</v>
+        <f>[7]Main!$C$6*E27</f>
+        <v>17.849999999999998</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$28</f>
-        <v>1731.8154</v>
+        <f>[7]Main!$C$8*$E$27</f>
+        <v>1653.9809999999998</v>
       </c>
       <c r="H9" s="49"/>
       <c r="I9" s="4"/>
@@ -8710,20 +8884,20 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E28</f>
-        <v>9.1135999999999999</v>
+        <f>[8]Main!$C$6*E27</f>
+        <v>8.7040000000000006</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E28</f>
-        <v>1535.2770560000001</v>
+        <f>[8]Main!$C$8*E27</f>
+        <v>1466.27584</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$28</f>
-        <v>-157.53</v>
+        <f>[8]Main!$C$11*$E$27</f>
+        <v>-150.44999999999999</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$28</f>
-        <v>1692.8070560000001</v>
+        <f>[8]Main!$C$12*$E$27</f>
+        <v>1616.7258400000001</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>[8]Main!$C$28</f>
@@ -8734,12 +8908,12 @@
         <v>59.925343415248761</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$16*E28</f>
-        <v>373.46713999999986</v>
+        <f>'[8]Financial Model'!$Z$16*E27</f>
+        <v>356.68209999999988</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$16*F28</f>
-        <v>-235.21011235955083</v>
+        <f>'[8]Financial Model'!$Y$16*F27</f>
+        <v>-246.27882352941202</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="52">
@@ -8773,8 +8947,8 @@
         <v>0.23990612577230669</v>
       </c>
       <c r="AD10" s="56">
-        <f>[8]Main!$C$26*E28</f>
-        <v>607.06900000000007</v>
+        <f>[8]Main!$C$26*E27</f>
+        <v>579.78499999999997</v>
       </c>
       <c r="AE10" s="53">
         <f>'[8]Financial Model'!$O$71</f>
@@ -8933,20 +9107,20 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E28</f>
-        <v>15.788599999999999</v>
+        <f>[10]Main!$C$6*E27</f>
+        <v>15.078999999999999</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E28</f>
-        <v>796.39277259999994</v>
+        <f>[10]Main!$C$8*E27</f>
+        <v>760.59983899999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E28</f>
-        <v>58.505930000000021</v>
+        <f>[10]Main!$C$11*E27</f>
+        <v>55.87645000000002</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E28</f>
-        <v>737.88684259999991</v>
+        <f>[10]Main!$C$12*E27</f>
+        <v>704.72338899999988</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>[10]Main!$C$27</f>
@@ -8966,16 +9140,16 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E28</f>
-        <v>234.07889999999975</v>
+        <f>'[10]Financial Model'!$X$18*E27</f>
+        <v>223.55849999999975</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$28</f>
-        <v>-101.47869000000014</v>
+        <f>'[10]Financial Model'!$W$18*$E$27</f>
+        <v>-96.917850000000129</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$28</f>
-        <v>35.028620000000551</v>
+        <f>'[10]Financial Model'!$V$18*$E$27</f>
+        <v>33.454300000000522</v>
       </c>
       <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
@@ -9019,8 +9193,8 @@
         <v>-0.61857707509881543</v>
       </c>
       <c r="AD12" s="56">
-        <f>'[10]Financial Model'!$P$41*E28</f>
-        <v>630.14135999999996</v>
+        <f>'[10]Financial Model'!$P$41*E27</f>
+        <v>601.82039999999995</v>
       </c>
       <c r="AE12" s="53">
         <f>'[10]Financial Model'!$X$69</f>
@@ -9158,84 +9332,86 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="1:36" s="112" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="113" t="s">
         <v>391</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="112" t="s">
         <v>392</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="115">
         <f>[12]Main!$C$6</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="G14" s="49">
+      <c r="G14" s="116">
         <f>[12]Main!$C$8</f>
         <v>201.23580000000001</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="117">
         <f>[12]Main!$C$11</f>
         <v>14.5</v>
       </c>
-      <c r="I14" s="58">
+      <c r="I14" s="117">
         <f>[12]Main!$C$12</f>
         <v>186.73580000000001</v>
       </c>
-      <c r="J14" s="4" t="str">
+      <c r="J14" s="114" t="str">
         <f>[12]Main!$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="53">
+      <c r="K14" s="114"/>
+      <c r="Q14" s="114"/>
+      <c r="U14" s="118"/>
+      <c r="V14" s="118">
         <f>'[12]Financial Model'!$T$23</f>
         <v>0.20588400900900905</v>
       </c>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="53">
+      <c r="W14" s="114"/>
+      <c r="X14" s="114"/>
+      <c r="Y14" s="118">
         <f>'[12]Financial Model'!$T$26</f>
         <v>0.55486890948567691</v>
       </c>
-      <c r="Z14" s="53">
+      <c r="Z14" s="118">
         <f>'[12]Financial Model'!$T$27</f>
         <v>-8.0487007680993719E-2</v>
       </c>
-      <c r="AA14" s="53">
+      <c r="AA14" s="118">
         <f>'[12]Financial Model'!$T$28</f>
         <v>-8.2866014521513875E-2</v>
       </c>
-      <c r="AB14" s="53">
+      <c r="AB14" s="118">
         <f>'[12]Financial Model'!$T$29</f>
         <v>0.19258416742493159</v>
       </c>
-      <c r="AD14" s="56">
+      <c r="AD14" s="119">
         <f>[12]Main!$C$26</f>
         <v>103.071</v>
       </c>
-      <c r="AE14" s="53">
+      <c r="AE14" s="118">
         <f>'[12]Financial Model'!$T$74</f>
         <v>0.17328795191694746</v>
       </c>
-      <c r="AG14" s="53">
+      <c r="AF14" s="114"/>
+      <c r="AG14" s="118">
         <f>'[12]Financial Model'!$T$76</f>
         <v>0.24063455746737328</v>
       </c>
-      <c r="AH14" s="4">
+      <c r="AH14" s="114">
         <f>[12]Main!$C$25</f>
         <v>85</v>
       </c>
-      <c r="AI14" s="4">
+      <c r="AI14" s="114">
         <f>[12]Main!$C$24</f>
         <v>1987</v>
       </c>
-      <c r="AJ14" s="4" t="str">
+      <c r="AJ14" s="114" t="str">
         <f>[12]Main!$C$23</f>
         <v>London, UK</v>
       </c>
@@ -9255,11 +9431,11 @@
       </c>
       <c r="F15" s="7">
         <f>[13]Main!$C$6</f>
-        <v>1.1299999999999999</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="G15" s="49">
         <f>[13]Main!$C$8</f>
-        <v>92.523351359999978</v>
+        <v>94.324690943999983</v>
       </c>
       <c r="H15" s="49">
         <f>[13]Main!$C$11</f>
@@ -9267,7 +9443,7 @@
       </c>
       <c r="I15" s="49">
         <f>[13]Main!$C$12</f>
-        <v>84.223351359999981</v>
+        <v>86.024690943999985</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>[13]Main!$C$29</f>
@@ -9279,7 +9455,7 @@
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>3.7102797955947073</v>
+        <v>3.7896339622907425</v>
       </c>
       <c r="N15" s="1">
         <f xml:space="preserve"> '[13]Financial Model'!$T$17</f>
@@ -9299,15 +9475,15 @@
       </c>
       <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>4.0759185621145306</v>
+        <v>4.1552727288105658</v>
       </c>
       <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
-        <v>-2.5676413418282564</v>
+        <v>-2.6176308192797801</v>
       </c>
       <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>0.89050386294513961</v>
+        <v>0.90784110629451398</v>
       </c>
       <c r="U15" s="53">
         <f xml:space="preserve"> '[13]Financial Model'!$T$21</f>
@@ -9370,72 +9546,138 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="B16" s="3"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="L16" s="50"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="53"/>
-      <c r="W16" s="53"/>
-      <c r="X16" s="53"/>
-      <c r="Y16" s="53"/>
-      <c r="Z16" s="53"/>
-      <c r="AA16" s="53"/>
-      <c r="AB16" s="53"/>
-      <c r="AD16" s="55"/>
-      <c r="AE16" s="53"/>
-      <c r="AH16" s="57"/>
-      <c r="AI16" s="4"/>
-      <c r="AJ16" s="4"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>13</v>
-      </c>
+    <row r="16" spans="1:36" s="92" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="93" t="s">
+        <v>445</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>446</v>
+      </c>
+      <c r="D16" s="94" t="s">
+        <v>489</v>
+      </c>
+      <c r="E16" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="108">
+        <f>[14]Main!$C$6</f>
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="G16" s="103">
+        <f>[14]Main!$C$8</f>
+        <v>10.16966</v>
+      </c>
+      <c r="H16" s="103">
+        <f>[14]Main!$C$11</f>
+        <v>-6.5050000000000026</v>
+      </c>
+      <c r="I16" s="103">
+        <f>[14]Main!$C$12</f>
+        <v>16.674660000000003</v>
+      </c>
+      <c r="J16" s="109" t="str">
+        <f>[14]Main!$C$28</f>
+        <v>H122</v>
+      </c>
+      <c r="K16" s="110">
+        <f>[14]Main!$D$28</f>
+        <v>44600</v>
+      </c>
+      <c r="L16" s="96"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="96"/>
+      <c r="T16" s="111">
+        <f>[14]Main!$C$33</f>
+        <v>0.20742534761796225</v>
+      </c>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
+      <c r="W16" s="94"/>
+      <c r="Y16" s="95">
+        <f>'[14]Financial Model'!$K$21</f>
+        <v>0.50353090223741115</v>
+      </c>
+      <c r="Z16" s="95">
+        <f>'[14]Financial Model'!$K$22</f>
+        <v>2.5932384981739429E-2</v>
+      </c>
+      <c r="AA16" s="95">
+        <f>'[14]Financial Model'!$K$23</f>
+        <v>1.7767906718489747E-2</v>
+      </c>
+      <c r="AB16" s="95">
+        <f>'[14]Financial Model'!$K$23</f>
+        <v>1.7767906718489747E-2</v>
+      </c>
+      <c r="AD16" s="96">
+        <f>[14]Main!$C$26</f>
+        <v>61.878</v>
+      </c>
+      <c r="AE16" s="95">
+        <f>'[14]Financial Model'!$K$65</f>
+        <v>0.44899775196702874</v>
+      </c>
+      <c r="AF16" s="94"/>
+      <c r="AG16" s="94"/>
+      <c r="AI16" s="94">
+        <f>[14]Main!$C$24</f>
+        <v>1989</v>
+      </c>
+      <c r="AJ16" s="92" t="str">
+        <f>[14]Main!$C$23</f>
+        <v>Market Harborough</v>
+      </c>
+    </row>
+    <row r="17" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="B17" s="3"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="L17" s="50"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+      <c r="AB17" s="53"/>
+      <c r="AD17" s="55"/>
+      <c r="AE17" s="53"/>
+      <c r="AH17" s="57"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+    </row>
+    <row r="18" spans="2:36" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>214</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>489</v>
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="I18" s="49"/>
       <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="2:36" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>445</v>
+        <v>214</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>446</v>
+        <v>488</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>489</v>
@@ -9449,7 +9691,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9468,7 +9710,19 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="B21" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>505</v>
+      </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -9478,12 +9732,12 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>492</v>
+        <v>511</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>493</v>
+        <v>512</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>31</v>
@@ -9500,29 +9754,15 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B23" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>505</v>
-      </c>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
       <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="56"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G24" s="49"/>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
@@ -9530,7 +9770,7 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
@@ -9538,77 +9778,69 @@
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="D26" s="105" t="s">
+        <v>495</v>
+      </c>
+      <c r="E26" s="106"/>
+      <c r="F26" s="42" t="s">
+        <v>496</v>
+      </c>
       <c r="G26" s="49"/>
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="D27" s="92" t="s">
-        <v>495</v>
-      </c>
-      <c r="E27" s="93"/>
-      <c r="F27" s="42" t="s">
-        <v>496</v>
+    </row>
+    <row r="27" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="D27" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="E27" s="44">
+        <v>0.85</v>
+      </c>
+      <c r="F27" s="45">
+        <f>1/E27</f>
+        <v>1.1764705882352942</v>
       </c>
       <c r="G27" s="49"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="D28" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E28" s="44">
-        <v>0.89</v>
-      </c>
-      <c r="F28" s="45">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="D28" s="46" t="s">
+        <v>498</v>
+      </c>
+      <c r="E28" s="48">
+        <v>0.87</v>
+      </c>
+      <c r="F28" s="47">
         <f>1/E28</f>
-        <v>1.1235955056179776</v>
+        <v>1.1494252873563218</v>
       </c>
       <c r="G28" s="49"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="D29" s="46" t="s">
-        <v>498</v>
-      </c>
-      <c r="E29" s="48">
-        <v>0.88</v>
-      </c>
-      <c r="F29" s="47">
-        <f>1/E29</f>
-        <v>1.1363636363636365</v>
-      </c>
+    <row r="29" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G29" s="49"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.15">
       <c r="G32" s="49"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G33" s="49"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.15">
-      <c r="G34" s="49"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -9625,9 +9857,10 @@
     <hyperlink ref="B9" r:id="rId11" xr:uid="{22F29850-B0EF-7041-BC72-9669C31D8AD8}"/>
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId14"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId15"/>
   <ignoredErrors>
     <ignoredError sqref="AH12 G12" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Add backdated £JOUL data for further analysis of collapse
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DA6752-794E-D44F-AEEF-BDBCC1204AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11C3D45-1147-4644-A039-A0A0A137DFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="500" windowWidth="27640" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="541">
   <si>
     <t>Ticker</t>
   </si>
@@ -1667,6 +1667,15 @@
   </si>
   <si>
     <t>(GBP)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Acquired by £FRAS 2022</t>
+  </si>
+  <si>
+    <t>Collapsed into administration Nov 2022</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1776,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1843,6 +1852,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1979,7 +2000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2263,15 +2284,6 @@
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="171" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2302,6 +2314,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3024,26 +3082,69 @@
             <v>0.20742534761796225</v>
           </cell>
         </row>
+        <row r="36">
+          <cell r="C36">
+            <v>8.2793743793445529</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>5.0560966752336345</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="21">
-          <cell r="K21">
-            <v>0.50353090223741115</v>
+        <row r="15">
+          <cell r="R15">
+            <v>-20.27600000000001</v>
+          </cell>
+          <cell r="S15">
+            <v>0.89299999999999291</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="S19">
+            <v>4.2969896440400834E-2</v>
           </cell>
         </row>
         <row r="22">
           <cell r="K22">
-            <v>2.5932384981739429E-2</v>
+            <v>0.50353090223741115</v>
           </cell>
         </row>
         <row r="23">
           <cell r="K23">
+            <v>2.5932384981739429E-2</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="K24">
             <v>1.7767906718489747E-2</v>
           </cell>
         </row>
-        <row r="65">
-          <cell r="K65">
+        <row r="25">
+          <cell r="K25">
+            <v>0.10901960784313716</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="K66">
             <v>0.44899775196702874</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="K67">
+            <v>0.32717055593685651</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="S80">
+            <v>3.3990470378499706</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="S82">
+            <v>0.23428321616827549</v>
           </cell>
         </row>
       </sheetData>
@@ -4216,8 +4317,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4808,47 +4909,47 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:14" s="128" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="119" t="s">
         <v>312</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="120" t="s">
         <v>302</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="122" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="123" t="s">
         <v>313</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="123" t="s">
         <v>314</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="123">
         <v>17.72</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="123">
         <v>4.3499999999999996</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="124">
         <v>1.39</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="123" t="s">
         <v>315</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="125">
         <v>0.92459999999999998</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="126">
         <v>44776</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="127" t="s">
         <v>316</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="125">
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
@@ -5864,47 +5965,47 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+    <row r="38" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61" t="s">
         <v>445</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="62" t="s">
         <v>446</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="67" t="s">
         <v>447</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="67" t="s">
         <v>448</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="67">
         <v>28.63</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="67">
         <v>13.37</v>
       </c>
-      <c r="I38" s="16">
+      <c r="I38" s="67">
         <v>2.92</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="65" t="s">
         <v>449</v>
       </c>
-      <c r="K38" s="32">
+      <c r="K38" s="118">
         <v>0.4834</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="M38" s="19" t="s">
+      <c r="M38" s="70" t="s">
         <v>450</v>
       </c>
-      <c r="N38" s="17">
+      <c r="N38" s="68">
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
@@ -6243,7 +6344,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+      <selection activeCell="E33" sqref="B25:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7993,13 +8094,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AJ33"/>
+  <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE14" sqref="AE14"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8017,66 +8118,67 @@
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="9.1640625" style="4"/>
     <col min="34" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="131" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
       <c r="R1" s="104">
         <f>AVERAGE(R3:R16)</f>
-        <v>1.1609166178244328</v>
+        <v>1.550434623565353</v>
       </c>
       <c r="S1" s="104">
         <f>AVERAGE(S3:S16)</f>
-        <v>14.027290837255359</v>
+        <v>12.698760362329685</v>
       </c>
       <c r="T1" s="104">
         <f>AVERAGE(T3:T16)</f>
         <v>2.6126027375685812</v>
       </c>
       <c r="U1" s="88"/>
-      <c r="V1" s="89">
-        <f>AVERAGE(V3:V16)</f>
-        <v>0.15708636175947649</v>
-      </c>
-      <c r="W1" s="89">
-        <f>AVERAGE(W3:W16)</f>
+      <c r="V1" s="117">
+        <f t="shared" ref="V1:AB1" si="0">AVERAGE(V3:V16)</f>
+        <v>0.14757665631622019</v>
+      </c>
+      <c r="W1" s="117">
+        <f t="shared" si="0"/>
         <v>6.1523225008126764E-2</v>
       </c>
-      <c r="X1" s="89">
-        <f>AVERAGE(X3:X16)</f>
+      <c r="X1" s="117">
+        <f t="shared" si="0"/>
         <v>0.10798125173689554</v>
       </c>
-      <c r="Y1" s="89">
-        <f>AVERAGE(Y3:Y16)</f>
+      <c r="Y1" s="117">
+        <f t="shared" si="0"/>
         <v>0.48923458289668553</v>
       </c>
-      <c r="Z1" s="89">
-        <f>AVERAGE(Z3:Z16)</f>
+      <c r="Z1" s="117">
+        <f t="shared" si="0"/>
         <v>5.2286639531140301E-2</v>
       </c>
-      <c r="AA1" s="89">
-        <f>AVERAGE(AA3:AA16)</f>
+      <c r="AA1" s="117">
+        <f t="shared" si="0"/>
         <v>3.6692022922336129E-2</v>
       </c>
-      <c r="AB1" s="89">
-        <f>AVERAGE(AB3:AB16)</f>
-        <v>5.6940421959518615E-2</v>
+      <c r="AB1" s="117">
+        <f t="shared" si="0"/>
+        <v>6.454473038657256E-2</v>
       </c>
       <c r="AC1" s="88"/>
       <c r="AD1" s="90" t="s">
@@ -8088,18 +8190,19 @@
       </c>
       <c r="AF1" s="89">
         <f>AVERAGE(AF3:AF16)</f>
-        <v>7.1548191262848185E-2</v>
+        <v>0.10806567193056367</v>
       </c>
       <c r="AG1" s="89">
         <f>AVERAGE(AG3:AG16)</f>
-        <v>0.23482149153783663</v>
+        <v>0.23476168316344095</v>
       </c>
       <c r="AH1" s="91">
         <f>AVERAGE(AH3:AH16)</f>
         <v>665.09462510297612</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AI1" s="91"/>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8203,8 +8306,11 @@
       <c r="AJ2" s="5" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AK2" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8323,7 +8429,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8427,7 +8533,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8542,7 +8648,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8661,7 +8767,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="97" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:37" s="97" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="98" t="s">
         <v>526</v>
       </c>
@@ -8716,7 +8822,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8839,7 +8945,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8870,7 +8976,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -8967,7 +9073,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -9093,7 +9199,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9217,7 +9323,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9332,91 +9438,94 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="112" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="113" t="s">
+    <row r="14" spans="1:37" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="110" t="s">
         <v>391</v>
       </c>
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="109" t="s">
         <v>392</v>
       </c>
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="114" t="s">
+      <c r="E14" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="115">
+      <c r="F14" s="112">
         <f>[12]Main!$C$6</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="G14" s="116">
+      <c r="G14" s="113">
         <f>[12]Main!$C$8</f>
         <v>201.23580000000001</v>
       </c>
-      <c r="H14" s="117">
+      <c r="H14" s="114">
         <f>[12]Main!$C$11</f>
         <v>14.5</v>
       </c>
-      <c r="I14" s="117">
+      <c r="I14" s="114">
         <f>[12]Main!$C$12</f>
         <v>186.73580000000001</v>
       </c>
-      <c r="J14" s="114" t="str">
+      <c r="J14" s="111" t="str">
         <f>[12]Main!$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="K14" s="114"/>
-      <c r="Q14" s="114"/>
-      <c r="U14" s="118"/>
-      <c r="V14" s="118">
+      <c r="K14" s="111"/>
+      <c r="Q14" s="111"/>
+      <c r="U14" s="115"/>
+      <c r="V14" s="115">
         <f>'[12]Financial Model'!$T$23</f>
         <v>0.20588400900900905</v>
       </c>
-      <c r="W14" s="114"/>
-      <c r="X14" s="114"/>
-      <c r="Y14" s="118">
+      <c r="W14" s="111"/>
+      <c r="X14" s="111"/>
+      <c r="Y14" s="115">
         <f>'[12]Financial Model'!$T$26</f>
         <v>0.55486890948567691</v>
       </c>
-      <c r="Z14" s="118">
+      <c r="Z14" s="115">
         <f>'[12]Financial Model'!$T$27</f>
         <v>-8.0487007680993719E-2</v>
       </c>
-      <c r="AA14" s="118">
+      <c r="AA14" s="115">
         <f>'[12]Financial Model'!$T$28</f>
         <v>-8.2866014521513875E-2</v>
       </c>
-      <c r="AB14" s="118">
+      <c r="AB14" s="115">
         <f>'[12]Financial Model'!$T$29</f>
         <v>0.19258416742493159</v>
       </c>
-      <c r="AD14" s="119">
+      <c r="AD14" s="116">
         <f>[12]Main!$C$26</f>
         <v>103.071</v>
       </c>
-      <c r="AE14" s="118">
+      <c r="AE14" s="115">
         <f>'[12]Financial Model'!$T$74</f>
         <v>0.17328795191694746</v>
       </c>
-      <c r="AF14" s="114"/>
-      <c r="AG14" s="118">
+      <c r="AF14" s="111"/>
+      <c r="AG14" s="115">
         <f>'[12]Financial Model'!$T$76</f>
         <v>0.24063455746737328</v>
       </c>
-      <c r="AH14" s="114">
+      <c r="AH14" s="111">
         <f>[12]Main!$C$25</f>
         <v>85</v>
       </c>
-      <c r="AI14" s="114">
+      <c r="AI14" s="111">
         <f>[12]Main!$C$24</f>
         <v>1987</v>
       </c>
-      <c r="AJ14" s="114" t="str">
+      <c r="AJ14" s="111" t="str">
         <f>[12]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="AK14" s="109" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9546,7 +9655,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:36" s="92" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:37" s="92" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="93" t="s">
         <v>445</v>
       </c>
@@ -9559,7 +9668,7 @@
       <c r="E16" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="108">
+      <c r="F16" s="105">
         <f>[14]Main!$C$6</f>
         <v>9.2200000000000004E-2</v>
       </c>
@@ -9575,50 +9684,78 @@
         <f>[14]Main!$C$12</f>
         <v>16.674660000000003</v>
       </c>
-      <c r="J16" s="109" t="str">
+      <c r="J16" s="106" t="str">
         <f>[14]Main!$C$28</f>
         <v>H122</v>
       </c>
-      <c r="K16" s="110">
+      <c r="K16" s="107">
         <f>[14]Main!$D$28</f>
         <v>44600</v>
       </c>
-      <c r="L16" s="96"/>
+      <c r="L16" s="132">
+        <f>[14]Main!$C$36</f>
+        <v>8.2793743793445529</v>
+      </c>
       <c r="M16" s="96"/>
       <c r="N16" s="96"/>
-      <c r="T16" s="111">
+      <c r="O16" s="96">
+        <f>'[14]Financial Model'!$S$15</f>
+        <v>0.89299999999999291</v>
+      </c>
+      <c r="P16" s="96">
+        <f>'[14]Financial Model'!$R$15</f>
+        <v>-20.27600000000001</v>
+      </c>
+      <c r="R16" s="108">
+        <f>[14]Main!$C$37</f>
+        <v>5.0560966752336345</v>
+      </c>
+      <c r="S16" s="108">
+        <f>'[14]Financial Model'!$S$80</f>
+        <v>3.3990470378499706</v>
+      </c>
+      <c r="T16" s="108">
         <f>[14]Main!$C$33</f>
         <v>0.20742534761796225</v>
       </c>
       <c r="U16" s="94"/>
-      <c r="V16" s="94"/>
+      <c r="V16" s="95">
+        <f>'[14]Financial Model'!$S$19</f>
+        <v>4.2969896440400834E-2</v>
+      </c>
       <c r="W16" s="94"/>
       <c r="Y16" s="95">
-        <f>'[14]Financial Model'!$K$21</f>
+        <f>'[14]Financial Model'!$K$22</f>
         <v>0.50353090223741115</v>
       </c>
       <c r="Z16" s="95">
-        <f>'[14]Financial Model'!$K$22</f>
+        <f>'[14]Financial Model'!$K$23</f>
         <v>2.5932384981739429E-2</v>
       </c>
       <c r="AA16" s="95">
-        <f>'[14]Financial Model'!$K$23</f>
+        <f>'[14]Financial Model'!$K$24</f>
         <v>1.7767906718489747E-2</v>
       </c>
       <c r="AB16" s="95">
-        <f>'[14]Financial Model'!$K$23</f>
-        <v>1.7767906718489747E-2</v>
+        <f>'[14]Financial Model'!$K$25</f>
+        <v>0.10901960784313716</v>
       </c>
       <c r="AD16" s="96">
         <f>[14]Main!$C$26</f>
         <v>61.878</v>
       </c>
       <c r="AE16" s="95">
-        <f>'[14]Financial Model'!$K$65</f>
+        <f>'[14]Financial Model'!$K$66</f>
         <v>0.44899775196702874</v>
       </c>
-      <c r="AF16" s="94"/>
-      <c r="AG16" s="94"/>
+      <c r="AF16" s="95">
+        <f>'[14]Financial Model'!$K$67</f>
+        <v>0.32717055593685651</v>
+      </c>
+      <c r="AG16" s="95">
+        <f>'[14]Financial Model'!$S$82</f>
+        <v>0.23428321616827549</v>
+      </c>
       <c r="AI16" s="94">
         <f>[14]Main!$C$24</f>
         <v>1989</v>
@@ -9626,6 +9763,9 @@
       <c r="AJ16" s="92" t="str">
         <f>[14]Main!$C$23</f>
         <v>Market Harborough</v>
+      </c>
+      <c r="AK16" s="92" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.15">
@@ -9779,10 +9919,10 @@
       <c r="N25" s="56"/>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.15">
-      <c r="D26" s="105" t="s">
+      <c r="D26" s="129" t="s">
         <v>495</v>
       </c>
-      <c r="E26" s="106"/>
+      <c r="E26" s="130"/>
       <c r="F26" s="42" t="s">
         <v>496</v>
       </c>

</xml_diff>

<commit_message>
Create empty £BRBY model
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D31807-BEB1-2143-A779-E0E96673A989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6988D5-29D7-4515-A651-AE19DF18AABF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="500" windowWidth="27640" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="4665" yWindow="495" windowWidth="27645" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -32,28 +32,19 @@
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="544">
   <si>
     <t>Ticker</t>
   </si>
@@ -1676,6 +1667,15 @@
   </si>
   <si>
     <t>Collapsed into administration Nov 2022</t>
+  </si>
+  <si>
+    <t>£BRBY</t>
+  </si>
+  <si>
+    <t>£MUL</t>
+  </si>
+  <si>
+    <t>Mulberry Group Plc</t>
   </si>
 </sst>
 </file>
@@ -1683,14 +1683,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2092,7 +2092,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2101,13 +2101,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2136,8 +2136,11 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2145,21 +2148,18 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2197,7 +2197,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2215,7 +2215,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2236,7 +2236,7 @@
     <xf numFmtId="15" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2263,7 +2263,7 @@
     <xf numFmtId="9" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2272,28 +2272,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="170" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="15" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2304,16 +2304,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2348,7 +2348,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3148,6 +3148,47 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>20.806000000000001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>8041.1028800000004</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>8041.1028800000004</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>London, UK</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1856</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4317,29 +4358,29 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4381,7 +4422,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>241</v>
       </c>
@@ -4425,7 +4466,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4469,7 +4510,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4513,7 +4554,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>259</v>
       </c>
@@ -4557,7 +4598,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4601,7 +4642,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4645,7 +4686,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4689,7 +4730,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4733,7 +4774,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4777,7 +4818,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4821,7 +4862,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>301</v>
       </c>
@@ -4865,7 +4906,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -4909,7 +4950,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="128" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="128" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="119" t="s">
         <v>312</v>
       </c>
@@ -4953,7 +4994,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -4997,7 +5038,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -5041,7 +5082,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -5085,7 +5126,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -5129,7 +5170,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -5173,7 +5214,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -5217,7 +5258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -5261,7 +5302,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5305,7 +5346,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5349,7 +5390,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5393,7 +5434,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5437,7 +5478,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5481,7 +5522,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5525,7 +5566,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="61" t="s">
         <v>391</v>
       </c>
@@ -5569,7 +5610,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5613,7 +5654,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5657,7 +5698,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>10</v>
       </c>
@@ -5701,7 +5742,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5745,7 +5786,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5789,7 +5830,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5833,7 +5874,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -5877,7 +5918,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -5921,7 +5962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -5965,7 +6006,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="61" t="s">
         <v>445</v>
       </c>
@@ -6009,7 +6050,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -6053,7 +6094,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -6097,7 +6138,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -6141,7 +6182,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -6185,7 +6226,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -6229,7 +6270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6344,28 +6385,28 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="B25:E33"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6407,7 +6448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6451,7 +6492,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6495,7 +6536,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6539,7 +6580,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6583,7 +6624,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>56</v>
       </c>
@@ -6627,7 +6668,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6671,7 +6712,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6715,7 +6756,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6759,7 +6800,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6803,7 +6844,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="60" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73" t="s">
         <v>86</v>
       </c>
@@ -6847,7 +6888,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
@@ -6891,7 +6932,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -6935,7 +6976,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -6979,7 +7020,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -7023,7 +7064,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -7067,7 +7108,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>121</v>
       </c>
@@ -7111,7 +7152,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -7155,7 +7196,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -7199,7 +7240,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -7243,7 +7284,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7287,7 +7328,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7331,7 +7372,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7375,7 +7416,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7419,7 +7460,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7463,7 +7504,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7507,7 +7548,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7551,7 +7592,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7595,7 +7636,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7639,7 +7680,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7683,7 +7724,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7727,7 +7768,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7771,7 +7812,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7815,7 +7856,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -7859,7 +7900,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -7903,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -7947,7 +7988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -7991,7 +8032,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -8097,33 +8138,33 @@
   <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="AI23" sqref="AI23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="23" width="9.1640625" style="4"/>
-    <col min="24" max="29" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="23" width="9.140625" style="4"/>
+    <col min="24" max="29" width="9.140625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.1640625" style="4"/>
-    <col min="34" max="35" width="9.1640625" style="1"/>
+    <col min="31" max="33" width="9.140625" style="4"/>
+    <col min="34" max="35" width="9.140625" style="1"/>
     <col min="36" max="36" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.1640625" style="1"/>
+    <col min="37" max="37" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="132" t="s">
         <v>499</v>
@@ -8202,7 +8243,7 @@
       </c>
       <c r="AI1" s="91"/>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8310,7 +8351,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8429,7 +8470,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8533,7 +8574,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8648,7 +8689,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8767,7 +8808,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:37" s="97" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:37" s="97" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="98" t="s">
         <v>526</v>
       </c>
@@ -8822,7 +8863,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8945,7 +8986,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -8976,7 +9017,7 @@
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -9073,7 +9114,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -9199,7 +9240,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9323,7 +9364,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9438,7 +9479,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="109" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:37" s="109" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="110" t="s">
         <v>391</v>
       </c>
@@ -9525,7 +9566,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9655,7 +9696,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:37" s="92" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:37" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="93" t="s">
         <v>445</v>
       </c>
@@ -9768,7 +9809,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="F17" s="7"/>
       <c r="G17" s="49"/>
@@ -9792,7 +9833,7 @@
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
     </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
@@ -9812,7 +9853,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
@@ -9831,7 +9872,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9850,7 +9891,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>492</v>
       </c>
@@ -9872,7 +9913,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>511</v>
       </c>
@@ -9894,15 +9935,51 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.15">
-      <c r="G23" s="49"/>
-      <c r="I23" s="4"/>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="54">
+        <f>[15]Main!$C$6</f>
+        <v>20.806000000000001</v>
+      </c>
+      <c r="G23" s="49">
+        <f>[15]Main!$C$8</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="I23" s="85">
+        <f>[15]Main!$C$12</f>
+        <v>8041.1028800000004</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
-    </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.15">
+      <c r="AI23" s="4">
+        <f>[15]Main!$C$24</f>
+        <v>1856</v>
+      </c>
+      <c r="AJ23" s="4" t="str">
+        <f>[15]Main!$C$23</f>
+        <v>London, UK</v>
+      </c>
+    </row>
+    <row r="24" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>543</v>
+      </c>
       <c r="G24" s="49"/>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
@@ -9910,7 +9987,7 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
       <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
@@ -9918,7 +9995,7 @@
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.2">
       <c r="D26" s="130" t="s">
         <v>495</v>
       </c>
@@ -9931,7 +10008,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.2">
       <c r="D27" s="43" t="s">
         <v>497</v>
       </c>
@@ -9947,7 +10024,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
       <c r="D28" s="46" t="s">
         <v>498</v>
       </c>
@@ -9963,19 +10040,19 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
       <c r="G32" s="49"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="49"/>
     </row>
   </sheetData>
@@ -9998,9 +10075,10 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
+    <hyperlink ref="B23" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId15"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId16"/>
   <ignoredErrors>
     <ignoredError sqref="AH12 G12" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Add Avg Rating column to Overview sheet
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F6B8A5-BED8-4E6B-9D05-988D56CCC679}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664DF23-D800-475F-811A-F994B90C8FA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="495" windowWidth="27645" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="545">
   <si>
     <t>Ticker</t>
   </si>
@@ -1676,6 +1676,9 @@
   </si>
   <si>
     <t>Mulberry Group Plc</t>
+  </si>
+  <si>
+    <t>Avg Rating</t>
   </si>
 </sst>
 </file>
@@ -2000,7 +2003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2361,6 +2364,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2955,6 +2964,11 @@
             <v>-3.0239089360221629</v>
           </cell>
         </row>
+        <row r="42">
+          <cell r="C42">
+            <v>4.097646421860806</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="17">
@@ -3021,8 +3035,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3997,6 +4011,11 @@
             <v>5.4526753959501493</v>
           </cell>
         </row>
+        <row r="42">
+          <cell r="C42">
+            <v>3.5843551695103639</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="4">
@@ -4063,7 +4082,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8148,13 +8167,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AK33"/>
+  <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ9" sqref="AJ9"/>
+      <selection pane="bottomRight" activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8171,13 +8190,15 @@
     <col min="24" max="29" width="9.140625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="9.140625" style="4"/>
-    <col min="34" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="1"/>
+    <col min="34" max="34" width="9.140625" style="1"/>
+    <col min="35" max="35" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" style="1"/>
+    <col min="37" max="37" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="133" t="s">
         <v>499</v>
@@ -8254,9 +8275,13 @@
         <f>AVERAGE(AH3:AH16)</f>
         <v>665.09462510297612</v>
       </c>
-      <c r="AI1" s="91"/>
-    </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI1" s="135">
+        <f>AVERAGE(AI3:AI16)</f>
+        <v>3.8410007956855852</v>
+      </c>
+      <c r="AJ1" s="91"/>
+    </row>
+    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8355,16 +8380,19 @@
         <v>516</v>
       </c>
       <c r="AI2" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8474,16 +8502,16 @@
         <f>'[1]Financial Model'!$AD$85</f>
         <v>0.18026118604153288</v>
       </c>
-      <c r="AI3" s="4">
+      <c r="AJ3" s="4">
         <f>[1]Main!$C$24</f>
         <v>1964</v>
       </c>
-      <c r="AJ3" s="4" t="str">
+      <c r="AK3" s="4" t="str">
         <f>[1]Main!$C$23</f>
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8578,16 +8606,17 @@
         <f>[2]Main!$C$25</f>
         <v>1297</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AI4" s="57"/>
+      <c r="AJ4" s="4">
         <f>[2]Main!$C$24</f>
         <v>1899</v>
       </c>
-      <c r="AJ4" s="4" t="str">
+      <c r="AK4" s="4" t="str">
         <f>[2]Main!$C$23</f>
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8693,16 +8722,17 @@
         <f>[3]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AI5" s="57"/>
+      <c r="AJ5" s="4">
         <f>[3]Main!$C$24</f>
         <v>1864</v>
       </c>
-      <c r="AJ5" s="4" t="str">
+      <c r="AK5" s="4" t="str">
         <f>[3]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8812,16 +8842,17 @@
         <f>[4]Main!$C$25</f>
         <v>3402</v>
       </c>
-      <c r="AI6" s="4">
+      <c r="AI6" s="57"/>
+      <c r="AJ6" s="4">
         <f>[4]Main!$C$24</f>
         <v>1981</v>
       </c>
-      <c r="AJ6" s="4" t="str">
+      <c r="AK6" s="4" t="str">
         <f>[4]Main!$C$23</f>
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:37" s="97" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" s="97" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="98" t="s">
         <v>526</v>
       </c>
@@ -8867,16 +8898,17 @@
         <f>[5]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="AI7" s="99">
+      <c r="AI7" s="99"/>
+      <c r="AJ7" s="99">
         <f>[5]Main!$C$24</f>
         <v>1982</v>
       </c>
-      <c r="AJ7" s="99" t="str">
+      <c r="AK7" s="99" t="str">
         <f>[5]Main!$C$23</f>
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -8990,16 +9022,17 @@
         <f>[6]Main!$C$26</f>
         <v>437</v>
       </c>
-      <c r="AI8" s="4">
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="4">
         <f>[6]Main!$C$24</f>
         <v>1996</v>
       </c>
-      <c r="AJ8" s="4" t="str">
+      <c r="AK8" s="4" t="str">
         <f>[6]Main!$C$23</f>
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -9029,16 +9062,16 @@
       <c r="N9" s="56"/>
       <c r="U9" s="53"/>
       <c r="AD9" s="56"/>
-      <c r="AI9" s="4">
+      <c r="AJ9" s="4">
         <f>[7]Main!$C$24</f>
         <v>1970</v>
       </c>
-      <c r="AJ9" s="4" t="str">
+      <c r="AK9" s="4" t="str">
         <f>[7]Main!$C$23</f>
         <v>Philadelphia, PA</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -9126,16 +9159,17 @@
         <f>[8]Main!$C$25</f>
         <v>1141</v>
       </c>
-      <c r="AI10" s="4">
+      <c r="AI10" s="57"/>
+      <c r="AJ10" s="4">
         <f>[8]Main!$C$24</f>
         <v>1977</v>
       </c>
-      <c r="AJ10" s="4" t="str">
+      <c r="AK10" s="4" t="str">
         <f>[8]Main!$C$23</f>
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -9252,16 +9286,20 @@
       <c r="AH11" s="57">
         <v>0</v>
       </c>
-      <c r="AI11" s="4">
+      <c r="AI11" s="134">
+        <f>[9]Main!$C$42</f>
+        <v>3.5843551695103639</v>
+      </c>
+      <c r="AJ11" s="4">
         <f>[9]Main!$C$24</f>
         <v>2000</v>
       </c>
-      <c r="AJ11" s="85" t="str">
+      <c r="AK11" s="85" t="str">
         <f>[9]Main!$C$23</f>
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9376,16 +9414,17 @@
         <f>[10]Main!$C$25</f>
         <v>734</v>
       </c>
-      <c r="AI12" s="4">
+      <c r="AI12" s="57"/>
+      <c r="AJ12" s="4">
         <f>[10]Main!$C$24</f>
         <v>1892</v>
       </c>
-      <c r="AJ12" s="4" t="str">
+      <c r="AK12" s="4" t="str">
         <f>[10]Main!$C$23</f>
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9491,16 +9530,17 @@
         <f>'[6]Financial Model'!$Y$24</f>
         <v>4.0876132736743287E-2</v>
       </c>
-      <c r="AI13" s="4">
+      <c r="AI13" s="53"/>
+      <c r="AJ13" s="4">
         <f>[11]Main!$C$24</f>
         <v>2006</v>
       </c>
-      <c r="AJ13" s="4" t="str">
+      <c r="AK13" s="4" t="str">
         <f>[11]Main!$C$23</f>
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="109" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" s="109" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="110" t="s">
         <v>391</v>
       </c>
@@ -9575,19 +9615,20 @@
         <f>[12]Main!$C$25</f>
         <v>85</v>
       </c>
-      <c r="AI14" s="111">
+      <c r="AI14" s="111"/>
+      <c r="AJ14" s="111">
         <f>[12]Main!$C$24</f>
         <v>1987</v>
       </c>
-      <c r="AJ14" s="111" t="str">
+      <c r="AK14" s="111" t="str">
         <f>[12]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AK14" s="109" t="s">
+      <c r="AL14" s="109" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9708,16 +9749,20 @@
         <f>[13]Main!$C$26</f>
         <v>220</v>
       </c>
-      <c r="AI15" s="4">
+      <c r="AI15" s="134">
+        <f>[13]Main!$C$42</f>
+        <v>4.097646421860806</v>
+      </c>
+      <c r="AJ15" s="4">
         <f>[13]Main!$C$25</f>
         <v>1985</v>
       </c>
-      <c r="AJ15" s="4" t="str">
+      <c r="AK15" s="4" t="str">
         <f>[13]Main!$C$24</f>
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:37" s="92" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="93" t="s">
         <v>445</v>
       </c>
@@ -9818,19 +9863,19 @@
         <f>'[14]Financial Model'!$S$82</f>
         <v>0.23428321616827549</v>
       </c>
-      <c r="AI16" s="94">
+      <c r="AJ16" s="94">
         <f>[14]Main!$C$24</f>
         <v>1989</v>
       </c>
-      <c r="AJ16" s="92" t="str">
+      <c r="AK16" s="92" t="str">
         <f>[14]Main!$C$23</f>
         <v>Market Harborough</v>
       </c>
-      <c r="AK16" s="92" t="s">
+      <c r="AL16" s="92" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="F17" s="7"/>
       <c r="G17" s="49"/>
@@ -9851,10 +9896,11 @@
       <c r="AD17" s="55"/>
       <c r="AE17" s="53"/>
       <c r="AH17" s="57"/>
-      <c r="AI17" s="4"/>
+      <c r="AI17" s="57"/>
       <c r="AJ17" s="4"/>
-    </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AK17" s="4"/>
+    </row>
+    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
@@ -9874,7 +9920,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
@@ -9897,7 +9943,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -9916,7 +9962,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>492</v>
       </c>
@@ -9938,7 +9984,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>511</v>
       </c>
@@ -9960,7 +10006,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>541</v>
       </c>
@@ -9989,16 +10035,16 @@
       <c r="K23" s="1"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
-      <c r="AI23" s="4">
+      <c r="AJ23" s="4">
         <f>[15]Main!$C$24</f>
         <v>1856</v>
       </c>
-      <c r="AJ23" s="4" t="str">
+      <c r="AK23" s="4" t="str">
         <f>[15]Main!$C$23</f>
         <v>London, UK</v>
       </c>
     </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>542</v>
       </c>
@@ -10012,7 +10058,7 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
@@ -10020,7 +10066,7 @@
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D26" s="131" t="s">
         <v>495</v>
       </c>
@@ -10033,7 +10079,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D27" s="43" t="s">
         <v>497</v>
       </c>
@@ -10049,7 +10095,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D28" s="46" t="s">
         <v>498</v>
       </c>
@@ -10065,16 +10111,16 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G32" s="49"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Q222 data for $AEO, more backdated metric calculations
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664DF23-D800-475F-811A-F994B90C8FA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FA0D16-6B8E-4BD7-B93D-EA18D8A1CBB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="495" windowWidth="27645" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="545">
   <si>
     <t>Ticker</t>
   </si>
@@ -3073,7 +3073,7 @@
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Market Harborough</v>
+            <v>Market Harborough, UK</v>
           </cell>
         </row>
         <row r="24">
@@ -3844,17 +3844,17 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>2176.5032000000001</v>
+            <v>2328.0418799999998</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-177</v>
+            <v>-278.30799999999999</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>2353.5032000000001</v>
+            <v>2606.3498799999998</v>
           </cell>
         </row>
         <row r="23">
@@ -3869,72 +3869,95 @@
         </row>
         <row r="25">
           <cell r="C25">
-            <v>1141</v>
+            <v>1160</v>
           </cell>
         </row>
         <row r="26">
           <cell r="C26">
-            <v>682.1</v>
+            <v>687.04600000000005</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28" t="str">
-            <v>Q122</v>
+            <v>Q222</v>
+          </cell>
+          <cell r="D28">
+            <v>44811</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>74.149439193446582</v>
+            <v>8.3153867603378018</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>5.160629036332355</v>
+            <v>11.122029267148672</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>1.573748197766315</v>
+            <v>1.6956827731781026</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>8.8873061964701936</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39">
+            <v>8.663850071253929</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="16">
-          <cell r="Y16">
+        <row r="17">
+          <cell r="Y17">
             <v>-209.33700000000022</v>
           </cell>
-          <cell r="Z16">
+          <cell r="Z17">
             <v>419.62599999999986</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="Z20">
+        <row r="21">
+          <cell r="Z21">
             <v>0.33299379683036578</v>
           </cell>
         </row>
-        <row r="23">
-          <cell r="O23">
-            <v>0.36778425780328089</v>
-          </cell>
-        </row>
         <row r="24">
-          <cell r="O24">
-            <v>3.9716142656608319E-2</v>
+          <cell r="P24">
+            <v>0.30883030470969619</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="O25">
-            <v>3.0084252969327211E-2</v>
+          <cell r="P25">
+            <v>1.1696619047778077E-2</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="O26">
-            <v>0.23990612577230669</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="O71">
-            <v>0.4615447248541884</v>
+          <cell r="P26">
+            <v>-3.5443743719347866E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="P27">
+            <v>0.10849393290506794</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="P72">
+            <v>0.36452124796676122</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="P73">
+            <v>7.2511361970386545E-3</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="P89">
+            <v>0.13644925222077642</v>
           </cell>
         </row>
       </sheetData>
@@ -4391,7 +4414,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:N23"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6416,7 +6439,7 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8170,10 +8193,10 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE11" sqref="AE11"/>
+      <selection pane="bottomRight" activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8193,7 +8216,7 @@
     <col min="34" max="34" width="9.140625" style="1"/>
     <col min="35" max="35" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.140625" style="1"/>
-    <col min="37" max="37" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -8216,15 +8239,15 @@
       <c r="Q1" s="133"/>
       <c r="R1" s="104">
         <f>AVERAGE(R3:R16)</f>
-        <v>2.253020008158559</v>
+        <v>2.8491600312401912</v>
       </c>
       <c r="S1" s="104">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.691069003608686</v>
+        <v>13.157317580593297</v>
       </c>
       <c r="T1" s="104">
         <f>AVERAGE(T3:T16)</f>
-        <v>2.960123877106037</v>
+        <v>2.9712088385071094</v>
       </c>
       <c r="U1" s="88"/>
       <c r="V1" s="117">
@@ -8241,19 +8264,19 @@
       </c>
       <c r="Y1" s="117">
         <f t="shared" si="0"/>
-        <v>0.48923458289668553</v>
+        <v>0.48432175347222012</v>
       </c>
       <c r="Z1" s="117">
         <f t="shared" si="0"/>
-        <v>5.2286639531140301E-2</v>
+        <v>4.9951679230404444E-2</v>
       </c>
       <c r="AA1" s="117">
         <f t="shared" si="0"/>
-        <v>3.6692022922336129E-2</v>
+        <v>3.12313565316132E-2</v>
       </c>
       <c r="AB1" s="117">
         <f t="shared" si="0"/>
-        <v>6.454473038657256E-2</v>
+        <v>5.3593714314302675E-2</v>
       </c>
       <c r="AC1" s="88"/>
       <c r="AD1" s="90" t="s">
@@ -8261,19 +8284,19 @@
       </c>
       <c r="AE1" s="89">
         <f>AVERAGE(AE3:AE16)</f>
-        <v>0.28208478568596257</v>
+        <v>0.27399949594534373</v>
       </c>
       <c r="AF1" s="89">
         <f>AVERAGE(AF3:AF16)</f>
-        <v>0.10806567193056367</v>
+        <v>9.5463854963873038E-2</v>
       </c>
       <c r="AG1" s="89">
         <f>AVERAGE(AG3:AG16)</f>
-        <v>0.23476168316344095</v>
+        <v>0.22493044006917443</v>
       </c>
       <c r="AH1" s="91">
         <f>AVERAGE(AH3:AH16)</f>
-        <v>665.09462510297612</v>
+        <v>666.82189783024887</v>
       </c>
       <c r="AI1" s="135">
         <f>AVERAGE(AI3:AI16)</f>
@@ -9090,74 +9113,94 @@
       </c>
       <c r="G10" s="49">
         <f>[8]Main!$C$8*E27</f>
-        <v>1828.262688</v>
+        <v>1955.5551791999997</v>
       </c>
       <c r="H10" s="49">
         <f>[8]Main!$C$11*$E$27</f>
-        <v>-148.68</v>
+        <v>-233.77871999999999</v>
       </c>
       <c r="I10" s="49">
         <f>[8]Main!$C$12*$E$27</f>
-        <v>1976.9426880000001</v>
+        <v>2189.3338991999999</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>[8]Main!$C$28</f>
-        <v>Q122</v>
+        <v>Q222</v>
+      </c>
+      <c r="K10" s="86">
+        <f>[8]Main!$D$28</f>
+        <v>44811</v>
       </c>
       <c r="L10" s="50">
         <f>[8]Main!$C$33</f>
-        <v>74.149439193446582</v>
+        <v>8.3153867603378018</v>
+      </c>
+      <c r="M10" s="50">
+        <f>[8]Main!$C$39</f>
+        <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$16*E27</f>
+        <f>'[8]Financial Model'!$Z$17*E27</f>
         <v>352.48583999999988</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$16*F27</f>
+        <f>'[8]Financial Model'!$Y$17*F27</f>
         <v>-249.21071428571454</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="52">
         <f>[8]Main!$C$34</f>
-        <v>5.160629036332355</v>
+        <v>11.122029267148672</v>
+      </c>
+      <c r="S10" s="52">
+        <f>[8]Main!$C$38</f>
+        <v>8.8873061964701936</v>
       </c>
       <c r="T10" s="52">
         <f>[8]Main!$C$36</f>
-        <v>1.573748197766315</v>
+        <v>1.6956827731781026</v>
       </c>
       <c r="U10" s="53"/>
       <c r="V10" s="53">
-        <f>'[8]Financial Model'!$Z$20</f>
+        <f>'[8]Financial Model'!$Z$21</f>
         <v>0.33299379683036578</v>
       </c>
       <c r="X10" s="4"/>
       <c r="Y10" s="53">
-        <f>'[8]Financial Model'!$O$23</f>
-        <v>0.36778425780328089</v>
+        <f>'[8]Financial Model'!$P$24</f>
+        <v>0.30883030470969619</v>
       </c>
       <c r="Z10" s="53">
-        <f>'[8]Financial Model'!$O$24</f>
-        <v>3.9716142656608319E-2</v>
+        <f>'[8]Financial Model'!$P$25</f>
+        <v>1.1696619047778077E-2</v>
       </c>
       <c r="AA10" s="53">
-        <f>'[8]Financial Model'!$O$25</f>
-        <v>3.0084252969327211E-2</v>
+        <f>'[8]Financial Model'!$P$26</f>
+        <v>-3.5443743719347866E-2</v>
       </c>
       <c r="AB10" s="53">
-        <f>'[8]Financial Model'!$O$26</f>
-        <v>0.23990612577230669</v>
+        <f>'[8]Financial Model'!$P$27</f>
+        <v>0.10849393290506794</v>
       </c>
       <c r="AD10" s="56">
         <f>[8]Main!$C$26*E27</f>
-        <v>572.96399999999994</v>
+        <v>577.11864000000003</v>
       </c>
       <c r="AE10" s="53">
-        <f>'[8]Financial Model'!$O$71</f>
-        <v>0.4615447248541884</v>
+        <f>'[8]Financial Model'!$P$72</f>
+        <v>0.36452124796676122</v>
+      </c>
+      <c r="AF10" s="53">
+        <f>'[8]Financial Model'!$P$73</f>
+        <v>7.2511361970386545E-3</v>
+      </c>
+      <c r="AG10" s="53">
+        <f>'[8]Financial Model'!$P$89</f>
+        <v>0.13644925222077642</v>
       </c>
       <c r="AH10" s="57">
         <f>[8]Main!$C$25</f>
-        <v>1141</v>
+        <v>1160</v>
       </c>
       <c r="AI10" s="57"/>
       <c r="AJ10" s="4">
@@ -9869,7 +9912,7 @@
       </c>
       <c r="AK16" s="92" t="str">
         <f>[14]Main!$C$23</f>
-        <v>Market Harborough</v>
+        <v>Market Harborough, UK</v>
       </c>
       <c r="AL16" s="92" t="s">
         <v>540</v>
@@ -10050,6 +10093,15 @@
       </c>
       <c r="C24" s="1" t="s">
         <v>543</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2.9</v>
       </c>
       <c r="G24" s="49"/>
       <c r="I24" s="4"/>

</xml_diff>

<commit_message>
Add £FRAS financial data, calc basic metrics
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B1E8F-E715-6749-B2F2-4EB41DD82760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A26CEE2-830E-4A5E-9B52-4267FFDA9930}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="500" windowWidth="27640" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="4665" yWindow="495" windowWidth="27645" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -39,16 +39,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1696,14 +1686,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2007,7 +1997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2099,7 +2089,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2108,13 +2098,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2143,8 +2133,11 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2152,21 +2145,18 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -2203,7 +2193,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2221,7 +2211,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2242,7 +2232,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2269,7 +2259,7 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2278,28 +2268,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2310,16 +2300,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2354,7 +2344,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2373,6 +2363,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3615,17 +3612,17 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>3929.6604000000002</v>
+            <v>3884.3565708599999</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>0</v>
+            <v>-275.20000000000005</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>3929.6604000000002</v>
+            <v>4159.5565708599997</v>
           </cell>
         </row>
         <row r="23">
@@ -3638,14 +3635,94 @@
             <v>1982</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="C25"/>
-        </row>
-        <row r="26">
-          <cell r="C26"/>
+        <row r="27">
+          <cell r="C27">
+            <v>1277.5999999999999</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>FY22</v>
+          </cell>
+          <cell r="D29">
+            <v>44765</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>15.120111213935388</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>0.8656184985037354</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>2.9683299486932606</v>
+          </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="24">
+          <cell r="S24">
+            <v>100.99999999999994</v>
+          </cell>
+          <cell r="T24">
+            <v>-77.999999999999801</v>
+          </cell>
+          <cell r="U24">
+            <v>256.89999999999992</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="S28">
+            <v>6.9018612064075224E-2</v>
+          </cell>
+          <cell r="T28">
+            <v>-8.3918734522666405E-2</v>
+          </cell>
+          <cell r="U28">
+            <v>0.3254903042506827</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="U31">
+            <v>0.43466588974673792</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="U32">
+            <v>6.8757413689051639E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="U33">
+            <v>5.3461802592970245E-2</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="U34">
+            <v>0.2345053635280096</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="U76">
+            <v>0.16505562648185301</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="U78">
+            <v>0.26587309845379059</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="U87">
+            <v>12.474551050136244</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4474,25 +4551,25 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4534,7 +4611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -4578,7 +4655,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4622,7 +4699,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -4666,7 +4743,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -4710,7 +4787,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -4754,7 +4831,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -4798,7 +4875,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -4842,7 +4919,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -4886,7 +4963,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -4930,7 +5007,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -4974,7 +5051,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -5018,7 +5095,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -5062,7 +5139,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="127" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="127" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="118" t="s">
         <v>312</v>
       </c>
@@ -5106,7 +5183,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -5150,7 +5227,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -5194,7 +5271,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -5238,7 +5315,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -5282,7 +5359,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -5326,7 +5403,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -5370,7 +5447,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -5414,7 +5491,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5458,7 +5535,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5502,7 +5579,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5546,7 +5623,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5590,7 +5667,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5634,7 +5711,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -5678,7 +5755,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -5722,7 +5799,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -5766,7 +5843,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -5810,7 +5887,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -5854,7 +5931,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -5898,7 +5975,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -5942,7 +6019,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -5986,7 +6063,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -6030,7 +6107,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -6074,7 +6151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -6118,7 +6195,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -6162,7 +6239,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -6206,7 +6283,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -6250,7 +6327,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -6294,7 +6371,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -6338,7 +6415,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -6382,7 +6459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6500,25 +6577,25 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6560,7 +6637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6604,7 +6681,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6648,7 +6725,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -6692,7 +6769,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -6736,7 +6813,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -6780,7 +6857,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -6824,7 +6901,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -6868,7 +6945,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -6912,7 +6989,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -6956,7 +7033,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -7000,7 +7077,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -7044,7 +7121,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -7088,7 +7165,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -7132,7 +7209,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -7176,7 +7253,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -7220,7 +7297,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -7264,7 +7341,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -7308,7 +7385,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -7352,7 +7429,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -7396,7 +7473,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7440,7 +7517,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7484,7 +7561,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7528,7 +7605,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7572,7 +7649,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7616,7 +7693,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -7660,7 +7737,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -7704,7 +7781,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -7748,7 +7825,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -7792,7 +7869,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -7836,7 +7913,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -7880,7 +7957,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -7924,7 +8001,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -7968,7 +8045,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -8012,7 +8089,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -8056,7 +8133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -8100,7 +8177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -8144,7 +8221,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -8253,32 +8330,32 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="23" width="9.1640625" style="4"/>
-    <col min="24" max="29" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="23" width="9.140625" style="4"/>
+    <col min="24" max="29" width="9.140625" style="1"/>
     <col min="30" max="30" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.1640625" style="4"/>
-    <col min="34" max="34" width="9.1640625" style="1"/>
-    <col min="35" max="35" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.1640625" style="1"/>
-    <col min="37" max="37" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.1640625" style="1"/>
+    <col min="31" max="33" width="9.140625" style="4"/>
+    <col min="34" max="34" width="9.140625" style="1"/>
+    <col min="35" max="35" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" style="1"/>
+    <col min="37" max="37" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="134" t="s">
         <v>499</v>
@@ -8296,44 +8373,44 @@
       <c r="Q1" s="134"/>
       <c r="R1" s="103">
         <f>AVERAGE(R3:R16)</f>
-        <v>2.8491600312401912</v>
+        <v>3.9647010478488456</v>
       </c>
       <c r="S1" s="103">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.157317580593297</v>
+        <v>13.089040927547591</v>
       </c>
       <c r="T1" s="103">
         <f>AVERAGE(T3:T16)</f>
-        <v>2.8418722706699513</v>
+        <v>2.8515997843640526</v>
       </c>
       <c r="U1" s="87"/>
       <c r="V1" s="116">
         <f t="shared" ref="V1:AB1" si="0">AVERAGE(V3:V16)</f>
-        <v>0.14757665631622019</v>
+        <v>0.16126232154194811</v>
       </c>
       <c r="W1" s="116">
         <f t="shared" si="0"/>
-        <v>6.1523225008126764E-2</v>
+        <v>4.5363007282483075E-2</v>
       </c>
       <c r="X1" s="116">
         <f t="shared" si="0"/>
-        <v>0.10798125173689554</v>
-      </c>
-      <c r="Y1" s="116">
+        <v>0.10365206955102663</v>
+      </c>
+      <c r="Y1" s="88">
         <f t="shared" si="0"/>
-        <v>0.47141301821392373</v>
-      </c>
-      <c r="Z1" s="116">
+        <v>0.46878822332341041</v>
+      </c>
+      <c r="Z1" s="88">
         <f t="shared" si="0"/>
-        <v>5.1687619547455682E-2</v>
-      </c>
-      <c r="AA1" s="116">
+        <v>5.2906890557569683E-2</v>
+      </c>
+      <c r="AA1" s="88">
         <f t="shared" si="0"/>
-        <v>3.2694833069821697E-2</v>
-      </c>
-      <c r="AB1" s="116">
+        <v>3.4178188035760886E-2</v>
+      </c>
+      <c r="AB1" s="88">
         <f t="shared" si="0"/>
-        <v>7.1642340944028784E-2</v>
+        <v>8.3275413985741703E-2</v>
       </c>
       <c r="AC1" s="87"/>
       <c r="AD1" s="89" t="s">
@@ -8341,7 +8418,7 @@
       </c>
       <c r="AE1" s="88">
         <f>AVERAGE(AE3:AE16)</f>
-        <v>0.28704593489811547</v>
+        <v>0.278332341439811</v>
       </c>
       <c r="AF1" s="88">
         <f>AVERAGE(AF3:AF16)</f>
@@ -8349,7 +8426,7 @@
       </c>
       <c r="AG1" s="88">
         <f>AVERAGE(AG3:AG16)</f>
-        <v>0.22493044006917443</v>
+        <v>0.22865249992232137</v>
       </c>
       <c r="AH1" s="90">
         <f>AVERAGE(AH3:AH16)</f>
@@ -8361,7 +8438,7 @@
       </c>
       <c r="AJ1" s="90"/>
     </row>
-    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8472,7 +8549,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8591,7 +8668,7 @@
         <v>Beaverton, OR</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8696,7 +8773,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -8812,7 +8889,7 @@
         <v>Leicester, UK</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8932,7 +9009,7 @@
         <v>Bury, UK</v>
       </c>
     </row>
-    <row r="7" spans="1:38" s="96" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:38" s="96" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="97" t="s">
         <v>526</v>
       </c>
@@ -8951,31 +9028,96 @@
       </c>
       <c r="G7" s="100">
         <f>[5]Main!$C$8</f>
-        <v>3929.6604000000002</v>
+        <v>3884.3565708599999</v>
       </c>
       <c r="H7" s="100">
         <f>[5]Main!$C$11</f>
-        <v>0</v>
+        <v>-275.20000000000005</v>
       </c>
       <c r="I7" s="100">
         <f>[5]Main!$C$12</f>
-        <v>3929.6604000000002</v>
-      </c>
-      <c r="K7" s="98"/>
-      <c r="Q7" s="98"/>
+        <v>4159.5565708599997</v>
+      </c>
+      <c r="J7" s="98" t="str">
+        <f>[5]Main!$C$29</f>
+        <v>FY22</v>
+      </c>
+      <c r="K7" s="137">
+        <f>[5]Main!$D$29</f>
+        <v>44765</v>
+      </c>
+      <c r="L7" s="136">
+        <f>[5]Main!$C$36</f>
+        <v>0.8656184985037354</v>
+      </c>
+      <c r="O7" s="96">
+        <f>'[5]Financial Model'!$U$24</f>
+        <v>256.89999999999992</v>
+      </c>
+      <c r="P7" s="135">
+        <f>'[5]Financial Model'!$T$24</f>
+        <v>-77.999999999999801</v>
+      </c>
+      <c r="Q7" s="55">
+        <f>'[5]Financial Model'!$S$24</f>
+        <v>100.99999999999994</v>
+      </c>
+      <c r="R7" s="136">
+        <f>[5]Main!$C$35</f>
+        <v>15.120111213935388</v>
+      </c>
+      <c r="S7" s="136">
+        <f>'[5]Financial Model'!$U$87</f>
+        <v>12.474551050136244</v>
+      </c>
+      <c r="T7" s="136">
+        <f>[5]Main!$C$37</f>
+        <v>2.9683299486932606</v>
+      </c>
       <c r="U7" s="101"/>
-      <c r="V7" s="98"/>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
+      <c r="V7" s="101">
+        <f>'[5]Financial Model'!$U$28</f>
+        <v>0.3254903042506827</v>
+      </c>
+      <c r="W7" s="101">
+        <f>'[5]Financial Model'!$T$28</f>
+        <v>-8.3918734522666405E-2</v>
+      </c>
+      <c r="X7" s="101">
+        <f>'[5]Financial Model'!$S$28</f>
+        <v>6.9018612064075224E-2</v>
+      </c>
+      <c r="Y7" s="101">
+        <f>'[5]Financial Model'!$U$31</f>
+        <v>0.43466588974673792</v>
+      </c>
+      <c r="Z7" s="101">
+        <f>'[5]Financial Model'!$U$32</f>
+        <v>6.8757413689051639E-2</v>
+      </c>
+      <c r="AA7" s="101">
+        <f>'[5]Financial Model'!$U$33</f>
+        <v>5.3461802592970245E-2</v>
+      </c>
+      <c r="AB7" s="101">
+        <f>'[5]Financial Model'!$U$34</f>
+        <v>0.2345053635280096</v>
+      </c>
       <c r="AD7" s="100">
+        <f>[5]Main!$C$27</f>
+        <v>1277.5999999999999</v>
+      </c>
+      <c r="AE7" s="101">
+        <f>'[5]Financial Model'!$U$76</f>
+        <v>0.16505562648185301</v>
+      </c>
+      <c r="AF7" s="98"/>
+      <c r="AG7" s="101">
+        <f>'[5]Financial Model'!$U$78</f>
+        <v>0.26587309845379059</v>
+      </c>
+      <c r="AH7" s="98">
         <f>[5]Main!$C$26</f>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="98"/>
-      <c r="AF7" s="98"/>
-      <c r="AG7" s="98"/>
-      <c r="AH7" s="98">
-        <f>[5]Main!$C$25</f>
         <v>0</v>
       </c>
       <c r="AI7" s="98"/>
@@ -8988,7 +9130,7 @@
         <v>Mansfiled, UK</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -9112,7 +9254,7 @@
         <v>Baltimore, US</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -9190,7 +9332,7 @@
         <v>Philadelphia, PA</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -9308,7 +9450,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -9438,7 +9580,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9563,7 +9705,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -9679,7 +9821,7 @@
         <v>Manchester, UK</v>
       </c>
     </row>
-    <row r="14" spans="1:38" s="108" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:38" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="109" t="s">
         <v>391</v>
       </c>
@@ -9767,7 +9909,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -9901,7 +10043,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="91" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:38" s="91" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -10014,7 +10156,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="F17" s="7"/>
       <c r="G17" s="49"/>
@@ -10039,7 +10181,7 @@
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
@@ -10059,7 +10201,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
@@ -10082,7 +10224,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -10101,7 +10243,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>492</v>
       </c>
@@ -10123,7 +10265,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>511</v>
       </c>
@@ -10145,7 +10287,7 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>541</v>
       </c>
@@ -10183,7 +10325,7 @@
         <v>London, UK</v>
       </c>
     </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>542</v>
       </c>
@@ -10206,7 +10348,7 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
@@ -10214,7 +10356,7 @@
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D26" s="132" t="s">
         <v>495</v>
       </c>
@@ -10227,7 +10369,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D27" s="43" t="s">
         <v>497</v>
       </c>
@@ -10243,7 +10385,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
       <c r="D28" s="46" t="s">
         <v>498</v>
       </c>
@@ -10259,19 +10401,19 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
       <c r="G32" s="49"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="49"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some company metadata to Fashion Retailers overview
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB481464-B497-433E-AC6D-3645A69EC9DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDBCDAA-3D6A-44A9-983A-DC505A7B1332}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="495" windowWidth="27645" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="551">
   <si>
     <t>Ticker</t>
   </si>
@@ -1663,9 +1663,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Acquired by £FRAS 2022</t>
-  </si>
-  <si>
     <t>Collapsed into administration Nov 2022</t>
   </si>
   <si>
@@ -1679,6 +1676,27 @@
   </si>
   <si>
     <t>Avg Rating</t>
+  </si>
+  <si>
+    <t>Fashion &amp; Home</t>
+  </si>
+  <si>
+    <t>Food, Fashion &amp; Home</t>
+  </si>
+  <si>
+    <t>Luxury Goods</t>
+  </si>
+  <si>
+    <t>Acquired by Authentic Brands Group 2022</t>
+  </si>
+  <si>
+    <t>Online Outlet</t>
+  </si>
+  <si>
+    <t>Sports Fashion</t>
+  </si>
+  <si>
+    <t>Retail Conglomerate, Sports Fashion</t>
   </si>
 </sst>
 </file>
@@ -1997,7 +2015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2370,6 +2388,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2842,8 +2863,21 @@
             <v>FY22</v>
           </cell>
         </row>
+        <row r="36">
+          <cell r="C36">
+            <v>1.6714759317373831</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="19">
+          <cell r="S19">
+            <v>-86.51600000000002</v>
+          </cell>
+          <cell r="T19">
+            <v>-35.494000000000035</v>
+          </cell>
+        </row>
         <row r="23">
           <cell r="T23">
             <v>0.20588400900900905</v>
@@ -8335,10 +8369,10 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8359,7 +8393,7 @@
     <col min="35" max="35" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.140625" style="1"/>
     <col min="37" max="37" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -8389,7 +8423,7 @@
       </c>
       <c r="T1" s="103">
         <f>AVERAGE(T3:T16)</f>
-        <v>2.846561257217036</v>
+        <v>2.7626265911113466</v>
       </c>
       <c r="U1" s="87"/>
       <c r="V1" s="116">
@@ -8545,7 +8579,7 @@
         <v>516</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>521</v>
@@ -8553,7 +8587,7 @@
       <c r="AK2" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AL2" s="5" t="s">
         <v>538</v>
       </c>
     </row>
@@ -8675,6 +8709,9 @@
         <f>[1]Main!$C$23</f>
         <v>Beaverton, OR</v>
       </c>
+      <c r="AL3" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
@@ -8896,6 +8933,9 @@
         <f>[3]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
+      <c r="AL5" s="4" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -9016,6 +9056,9 @@
         <f>[4]Main!$C$23</f>
         <v>Bury, UK</v>
       </c>
+      <c r="AL6" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="7" spans="1:38" s="96" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="97" t="s">
@@ -9137,6 +9180,9 @@
         <f>[5]Main!$C$23</f>
         <v>Mansfiled, UK</v>
       </c>
+      <c r="AL7" s="98" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -9261,6 +9307,9 @@
         <f>[6]Main!$C$23</f>
         <v>Baltimore, US</v>
       </c>
+      <c r="AL8" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
@@ -9284,12 +9333,12 @@
         <v>1976.693296032</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11</f>
-        <v>389.041</v>
+        <f>[7]Main!$C$11*E27</f>
+        <v>326.79444000000001</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12</f>
-        <v>1964.1653048000001</v>
+        <f>[7]Main!$C$12*E27</f>
+        <v>1649.8988560319999</v>
       </c>
       <c r="J9" s="98" t="str">
         <f>[7]Main!$C$29</f>
@@ -9324,8 +9373,8 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AD9" s="56">
-        <f>[7]Main!$C$26</f>
-        <v>743.57899999999995</v>
+        <f>[7]Main!$C$26*E27</f>
+        <v>624.60635999999988</v>
       </c>
       <c r="AE9" s="53">
         <f>'[7]Financial Model'!$M$63</f>
@@ -9591,6 +9640,9 @@
         <f>[9]Main!$C$23</f>
         <v>London, UK</v>
       </c>
+      <c r="AL11" s="4" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
@@ -9832,6 +9884,9 @@
         <f>[11]Main!$C$23</f>
         <v>Manchester, UK</v>
       </c>
+      <c r="AL13" s="4" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="14" spans="1:38" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="109" t="s">
@@ -9867,7 +9922,19 @@
         <v>FY22</v>
       </c>
       <c r="K14" s="110"/>
+      <c r="O14" s="115">
+        <f>'[12]Financial Model'!$T$19</f>
+        <v>-35.494000000000035</v>
+      </c>
+      <c r="P14" s="115">
+        <f>'[12]Financial Model'!$S$19</f>
+        <v>-86.51600000000002</v>
+      </c>
       <c r="Q14" s="110"/>
+      <c r="T14" s="138">
+        <f>[12]Main!$C$36</f>
+        <v>1.6714759317373831</v>
+      </c>
       <c r="U14" s="114"/>
       <c r="V14" s="114">
         <f>'[12]Financial Model'!$T$23</f>
@@ -9917,8 +9984,8 @@
         <f>[12]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AL14" s="108" t="s">
-        <v>539</v>
+      <c r="AL14" s="110" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
@@ -10164,11 +10231,11 @@
         <f>[14]Main!$C$23</f>
         <v>Market Harborough, UK</v>
       </c>
-      <c r="AL16" s="91" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AL16" s="93" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="17" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="F17" s="7"/>
       <c r="G17" s="49"/>
@@ -10193,7 +10260,7 @@
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
@@ -10212,8 +10279,11 @@
       <c r="L18" s="56"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AL18" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="19" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
@@ -10236,7 +10306,7 @@
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>503</v>
       </c>
@@ -10255,7 +10325,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>492</v>
       </c>
@@ -10277,7 +10347,7 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>511</v>
       </c>
@@ -10298,10 +10368,13 @@
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
-    </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AL22" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="23" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>260</v>
@@ -10336,13 +10409,16 @@
         <f>[15]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-    </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AL23" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="24" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>543</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>489</v>
@@ -10359,8 +10435,11 @@
       <c r="K24" s="1"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
-    </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AL24" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="25" spans="2:38" x14ac:dyDescent="0.2">
       <c r="G25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
@@ -10368,7 +10447,7 @@
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:38" x14ac:dyDescent="0.2">
       <c r="D26" s="135" t="s">
         <v>495</v>
       </c>
@@ -10381,7 +10460,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:38" x14ac:dyDescent="0.2">
       <c r="D27" s="43" t="s">
         <v>497</v>
       </c>
@@ -10397,7 +10476,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:38" x14ac:dyDescent="0.2">
       <c r="D28" s="46" t="s">
         <v>498</v>
       </c>
@@ -10413,16 +10492,16 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:38" x14ac:dyDescent="0.2">
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:38" x14ac:dyDescent="0.2">
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:38" x14ac:dyDescent="0.2">
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:38" x14ac:dyDescent="0.2">
       <c r="G32" s="49"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Start £ITS model, add to Fashion Retailer overview
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842B2B72-7BC1-41FD-B77A-30CC1E2648BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7211D54-14F0-467D-87D7-E3146C009BB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2025" yWindow="495" windowWidth="30285" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -33,6 +33,7 @@
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="556">
   <si>
     <t>Ticker</t>
   </si>
@@ -1700,6 +1701,18 @@
   </si>
   <si>
     <t>ROCE</t>
+  </si>
+  <si>
+    <t>Luxury Fashion &amp; Cosmetics</t>
+  </si>
+  <si>
+    <t>Luxury Fashion</t>
+  </si>
+  <si>
+    <t>Luxury Apparel</t>
+  </si>
+  <si>
+    <t>Online Womenswear &amp; Wholesale</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1729,7 @@
     <numFmt numFmtId="169" formatCode="0.0"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1807,6 +1820,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2035,7 +2056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2422,6 +2443,7 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2990,12 +3012,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>1.3308</v>
+            <v>1.05</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>108.96466901759999</v>
+            <v>85.9730256</v>
           </cell>
         </row>
         <row r="11">
@@ -3005,7 +3027,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>100.66466901759999</v>
+            <v>77.673025600000003</v>
           </cell>
         </row>
         <row r="24">
@@ -3038,17 +3060,17 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>4.4345669170748829</v>
+            <v>3.4217191894273076</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>4.8002056835947062</v>
+            <v>3.7873579559471304</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1.048745611333975</v>
+            <v>0.82745934167468738</v>
           </cell>
         </row>
         <row r="38">
@@ -3058,12 +3080,12 @@
         </row>
         <row r="39">
           <cell r="C39">
-            <v>-3.0239089360221629</v>
+            <v>-2.3858614238227163</v>
           </cell>
         </row>
         <row r="42">
           <cell r="C42">
-            <v>4.097646421860806</v>
+            <v>4.0934845655588719</v>
           </cell>
         </row>
       </sheetData>
@@ -3132,8 +3154,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3306,8 +3328,97 @@
             <v>1856</v>
           </cell>
         </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D29">
+            <v>44882</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="K28">
+            <v>0.70111524163568772</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="K29">
+            <v>0.19553903345724907</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="K30">
+            <v>0.14423791821561338</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="K31">
+            <v>0.22709163346613545</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>0.13569999999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>7.1242499999999991</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>7.1242499999999991</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Salford, UK</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2013</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>FH123</v>
+          </cell>
+          <cell r="D28">
+            <v>44903</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="17">
+          <cell r="K17">
+            <v>0.48510270107591608</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3325,12 +3436,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>33.08</v>
+            <v>33.22</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>12824.719039999998</v>
+            <v>12878.995359999999</v>
           </cell>
         </row>
         <row r="11">
@@ -3340,7 +3451,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>17490.75404</v>
+            <v>17545.030359999997</v>
           </cell>
         </row>
         <row r="23">
@@ -3373,17 +3484,17 @@
         </row>
         <row r="33">
           <cell r="C33">
-            <v>12.611393343865217</v>
+            <v>12.65052830735576</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>9.3091188772666609</v>
+            <v>9.3485165992381649</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>4.156264394115186</v>
+            <v>4.1738543885280066</v>
           </cell>
         </row>
       </sheetData>
@@ -3742,6 +3853,9 @@
             <v>1982</v>
           </cell>
         </row>
+        <row r="26">
+          <cell r="C26"/>
+        </row>
         <row r="27">
           <cell r="C27">
             <v>1277.5999999999999</v>
@@ -3983,7 +4097,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4307,18 +4421,18 @@
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="4">
-          <cell r="Q4">
-            <v>2733.5</v>
-          </cell>
-          <cell r="R4">
-            <v>3263.5</v>
-          </cell>
-          <cell r="S4">
-            <v>3910.5</v>
-          </cell>
-          <cell r="T4">
-            <v>3936.5</v>
+        <row r="15">
+          <cell r="Q15">
+            <v>24.599999999999909</v>
+          </cell>
+          <cell r="R15">
+            <v>113.30000000000014</v>
+          </cell>
+          <cell r="S15">
+            <v>128.40000000000015</v>
+          </cell>
+          <cell r="T15">
+            <v>-30.80000000000009</v>
           </cell>
         </row>
         <row r="19">
@@ -4371,7 +4485,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8456,13 +8570,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AM33"/>
+  <dimension ref="A1:AM36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:Q1"/>
+      <selection pane="bottomRight" activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8489,31 +8603,31 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="145" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="144"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
       <c r="R1" s="103">
         <f>AVERAGE(R3:R16)</f>
-        <v>14.447275691579479</v>
+        <v>14.358780236518021</v>
       </c>
       <c r="S1" s="103">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.176053771165707</v>
+        <v>13.239858522385651</v>
       </c>
       <c r="T1" s="103">
         <f>AVERAGE(T3:T16)</f>
-        <v>2.7839366083880521</v>
+        <v>2.7693868744418757</v>
       </c>
       <c r="U1" s="116">
         <f t="shared" ref="U1:AC1" si="0">AVERAGE(U3:U16)</f>
@@ -8533,8 +8647,8 @@
         <v>0.10365206955102663</v>
       </c>
       <c r="Z1" s="88">
-        <f t="shared" si="0"/>
-        <v>0.46881441387493933</v>
+        <f>AVERAGE(Z3:Z17)</f>
+        <v>0.4699002996883378</v>
       </c>
       <c r="AA1" s="88">
         <f t="shared" si="0"/>
@@ -8570,7 +8684,7 @@
       </c>
       <c r="AJ1" s="131">
         <f>AVERAGE(AJ3:AJ16)</f>
-        <v>3.8410007956855852</v>
+        <v>3.8389198675346181</v>
       </c>
       <c r="AK1" s="90"/>
     </row>
@@ -8702,19 +8816,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$27</f>
+        <f>[1]Main!$C$6*$E$30</f>
         <v>87.498599999999996</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$27</f>
+        <f>[1]Main!$C$8*$E$30</f>
         <v>137119.05606</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$27</f>
+        <f>[1]Main!$C$11*$E$30</f>
         <v>2029.35</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$27</f>
+        <f>[1]Main!$C$12*$E$30</f>
         <v>135089.70606</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -8730,15 +8844,15 @@
         <v>26.920059874297088</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E27</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E30</f>
         <v>5018.1799999999939</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AC$21*1000*E27</f>
+        <f>'[1]Financial Model'!$AC$21*1000*E30</f>
         <v>4753.409999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AB$21*1000*E27</f>
+        <f>'[1]Financial Model'!$AB$21*1000*E30</f>
         <v>2107.37</v>
       </c>
       <c r="R3" s="51">
@@ -8784,7 +8898,7 @@
         <v>0.19693654266958391</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E27</f>
+        <f>[1]Main!$C$26*E30</f>
         <v>8019.46</v>
       </c>
       <c r="AF3" s="53">
@@ -8825,20 +8939,20 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$27</f>
-        <v>27.456399999999999</v>
+        <f>[2]Main!$C$6*$E$30</f>
+        <v>27.572599999999998</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$27</f>
-        <v>10644.516803199998</v>
+        <f>[2]Main!$C$8*$E$30</f>
+        <v>10689.566148799999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$27</f>
+        <f>[2]Main!$C$11*$E$30</f>
         <v>-3872.8090499999998</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$27</f>
-        <v>14517.3258532</v>
+        <f>[2]Main!$C$12*$E$30</f>
+        <v>14562.375198799997</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>[2]Main!$C$28</f>
@@ -8850,27 +8964,27 @@
       </c>
       <c r="L4" s="50">
         <f>[2]Main!$C$33</f>
-        <v>12.611393343865217</v>
+        <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E27</f>
+        <f>'[2]Financial Model'!$AA$22*E30</f>
         <v>1151.127829999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$27</f>
+        <f>'[2]Financial Model'!$Z$22*$E$30</f>
         <v>338.51467000000116</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$27</f>
+        <f>'[2]Financial Model'!$Y$22*$E$30</f>
         <v>563.94267000000013</v>
       </c>
       <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
-        <v>9.3091188772666609</v>
+        <v>9.3485165992381649</v>
       </c>
       <c r="T4" s="51">
         <f>[2]Main!$C$36</f>
-        <v>4.156264394115186</v>
+        <v>4.1738543885280066</v>
       </c>
       <c r="U4" s="53"/>
       <c r="V4" s="53"/>
@@ -8896,7 +9010,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E27</f>
+        <f>[2]Main!$C$26*E30</f>
         <v>1943.3578499999999</v>
       </c>
       <c r="AF4" s="53">
@@ -9306,19 +9420,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E27</f>
+        <f>[6]Main!$C$6*E30</f>
         <v>6.8806999999999992</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E27</f>
+        <f>[6]Main!$C$8*E30</f>
         <v>3126.0533853999996</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$27</f>
+        <f>[6]Main!$C$11*$E$30</f>
         <v>149.62410000000008</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$27</f>
+        <f>[6]Main!$C$12*$E$30</f>
         <v>2976.4292853999996</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -9334,15 +9448,15 @@
         <v>24.790599499495396</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$27</f>
+        <f>'[6]Financial Model'!$AA$20*$E$30</f>
         <v>-455.81691000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$27</f>
+        <f>'[6]Financial Model'!$Z$20*$E$30</f>
         <v>76.477859999999353</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$27</f>
+        <f>'[6]Financial Model'!$Y$20*$E$30</f>
         <v>-38.43066000000033</v>
       </c>
       <c r="R8" s="52">
@@ -9391,7 +9505,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E27</f>
+        <f>[6]Main!$C$27*E30</f>
         <v>896.74860000000001</v>
       </c>
       <c r="AF8" s="53">
@@ -9437,19 +9551,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E27</f>
+        <f>[7]Main!$C$6*E30</f>
         <v>21.189900000000002</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$27</f>
+        <f>[7]Main!$C$8*$E$30</f>
         <v>1953.161232984</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E27</f>
+        <f>[7]Main!$C$11*E30</f>
         <v>322.90402999999998</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E27</f>
+        <f>[7]Main!$C$12*E30</f>
         <v>1630.2572029840001</v>
       </c>
       <c r="J9" s="98" t="str">
@@ -9486,7 +9600,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E27</f>
+        <f>[7]Main!$C$26*E30</f>
         <v>617.17056999999988</v>
       </c>
       <c r="AF9" s="53">
@@ -9520,19 +9634,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E27</f>
+        <f>[8]Main!$C$6*E30</f>
         <v>10.723599999999999</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E27</f>
+        <f>[8]Main!$C$8*E30</f>
         <v>1932.2747603999996</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$27</f>
+        <f>[8]Main!$C$11*$E$30</f>
         <v>-230.99563999999998</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$27</f>
+        <f>[8]Main!$C$12*$E$30</f>
         <v>2163.2704003999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -9552,11 +9666,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E27</f>
+        <f>'[8]Financial Model'!$Z$17*E30</f>
         <v>348.28957999999989</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F27</f>
+        <f>'[8]Financial Model'!$Y$17*F30</f>
         <v>-252.21325301204848</v>
       </c>
       <c r="Q10" s="4"/>
@@ -9599,7 +9713,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E27</f>
+        <f>[8]Main!$C$26*E30</f>
         <v>570.24818000000005</v>
       </c>
       <c r="AF10" s="53">
@@ -9667,20 +9781,20 @@
       </c>
       <c r="L11" s="56"/>
       <c r="N11" s="56">
-        <f>'[9]Financial Model'!$T$4</f>
-        <v>3936.5</v>
+        <f>'[9]Financial Model'!$T$15</f>
+        <v>-30.80000000000009</v>
       </c>
       <c r="O11" s="56">
-        <f>'[9]Financial Model'!$S$4</f>
-        <v>3910.5</v>
+        <f>'[9]Financial Model'!$S$15</f>
+        <v>128.40000000000015</v>
       </c>
       <c r="P11" s="56">
-        <f>'[9]Financial Model'!$R$4</f>
-        <v>3263.5</v>
+        <f>'[9]Financial Model'!$R$15</f>
+        <v>113.30000000000014</v>
       </c>
       <c r="Q11" s="56">
-        <f>'[9]Financial Model'!$Q$4</f>
-        <v>2733.5</v>
+        <f>'[9]Financial Model'!$Q$15</f>
+        <v>24.599999999999909</v>
       </c>
       <c r="R11" s="52">
         <f>[9]Main!$C$36</f>
@@ -9779,19 +9893,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E27</f>
+        <f>[10]Main!$C$6*E30</f>
         <v>18.7746</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E27</f>
+        <f>[10]Main!$C$8*E30</f>
         <v>929.07985559999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E27</f>
+        <f>[10]Main!$C$11*E30</f>
         <v>123.55711999999997</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E27</f>
+        <f>[10]Main!$C$12*E30</f>
         <v>805.52273559999992</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -9812,15 +9926,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E27</f>
+        <f>'[10]Financial Model'!$X$18*E30</f>
         <v>218.29829999999976</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$27</f>
+        <f>'[10]Financial Model'!$W$18*$E$30</f>
         <v>-94.637430000000123</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$27</f>
+        <f>'[10]Financial Model'!$V$18*$E$30</f>
         <v>32.667140000000508</v>
       </c>
       <c r="R12" s="52">
@@ -9869,7 +9983,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E27</f>
+        <f>'[10]Financial Model'!$Q$41*E30</f>
         <v>615.8292899999999</v>
       </c>
       <c r="AF12" s="53">
@@ -10139,11 +10253,11 @@
       </c>
       <c r="F15" s="7">
         <f>[13]Main!$C$6</f>
-        <v>1.3308</v>
+        <v>1.05</v>
       </c>
       <c r="G15" s="49">
         <f>[13]Main!$C$8</f>
-        <v>108.96466901759999</v>
+        <v>85.9730256</v>
       </c>
       <c r="H15" s="49">
         <f>[13]Main!$C$11</f>
@@ -10151,7 +10265,7 @@
       </c>
       <c r="I15" s="49">
         <f>[13]Main!$C$12</f>
-        <v>100.66466901759999</v>
+        <v>77.673025600000003</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>[13]Main!$C$29</f>
@@ -10163,7 +10277,7 @@
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>4.4345669170748829</v>
+        <v>3.4217191894273076</v>
       </c>
       <c r="N15" s="1">
         <f xml:space="preserve"> '[13]Financial Model'!$T$17</f>
@@ -10183,15 +10297,15 @@
       </c>
       <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>4.8002056835947062</v>
+        <v>3.7873579559471304</v>
       </c>
       <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
-        <v>-3.0239089360221629</v>
+        <v>-2.3858614238227163</v>
       </c>
       <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>1.048745611333975</v>
+        <v>0.82745934167468738</v>
       </c>
       <c r="U15" s="139">
         <f>[13]Main!$C$38</f>
@@ -10251,7 +10365,7 @@
       </c>
       <c r="AJ15" s="130">
         <f>[13]Main!$C$42</f>
-        <v>4.097646421860806</v>
+        <v>4.0934845655588719</v>
       </c>
       <c r="AK15" s="4">
         <f>[13]Main!$C$25</f>
@@ -10380,91 +10494,128 @@
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="L17" s="50"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="53"/>
-      <c r="Z17" s="53"/>
-      <c r="AA17" s="53"/>
-      <c r="AB17" s="53"/>
-      <c r="AC17" s="53"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="53"/>
-      <c r="AI17" s="57"/>
-      <c r="AJ17" s="57"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="7">
+        <f>[16]Main!$C$6</f>
+        <v>0.13569999999999999</v>
+      </c>
+      <c r="G17" s="49">
+        <f>[16]Main!$C$8</f>
+        <v>7.1242499999999991</v>
+      </c>
+      <c r="H17" s="49">
+        <f>[16]Main!$C$11</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="49">
+        <f>[16]Main!$C$12</f>
+        <v>7.1242499999999991</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f>[16]Main!$C$28</f>
+        <v>FH123</v>
+      </c>
+      <c r="K17" s="85">
+        <f>[16]Main!$D$28</f>
+        <v>44903</v>
+      </c>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="Z17" s="53">
+        <f>'[16]Financial Model'!$K$17</f>
+        <v>0.48510270107591608</v>
+      </c>
+      <c r="AK17" s="4">
+        <f>[16]Main!$C$24</f>
+        <v>2013</v>
+      </c>
+      <c r="AL17" s="4" t="str">
+        <f>[16]Main!$C$23</f>
+        <v>Salford, UK</v>
+      </c>
+      <c r="AM17" s="4" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="18" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
-      <c r="J18" s="1"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="AM18" s="4" t="s">
-        <v>545</v>
-      </c>
+      <c r="L18" s="50"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="53"/>
+      <c r="Z18" s="53"/>
+      <c r="AA18" s="53"/>
+      <c r="AB18" s="53"/>
+      <c r="AC18" s="53"/>
+      <c r="AE18" s="55"/>
+      <c r="AF18" s="53"/>
+      <c r="AI18" s="57"/>
+      <c r="AJ18" s="57"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
     </row>
     <row r="19" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>214</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>489</v>
+        <v>13</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="7"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
-      <c r="I19" s="4"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
       <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="AM19" s="4" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>503</v>
+        <v>214</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>489</v>
       </c>
+      <c r="E20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
-      <c r="I20" s="84"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="56"/>
@@ -10493,159 +10644,199 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="AM22" s="4" t="s">
-        <v>546</v>
-      </c>
-    </row>
     <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="54">
-        <f>[15]Main!$C$6</f>
-        <v>20.806000000000001</v>
-      </c>
-      <c r="G23" s="49">
-        <f>[15]Main!$C$8</f>
-        <v>8041.1028800000004</v>
-      </c>
-      <c r="I23" s="84">
-        <f>[15]Main!$C$12</f>
-        <v>8041.1028800000004</v>
-      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
+      <c r="L23" s="56"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
-      <c r="AK23" s="4">
-        <f>[15]Main!$C$24</f>
-        <v>1856</v>
-      </c>
-      <c r="AL23" s="4" t="str">
-        <f>[15]Main!$C$23</f>
-        <v>London, UK</v>
-      </c>
-      <c r="AM23" s="4" t="s">
-        <v>546</v>
-      </c>
     </row>
     <row r="24" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2.9</v>
+      <c r="C24" s="142" t="s">
+        <v>554</v>
       </c>
       <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
+      <c r="L24" s="56"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
-      <c r="AM24" s="4" t="s">
-        <v>546</v>
-      </c>
     </row>
     <row r="25" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F25" s="7">
+        <f>18.22*E30</f>
+        <v>15.122599999999998</v>
+      </c>
       <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
+      <c r="L25" s="56"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
+      <c r="AM25" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="26" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D26" s="142" t="s">
-        <v>495</v>
-      </c>
-      <c r="E26" s="143"/>
-      <c r="F26" s="42" t="s">
-        <v>496</v>
-      </c>
-      <c r="G26" s="49"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="54">
+        <f>[15]Main!$C$6</f>
+        <v>20.806000000000001</v>
+      </c>
+      <c r="G26" s="49">
+        <f>[15]Main!$C$8</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="I26" s="84">
+        <f>[15]Main!$C$12</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="J26" s="4" t="str">
+        <f>[15]Main!$C$29</f>
+        <v>H122</v>
+      </c>
+      <c r="K26" s="85">
+        <f>[15]Main!$D$29</f>
+        <v>44882</v>
+      </c>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="Z26" s="53">
+        <f>'[15]Financial Model'!$K$28</f>
+        <v>0.70111524163568772</v>
+      </c>
+      <c r="AA26" s="53">
+        <f>'[15]Financial Model'!$K$29</f>
+        <v>0.19553903345724907</v>
+      </c>
+      <c r="AB26" s="53">
+        <f>'[15]Financial Model'!$K$30</f>
+        <v>0.14423791821561338</v>
+      </c>
+      <c r="AC26" s="53">
+        <f>'[15]Financial Model'!$K$31</f>
+        <v>0.22709163346613545</v>
+      </c>
+      <c r="AK26" s="4">
+        <f>[15]Main!$C$24</f>
+        <v>1856</v>
+      </c>
+      <c r="AL26" s="4" t="str">
+        <f>[15]Main!$C$23</f>
+        <v>London, UK</v>
+      </c>
+      <c r="AM26" s="4" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="27" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D27" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E27" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="F27" s="45">
-        <f>1/E27</f>
-        <v>1.2048192771084338</v>
+      <c r="B27" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2.9</v>
       </c>
       <c r="G27" s="49"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="AM27" s="4" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="28" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D28" s="46" t="s">
-        <v>498</v>
-      </c>
-      <c r="E28" s="48">
-        <v>0.87</v>
-      </c>
-      <c r="F28" s="47">
-        <f>1/E28</f>
-        <v>1.1494252873563218</v>
-      </c>
       <c r="G28" s="49"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
     </row>
     <row r="29" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="D29" s="143" t="s">
+        <v>495</v>
+      </c>
+      <c r="E29" s="144"/>
+      <c r="F29" s="42" t="s">
+        <v>496</v>
+      </c>
       <c r="G29" s="49"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
     </row>
     <row r="30" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="D30" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="E30" s="44">
+        <v>0.83</v>
+      </c>
+      <c r="F30" s="45">
+        <f>1/E30</f>
+        <v>1.2048192771084338</v>
+      </c>
       <c r="G30" s="49"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
     </row>
     <row r="31" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="D31" s="46" t="s">
+        <v>498</v>
+      </c>
+      <c r="E31" s="48">
+        <v>0.87</v>
+      </c>
+      <c r="F31" s="47">
+        <f>1/E31</f>
+        <v>1.1494252873563218</v>
+      </c>
       <c r="G31" s="49"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="2:39" x14ac:dyDescent="0.2">
       <c r="G32" s="49"/>
@@ -10653,9 +10844,18 @@
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="49"/>
     </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="49"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="49"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="49"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -10673,10 +10873,11 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
-    <hyperlink ref="B23" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B26" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{183ACAEF-5A70-4D85-94EE-2D4C25FF95CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId16"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId17"/>
   <ignoredErrors>
     <ignoredError sqref="AI12 G12" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Start add Fast Retailing Co, Ltd & Private Equity tab
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A1B95-4361-4083-AE94-54839D3E0813}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FBBC0D-F234-7349-948A-940351869B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="495" windowWidth="30285" windowHeight="18855" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="2020" yWindow="500" windowWidth="30280" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
     <sheet name="Screener - Apparel Retail" sheetId="2" r:id="rId2"/>
     <sheet name="Main" sheetId="1" r:id="rId3"/>
+    <sheet name="Private Equity" sheetId="6" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
@@ -34,18 +34,30 @@
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="567">
   <si>
     <t>Ticker</t>
   </si>
@@ -1713,6 +1725,39 @@
   </si>
   <si>
     <t>Online Womenswear Outlet</t>
+  </si>
+  <si>
+    <t>$LULU</t>
+  </si>
+  <si>
+    <t>Luluemon Athletica Inc.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>Fast Retailing Co, Ltd.</t>
+  </si>
+  <si>
+    <t>Japanese Fashion Holding Company</t>
+  </si>
+  <si>
+    <t>Yamaguchi, Japan</t>
+  </si>
+  <si>
+    <t>JPYGBP</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>TSE</t>
   </si>
 </sst>
 </file>
@@ -1720,14 +1765,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -2056,7 +2101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2148,7 +2193,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2157,13 +2202,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2192,11 +2237,8 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2204,18 +2246,21 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -2252,7 +2297,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2270,7 +2315,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2291,7 +2336,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2318,24 +2363,24 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2346,16 +2391,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2390,7 +2435,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2402,7 +2447,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2429,6 +2474,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3375,6 +3426,52 @@
 </file>
 
 <file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>331.41</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>40531.442999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>40531.442999999999</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Vancouver, Canada</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1998</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4817,25 +4914,25 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -4877,7 +4974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -4921,7 +5018,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -4965,7 +5062,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -5009,7 +5106,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -5053,7 +5150,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>265</v>
       </c>
@@ -5097,7 +5194,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>271</v>
       </c>
@@ -5141,7 +5238,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -5185,7 +5282,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -5229,7 +5326,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -5273,7 +5370,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -5317,7 +5414,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -5361,7 +5458,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -5405,7 +5502,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -5449,7 +5546,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -5493,7 +5590,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -5537,7 +5634,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -5581,7 +5678,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -5625,7 +5722,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -5669,7 +5766,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>347</v>
       </c>
@@ -5713,7 +5810,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -5757,7 +5854,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -5801,7 +5898,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -5845,7 +5942,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -5889,7 +5986,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -5933,7 +6030,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -5977,7 +6074,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -6021,7 +6118,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -6065,7 +6162,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -6109,7 +6206,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -6153,7 +6250,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -6197,7 +6294,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -6241,7 +6338,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -6285,7 +6382,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -6329,7 +6426,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -6373,7 +6470,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -6417,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -6461,7 +6558,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -6505,7 +6602,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -6549,7 +6646,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -6593,7 +6690,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -6637,7 +6734,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -6681,7 +6778,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -6725,7 +6822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -6843,25 +6940,25 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6903,7 +7000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -6947,7 +7044,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -6991,7 +7088,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -7035,7 +7132,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -7079,7 +7176,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -7123,7 +7220,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -7167,7 +7264,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -7211,7 +7308,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -7255,7 +7352,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -7299,7 +7396,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -7343,7 +7440,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -7387,7 +7484,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -7431,7 +7528,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -7475,7 +7572,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -7519,7 +7616,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -7563,7 +7660,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -7607,7 +7704,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -7651,7 +7748,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -7695,7 +7792,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -7739,7 +7836,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -7783,7 +7880,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -7827,7 +7924,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -7871,7 +7968,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -7915,7 +8012,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -7959,7 +8056,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -8003,7 +8100,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -8047,7 +8144,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -8091,7 +8188,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -8135,7 +8232,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -8179,7 +8276,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -8223,7 +8320,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -8267,7 +8364,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -8311,7 +8408,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -8355,7 +8452,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -8399,7 +8496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -8443,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -8487,7 +8584,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -8590,38 +8687,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AM36"/>
+  <dimension ref="A1:AM37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W17" sqref="W17"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="24" width="9.140625" style="4"/>
-    <col min="25" max="30" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="24" width="9.1640625" style="4"/>
+    <col min="25" max="30" width="9.1640625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.140625" style="4"/>
-    <col min="35" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="1"/>
+    <col min="32" max="34" width="9.1640625" style="4"/>
+    <col min="35" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="136" t="s">
         <v>499</v>
@@ -8650,7 +8747,7 @@
         <v>2.6465954770197686</v>
       </c>
       <c r="U1" s="111">
-        <f t="shared" ref="U1:AC1" si="0">AVERAGE(U3:U16)</f>
+        <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
         <v>4.375835462356302E-2</v>
       </c>
       <c r="V1" s="87"/>
@@ -8708,7 +8805,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8822,7 +8919,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -8836,19 +8933,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$30</f>
+        <f>[1]Main!$C$6*$E$31</f>
         <v>87.498599999999996</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$30</f>
+        <f>[1]Main!$C$8*$E$31</f>
         <v>137119.05606</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$30</f>
+        <f>[1]Main!$C$11*$E$31</f>
         <v>2029.35</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$30</f>
+        <f>[1]Main!$C$12*$E$31</f>
         <v>135089.70606</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -8864,15 +8961,15 @@
         <v>26.920059874297088</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E30</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E31</f>
         <v>5018.1799999999939</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AC$21*1000*E30</f>
+        <f>'[1]Financial Model'!$AC$21*1000*E31</f>
         <v>4753.409999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AB$21*1000*E30</f>
+        <f>'[1]Financial Model'!$AB$21*1000*E31</f>
         <v>2107.37</v>
       </c>
       <c r="R3" s="51">
@@ -8918,7 +9015,7 @@
         <v>0.19693654266958391</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E30</f>
+        <f>[1]Main!$C$26*E31</f>
         <v>8019.46</v>
       </c>
       <c r="AF3" s="53">
@@ -8945,7 +9042,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -8959,19 +9056,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$30</f>
+        <f>[2]Main!$C$6*$E$31</f>
         <v>27.572599999999998</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$30</f>
+        <f>[2]Main!$C$8*$E$31</f>
         <v>10689.566148799999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$30</f>
+        <f>[2]Main!$C$11*$E$31</f>
         <v>-3872.8090499999998</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$30</f>
+        <f>[2]Main!$C$12*$E$31</f>
         <v>14562.375198799997</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -8987,15 +9084,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E30</f>
+        <f>'[2]Financial Model'!$AA$22*E31</f>
         <v>1151.127829999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$30</f>
+        <f>'[2]Financial Model'!$Z$22*$E$31</f>
         <v>338.51467000000116</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$30</f>
+        <f>'[2]Financial Model'!$Y$22*$E$31</f>
         <v>563.94267000000013</v>
       </c>
       <c r="R4" s="51">
@@ -9030,7 +9127,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E30</f>
+        <f>[2]Main!$C$26*E31</f>
         <v>1943.3578499999999</v>
       </c>
       <c r="AF4" s="53">
@@ -9051,7 +9148,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -9171,7 +9268,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -9298,7 +9395,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -9425,7 +9522,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -9439,19 +9536,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E30</f>
+        <f>[6]Main!$C$6*E31</f>
         <v>6.8806999999999992</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E30</f>
+        <f>[6]Main!$C$8*E31</f>
         <v>3126.0533853999996</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$30</f>
+        <f>[6]Main!$C$11*$E$31</f>
         <v>149.62410000000008</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$30</f>
+        <f>[6]Main!$C$12*$E$31</f>
         <v>2976.4292853999996</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -9467,15 +9564,15 @@
         <v>24.790599499495396</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$30</f>
+        <f>'[6]Financial Model'!$AA$20*$E$31</f>
         <v>-455.81691000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$30</f>
+        <f>'[6]Financial Model'!$Z$20*$E$31</f>
         <v>76.477859999999353</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$30</f>
+        <f>'[6]Financial Model'!$Y$20*$E$31</f>
         <v>-38.43066000000033</v>
       </c>
       <c r="R8" s="52">
@@ -9524,7 +9621,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E30</f>
+        <f>[6]Main!$C$27*E31</f>
         <v>896.74860000000001</v>
       </c>
       <c r="AF8" s="53">
@@ -9556,7 +9653,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -9570,19 +9667,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E30</f>
+        <f>[7]Main!$C$6*E31</f>
         <v>21.189900000000002</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$30</f>
+        <f>[7]Main!$C$8*$E$31</f>
         <v>1953.161232984</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E30</f>
+        <f>[7]Main!$C$11*E31</f>
         <v>322.90402999999998</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E30</f>
+        <f>[7]Main!$C$12*E31</f>
         <v>1630.2572029840001</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -9619,7 +9716,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E30</f>
+        <f>[7]Main!$C$26*E31</f>
         <v>617.17056999999988</v>
       </c>
       <c r="AF9" s="53">
@@ -9639,7 +9736,7 @@
         <v>Philadelphia, PA</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -9653,19 +9750,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E30</f>
+        <f>[8]Main!$C$6*E31</f>
         <v>10.723599999999999</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E30</f>
+        <f>[8]Main!$C$8*E31</f>
         <v>1932.2747603999996</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$30</f>
+        <f>[8]Main!$C$11*$E$31</f>
         <v>-230.99563999999998</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$30</f>
+        <f>[8]Main!$C$12*$E$31</f>
         <v>2163.2704003999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -9685,11 +9782,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E30</f>
+        <f>'[8]Financial Model'!$Z$17*E31</f>
         <v>348.28957999999989</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F30</f>
+        <f>'[8]Financial Model'!$Y$17*F31</f>
         <v>-252.21325301204848</v>
       </c>
       <c r="Q10" s="4"/>
@@ -9732,7 +9829,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E30</f>
+        <f>[8]Main!$C$26*E31</f>
         <v>570.24818000000005</v>
       </c>
       <c r="AF10" s="53">
@@ -9761,7 +9858,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -9898,7 +9995,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -9912,19 +10009,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E30</f>
+        <f>[10]Main!$C$6*E31</f>
         <v>18.7746</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E30</f>
+        <f>[10]Main!$C$8*E31</f>
         <v>929.07985559999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E30</f>
+        <f>[10]Main!$C$11*E31</f>
         <v>123.55711999999997</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E30</f>
+        <f>[10]Main!$C$12*E31</f>
         <v>805.52273559999992</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -9945,15 +10042,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E30</f>
+        <f>'[10]Financial Model'!$X$18*E31</f>
         <v>218.29829999999976</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$30</f>
+        <f>'[10]Financial Model'!$W$18*$E$31</f>
         <v>-94.637430000000123</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$30</f>
+        <f>'[10]Financial Model'!$V$18*$E$31</f>
         <v>32.667140000000508</v>
       </c>
       <c r="R12" s="52">
@@ -10002,7 +10099,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E30</f>
+        <f>'[10]Financial Model'!$Q$41*E31</f>
         <v>615.8292899999999</v>
       </c>
       <c r="AF12" s="53">
@@ -10031,7 +10128,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -10153,7 +10250,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="103" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -10257,7 +10354,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -10395,7 +10492,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -10512,7 +10609,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -10611,7 +10708,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -10637,7 +10734,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
@@ -10661,7 +10758,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>214</v>
       </c>
@@ -10684,7 +10781,7 @@
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>492</v>
       </c>
@@ -10706,20 +10803,78 @@
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B22" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F22" s="54">
+        <f>[16]Main!$C$6*E31</f>
+        <v>275.07030000000003</v>
+      </c>
+      <c r="G22" s="49">
+        <f>[16]Main!$C$8*E31</f>
+        <v>33641.097689999995</v>
+      </c>
+      <c r="H22" s="49">
+        <f>[16]Main!$C$11*E31</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="49">
+        <f>[16]Main!$C$12*E31</f>
+        <v>33641.097689999995</v>
+      </c>
+      <c r="AK22" s="4">
+        <f>[16]Main!$C$24</f>
+        <v>1998</v>
+      </c>
+      <c r="AL22" s="4" t="str">
+        <f>[16]Main!$C$23</f>
+        <v>Vancouver, Canada</v>
+      </c>
+      <c r="AM22" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B23" s="138">
+        <v>9983</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F23" s="54">
+        <f>81600*E33</f>
+        <v>489.6</v>
+      </c>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-    </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C24" s="133" t="s">
-        <v>554</v>
-      </c>
+      <c r="I23" s="49"/>
+      <c r="AK23" s="4">
+        <v>1949</v>
+      </c>
+      <c r="AL23" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="AM23" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
       <c r="I24" s="4"/>
@@ -10729,22 +10884,9 @@
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="F25" s="7">
-        <f>18.22*E30</f>
-        <v>15.122599999999998</v>
+    <row r="25" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="C25" s="133" t="s">
+        <v>554</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -10754,79 +10896,42 @@
       <c r="L25" s="56"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
-      <c r="AM25" s="4" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>540</v>
+    </row>
+    <row r="26" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B26" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>260</v>
+        <v>512</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>489</v>
+        <v>31</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="54">
-        <f>[16]Main!$C$6</f>
-        <v>20.806000000000001</v>
-      </c>
-      <c r="G26" s="49">
-        <f>[16]Main!$C$8</f>
-        <v>8041.1028800000004</v>
-      </c>
-      <c r="I26" s="84">
-        <f>[16]Main!$C$12</f>
-        <v>8041.1028800000004</v>
-      </c>
-      <c r="J26" s="4" t="str">
-        <f>[16]Main!$C$29</f>
-        <v>H122</v>
-      </c>
-      <c r="K26" s="85">
-        <f>[16]Main!$D$29</f>
-        <v>44882</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="F26" s="7">
+        <f>18.22*E31</f>
+        <v>15.122599999999998</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="56"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
-      <c r="Z26" s="53">
-        <f>'[16]Financial Model'!$K$28</f>
-        <v>0.70111524163568772</v>
-      </c>
-      <c r="AA26" s="53">
-        <f>'[16]Financial Model'!$K$29</f>
-        <v>0.19553903345724907</v>
-      </c>
-      <c r="AB26" s="53">
-        <f>'[16]Financial Model'!$K$30</f>
-        <v>0.14423791821561338</v>
-      </c>
-      <c r="AC26" s="53">
-        <f>'[16]Financial Model'!$K$31</f>
-        <v>0.22709163346613545</v>
-      </c>
-      <c r="AK26" s="4">
-        <f>[16]Main!$C$24</f>
-        <v>1856</v>
-      </c>
-      <c r="AL26" s="4" t="str">
-        <f>[16]Main!$C$23</f>
-        <v>London, UK</v>
-      </c>
       <c r="AM26" s="4" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>541</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="27" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B27" s="3" t="s">
+        <v>540</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>542</v>
+        <v>260</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>489</v>
@@ -10834,90 +10939,163 @@
       <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="7">
-        <v>2.9</v>
-      </c>
-      <c r="G27" s="49"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="F27" s="54">
+        <f>[17]Main!$C$6</f>
+        <v>20.806000000000001</v>
+      </c>
+      <c r="G27" s="49">
+        <f>[17]Main!$C$8</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="I27" s="84">
+        <f>[17]Main!$C$12</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="J27" s="4" t="str">
+        <f>[17]Main!$C$29</f>
+        <v>H122</v>
+      </c>
+      <c r="K27" s="85">
+        <f>[17]Main!$D$29</f>
+        <v>44882</v>
+      </c>
       <c r="M27" s="56"/>
       <c r="N27" s="56"/>
+      <c r="Z27" s="53">
+        <f>'[17]Financial Model'!$K$28</f>
+        <v>0.70111524163568772</v>
+      </c>
+      <c r="AA27" s="53">
+        <f>'[17]Financial Model'!$K$29</f>
+        <v>0.19553903345724907</v>
+      </c>
+      <c r="AB27" s="53">
+        <f>'[17]Financial Model'!$K$30</f>
+        <v>0.14423791821561338</v>
+      </c>
+      <c r="AC27" s="53">
+        <f>'[17]Financial Model'!$K$31</f>
+        <v>0.22709163346613545</v>
+      </c>
+      <c r="AK27" s="4">
+        <f>[17]Main!$C$24</f>
+        <v>1856</v>
+      </c>
+      <c r="AL27" s="4" t="str">
+        <f>[17]Main!$C$23</f>
+        <v>London, UK</v>
+      </c>
       <c r="AM27" s="4" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="28" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B28" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="7">
+        <v>2.9</v>
+      </c>
       <c r="G28" s="49"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
-    </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D29" s="134" t="s">
-        <v>495</v>
-      </c>
-      <c r="E29" s="135"/>
-      <c r="F29" s="42" t="s">
-        <v>496</v>
-      </c>
+      <c r="AM28" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="29" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G29" s="49"/>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D30" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E30" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="F30" s="45">
-        <f>1/E30</f>
-        <v>1.2048192771084338</v>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+    </row>
+    <row r="30" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="D30" s="134" t="s">
+        <v>495</v>
+      </c>
+      <c r="E30" s="135"/>
+      <c r="F30" s="42" t="s">
+        <v>496</v>
       </c>
       <c r="G30" s="49"/>
       <c r="I30" s="4"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D31" s="46" t="s">
-        <v>498</v>
-      </c>
-      <c r="E31" s="48">
-        <v>0.87</v>
-      </c>
-      <c r="F31" s="47">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="D31" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="E31" s="44">
+        <v>0.83</v>
+      </c>
+      <c r="F31" s="45">
         <f>1/E31</f>
-        <v>1.1494252873563218</v>
+        <v>1.2048192771084338</v>
       </c>
       <c r="G31" s="49"/>
       <c r="I31" s="4"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="D32" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E32" s="44">
+        <v>0.87</v>
+      </c>
+      <c r="F32" s="45">
+        <f>1/E32</f>
+        <v>1.1494252873563218</v>
+      </c>
       <c r="G32" s="49"/>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="I32" s="4"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D33" s="46" t="s">
+        <v>564</v>
+      </c>
+      <c r="E33" s="48">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F33" s="47">
+        <f>1/E33</f>
+        <v>166.66666666666666</v>
+      </c>
       <c r="G33" s="49"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.15">
       <c r="G34" s="49"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.15">
       <c r="G35" s="49"/>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.15">
       <c r="G36" s="49"/>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="G37" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -10935,13 +11113,178 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
-    <hyperlink ref="B26" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B27" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{183ACAEF-5A70-4D85-94EE-2D4C25FF95CC}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId17"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId18"/>
   <ignoredErrors>
     <ignoredError sqref="AI12 G12" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8C83D4-A3B8-FA43-9115-0C471E65D93F}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E1" s="90" t="e">
+        <f>AVERAGE(E3:E16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F1" s="126" t="e">
+        <f>AVERAGE(F3:F16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G1" s="90"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D2" s="137" t="s">
+        <v>559</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="E16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="E17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="133" t="s">
+        <v>554</v>
+      </c>
+      <c r="D24" s="133"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on Overview sheets to plan upcoming analysis
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4BE4C5-A27D-0846-86D1-7EC20ACB73A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729C645-7601-1547-BD9C-9FD024B39D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2000" yWindow="520" windowWidth="30280" windowHeight="18860" activeTab="2" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="588">
   <si>
     <t>Ticker</t>
   </si>
@@ -1758,6 +1758,69 @@
   </si>
   <si>
     <t>TSE</t>
+  </si>
+  <si>
+    <t>Footwear</t>
+  </si>
+  <si>
+    <t>DOCS</t>
+  </si>
+  <si>
+    <t>SHOE</t>
+  </si>
+  <si>
+    <t>Shoe Zone Plc</t>
+  </si>
+  <si>
+    <t>Dr. Martens Plc</t>
+  </si>
+  <si>
+    <t>Puma SE</t>
+  </si>
+  <si>
+    <t>XETRA</t>
+  </si>
+  <si>
+    <t>Hugo Boss AG</t>
+  </si>
+  <si>
+    <t>€BOSS</t>
+  </si>
+  <si>
+    <t>€PUM</t>
+  </si>
+  <si>
+    <t>€ADS</t>
+  </si>
+  <si>
+    <t>Addidas AG</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>$CROX</t>
+  </si>
+  <si>
+    <t>$SKX</t>
+  </si>
+  <si>
+    <t>$FL</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Fashion (Not Yet Analysed)</t>
+  </si>
+  <si>
+    <t>Crocs Inc</t>
+  </si>
+  <si>
+    <t>Skechers USA Inc</t>
+  </si>
+  <si>
+    <t>Foot Locker Inc</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1837,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1873,6 +1936,14 @@
       <u/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2101,7 +2172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2480,6 +2551,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3040,12 +3117,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>1.3508</v>
+            <v>1.5638000000000001</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>110.60225045759999</v>
+            <v>128.04249279359999</v>
           </cell>
         </row>
         <row r="11">
@@ -3055,7 +3132,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>102.3022504576</v>
+            <v>119.74249279359999</v>
           </cell>
         </row>
         <row r="24">
@@ -3088,17 +3165,17 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>4.5067070686167332</v>
+            <v>5.2749996825374366</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>4.8723458351365556</v>
+            <v>5.6406384490572599</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1.0645067416515883</v>
+            <v>1.2323627795341676</v>
           </cell>
         </row>
         <row r="38">
@@ -3108,7 +3185,7 @@
         </row>
         <row r="39">
           <cell r="C39">
-            <v>-3.0693539155235481</v>
+            <v>-3.5533429472132991</v>
           </cell>
         </row>
         <row r="42">
@@ -4609,7 +4686,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4897,7 +4974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8687,13 +8764,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AM37"/>
+  <dimension ref="A1:AM52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8736,15 +8813,15 @@
       <c r="Q1" s="138"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
-        <v>14.883448446973592</v>
+        <v>14.953293230057294</v>
       </c>
       <c r="S1" s="98">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.171509273215568</v>
+        <v>13.123110370046593</v>
       </c>
       <c r="T1" s="98">
         <f>AVERAGE(T3:T17)</f>
-        <v>2.7530197424288074</v>
+        <v>2.7642101449543128</v>
       </c>
       <c r="U1" s="111">
         <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
@@ -8933,19 +9010,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$31</f>
+        <f>[1]Main!$C$6*$E$46</f>
         <v>95.947999999999993</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$31</f>
+        <f>[1]Main!$C$8*$E$46</f>
         <v>149582.932</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$31</f>
+        <f>[1]Main!$C$11*$E$46</f>
         <v>987.69999999999993</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$31</f>
+        <f>[1]Main!$C$12*$E$46</f>
         <v>148595.23199999999</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -8961,15 +9038,15 @@
         <v>29.611379424412871</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AF$21*1000*E31</f>
+        <f>'[1]Financial Model'!$AF$21*1000*E46</f>
         <v>5018.1799999999939</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AE$21*1000*E31</f>
+        <f>'[1]Financial Model'!$AE$21*1000*E46</f>
         <v>4753.409999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E31</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E46</f>
         <v>2107.37</v>
       </c>
       <c r="R3" s="51">
@@ -9015,7 +9092,7 @@
         <v>0.19333333333333316</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E31</f>
+        <f>[1]Main!$C$26*E46</f>
         <v>8019.46</v>
       </c>
       <c r="AF3" s="53">
@@ -9056,19 +9133,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$31</f>
+        <f>[2]Main!$C$6*$E$46</f>
         <v>27.572599999999998</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$31</f>
+        <f>[2]Main!$C$8*$E$46</f>
         <v>10689.566148799999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$31</f>
+        <f>[2]Main!$C$11*$E$46</f>
         <v>-3872.8090499999998</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$31</f>
+        <f>[2]Main!$C$12*$E$46</f>
         <v>14562.375198799997</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -9084,15 +9161,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E31</f>
+        <f>'[2]Financial Model'!$AA$22*E46</f>
         <v>1151.127829999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$31</f>
+        <f>'[2]Financial Model'!$Z$22*$E$46</f>
         <v>338.51467000000116</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$31</f>
+        <f>'[2]Financial Model'!$Y$22*$E$46</f>
         <v>563.94267000000013</v>
       </c>
       <c r="R4" s="51">
@@ -9127,7 +9204,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E31</f>
+        <f>[2]Main!$C$26*E46</f>
         <v>1943.3578499999999</v>
       </c>
       <c r="AF4" s="53">
@@ -9536,19 +9613,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E31</f>
+        <f>[6]Main!$C$6*E46</f>
         <v>6.8806999999999992</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E31</f>
+        <f>[6]Main!$C$8*E46</f>
         <v>3126.0533853999996</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$31</f>
+        <f>[6]Main!$C$11*$E$46</f>
         <v>149.62410000000008</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$31</f>
+        <f>[6]Main!$C$12*$E$46</f>
         <v>2976.4292853999996</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -9564,15 +9641,15 @@
         <v>24.790599499495396</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$31</f>
+        <f>'[6]Financial Model'!$AA$20*$E$46</f>
         <v>-455.81691000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$31</f>
+        <f>'[6]Financial Model'!$Z$20*$E$46</f>
         <v>76.477859999999353</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$31</f>
+        <f>'[6]Financial Model'!$Y$20*$E$46</f>
         <v>-38.43066000000033</v>
       </c>
       <c r="R8" s="52">
@@ -9621,7 +9698,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E31</f>
+        <f>[6]Main!$C$27*E46</f>
         <v>896.74860000000001</v>
       </c>
       <c r="AF8" s="53">
@@ -9667,19 +9744,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E31</f>
+        <f>[7]Main!$C$6*E46</f>
         <v>21.189900000000002</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$31</f>
+        <f>[7]Main!$C$8*$E$46</f>
         <v>1953.161232984</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E31</f>
+        <f>[7]Main!$C$11*E46</f>
         <v>322.90402999999998</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E31</f>
+        <f>[7]Main!$C$12*E46</f>
         <v>1630.2572029840001</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -9716,7 +9793,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E31</f>
+        <f>[7]Main!$C$26*E46</f>
         <v>617.17056999999988</v>
       </c>
       <c r="AF9" s="53">
@@ -9750,19 +9827,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E31</f>
+        <f>[8]Main!$C$6*E46</f>
         <v>10.723599999999999</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E31</f>
+        <f>[8]Main!$C$8*E46</f>
         <v>1932.2747603999996</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$31</f>
+        <f>[8]Main!$C$11*$E$46</f>
         <v>-230.99563999999998</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$31</f>
+        <f>[8]Main!$C$12*$E$46</f>
         <v>2163.2704003999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -9782,11 +9859,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E31</f>
+        <f>'[8]Financial Model'!$Z$17*E46</f>
         <v>348.28957999999989</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F31</f>
+        <f>'[8]Financial Model'!$Y$17*F46</f>
         <v>-252.21325301204848</v>
       </c>
       <c r="Q10" s="4"/>
@@ -9829,7 +9906,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E31</f>
+        <f>[8]Main!$C$26*E46</f>
         <v>570.24818000000005</v>
       </c>
       <c r="AF10" s="53">
@@ -10009,19 +10086,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E31</f>
+        <f>[10]Main!$C$6*E46</f>
         <v>18.7746</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E31</f>
+        <f>[10]Main!$C$8*E46</f>
         <v>929.07985559999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E31</f>
+        <f>[10]Main!$C$11*E46</f>
         <v>123.55711999999997</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E31</f>
+        <f>[10]Main!$C$12*E46</f>
         <v>805.52273559999992</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -10042,15 +10119,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E31</f>
+        <f>'[10]Financial Model'!$X$18*E46</f>
         <v>218.29829999999976</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$31</f>
+        <f>'[10]Financial Model'!$W$18*$E$46</f>
         <v>-94.637430000000123</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$31</f>
+        <f>'[10]Financial Model'!$V$18*$E$46</f>
         <v>32.667140000000508</v>
       </c>
       <c r="R12" s="52">
@@ -10099,7 +10176,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E31</f>
+        <f>'[10]Financial Model'!$Q$41*E46</f>
         <v>615.8292899999999</v>
       </c>
       <c r="AF12" s="53">
@@ -10369,11 +10446,11 @@
       </c>
       <c r="F15" s="7">
         <f>[13]Main!$C$6</f>
-        <v>1.3508</v>
+        <v>1.5638000000000001</v>
       </c>
       <c r="G15" s="49">
         <f>[13]Main!$C$8</f>
-        <v>110.60225045759999</v>
+        <v>128.04249279359999</v>
       </c>
       <c r="H15" s="49">
         <f>[13]Main!$C$11</f>
@@ -10381,7 +10458,7 @@
       </c>
       <c r="I15" s="49">
         <f>[13]Main!$C$12</f>
-        <v>102.3022504576</v>
+        <v>119.74249279359999</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>[13]Main!$C$29</f>
@@ -10393,7 +10470,7 @@
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>4.5067070686167332</v>
+        <v>5.2749996825374366</v>
       </c>
       <c r="N15" s="1">
         <f xml:space="preserve"> '[13]Financial Model'!$T$17</f>
@@ -10413,15 +10490,15 @@
       </c>
       <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>4.8723458351365556</v>
+        <v>5.6406384490572599</v>
       </c>
       <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
-        <v>-3.0693539155235481</v>
+        <v>-3.5533429472132991</v>
       </c>
       <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>1.0645067416515883</v>
+        <v>1.2323627795341676</v>
       </c>
       <c r="U15" s="131">
         <f>[13]Main!$C$38</f>
@@ -10735,65 +10812,74 @@
       <c r="AL18" s="4"/>
     </row>
     <row r="19" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="139" t="s">
+        <v>583</v>
+      </c>
+      <c r="C19" s="133" t="s">
+        <v>584</v>
+      </c>
+      <c r="F19" s="7"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
-      <c r="J19" s="1"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="AM19" s="4" t="s">
-        <v>545</v>
-      </c>
+      <c r="L19" s="50"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="53"/>
+      <c r="Z19" s="53"/>
+      <c r="AA19" s="53"/>
+      <c r="AB19" s="53"/>
+      <c r="AC19" s="53"/>
+      <c r="AE19" s="55"/>
+      <c r="AF19" s="53"/>
+      <c r="AI19" s="57"/>
+      <c r="AJ19" s="57"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="4"/>
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>214</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>489</v>
+        <v>13</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="7"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
       <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="AM20" s="4" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="21" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>492</v>
+        <v>214</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>31</v>
+        <v>489</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>505</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F21" s="7"/>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="4"/>
@@ -10804,298 +10890,520 @@
       <c r="N21" s="56"/>
     </row>
     <row r="22" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B22" s="3" t="s">
-        <v>556</v>
+      <c r="B22" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>557</v>
+        <v>493</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="F22" s="54">
-        <f>[16]Main!$C$6*E31</f>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+    </row>
+    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B23" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F23" s="54">
+        <f>[16]Main!$C$6*E46</f>
         <v>275.07030000000003</v>
       </c>
-      <c r="G22" s="49">
-        <f>[16]Main!$C$8*E31</f>
+      <c r="G23" s="49">
+        <f>[16]Main!$C$8*E46</f>
         <v>33641.097689999995</v>
       </c>
-      <c r="H22" s="49">
-        <f>[16]Main!$C$11*E31</f>
+      <c r="H23" s="49">
+        <f>[16]Main!$C$11*E46</f>
         <v>0</v>
       </c>
-      <c r="I22" s="49">
-        <f>[16]Main!$C$12*E31</f>
+      <c r="I23" s="49">
+        <f>[16]Main!$C$12*E46</f>
         <v>33641.097689999995</v>
       </c>
-      <c r="AK22" s="4">
+      <c r="AK23" s="4">
         <f>[16]Main!$C$24</f>
         <v>1998</v>
       </c>
-      <c r="AL22" s="4" t="str">
+      <c r="AL23" s="4" t="str">
         <f>[16]Main!$C$23</f>
         <v>Vancouver, Canada</v>
       </c>
-      <c r="AM22" s="4" t="s">
+      <c r="AM23" s="4" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B23" s="135">
+    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B24" s="135">
         <v>9983</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="F23" s="54">
-        <f>81600*E33</f>
+      <c r="F24" s="54">
+        <f>81600*E48</f>
         <v>489.6</v>
       </c>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="AK23" s="4">
-        <v>1949</v>
-      </c>
-      <c r="AL23" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="AM23" s="4" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
+      <c r="I24" s="49"/>
+      <c r="AK24" s="4">
+        <v>1949</v>
+      </c>
+      <c r="AL24" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="AM24" s="4" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="25" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="C25" s="133" t="s">
-        <v>554</v>
-      </c>
+      <c r="B25" s="135" t="s">
+        <v>577</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F25" s="54"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
+      <c r="I25" s="49"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
     </row>
     <row r="26" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B26" s="1" t="s">
-        <v>511</v>
+      <c r="B26" s="135" t="s">
+        <v>576</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>512</v>
+        <v>572</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>31</v>
+        <v>573</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="F26" s="7">
-        <f>18.22*E31</f>
-        <v>15.122599999999998</v>
-      </c>
+        <v>579</v>
+      </c>
+      <c r="F26" s="54"/>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="AM26" s="4" t="s">
-        <v>553</v>
-      </c>
+      <c r="I26" s="49"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
     </row>
     <row r="27" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B27" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="54">
-        <f>[17]Main!$C$6</f>
-        <v>20.806000000000001</v>
-      </c>
-      <c r="G27" s="49">
-        <f>[17]Main!$C$8</f>
-        <v>8041.1028800000004</v>
-      </c>
-      <c r="I27" s="84">
-        <f>[17]Main!$C$12</f>
-        <v>8041.1028800000004</v>
-      </c>
-      <c r="J27" s="4" t="str">
-        <f>[17]Main!$C$29</f>
-        <v>H122</v>
-      </c>
-      <c r="K27" s="85">
-        <f>[17]Main!$D$29</f>
-        <v>44882</v>
-      </c>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="56"/>
       <c r="M27" s="56"/>
       <c r="N27" s="56"/>
-      <c r="Z27" s="53">
-        <f>'[17]Financial Model'!$K$28</f>
-        <v>0.70111524163568772</v>
-      </c>
-      <c r="AA27" s="53">
-        <f>'[17]Financial Model'!$K$29</f>
-        <v>0.19553903345724907</v>
-      </c>
-      <c r="AB27" s="53">
-        <f>'[17]Financial Model'!$K$30</f>
-        <v>0.14423791821561338</v>
-      </c>
-      <c r="AC27" s="53">
-        <f>'[17]Financial Model'!$K$31</f>
-        <v>0.22709163346613545</v>
-      </c>
-      <c r="AK27" s="4">
-        <f>[17]Main!$C$24</f>
-        <v>1856</v>
-      </c>
-      <c r="AL27" s="4" t="str">
-        <f>[17]Main!$C$23</f>
-        <v>London, UK</v>
-      </c>
-      <c r="AM27" s="4" t="s">
-        <v>552</v>
-      </c>
     </row>
     <row r="28" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B28" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="7">
-        <v>2.9</v>
+      <c r="B28" s="140" t="s">
+        <v>583</v>
+      </c>
+      <c r="C28" s="133" t="s">
+        <v>554</v>
       </c>
       <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
+      <c r="L28" s="56"/>
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
-      <c r="AM28" s="4" t="s">
-        <v>546</v>
-      </c>
     </row>
     <row r="29" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B29" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F29" s="7">
+        <f>18.22*E46</f>
+        <v>15.122599999999998</v>
+      </c>
       <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
+      <c r="L29" s="56"/>
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
+      <c r="AM29" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="30" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="D30" s="136" t="s">
-        <v>495</v>
-      </c>
-      <c r="E30" s="137"/>
-      <c r="F30" s="42" t="s">
-        <v>496</v>
-      </c>
-      <c r="G30" s="49"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="B30" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="54">
+        <f>[17]Main!$C$6</f>
+        <v>20.806000000000001</v>
+      </c>
+      <c r="G30" s="49">
+        <f>[17]Main!$C$8</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="I30" s="84">
+        <f>[17]Main!$C$12</f>
+        <v>8041.1028800000004</v>
+      </c>
+      <c r="J30" s="4" t="str">
+        <f>[17]Main!$C$29</f>
+        <v>H122</v>
+      </c>
+      <c r="K30" s="85">
+        <f>[17]Main!$D$29</f>
+        <v>44882</v>
+      </c>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="Z30" s="53">
+        <f>'[17]Financial Model'!$K$28</f>
+        <v>0.70111524163568772</v>
+      </c>
+      <c r="AA30" s="53">
+        <f>'[17]Financial Model'!$K$29</f>
+        <v>0.19553903345724907</v>
+      </c>
+      <c r="AB30" s="53">
+        <f>'[17]Financial Model'!$K$30</f>
+        <v>0.14423791821561338</v>
+      </c>
+      <c r="AC30" s="53">
+        <f>'[17]Financial Model'!$K$31</f>
+        <v>0.22709163346613545</v>
+      </c>
+      <c r="AK30" s="4">
+        <f>[17]Main!$C$24</f>
+        <v>1856</v>
+      </c>
+      <c r="AL30" s="4" t="str">
+        <f>[17]Main!$C$23</f>
+        <v>London, UK</v>
+      </c>
+      <c r="AM30" s="4" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="31" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="D31" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E31" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="F31" s="45">
-        <f>1/E31</f>
-        <v>1.2048192771084338</v>
+      <c r="B31" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="7">
+        <v>2.9</v>
       </c>
       <c r="G31" s="49"/>
       <c r="I31" s="4"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="AM31" s="4" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="32" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="D32" s="43" t="s">
-        <v>498</v>
-      </c>
-      <c r="E32" s="44">
-        <v>0.87</v>
-      </c>
-      <c r="F32" s="45">
-        <f>1/E32</f>
-        <v>1.1494252873563218</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F32" s="7"/>
       <c r="G32" s="49"/>
       <c r="I32" s="4"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.15">
-      <c r="D33" s="46" t="s">
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G33" s="49"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B34" s="140" t="s">
+        <v>583</v>
+      </c>
+      <c r="C34" s="133" t="s">
+        <v>567</v>
+      </c>
+      <c r="G34" s="49"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="G35" s="49"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="G36" s="49"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B37" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="G37" s="49"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B38" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="49"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B39" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="49"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G40" s="49"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="56"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G41" s="49"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G42" s="49"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G43" s="49"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="G44" s="49"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="D45" s="136" t="s">
+        <v>495</v>
+      </c>
+      <c r="E45" s="137"/>
+      <c r="F45" s="42" t="s">
+        <v>496</v>
+      </c>
+      <c r="G45" s="49"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="D46" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="E46" s="44">
+        <v>0.83</v>
+      </c>
+      <c r="F46" s="45">
+        <f>1/E46</f>
+        <v>1.2048192771084338</v>
+      </c>
+      <c r="G46" s="49"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="D47" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E47" s="44">
+        <v>0.87</v>
+      </c>
+      <c r="F47" s="45">
+        <f>1/E47</f>
+        <v>1.1494252873563218</v>
+      </c>
+      <c r="G47" s="49"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="D48" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="E33" s="48">
+      <c r="E48" s="48">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F33" s="47">
-        <f>1/E33</f>
+      <c r="F48" s="47">
+        <f>1/E48</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="G33" s="49"/>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.15">
-      <c r="G34" s="49"/>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.15">
-      <c r="G35" s="49"/>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.15">
-      <c r="G36" s="49"/>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.15">
-      <c r="G37" s="49"/>
+      <c r="G48" s="49"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G49" s="49"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G50" s="49"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G51" s="49"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G52" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -11113,12 +11421,15 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
-    <hyperlink ref="B27" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B30" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{183ACAEF-5A70-4D85-94EE-2D4C25FF95CC}"/>
-    <hyperlink ref="B22" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
+    <hyperlink ref="B23" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
+    <hyperlink ref="B34" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
+    <hyperlink ref="B28" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
+    <hyperlink ref="B19" r:id="rId20" xr:uid="{8B27DD55-F39A-E042-A7A2-82BE3E8447D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId18"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId21"/>
   <ignoredErrors>
     <ignoredError sqref="AI12 G12 Z1 T1" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Update £SHOE on Fashion Overview
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBBF552-5163-40F3-8348-D0B10CDC5D16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9A3B1E-6CCD-2046-B8FD-DD8614F0D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -44,12 +44,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -57,7 +67,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -66,42 +76,42 @@
   <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
@@ -136,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="980">
   <si>
     <t>Ticker</t>
   </si>
@@ -3067,6 +3077,15 @@
   </si>
   <si>
     <t>Budget Footwear</t>
+  </si>
+  <si>
+    <t>$HBI</t>
+  </si>
+  <si>
+    <t>Hanesbrands Inc.</t>
+  </si>
+  <si>
+    <t>Multinational Fashion Brands</t>
   </si>
 </sst>
 </file>
@@ -3074,14 +3093,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3432,7 +3451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3524,7 +3543,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3533,13 +3552,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3568,16 +3587,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3586,12 +3605,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3628,7 +3647,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3646,7 +3665,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3667,7 +3686,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3694,15 +3713,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3711,7 +3730,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3722,16 +3741,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3766,7 +3785,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3778,7 +3797,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3813,7 +3832,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3841,8 +3860,7 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4919,17 +4937,17 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>116.64249999999998</v>
+            <v>120.24999999999999</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>0</v>
+            <v>13.872</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>116.64249999999998</v>
+            <v>106.37799999999999</v>
           </cell>
         </row>
         <row r="23">
@@ -4942,8 +4960,95 @@
             <v>1917</v>
           </cell>
         </row>
+        <row r="25">
+          <cell r="C25">
+            <v>388</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>31.096</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D29">
+            <v>45063</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>4.0893015030946032</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>10.025846256461564</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>8.8692679673169916</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="16">
+          <cell r="S16">
+            <v>-11.902999999999997</v>
+          </cell>
+          <cell r="T16">
+            <v>7.0139999999999958</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="T21">
+            <v>-2.7951830820442503E-2</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="K26">
+            <v>0.19490724836825837</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="K27">
+            <v>5.2401809229359962E-2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="K28">
+            <v>4.1008244589488214E-2</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="K29">
+            <v>6.4337034617896707E-2</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="K72">
+            <v>9.3658776773467567E-2</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="K73">
+            <v>0.23735625323305887</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="K74">
+            <v>0.20930060375174159</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="T83">
+            <v>4.5587396635300852</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6407,25 +6512,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6467,7 +6572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6511,7 +6616,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6555,7 +6660,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6599,7 +6704,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -6643,7 +6748,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -6687,7 +6792,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -6731,7 +6836,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -6775,7 +6880,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -6819,7 +6924,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -6863,7 +6968,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -6907,7 +7012,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -6951,7 +7056,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -6995,7 +7100,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7039,7 +7144,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7083,7 +7188,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7127,7 +7232,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7171,7 +7276,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7215,7 +7320,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7259,7 +7364,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7303,7 +7408,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7347,7 +7452,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7391,7 +7496,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7435,7 +7540,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7479,7 +7584,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7523,7 +7628,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7567,7 +7672,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -7611,7 +7716,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -7655,7 +7760,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -7699,7 +7804,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -7743,7 +7848,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -7787,7 +7892,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -7831,7 +7936,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -7875,7 +7980,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -7919,7 +8024,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -7963,7 +8068,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8007,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8051,7 +8156,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8095,7 +8200,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8139,7 +8244,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8183,7 +8288,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8227,7 +8332,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8271,7 +8376,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8315,7 +8420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8429,29 +8534,29 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8493,7 +8598,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8537,7 +8642,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8581,7 +8686,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -8625,7 +8730,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -8669,7 +8774,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -8713,7 +8818,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -8757,7 +8862,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -8801,7 +8906,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -8845,7 +8950,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -8889,7 +8994,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -8933,7 +9038,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -8977,7 +9082,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9021,7 +9126,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9065,7 +9170,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9109,7 +9214,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9153,7 +9258,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9197,7 +9302,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9241,7 +9346,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9285,7 +9390,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9329,7 +9434,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9373,7 +9478,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9417,7 +9522,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9461,7 +9566,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9505,7 +9610,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9549,7 +9654,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9593,7 +9698,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -9637,7 +9742,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -9681,7 +9786,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -9725,7 +9830,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -9769,7 +9874,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -9813,7 +9918,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -9857,7 +9962,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -9901,7 +10006,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -9945,7 +10050,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -9989,7 +10094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10033,7 +10138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10077,7 +10182,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10185,20 +10290,20 @@
   </sheetPr>
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10240,7 +10345,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="150" t="s">
         <v>590</v>
       </c>
@@ -10284,7 +10389,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="150" t="s">
         <v>590</v>
       </c>
@@ -10328,7 +10433,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="150" t="s">
         <v>598</v>
       </c>
@@ -10372,7 +10477,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="150" t="s">
         <v>605</v>
       </c>
@@ -10416,7 +10521,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="150" t="s">
         <v>609</v>
       </c>
@@ -10460,7 +10565,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="150" t="s">
         <v>615</v>
       </c>
@@ -10504,7 +10609,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="150" t="s">
         <v>620</v>
       </c>
@@ -10548,7 +10653,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="150" t="s">
         <v>623</v>
       </c>
@@ -10592,7 +10697,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="150" t="s">
         <v>628</v>
       </c>
@@ -10636,7 +10741,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="150" t="s">
         <v>633</v>
       </c>
@@ -10680,7 +10785,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="150" t="s">
         <v>636</v>
       </c>
@@ -10724,7 +10829,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="150" t="s">
         <v>642</v>
       </c>
@@ -10768,7 +10873,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="150" t="s">
         <v>647</v>
       </c>
@@ -10812,7 +10917,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="150" t="s">
         <v>653</v>
       </c>
@@ -10856,7 +10961,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -10900,7 +11005,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="150" t="s">
         <v>662</v>
       </c>
@@ -10944,7 +11049,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="150" t="s">
         <v>667</v>
       </c>
@@ -10988,7 +11093,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="150" t="s">
         <v>667</v>
       </c>
@@ -11032,7 +11137,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="150" t="s">
         <v>679</v>
       </c>
@@ -11076,7 +11181,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="150" t="s">
         <v>685</v>
       </c>
@@ -11120,7 +11225,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="150" t="s">
         <v>691</v>
       </c>
@@ -11164,7 +11269,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
         <v>697</v>
       </c>
@@ -11208,7 +11313,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="150" t="s">
         <v>700</v>
       </c>
@@ -11252,7 +11357,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11296,7 +11401,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11340,7 +11445,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="150" t="s">
         <v>715</v>
       </c>
@@ -11384,7 +11489,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="150" t="s">
         <v>721</v>
       </c>
@@ -11428,7 +11533,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11472,7 +11577,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="150" t="s">
         <v>732</v>
       </c>
@@ -11516,7 +11621,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11560,7 +11665,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="150" t="s">
         <v>742</v>
       </c>
@@ -11604,7 +11709,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="150" t="s">
         <v>748</v>
       </c>
@@ -11648,7 +11753,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="150" t="s">
         <v>753</v>
       </c>
@@ -11692,7 +11797,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -11737,7 +11842,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="150" t="s">
         <v>763</v>
       </c>
@@ -11781,7 +11886,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -11825,7 +11930,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="150" t="s">
         <v>774</v>
       </c>
@@ -11869,7 +11974,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="150" t="s">
         <v>780</v>
       </c>
@@ -11913,7 +12018,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="150" t="s">
         <v>786</v>
       </c>
@@ -11957,7 +12062,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="150" t="s">
         <v>791</v>
       </c>
@@ -12001,7 +12106,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12045,7 +12150,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="150" t="s">
         <v>801</v>
       </c>
@@ -12089,7 +12194,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12133,7 +12238,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12177,7 +12282,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12222,7 +12327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12266,7 +12371,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="150" t="s">
         <v>825</v>
       </c>
@@ -12310,7 +12415,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12354,7 +12459,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="150" t="s">
         <v>836</v>
       </c>
@@ -12398,7 +12503,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="150" t="s">
         <v>825</v>
       </c>
@@ -12442,7 +12547,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="152" t="s">
         <v>846</v>
       </c>
@@ -12486,7 +12591,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="152" t="s">
         <v>846</v>
       </c>
@@ -12530,7 +12635,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="152" t="s">
         <v>856</v>
       </c>
@@ -12574,7 +12679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -12618,7 +12723,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -12663,7 +12768,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -12707,7 +12812,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="152" t="s">
         <v>871</v>
       </c>
@@ -12751,7 +12856,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -12795,7 +12900,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -12840,7 +12945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="152" t="s">
         <v>884</v>
       </c>
@@ -12884,7 +12989,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="152" t="s">
         <v>890</v>
       </c>
@@ -12928,7 +13033,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="152" t="s">
         <v>890</v>
       </c>
@@ -12972,7 +13077,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="152" t="s">
         <v>900</v>
       </c>
@@ -13016,7 +13121,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13061,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13105,7 +13210,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13149,7 +13254,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="152" t="s">
         <v>920</v>
       </c>
@@ -13193,7 +13298,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="152" t="s">
         <v>926</v>
       </c>
@@ -13237,7 +13342,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="152" t="s">
         <v>932</v>
       </c>
@@ -13281,7 +13386,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="152" t="s">
         <v>937</v>
       </c>
@@ -13325,7 +13430,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="152" t="s">
         <v>943</v>
       </c>
@@ -13369,7 +13474,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="152" t="s">
         <v>949</v>
       </c>
@@ -13413,7 +13518,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="152" t="s">
         <v>949</v>
       </c>
@@ -13457,7 +13562,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13501,7 +13606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13545,7 +13650,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="152" t="s">
         <v>968</v>
       </c>
@@ -13589,7 +13694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -13733,38 +13838,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AM54"/>
+  <dimension ref="A1:AM55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Y27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK41" sqref="AK41"/>
+      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="24" width="9.140625" style="4"/>
-    <col min="25" max="30" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="24" width="9.1640625" style="4"/>
+    <col min="25" max="30" width="9.1640625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.140625" style="4"/>
-    <col min="35" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="1"/>
+    <col min="32" max="34" width="9.1640625" style="4"/>
+    <col min="35" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="155" t="s">
         <v>499</v>
@@ -13851,7 +13956,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -13965,7 +14070,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -13979,19 +14084,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$48</f>
+        <f>[1]Main!$C$6*$E$49</f>
         <v>95.947999999999993</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$48</f>
+        <f>[1]Main!$C$8*$E$49</f>
         <v>149582.932</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$48</f>
+        <f>[1]Main!$C$11*$E$49</f>
         <v>987.69999999999993</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$48</f>
+        <f>[1]Main!$C$12*$E$49</f>
         <v>148595.23199999999</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -14007,15 +14112,15 @@
         <v>29.611379424412871</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AF$21*1000*E48</f>
+        <f>'[1]Financial Model'!$AF$21*1000*E49</f>
         <v>5018.1799999999939</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AE$21*1000*E48</f>
+        <f>'[1]Financial Model'!$AE$21*1000*E49</f>
         <v>4753.409999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E48</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E49</f>
         <v>2107.37</v>
       </c>
       <c r="R3" s="51">
@@ -14061,7 +14166,7 @@
         <v>0.19333333333333316</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E48</f>
+        <f>[1]Main!$C$26*E49</f>
         <v>8019.46</v>
       </c>
       <c r="AF3" s="53">
@@ -14088,7 +14193,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14102,19 +14207,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$48</f>
+        <f>[2]Main!$C$6*$E$49</f>
         <v>27.572599999999998</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$48</f>
+        <f>[2]Main!$C$8*$E$49</f>
         <v>10689.566148799999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$48</f>
+        <f>[2]Main!$C$11*$E$49</f>
         <v>-3872.8090499999998</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$48</f>
+        <f>[2]Main!$C$12*$E$49</f>
         <v>14562.375198799997</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -14130,15 +14235,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E48</f>
+        <f>'[2]Financial Model'!$AA$22*E49</f>
         <v>1151.127829999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$48</f>
+        <f>'[2]Financial Model'!$Z$22*$E$49</f>
         <v>338.51467000000116</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$48</f>
+        <f>'[2]Financial Model'!$Y$22*$E$49</f>
         <v>563.94267000000013</v>
       </c>
       <c r="R4" s="51">
@@ -14173,7 +14278,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E48</f>
+        <f>[2]Main!$C$26*E49</f>
         <v>1943.3578499999999</v>
       </c>
       <c r="AF4" s="53">
@@ -14194,7 +14299,7 @@
         <v>Denver, US</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14314,7 +14419,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14441,7 +14546,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14568,7 +14673,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -14582,19 +14687,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E48</f>
+        <f>[6]Main!$C$6*E49</f>
         <v>6.8806999999999992</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E48</f>
+        <f>[6]Main!$C$8*E49</f>
         <v>3126.0533853999996</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$48</f>
+        <f>[6]Main!$C$11*$E$49</f>
         <v>149.62410000000008</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$48</f>
+        <f>[6]Main!$C$12*$E$49</f>
         <v>2976.4292853999996</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -14610,15 +14715,15 @@
         <v>24.790599499495396</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$48</f>
+        <f>'[6]Financial Model'!$AA$20*$E$49</f>
         <v>-455.81691000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$48</f>
+        <f>'[6]Financial Model'!$Z$20*$E$49</f>
         <v>76.477859999999353</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$48</f>
+        <f>'[6]Financial Model'!$Y$20*$E$49</f>
         <v>-38.43066000000033</v>
       </c>
       <c r="R8" s="52">
@@ -14667,7 +14772,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E48</f>
+        <f>[6]Main!$C$27*E49</f>
         <v>896.74860000000001</v>
       </c>
       <c r="AF8" s="53">
@@ -14699,7 +14804,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -14713,19 +14818,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E48</f>
+        <f>[7]Main!$C$6*E49</f>
         <v>21.189900000000002</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$48</f>
+        <f>[7]Main!$C$8*$E$49</f>
         <v>1953.161232984</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E48</f>
+        <f>[7]Main!$C$11*E49</f>
         <v>322.90402999999998</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E48</f>
+        <f>[7]Main!$C$12*E49</f>
         <v>1630.2572029840001</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -14762,7 +14867,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E48</f>
+        <f>[7]Main!$C$26*E49</f>
         <v>617.17056999999988</v>
       </c>
       <c r="AF9" s="53">
@@ -14782,7 +14887,7 @@
         <v>Philadelphia, PA</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -14796,19 +14901,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E48</f>
+        <f>[8]Main!$C$6*E49</f>
         <v>10.723599999999999</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E48</f>
+        <f>[8]Main!$C$8*E49</f>
         <v>1932.2747603999996</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$48</f>
+        <f>[8]Main!$C$11*$E$49</f>
         <v>-230.99563999999998</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$48</f>
+        <f>[8]Main!$C$12*$E$49</f>
         <v>2163.2704003999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -14828,11 +14933,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E48</f>
+        <f>'[8]Financial Model'!$Z$17*E49</f>
         <v>348.28957999999989</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F48</f>
+        <f>'[8]Financial Model'!$Y$17*F49</f>
         <v>-252.21325301204848</v>
       </c>
       <c r="Q10" s="4"/>
@@ -14875,7 +14980,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E48</f>
+        <f>[8]Main!$C$26*E49</f>
         <v>570.24818000000005</v>
       </c>
       <c r="AF10" s="53">
@@ -14904,7 +15009,7 @@
         <v>Pittsburgh, US</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15041,7 +15146,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15055,19 +15160,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E48</f>
+        <f>[10]Main!$C$6*E49</f>
         <v>18.7746</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E48</f>
+        <f>[10]Main!$C$8*E49</f>
         <v>929.07985559999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E48</f>
+        <f>[10]Main!$C$11*E49</f>
         <v>123.55711999999997</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E48</f>
+        <f>[10]Main!$C$12*E49</f>
         <v>805.52273559999992</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -15088,15 +15193,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E48</f>
+        <f>'[10]Financial Model'!$X$18*E49</f>
         <v>218.29829999999976</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$48</f>
+        <f>'[10]Financial Model'!$W$18*$E$49</f>
         <v>-94.637430000000123</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$48</f>
+        <f>'[10]Financial Model'!$V$18*$E$49</f>
         <v>32.667140000000508</v>
       </c>
       <c r="R12" s="52">
@@ -15145,7 +15250,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E48</f>
+        <f>'[10]Financial Model'!$Q$41*E49</f>
         <v>615.8292899999999</v>
       </c>
       <c r="AF12" s="53">
@@ -15174,7 +15279,7 @@
         <v>Ohio, US</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15296,7 +15401,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="103" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15400,7 +15505,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15538,7 +15643,7 @@
         <v>Cheltenham, UK</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -15655,7 +15760,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -15754,7 +15859,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -15780,7 +15885,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B19" s="136" t="s">
         <v>583</v>
       </c>
@@ -15788,9 +15893,9 @@
         <v>584</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="156"/>
-      <c r="H19" s="156"/>
-      <c r="I19" s="156"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
       <c r="L19" s="50"/>
       <c r="R19" s="51"/>
       <c r="S19" s="51"/>
@@ -15811,172 +15916,175 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B20" s="135" t="s">
+        <v>977</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="21" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="156"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="1"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="AM20" s="4" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>489</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="156"/>
-      <c r="H21" s="156"/>
-      <c r="I21" s="157"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
       <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-    </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="AM21" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="22" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>492</v>
+        <v>214</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>31</v>
+        <v>489</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="G22" s="156"/>
-      <c r="H22" s="156"/>
-      <c r="I22" s="157"/>
+        <v>15</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>556</v>
+    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B23" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>557</v>
+        <v>493</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="F23" s="54">
-        <f>[16]Main!$C$6*E48</f>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+    </row>
+    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B24" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F24" s="54">
+        <f>[16]Main!$C$6*E49</f>
         <v>275.07030000000003</v>
       </c>
-      <c r="G23" s="156">
-        <f>[16]Main!$C$8*E48</f>
+      <c r="G24" s="56">
+        <f>[16]Main!$C$8*E49</f>
         <v>33641.097689999995</v>
       </c>
-      <c r="H23" s="156">
-        <f>[16]Main!$C$11*E48</f>
+      <c r="H24" s="56">
+        <f>[16]Main!$C$11*E49</f>
         <v>0</v>
       </c>
-      <c r="I23" s="156">
-        <f>[16]Main!$C$12*E48</f>
+      <c r="I24" s="56">
+        <f>[16]Main!$C$12*E49</f>
         <v>33641.097689999995</v>
       </c>
-      <c r="AK23" s="4">
+      <c r="AK24" s="4">
         <f>[16]Main!$C$24</f>
         <v>1998</v>
       </c>
-      <c r="AL23" s="4" t="str">
+      <c r="AL24" s="4" t="str">
         <f>[16]Main!$C$23</f>
         <v>Vancouver, Canada</v>
       </c>
-      <c r="AM23" s="4" t="s">
+      <c r="AM24" s="4" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B24" s="135">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B25" s="135">
         <v>9983</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="F24" s="54">
-        <f>81600*E50</f>
+      <c r="F25" s="54">
+        <f>81600*E51</f>
         <v>489.6</v>
       </c>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="AK24" s="4">
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="AK25" s="4">
         <v>1949</v>
       </c>
-      <c r="AL24" s="4" t="s">
+      <c r="AL25" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="AM24" s="4" t="s">
+      <c r="AM25" s="4" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B25" s="135" t="s">
+    <row r="26" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-    </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B26" s="135" t="s">
-        <v>576</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>572</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>573</v>
@@ -15985,208 +16093,210 @@
         <v>579</v>
       </c>
       <c r="F26" s="54"/>
-      <c r="G26" s="156"/>
-      <c r="H26" s="156"/>
-      <c r="I26" s="156"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G27" s="156"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="157"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-    </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B28" s="136" t="s">
-        <v>583</v>
-      </c>
-      <c r="C28" s="133" t="s">
-        <v>554</v>
-      </c>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="157"/>
+    <row r="27" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B27" s="135" t="s">
+        <v>576</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F27" s="54"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+    </row>
+    <row r="28" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="56"/>
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="F29" s="7">
-        <f>18.22*E48</f>
-        <v>15.122599999999998</v>
-      </c>
-      <c r="G29" s="156"/>
-      <c r="H29" s="156"/>
-      <c r="I29" s="157"/>
+    <row r="29" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B29" s="136" t="s">
+        <v>583</v>
+      </c>
+      <c r="C29" s="133" t="s">
+        <v>554</v>
+      </c>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="56"/>
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
-      <c r="AM29" s="4" t="s">
+    </row>
+    <row r="30" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B30" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F30" s="7">
+        <f>18.22*E49</f>
+        <v>15.122599999999998</v>
+      </c>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="AM30" s="4" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B31" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="54">
+      <c r="F31" s="54">
         <f>[17]Main!$C$6</f>
         <v>20.806000000000001</v>
       </c>
-      <c r="G30" s="156">
+      <c r="G31" s="56">
         <f>[17]Main!$C$8</f>
         <v>8041.1028800000004</v>
       </c>
-      <c r="H30" s="157"/>
-      <c r="I30" s="156">
+      <c r="H31" s="1"/>
+      <c r="I31" s="56">
         <f>[17]Main!$C$12</f>
         <v>8041.1028800000004</v>
       </c>
-      <c r="J30" s="4" t="str">
+      <c r="J31" s="4" t="str">
         <f>[17]Main!$C$29</f>
         <v>H122</v>
       </c>
-      <c r="K30" s="85">
+      <c r="K31" s="85">
         <f>[17]Main!$D$29</f>
         <v>44882</v>
       </c>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="Z30" s="53">
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="Z31" s="53">
         <f>'[17]Financial Model'!$K$28</f>
         <v>0.70111524163568772</v>
       </c>
-      <c r="AA30" s="53">
+      <c r="AA31" s="53">
         <f>'[17]Financial Model'!$K$29</f>
         <v>0.19553903345724907</v>
       </c>
-      <c r="AB30" s="53">
+      <c r="AB31" s="53">
         <f>'[17]Financial Model'!$K$30</f>
         <v>0.14423791821561338</v>
       </c>
-      <c r="AC30" s="53">
+      <c r="AC31" s="53">
         <f>'[17]Financial Model'!$K$31</f>
         <v>0.22709163346613545</v>
       </c>
-      <c r="AK30" s="4">
+      <c r="AK31" s="4">
         <f>[17]Main!$C$24</f>
         <v>1856</v>
       </c>
-      <c r="AL30" s="4" t="str">
+      <c r="AL31" s="4" t="str">
         <f>[17]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AM30" s="4" t="s">
+      <c r="AM31" s="4" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B32" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F32" s="7">
         <v>2.9</v>
       </c>
-      <c r="G31" s="156"/>
-      <c r="H31" s="157"/>
-      <c r="I31" s="157"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="AM31" s="4" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="156"/>
-      <c r="H32" s="157"/>
-      <c r="I32" s="157"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="M32" s="56"/>
       <c r="N32" s="56"/>
-    </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="AM32" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="33" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>266</v>
+        <v>574</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>31</v>
+        <v>573</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>579</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="156"/>
-      <c r="H33" s="157"/>
-      <c r="I33" s="157"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="M33" s="56"/>
       <c r="N33" s="56"/>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>31</v>
@@ -16195,186 +16305,274 @@
         <v>579</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="156"/>
-      <c r="H34" s="157"/>
-      <c r="I34" s="157"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="M34" s="56"/>
       <c r="N34" s="56"/>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>579</v>
+      </c>
       <c r="F35" s="7"/>
-      <c r="G35" s="156"/>
-      <c r="H35" s="157"/>
-      <c r="I35" s="157"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="M35" s="56"/>
       <c r="N35" s="56"/>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B36" s="136" t="s">
-        <v>583</v>
-      </c>
-      <c r="C36" s="133" t="s">
-        <v>567</v>
-      </c>
-      <c r="G36" s="156"/>
-      <c r="H36" s="157"/>
-      <c r="I36" s="157"/>
+    <row r="36" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="F36" s="7"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="M36" s="56"/>
       <c r="N36" s="56"/>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="G37" s="156"/>
-      <c r="H37" s="157"/>
-      <c r="I37" s="157"/>
+    <row r="37" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B37" s="136" t="s">
+        <v>583</v>
+      </c>
+      <c r="C37" s="133" t="s">
+        <v>567</v>
+      </c>
+      <c r="G37" s="56"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="G38" s="156"/>
-      <c r="H38" s="157"/>
-      <c r="I38" s="157"/>
+        <v>585</v>
+      </c>
+      <c r="G38" s="56"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="G39" s="156"/>
-      <c r="H39" s="157"/>
-      <c r="I39" s="157"/>
+        <v>586</v>
+      </c>
+      <c r="G39" s="56"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>568</v>
+        <v>582</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="156"/>
-      <c r="H40" s="157"/>
-      <c r="I40" s="157"/>
+        <v>587</v>
+      </c>
+      <c r="G40" s="56"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
-        <v>569</v>
+    <row r="41" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B41" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>489</v>
+        <v>13</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="54">
-        <f>[18]Main!$C$6</f>
-        <v>2.4049999999999998</v>
-      </c>
-      <c r="G41" s="156">
-        <f>[18]Main!$C$8</f>
-        <v>116.64249999999998</v>
-      </c>
-      <c r="H41" s="156">
-        <f>[18]Main!$C$11</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="156">
-        <f>[18]Main!$C$12</f>
-        <v>116.64249999999998</v>
-      </c>
+      <c r="G41" s="56"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
-      <c r="AK41" s="4">
+    </row>
+    <row r="42" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="54">
+        <f>[18]Main!$C$6</f>
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="G42" s="56">
+        <f>[18]Main!$C$8</f>
+        <v>120.24999999999999</v>
+      </c>
+      <c r="H42" s="56">
+        <f>[18]Main!$C$11</f>
+        <v>13.872</v>
+      </c>
+      <c r="I42" s="56">
+        <f>[18]Main!$C$12</f>
+        <v>106.37799999999999</v>
+      </c>
+      <c r="J42" s="4" t="str">
+        <f>[18]Main!$C$29</f>
+        <v>H122</v>
+      </c>
+      <c r="K42" s="85">
+        <f>[18]Main!$D$29</f>
+        <v>45063</v>
+      </c>
+      <c r="L42" s="50">
+        <f>[18]Main!$C$38</f>
+        <v>8.8692679673169916</v>
+      </c>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56">
+        <f>'[18]Financial Model'!$T$16</f>
+        <v>7.0139999999999958</v>
+      </c>
+      <c r="P42" s="56">
+        <f>'[18]Financial Model'!$S$16</f>
+        <v>-11.902999999999997</v>
+      </c>
+      <c r="Q42" s="56">
+        <f>'[18]Financial Model'!$R$17</f>
+        <v>0</v>
+      </c>
+      <c r="R42" s="51">
+        <f>[18]Main!$C$37</f>
+        <v>10.025846256461564</v>
+      </c>
+      <c r="S42" s="156">
+        <f>'[18]Financial Model'!$T$83</f>
+        <v>4.5587396635300852</v>
+      </c>
+      <c r="T42" s="51">
+        <f>[18]Main!$C$34</f>
+        <v>4.0893015030946032</v>
+      </c>
+      <c r="W42" s="53">
+        <f>'[18]Financial Model'!$T$21</f>
+        <v>-2.7951830820442503E-2</v>
+      </c>
+      <c r="Z42" s="53">
+        <f>'[18]Financial Model'!$K$26</f>
+        <v>0.19490724836825837</v>
+      </c>
+      <c r="AA42" s="53">
+        <f>'[18]Financial Model'!$K$27</f>
+        <v>5.2401809229359962E-2</v>
+      </c>
+      <c r="AB42" s="53">
+        <f>'[18]Financial Model'!$K$28</f>
+        <v>4.1008244589488214E-2</v>
+      </c>
+      <c r="AC42" s="53">
+        <f>'[18]Financial Model'!$K$29</f>
+        <v>6.4337034617896707E-2</v>
+      </c>
+      <c r="AE42" s="56">
+        <f>[18]Main!$C$27</f>
+        <v>31.096</v>
+      </c>
+      <c r="AF42" s="53">
+        <f>'[18]Financial Model'!$K$72</f>
+        <v>9.3658776773467567E-2</v>
+      </c>
+      <c r="AG42" s="53">
+        <f>'[18]Financial Model'!$K$73</f>
+        <v>0.23735625323305887</v>
+      </c>
+      <c r="AH42" s="53">
+        <f>'[18]Financial Model'!$K$74</f>
+        <v>0.20930060375174159</v>
+      </c>
+      <c r="AI42" s="4">
+        <f>[18]Main!$C$25</f>
+        <v>388</v>
+      </c>
+      <c r="AK42" s="4">
         <f>[18]Main!$C$24</f>
         <v>1917</v>
       </c>
-      <c r="AL41" s="4" t="str">
+      <c r="AL42" s="4" t="str">
         <f>[18]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
-      <c r="AM41" s="4" t="s">
+      <c r="AM42" s="4" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G42" s="156"/>
-      <c r="H42" s="157"/>
-      <c r="I42" s="157"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-    </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G43" s="156"/>
-      <c r="H43" s="157"/>
-      <c r="I43" s="157"/>
+    <row r="43" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="G43" s="56"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="M43" s="56"/>
       <c r="N43" s="56"/>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G44" s="156"/>
-      <c r="H44" s="157"/>
-      <c r="I44" s="157"/>
+    <row r="44" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="G44" s="56"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G45" s="49"/>
-      <c r="I45" s="4"/>
+    <row r="45" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="G45" s="56"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G46" s="49"/>
       <c r="I46" s="4"/>
       <c r="J46" s="1"/>
@@ -16382,79 +16580,87 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D47" s="153" t="s">
-        <v>495</v>
-      </c>
-      <c r="E47" s="154"/>
-      <c r="F47" s="42" t="s">
-        <v>496</v>
-      </c>
+    <row r="47" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G47" s="49"/>
       <c r="I47" s="4"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D48" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E48" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="F48" s="45">
-        <f>1/E48</f>
-        <v>1.2048192771084338</v>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+    </row>
+    <row r="48" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="D48" s="153" t="s">
+        <v>495</v>
+      </c>
+      <c r="E48" s="154"/>
+      <c r="F48" s="42" t="s">
+        <v>496</v>
       </c>
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D49" s="43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E49" s="44">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="F49" s="45">
         <f>1/E49</f>
-        <v>1.1494252873563218</v>
+        <v>1.2048192771084338</v>
       </c>
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D50" s="46" t="s">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.15">
+      <c r="D50" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E50" s="44">
+        <v>0.87</v>
+      </c>
+      <c r="F50" s="45">
+        <f>1/E50</f>
+        <v>1.1494252873563218</v>
+      </c>
+      <c r="G50" s="49"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.15">
+      <c r="D51" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="E50" s="48">
+      <c r="E51" s="48">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F50" s="47">
-        <f>1/E50</f>
+      <c r="F51" s="47">
+        <f>1/E51</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="G50" s="49"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G51" s="49"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G54" s="49"/>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.15">
+      <c r="G55" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -16472,13 +16678,13 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
-    <hyperlink ref="B30" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B31" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{183ACAEF-5A70-4D85-94EE-2D4C25FF95CC}"/>
-    <hyperlink ref="B23" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
-    <hyperlink ref="B36" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
-    <hyperlink ref="B28" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
+    <hyperlink ref="B24" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
+    <hyperlink ref="B37" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
+    <hyperlink ref="B29" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
     <hyperlink ref="B19" r:id="rId20" xr:uid="{8B27DD55-F39A-E042-A7A2-82BE3E8447D7}"/>
-    <hyperlink ref="B41" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
+    <hyperlink ref="B42" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId22"/>
@@ -16499,21 +16705,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -16524,7 +16730,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -16551,98 +16757,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
Update Overview - Fashion Retailers.xlsx
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9A3B1E-6CCD-2046-B8FD-DD8614F0D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13943ADB-041A-D641-8EF4-3613569553AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="986">
   <si>
     <t>Ticker</t>
   </si>
@@ -3076,9 +3076,6 @@
     <t>HKD$0.024</t>
   </si>
   <si>
-    <t>Budget Footwear</t>
-  </si>
-  <si>
     <t>$HBI</t>
   </si>
   <si>
@@ -3086,6 +3083,27 @@
   </si>
   <si>
     <t>Multinational Fashion Brands</t>
+  </si>
+  <si>
+    <t>Sports &amp; Footwear Retail</t>
+  </si>
+  <si>
+    <t>Budget Footwear Retail</t>
+  </si>
+  <si>
+    <t>Casual Footwear</t>
+  </si>
+  <si>
+    <t>Athletic &amp; Casual Footwear</t>
+  </si>
+  <si>
+    <t>Casual Fashion</t>
+  </si>
+  <si>
+    <t>Fast-Fashion Retailer</t>
+  </si>
+  <si>
+    <t>Casual &amp; Workwear Fashion Brands</t>
   </si>
 </sst>
 </file>
@@ -13841,10 +13859,10 @@
   <dimension ref="A1:AM55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14298,6 +14316,9 @@
         <f>[2]Main!$C$23</f>
         <v>Denver, US</v>
       </c>
+      <c r="AM4" s="4" t="s">
+        <v>985</v>
+      </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
@@ -14886,6 +14907,9 @@
         <f>[7]Main!$C$23</f>
         <v>Philadelphia, PA</v>
       </c>
+      <c r="AM9" s="4" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
@@ -15008,6 +15032,9 @@
         <f>[8]Main!$C$23</f>
         <v>Pittsburgh, US</v>
       </c>
+      <c r="AM10" s="4" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
@@ -15277,6 +15304,9 @@
       <c r="AL12" s="4" t="str">
         <f>[10]Main!$C$23</f>
         <v>Ohio, US</v>
+      </c>
+      <c r="AM12" s="4" t="s">
+        <v>983</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.15">
@@ -15641,6 +15671,9 @@
       <c r="AL15" s="4" t="str">
         <f>[13]Main!$C$24</f>
         <v>Cheltenham, UK</v>
+      </c>
+      <c r="AM15" s="4" t="s">
+        <v>983</v>
       </c>
     </row>
     <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.15">
@@ -15918,10 +15951,10 @@
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B20" s="135" t="s">
+        <v>976</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>977</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>978</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>31</v>
@@ -15936,7 +15969,7 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="21" spans="2:39" x14ac:dyDescent="0.15">
@@ -15985,6 +16018,9 @@
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
+      <c r="AM22" s="4" t="s">
+        <v>984</v>
+      </c>
     </row>
     <row r="23" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
@@ -16007,6 +16043,9 @@
       <c r="L23" s="56"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
+      <c r="AM23" s="4" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="24" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
@@ -16098,6 +16137,9 @@
       <c r="I26" s="56"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
+      <c r="AM26" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="27" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B27" s="135" t="s">
@@ -16118,6 +16160,9 @@
       <c r="I27" s="56"/>
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
+      <c r="AM27" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="28" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G28" s="56"/>
@@ -16290,6 +16335,9 @@
       <c r="K33" s="1"/>
       <c r="M33" s="56"/>
       <c r="N33" s="56"/>
+      <c r="AM33" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="34" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
@@ -16312,6 +16360,9 @@
       <c r="K34" s="1"/>
       <c r="M34" s="56"/>
       <c r="N34" s="56"/>
+      <c r="AM34" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="35" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
@@ -16334,6 +16385,9 @@
       <c r="K35" s="1"/>
       <c r="M35" s="56"/>
       <c r="N35" s="56"/>
+      <c r="AM35" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="36" spans="2:39" x14ac:dyDescent="0.15">
       <c r="F36" s="7"/>
@@ -16374,6 +16428,9 @@
       <c r="K38" s="1"/>
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
+      <c r="AM38" s="4" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="39" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
@@ -16389,6 +16446,9 @@
       <c r="K39" s="1"/>
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
+      <c r="AM39" s="4" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="40" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
@@ -16396,6 +16456,9 @@
       </c>
       <c r="C40" s="1" t="s">
         <v>587</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="G40" s="56"/>
       <c r="H40" s="1"/>
@@ -16404,6 +16467,9 @@
       <c r="K40" s="1"/>
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
+      <c r="AM40" s="4" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="41" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
@@ -16425,6 +16491,9 @@
       <c r="K41" s="1"/>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
+      <c r="AM41" s="4" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="42" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B42" s="3" t="s">
@@ -16542,7 +16611,7 @@
         <v>Leicester, UK</v>
       </c>
       <c r="AM42" s="4" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
     </row>
     <row r="43" spans="2:39" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update Fashion Retailers Overview to include details of owned brands/stores
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13943ADB-041A-D641-8EF4-3613569553AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D58741-CDE4-184E-AAAD-343C696DFB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="1013">
   <si>
     <t>Ticker</t>
   </si>
@@ -1882,9 +1882,6 @@
     <t>€ADS</t>
   </si>
   <si>
-    <t>Addidas AG</t>
-  </si>
-  <si>
     <t>€</t>
   </si>
   <si>
@@ -3104,6 +3101,90 @@
   </si>
   <si>
     <t>Casual &amp; Workwear Fashion Brands</t>
+  </si>
+  <si>
+    <t>$GCO</t>
+  </si>
+  <si>
+    <t>Genesco, Inc.</t>
+  </si>
+  <si>
+    <t>Casual Footwear Retailer</t>
+  </si>
+  <si>
+    <t>Schuh, Johnston &amp; Murphy, Dockers, Journeys</t>
+  </si>
+  <si>
+    <t>Nike, Converse, Jordan</t>
+  </si>
+  <si>
+    <t>Vans, North Face, Timberland, Dickies</t>
+  </si>
+  <si>
+    <t>Owned Brands / Companies</t>
+  </si>
+  <si>
+    <t>Sports Direct, Game, House of Fraser</t>
+  </si>
+  <si>
+    <t>Abercrombie &amp; Fitch, Hollister</t>
+  </si>
+  <si>
+    <t>American Eagle Outfitters, Aerie</t>
+  </si>
+  <si>
+    <t>Under Armour, MyFitnessPal</t>
+  </si>
+  <si>
+    <t>UNIQLO, GU, PLST, Theory</t>
+  </si>
+  <si>
+    <t>ASOS, TopShop/TopMan &amp; more</t>
+  </si>
+  <si>
+    <t>boohoo, PrettyLittleThing, Debehnhams &amp; more</t>
+  </si>
+  <si>
+    <t>Made.com, JV to save £JOUL</t>
+  </si>
+  <si>
+    <t>Go Outdoors, Shoe Palace, Blacks &amp; more</t>
+  </si>
+  <si>
+    <t>Anthrapologie, Free People, BHLDN.&amp; more</t>
+  </si>
+  <si>
+    <t>Ted Baker</t>
+  </si>
+  <si>
+    <t>Superdry</t>
+  </si>
+  <si>
+    <t>Joules, Little Joules, Baby Joule</t>
+  </si>
+  <si>
+    <t>Rescued in Dec 22 in Joint Venture by £NXT &amp; founder Tom Joule</t>
+  </si>
+  <si>
+    <t>Acquired by Authentic Brands Group for £211m in October 22</t>
+  </si>
+  <si>
+    <t>Hanes, Champion, Playtex &amp; more</t>
+  </si>
+  <si>
+    <t>Adidas, Reebok &amp; Taylor Made</t>
+  </si>
+  <si>
+    <t>Adidas AG</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>Sub-Sector / Notes</t>
+  </si>
+  <si>
+    <t>Key Notes</t>
   </si>
 </sst>
 </file>
@@ -3869,6 +3950,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3878,7 +3960,6 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4945,6 +5026,7 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -5067,6 +5149,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10365,7 +10448,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="150" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B2" s="138" t="s">
         <v>513</v>
@@ -10377,10 +10460,10 @@
         <v>567</v>
       </c>
       <c r="E2" s="139" t="s">
+        <v>590</v>
+      </c>
+      <c r="F2" s="139" t="s">
         <v>591</v>
-      </c>
-      <c r="F2" s="139" t="s">
-        <v>592</v>
       </c>
       <c r="G2" s="140">
         <v>35.64</v>
@@ -10401,7 +10484,7 @@
         <v>45005</v>
       </c>
       <c r="M2" s="138" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N2" s="143">
         <v>-4.0000000000000002E-4</v>
@@ -10409,10 +10492,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="150" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B3" s="138" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C3" s="148" t="s">
         <v>573</v>
@@ -10421,10 +10504,10 @@
         <v>567</v>
       </c>
       <c r="E3" s="139" t="s">
+        <v>594</v>
+      </c>
+      <c r="F3" s="139" t="s">
         <v>595</v>
-      </c>
-      <c r="F3" s="139" t="s">
-        <v>596</v>
       </c>
       <c r="G3" s="140">
         <v>30.07</v>
@@ -10436,7 +10519,7 @@
         <v>1.64</v>
       </c>
       <c r="J3" s="140" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K3" s="141">
         <v>0.83240000000000003</v>
@@ -10453,22 +10536,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="150" t="s">
+        <v>597</v>
+      </c>
+      <c r="B4" s="138" t="s">
         <v>598</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="C4" s="148" t="s">
         <v>599</v>
-      </c>
-      <c r="C4" s="148" t="s">
-        <v>600</v>
       </c>
       <c r="D4" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E4" s="139" t="s">
+        <v>600</v>
+      </c>
+      <c r="F4" s="139" t="s">
         <v>601</v>
-      </c>
-      <c r="F4" s="139" t="s">
-        <v>602</v>
       </c>
       <c r="G4" s="139">
         <v>19.149999999999999</v>
@@ -10480,7 +10563,7 @@
         <v>1.3</v>
       </c>
       <c r="J4" s="140" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K4" s="143">
         <v>3.5999999999999999E-3</v>
@@ -10489,7 +10572,7 @@
         <v>54</v>
       </c>
       <c r="M4" s="138" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N4" s="141">
         <v>2.3099999999999999E-2</v>
@@ -10497,22 +10580,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="150" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5" s="138" t="s">
+        <v>598</v>
+      </c>
+      <c r="C5" s="148" t="s">
         <v>605</v>
-      </c>
-      <c r="B5" s="138" t="s">
-        <v>599</v>
-      </c>
-      <c r="C5" s="148" t="s">
-        <v>606</v>
       </c>
       <c r="D5" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E5" s="139" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F5" s="139" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G5" s="140">
         <v>31.59</v>
@@ -10524,7 +10607,7 @@
         <v>1.3</v>
       </c>
       <c r="J5" s="145" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K5" s="146">
         <v>0.26879999999999998</v>
@@ -10541,22 +10624,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="150" t="s">
+        <v>608</v>
+      </c>
+      <c r="B6" s="138" t="s">
         <v>609</v>
       </c>
-      <c r="B6" s="138" t="s">
-        <v>610</v>
-      </c>
       <c r="C6" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D6" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E6" s="139" t="s">
+        <v>610</v>
+      </c>
+      <c r="F6" s="139" t="s">
         <v>611</v>
-      </c>
-      <c r="F6" s="139" t="s">
-        <v>612</v>
       </c>
       <c r="G6" s="139">
         <v>17.54</v>
@@ -10568,7 +10651,7 @@
         <v>1.9</v>
       </c>
       <c r="J6" s="145" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K6" s="143">
         <v>1.1000000000000001E-3</v>
@@ -10577,7 +10660,7 @@
         <v>54</v>
       </c>
       <c r="M6" s="138" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="N6" s="141">
         <v>2.1600000000000001E-2</v>
@@ -10585,22 +10668,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="150" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B7" s="138" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C7" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D7" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E7" s="139" t="s">
+        <v>615</v>
+      </c>
+      <c r="F7" s="139" t="s">
         <v>616</v>
-      </c>
-      <c r="F7" s="139" t="s">
-        <v>617</v>
       </c>
       <c r="G7" s="139">
         <v>17.59</v>
@@ -10612,7 +10695,7 @@
         <v>1.82</v>
       </c>
       <c r="J7" s="140" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K7" s="146">
         <v>0.47870000000000001</v>
@@ -10621,7 +10704,7 @@
         <v>54</v>
       </c>
       <c r="M7" s="138" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="N7" s="141">
         <v>3.3700000000000001E-2</v>
@@ -10629,10 +10712,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="150" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B8" s="138" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C8" s="148" t="s">
         <v>573</v>
@@ -10641,10 +10724,10 @@
         <v>567</v>
       </c>
       <c r="E8" s="139" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F8" s="139" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G8" s="140">
         <v>65.37</v>
@@ -10656,7 +10739,7 @@
         <v>1.9</v>
       </c>
       <c r="J8" s="139" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K8" s="146">
         <v>0.4647</v>
@@ -10673,10 +10756,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="150" t="s">
+        <v>622</v>
+      </c>
+      <c r="B9" s="138" t="s">
         <v>623</v>
-      </c>
-      <c r="B9" s="138" t="s">
-        <v>624</v>
       </c>
       <c r="C9" s="148" t="s">
         <v>31</v>
@@ -10685,10 +10768,10 @@
         <v>567</v>
       </c>
       <c r="E9" s="139" t="s">
+        <v>624</v>
+      </c>
+      <c r="F9" s="139" t="s">
         <v>625</v>
-      </c>
-      <c r="F9" s="139" t="s">
-        <v>626</v>
       </c>
       <c r="G9" s="145">
         <v>24.8</v>
@@ -10709,7 +10792,7 @@
         <v>44959</v>
       </c>
       <c r="M9" s="138" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="N9" s="141">
         <v>1.5299999999999999E-2</v>
@@ -10717,10 +10800,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="150" t="s">
+        <v>627</v>
+      </c>
+      <c r="B10" s="138" t="s">
         <v>628</v>
-      </c>
-      <c r="B10" s="138" t="s">
-        <v>629</v>
       </c>
       <c r="C10" s="148" t="s">
         <v>573</v>
@@ -10729,10 +10812,10 @@
         <v>567</v>
       </c>
       <c r="E10" s="139" t="s">
+        <v>629</v>
+      </c>
+      <c r="F10" s="139" t="s">
         <v>630</v>
-      </c>
-      <c r="F10" s="139" t="s">
-        <v>631</v>
       </c>
       <c r="G10" s="145">
         <v>22.7</v>
@@ -10744,7 +10827,7 @@
         <v>1.56</v>
       </c>
       <c r="J10" s="139" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K10" s="141">
         <v>0.67789999999999995</v>
@@ -10761,22 +10844,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="150" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B11" s="138" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C11" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D11" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E11" s="139" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F11" s="139" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G11" s="139">
         <v>4.93</v>
@@ -10797,7 +10880,7 @@
         <v>54</v>
       </c>
       <c r="M11" s="138" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="N11" s="141">
         <v>4.65E-2</v>
@@ -10805,10 +10888,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="150" t="s">
+        <v>635</v>
+      </c>
+      <c r="B12" s="138" t="s">
         <v>636</v>
-      </c>
-      <c r="B12" s="138" t="s">
-        <v>637</v>
       </c>
       <c r="C12" s="148" t="s">
         <v>31</v>
@@ -10817,10 +10900,10 @@
         <v>567</v>
       </c>
       <c r="E12" s="139" t="s">
+        <v>637</v>
+      </c>
+      <c r="F12" s="139" t="s">
         <v>638</v>
-      </c>
-      <c r="F12" s="139" t="s">
-        <v>639</v>
       </c>
       <c r="G12" s="139">
         <v>10.33</v>
@@ -10832,7 +10915,7 @@
         <v>0.9</v>
       </c>
       <c r="J12" s="139" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="K12" s="141">
         <v>0.96950000000000003</v>
@@ -10841,7 +10924,7 @@
         <v>44959</v>
       </c>
       <c r="M12" s="138" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N12" s="143">
         <v>-6.1999999999999998E-3</v>
@@ -10849,10 +10932,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="150" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B13" s="138" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C13" s="148" t="s">
         <v>39</v>
@@ -10861,10 +10944,10 @@
         <v>567</v>
       </c>
       <c r="E13" s="139" t="s">
+        <v>642</v>
+      </c>
+      <c r="F13" s="139" t="s">
         <v>643</v>
-      </c>
-      <c r="F13" s="139" t="s">
-        <v>644</v>
       </c>
       <c r="G13" s="145">
         <v>13.45</v>
@@ -10876,7 +10959,7 @@
         <v>108.72</v>
       </c>
       <c r="J13" s="139" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K13" s="141">
         <v>0.82120000000000004</v>
@@ -10885,7 +10968,7 @@
         <v>44972</v>
       </c>
       <c r="M13" s="138" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N13" s="141">
         <v>3.8100000000000002E-2</v>
@@ -10893,22 +10976,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="150" t="s">
+        <v>646</v>
+      </c>
+      <c r="B14" s="138" t="s">
         <v>647</v>
       </c>
-      <c r="B14" s="138" t="s">
-        <v>648</v>
-      </c>
       <c r="C14" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D14" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E14" s="139" t="s">
+        <v>648</v>
+      </c>
+      <c r="F14" s="139" t="s">
         <v>649</v>
-      </c>
-      <c r="F14" s="139" t="s">
-        <v>650</v>
       </c>
       <c r="G14" s="145">
         <v>20.010000000000002</v>
@@ -10920,7 +11003,7 @@
         <v>5.98</v>
       </c>
       <c r="J14" s="140" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K14" s="143">
         <v>2E-3</v>
@@ -10929,7 +11012,7 @@
         <v>54</v>
       </c>
       <c r="M14" s="138" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="N14" s="143">
         <v>-4.0000000000000002E-4</v>
@@ -10937,22 +11020,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="150" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B15" s="138" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C15" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D15" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E15" s="139" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F15" s="139" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G15" s="139">
         <v>13.98</v>
@@ -10964,7 +11047,7 @@
         <v>5.98</v>
       </c>
       <c r="J15" s="140" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K15" s="141">
         <v>0.54590000000000005</v>
@@ -10973,7 +11056,7 @@
         <v>54</v>
       </c>
       <c r="M15" s="138" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N15" s="141">
         <v>2.5499999999999998E-2</v>
@@ -10984,19 +11067,19 @@
         <v>1910</v>
       </c>
       <c r="B16" s="138" t="s">
+        <v>656</v>
+      </c>
+      <c r="C16" s="148" t="s">
         <v>657</v>
-      </c>
-      <c r="C16" s="148" t="s">
-        <v>658</v>
       </c>
       <c r="D16" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E16" s="139" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F16" s="139" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G16" s="145">
         <v>13.48</v>
@@ -11008,7 +11091,7 @@
         <v>5.68</v>
       </c>
       <c r="J16" s="139" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K16" s="141">
         <v>0.53680000000000005</v>
@@ -11017,7 +11100,7 @@
         <v>44999</v>
       </c>
       <c r="M16" s="138" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="N16" s="141">
         <v>1.18E-2</v>
@@ -11025,10 +11108,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="150" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B17" s="138" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C17" s="148" t="s">
         <v>31</v>
@@ -11037,10 +11120,10 @@
         <v>567</v>
       </c>
       <c r="E17" s="139" t="s">
+        <v>662</v>
+      </c>
+      <c r="F17" s="139" t="s">
         <v>663</v>
-      </c>
-      <c r="F17" s="139" t="s">
-        <v>664</v>
       </c>
       <c r="G17" s="139">
         <v>8.89</v>
@@ -11052,7 +11135,7 @@
         <v>1.51</v>
       </c>
       <c r="J17" s="139" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K17" s="141">
         <v>0.9325</v>
@@ -11061,7 +11144,7 @@
         <v>44981</v>
       </c>
       <c r="M17" s="138" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="N17" s="143">
         <v>-2.8E-3</v>
@@ -11069,22 +11152,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="150" t="s">
+        <v>666</v>
+      </c>
+      <c r="B18" s="138" t="s">
         <v>667</v>
       </c>
-      <c r="B18" s="138" t="s">
+      <c r="C18" s="148" t="s">
         <v>668</v>
-      </c>
-      <c r="C18" s="148" t="s">
-        <v>669</v>
       </c>
       <c r="D18" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E18" s="139" t="s">
+        <v>669</v>
+      </c>
+      <c r="F18" s="139" t="s">
         <v>670</v>
-      </c>
-      <c r="F18" s="139" t="s">
-        <v>671</v>
       </c>
       <c r="G18" s="140">
         <v>97.06</v>
@@ -11096,7 +11179,7 @@
         <v>0.45</v>
       </c>
       <c r="J18" s="140" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K18" s="143">
         <v>8.48E-2</v>
@@ -11105,7 +11188,7 @@
         <v>54</v>
       </c>
       <c r="M18" s="138" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="N18" s="141">
         <v>7.1000000000000004E-3</v>
@@ -11113,22 +11196,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="150" t="s">
+        <v>666</v>
+      </c>
+      <c r="B19" s="138" t="s">
         <v>667</v>
       </c>
-      <c r="B19" s="138" t="s">
-        <v>668</v>
-      </c>
       <c r="C19" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D19" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E19" s="139" t="s">
+        <v>674</v>
+      </c>
+      <c r="F19" s="139" t="s">
         <v>675</v>
-      </c>
-      <c r="F19" s="139" t="s">
-        <v>676</v>
       </c>
       <c r="G19" s="140">
         <v>92.37</v>
@@ -11140,7 +11223,7 @@
         <v>0.35</v>
       </c>
       <c r="J19" s="140" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K19" s="143">
         <v>9.4700000000000006E-2</v>
@@ -11149,7 +11232,7 @@
         <v>44867</v>
       </c>
       <c r="M19" s="138" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="N19" s="141">
         <v>6.1000000000000004E-3</v>
@@ -11157,22 +11240,22 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="150" t="s">
+        <v>678</v>
+      </c>
+      <c r="B20" s="138" t="s">
         <v>679</v>
       </c>
-      <c r="B20" s="138" t="s">
-        <v>680</v>
-      </c>
       <c r="C20" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D20" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E20" s="139" t="s">
+        <v>680</v>
+      </c>
+      <c r="F20" s="139" t="s">
         <v>681</v>
-      </c>
-      <c r="F20" s="139" t="s">
-        <v>682</v>
       </c>
       <c r="G20" s="140">
         <v>141.47999999999999</v>
@@ -11184,7 +11267,7 @@
         <v>0.97</v>
       </c>
       <c r="J20" s="140" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="K20" s="146">
         <v>0.29060000000000002</v>
@@ -11193,7 +11276,7 @@
         <v>54</v>
       </c>
       <c r="M20" s="138" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N20" s="141">
         <v>8.0000000000000004E-4</v>
@@ -11201,10 +11284,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="150" t="s">
+        <v>684</v>
+      </c>
+      <c r="B21" s="138" t="s">
         <v>685</v>
-      </c>
-      <c r="B21" s="138" t="s">
-        <v>686</v>
       </c>
       <c r="C21" s="148" t="s">
         <v>39</v>
@@ -11213,10 +11296,10 @@
         <v>567</v>
       </c>
       <c r="E21" s="139" t="s">
+        <v>686</v>
+      </c>
+      <c r="F21" s="139" t="s">
         <v>687</v>
-      </c>
-      <c r="F21" s="139" t="s">
-        <v>688</v>
       </c>
       <c r="G21" s="139">
         <v>10.210000000000001</v>
@@ -11228,7 +11311,7 @@
         <v>0.66</v>
       </c>
       <c r="J21" s="139" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K21" s="141">
         <v>0.9698</v>
@@ -11237,7 +11320,7 @@
         <v>44980</v>
       </c>
       <c r="M21" s="138" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N21" s="143">
         <v>-5.9999999999999995E-4</v>
@@ -11245,10 +11328,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="150" t="s">
+        <v>690</v>
+      </c>
+      <c r="B22" s="138" t="s">
         <v>691</v>
-      </c>
-      <c r="B22" s="138" t="s">
-        <v>692</v>
       </c>
       <c r="C22" s="148" t="s">
         <v>13</v>
@@ -11257,10 +11340,10 @@
         <v>567</v>
       </c>
       <c r="E22" s="139" t="s">
+        <v>692</v>
+      </c>
+      <c r="F22" s="139" t="s">
         <v>693</v>
-      </c>
-      <c r="F22" s="139" t="s">
-        <v>694</v>
       </c>
       <c r="G22" s="139">
         <v>10.95</v>
@@ -11272,7 +11355,7 @@
         <v>1.62</v>
       </c>
       <c r="J22" s="139" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K22" s="141">
         <v>0.68240000000000001</v>
@@ -11281,7 +11364,7 @@
         <v>44889</v>
       </c>
       <c r="M22" s="138" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N22" s="141">
         <v>2.2100000000000002E-2</v>
@@ -11289,22 +11372,22 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B23" s="138" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C23" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D23" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E23" s="139" t="s">
+        <v>692</v>
+      </c>
+      <c r="F23" s="139" t="s">
         <v>693</v>
-      </c>
-      <c r="F23" s="139" t="s">
-        <v>694</v>
       </c>
       <c r="G23" s="140">
         <v>34.520000000000003</v>
@@ -11316,7 +11399,7 @@
         <v>1.62</v>
       </c>
       <c r="J23" s="140" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="K23" s="141">
         <v>0.6845</v>
@@ -11325,7 +11408,7 @@
         <v>54</v>
       </c>
       <c r="M23" s="138" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N23" s="141">
         <v>1.1900000000000001E-2</v>
@@ -11333,22 +11416,22 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="150" t="s">
+        <v>699</v>
+      </c>
+      <c r="B24" s="138" t="s">
         <v>700</v>
       </c>
-      <c r="B24" s="138" t="s">
-        <v>701</v>
-      </c>
       <c r="C24" s="148" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D24" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E24" s="139" t="s">
+        <v>701</v>
+      </c>
+      <c r="F24" s="139" t="s">
         <v>702</v>
-      </c>
-      <c r="F24" s="139" t="s">
-        <v>703</v>
       </c>
       <c r="G24" s="139">
         <v>7.44</v>
@@ -11360,7 +11443,7 @@
         <v>0.98</v>
       </c>
       <c r="J24" s="140" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K24" s="143">
         <v>0</v>
@@ -11369,7 +11452,7 @@
         <v>54</v>
       </c>
       <c r="M24" s="138" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N24" s="141">
         <v>1.7600000000000001E-2</v>
@@ -11380,19 +11463,19 @@
         <v>551</v>
       </c>
       <c r="B25" s="138" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C25" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D25" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E25" s="139" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F25" s="139" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G25" s="139">
         <v>8.0500000000000007</v>
@@ -11404,7 +11487,7 @@
         <v>0.98</v>
       </c>
       <c r="J25" s="139" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K25" s="146">
         <v>0.1731</v>
@@ -11413,7 +11496,7 @@
         <v>54</v>
       </c>
       <c r="M25" s="138" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N25" s="141">
         <v>3.8300000000000001E-2</v>
@@ -11424,19 +11507,19 @@
         <v>1121</v>
       </c>
       <c r="B26" s="138" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C26" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D26" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E26" s="139" t="s">
+        <v>710</v>
+      </c>
+      <c r="F26" s="140" t="s">
         <v>711</v>
-      </c>
-      <c r="F26" s="140" t="s">
-        <v>712</v>
       </c>
       <c r="G26" s="138" t="s">
         <v>54</v>
@@ -11448,7 +11531,7 @@
         <v>1.02</v>
       </c>
       <c r="J26" s="139" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K26" s="143">
         <v>1.52E-2</v>
@@ -11457,7 +11540,7 @@
         <v>54</v>
       </c>
       <c r="M26" s="138" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="N26" s="141">
         <v>1.67E-2</v>
@@ -11465,22 +11548,22 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="150" t="s">
+        <v>714</v>
+      </c>
+      <c r="B27" s="138" t="s">
         <v>715</v>
       </c>
-      <c r="B27" s="138" t="s">
-        <v>716</v>
-      </c>
       <c r="C27" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D27" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E27" s="145" t="s">
+        <v>716</v>
+      </c>
+      <c r="F27" s="139" t="s">
         <v>717</v>
-      </c>
-      <c r="F27" s="139" t="s">
-        <v>718</v>
       </c>
       <c r="G27" s="140">
         <v>65.83</v>
@@ -11492,7 +11575,7 @@
         <v>0.94</v>
       </c>
       <c r="J27" s="145" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K27" s="146">
         <v>0.22289999999999999</v>
@@ -11501,7 +11584,7 @@
         <v>44956</v>
       </c>
       <c r="M27" s="138" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="N27" s="141">
         <v>1.1999999999999999E-3</v>
@@ -11509,10 +11592,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="150" t="s">
+        <v>720</v>
+      </c>
+      <c r="B28" s="138" t="s">
         <v>721</v>
-      </c>
-      <c r="B28" s="138" t="s">
-        <v>722</v>
       </c>
       <c r="C28" s="148" t="s">
         <v>31</v>
@@ -11521,10 +11604,10 @@
         <v>567</v>
       </c>
       <c r="E28" s="145" t="s">
+        <v>722</v>
+      </c>
+      <c r="F28" s="139" t="s">
         <v>723</v>
-      </c>
-      <c r="F28" s="139" t="s">
-        <v>724</v>
       </c>
       <c r="G28" s="139">
         <v>6.75</v>
@@ -11536,7 +11619,7 @@
         <v>3.08</v>
       </c>
       <c r="J28" s="139" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="K28" s="141">
         <v>1</v>
@@ -11545,7 +11628,7 @@
         <v>44979</v>
       </c>
       <c r="M28" s="138" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="N28" s="141">
         <v>3.04E-2</v>
@@ -11556,19 +11639,19 @@
         <v>1836</v>
       </c>
       <c r="B29" s="138" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C29" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D29" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E29" s="145" t="s">
+        <v>727</v>
+      </c>
+      <c r="F29" s="139" t="s">
         <v>728</v>
-      </c>
-      <c r="F29" s="139" t="s">
-        <v>729</v>
       </c>
       <c r="G29" s="139">
         <v>8.3000000000000007</v>
@@ -11580,7 +11663,7 @@
         <v>0.3</v>
       </c>
       <c r="J29" s="139" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="K29" s="146">
         <v>0.11650000000000001</v>
@@ -11589,7 +11672,7 @@
         <v>54</v>
       </c>
       <c r="M29" s="138" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="N29" s="141">
         <v>2.5999999999999999E-3</v>
@@ -11597,10 +11680,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="150" t="s">
+        <v>731</v>
+      </c>
+      <c r="B30" s="138" t="s">
         <v>732</v>
-      </c>
-      <c r="B30" s="138" t="s">
-        <v>733</v>
       </c>
       <c r="C30" s="148" t="s">
         <v>31</v>
@@ -11609,10 +11692,10 @@
         <v>567</v>
       </c>
       <c r="E30" s="145" t="s">
+        <v>733</v>
+      </c>
+      <c r="F30" s="139" t="s">
         <v>734</v>
-      </c>
-      <c r="F30" s="139" t="s">
-        <v>735</v>
       </c>
       <c r="G30" s="139">
         <v>4.8099999999999996</v>
@@ -11624,7 +11707,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="J30" s="145" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K30" s="141">
         <v>0.91869999999999996</v>
@@ -11633,7 +11716,7 @@
         <v>44999</v>
       </c>
       <c r="M30" s="138" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="N30" s="141">
         <v>2.1600000000000001E-2</v>
@@ -11644,19 +11727,19 @@
         <v>3813</v>
       </c>
       <c r="B31" s="138" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C31" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D31" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E31" s="145" t="s">
+        <v>738</v>
+      </c>
+      <c r="F31" s="139" t="s">
         <v>739</v>
-      </c>
-      <c r="F31" s="139" t="s">
-        <v>740</v>
       </c>
       <c r="G31" s="138" t="s">
         <v>54</v>
@@ -11668,7 +11751,7 @@
         <v>1.06</v>
       </c>
       <c r="J31" s="139" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K31" s="143">
         <v>7.1900000000000006E-2</v>
@@ -11677,7 +11760,7 @@
         <v>54</v>
       </c>
       <c r="M31" s="138" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="N31" s="141">
         <v>3.3000000000000002E-2</v>
@@ -11685,22 +11768,22 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="150" t="s">
+        <v>741</v>
+      </c>
+      <c r="B32" s="138" t="s">
         <v>742</v>
       </c>
-      <c r="B32" s="138" t="s">
-        <v>743</v>
-      </c>
       <c r="C32" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D32" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E32" s="140" t="s">
+        <v>743</v>
+      </c>
+      <c r="F32" s="139" t="s">
         <v>744</v>
-      </c>
-      <c r="F32" s="139" t="s">
-        <v>745</v>
       </c>
       <c r="G32" s="140">
         <v>63.22</v>
@@ -11712,7 +11795,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="J32" s="140" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K32" s="146">
         <v>0.13880000000000001</v>
@@ -11721,7 +11804,7 @@
         <v>44963</v>
       </c>
       <c r="M32" s="138" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N32" s="143">
         <v>-2.9100000000000001E-2</v>
@@ -11729,22 +11812,22 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="150" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B33" s="138" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C33" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D33" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E33" s="140" t="s">
+        <v>748</v>
+      </c>
+      <c r="F33" s="139" t="s">
         <v>749</v>
-      </c>
-      <c r="F33" s="139" t="s">
-        <v>750</v>
       </c>
       <c r="G33" s="147">
         <v>1134.01</v>
@@ -11756,7 +11839,7 @@
         <v>0.8</v>
       </c>
       <c r="J33" s="140" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="K33" s="143">
         <v>5.4300000000000001E-2</v>
@@ -11765,7 +11848,7 @@
         <v>54</v>
       </c>
       <c r="M33" s="138" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="N33" s="143">
         <v>-2.7400000000000001E-2</v>
@@ -11773,22 +11856,22 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="150" t="s">
+        <v>752</v>
+      </c>
+      <c r="B34" s="138" t="s">
         <v>753</v>
       </c>
-      <c r="B34" s="138" t="s">
-        <v>754</v>
-      </c>
       <c r="C34" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D34" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E34" s="140" t="s">
+        <v>754</v>
+      </c>
+      <c r="F34" s="139" t="s">
         <v>755</v>
-      </c>
-      <c r="F34" s="139" t="s">
-        <v>756</v>
       </c>
       <c r="G34" s="145">
         <v>20.91</v>
@@ -11800,7 +11883,7 @@
         <v>0.87</v>
       </c>
       <c r="J34" s="145" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="K34" s="143">
         <v>4.58E-2</v>
@@ -11809,7 +11892,7 @@
         <v>54</v>
       </c>
       <c r="M34" s="138" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="N34" s="141">
         <v>7.51E-2</v>
@@ -11820,16 +11903,16 @@
         <v>1058</v>
       </c>
       <c r="B35" s="138" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C35" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D35" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E35" s="140" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F35" s="140" t="e" cm="1" vm="1">
         <f t="array" ref="F35">-_FV(HKD$31,"22")</f>
@@ -11845,7 +11928,7 @@
         <v>0.31</v>
       </c>
       <c r="J35" s="140" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K35" s="143">
         <v>0</v>
@@ -11854,7 +11937,7 @@
         <v>44865</v>
       </c>
       <c r="M35" s="138" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="N35" s="141">
         <v>1.4500000000000001E-2</v>
@@ -11862,22 +11945,22 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="150" t="s">
+        <v>762</v>
+      </c>
+      <c r="B36" s="138" t="s">
         <v>763</v>
       </c>
-      <c r="B36" s="138" t="s">
-        <v>764</v>
-      </c>
       <c r="C36" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D36" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E36" s="140" t="s">
+        <v>764</v>
+      </c>
+      <c r="F36" s="140" t="s">
         <v>765</v>
-      </c>
-      <c r="F36" s="140" t="s">
-        <v>766</v>
       </c>
       <c r="G36" s="138" t="s">
         <v>54</v>
@@ -11889,7 +11972,7 @@
         <v>1.19</v>
       </c>
       <c r="J36" s="139" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K36" s="143">
         <v>0</v>
@@ -11898,7 +11981,7 @@
         <v>54</v>
       </c>
       <c r="M36" s="138" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="N36" s="143">
         <v>-6.9400000000000003E-2</v>
@@ -11909,19 +11992,19 @@
         <v>210</v>
       </c>
       <c r="B37" s="138" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C37" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D37" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E37" s="140" t="s">
+        <v>769</v>
+      </c>
+      <c r="F37" s="145" t="s">
         <v>770</v>
-      </c>
-      <c r="F37" s="145" t="s">
-        <v>771</v>
       </c>
       <c r="G37" s="139">
         <v>6.6</v>
@@ -11933,7 +12016,7 @@
         <v>0.42</v>
       </c>
       <c r="J37" s="145" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="K37" s="143">
         <v>0</v>
@@ -11942,7 +12025,7 @@
         <v>54</v>
       </c>
       <c r="M37" s="138" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N37" s="141">
         <v>9.0899999999999995E-2</v>
@@ -11950,10 +12033,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="150" t="s">
+        <v>773</v>
+      </c>
+      <c r="B38" s="138" t="s">
         <v>774</v>
-      </c>
-      <c r="B38" s="138" t="s">
-        <v>775</v>
       </c>
       <c r="C38" s="148" t="s">
         <v>39</v>
@@ -11962,10 +12045,10 @@
         <v>567</v>
       </c>
       <c r="E38" s="140" t="s">
+        <v>775</v>
+      </c>
+      <c r="F38" s="145" t="s">
         <v>776</v>
-      </c>
-      <c r="F38" s="145" t="s">
-        <v>777</v>
       </c>
       <c r="G38" s="139">
         <v>8.31</v>
@@ -11977,7 +12060,7 @@
         <v>0.38</v>
       </c>
       <c r="J38" s="140" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="K38" s="146">
         <v>0.20050000000000001</v>
@@ -11986,7 +12069,7 @@
         <v>44992</v>
       </c>
       <c r="M38" s="138" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="N38" s="143">
         <v>-4.7000000000000002E-3</v>
@@ -11994,10 +12077,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="150" t="s">
+        <v>779</v>
+      </c>
+      <c r="B39" s="138" t="s">
         <v>780</v>
-      </c>
-      <c r="B39" s="138" t="s">
-        <v>781</v>
       </c>
       <c r="C39" s="148" t="s">
         <v>39</v>
@@ -12006,10 +12089,10 @@
         <v>567</v>
       </c>
       <c r="E39" s="140" t="s">
+        <v>781</v>
+      </c>
+      <c r="F39" s="145" t="s">
         <v>782</v>
-      </c>
-      <c r="F39" s="145" t="s">
-        <v>783</v>
       </c>
       <c r="G39" s="138" t="s">
         <v>54</v>
@@ -12021,7 +12104,7 @@
         <v>1.95</v>
       </c>
       <c r="J39" s="139" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K39" s="141">
         <v>0.78059999999999996</v>
@@ -12030,7 +12113,7 @@
         <v>44993</v>
       </c>
       <c r="M39" s="138" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N39" s="141">
         <v>2.1899999999999999E-2</v>
@@ -12038,10 +12121,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="B40" s="138" t="s">
         <v>786</v>
-      </c>
-      <c r="B40" s="138" t="s">
-        <v>787</v>
       </c>
       <c r="C40" s="148" t="s">
         <v>39</v>
@@ -12050,7 +12133,7 @@
         <v>567</v>
       </c>
       <c r="E40" s="140" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F40" s="138" t="s">
         <v>54</v>
@@ -12065,7 +12148,7 @@
         <v>2.16</v>
       </c>
       <c r="J40" s="140" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="K40" s="141">
         <v>0.78139999999999998</v>
@@ -12074,7 +12157,7 @@
         <v>44985</v>
       </c>
       <c r="M40" s="138" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="N40" s="141">
         <v>1.37E-2</v>
@@ -12082,7 +12165,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="150" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B41" s="138" t="s">
         <v>542</v>
@@ -12094,10 +12177,10 @@
         <v>567</v>
       </c>
       <c r="E41" s="140" t="s">
+        <v>791</v>
+      </c>
+      <c r="F41" s="140" t="s">
         <v>792</v>
-      </c>
-      <c r="F41" s="140" t="s">
-        <v>793</v>
       </c>
       <c r="G41" s="138" t="s">
         <v>54</v>
@@ -12109,7 +12192,7 @@
         <v>2.54</v>
       </c>
       <c r="J41" s="140" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="K41" s="143">
         <v>6.0000000000000001E-3</v>
@@ -12118,7 +12201,7 @@
         <v>44887</v>
       </c>
       <c r="M41" s="138" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="N41" s="143">
         <v>-7.4200000000000002E-2</v>
@@ -12129,19 +12212,19 @@
         <v>1488</v>
       </c>
       <c r="B42" s="138" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C42" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D42" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E42" s="140" t="s">
+        <v>796</v>
+      </c>
+      <c r="F42" s="140" t="s">
         <v>797</v>
-      </c>
-      <c r="F42" s="140" t="s">
-        <v>798</v>
       </c>
       <c r="G42" s="138" t="s">
         <v>54</v>
@@ -12153,7 +12236,7 @@
         <v>4.3</v>
       </c>
       <c r="J42" s="140" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K42" s="143">
         <v>0</v>
@@ -12162,7 +12245,7 @@
         <v>54</v>
       </c>
       <c r="M42" s="138" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="N42" s="141">
         <v>2.5000000000000001E-2</v>
@@ -12170,10 +12253,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="150" t="s">
+        <v>800</v>
+      </c>
+      <c r="B43" s="138" t="s">
         <v>801</v>
-      </c>
-      <c r="B43" s="138" t="s">
-        <v>802</v>
       </c>
       <c r="C43" s="148" t="s">
         <v>39</v>
@@ -12182,10 +12265,10 @@
         <v>567</v>
       </c>
       <c r="E43" s="140" t="s">
+        <v>802</v>
+      </c>
+      <c r="F43" s="140" t="s">
         <v>803</v>
-      </c>
-      <c r="F43" s="140" t="s">
-        <v>804</v>
       </c>
       <c r="G43" s="138" t="s">
         <v>54</v>
@@ -12197,7 +12280,7 @@
         <v>0.49</v>
       </c>
       <c r="J43" s="145" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K43" s="141">
         <v>0.75319999999999998</v>
@@ -12206,7 +12289,7 @@
         <v>44993</v>
       </c>
       <c r="M43" s="138" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="N43" s="141">
         <v>4.7500000000000001E-2</v>
@@ -12226,10 +12309,10 @@
         <v>567</v>
       </c>
       <c r="E44" s="140" t="s">
+        <v>806</v>
+      </c>
+      <c r="F44" s="140" t="s">
         <v>807</v>
-      </c>
-      <c r="F44" s="140" t="s">
-        <v>808</v>
       </c>
       <c r="G44" s="140">
         <v>979.17</v>
@@ -12241,7 +12324,7 @@
         <v>1.73</v>
       </c>
       <c r="J44" s="140" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="K44" s="146">
         <v>0.2656</v>
@@ -12250,7 +12333,7 @@
         <v>44936</v>
       </c>
       <c r="M44" s="138" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="N44" s="141">
         <v>2.3E-3</v>
@@ -12261,19 +12344,19 @@
         <v>1100</v>
       </c>
       <c r="B45" s="138" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C45" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D45" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E45" s="140" t="s">
+        <v>811</v>
+      </c>
+      <c r="F45" s="139" t="s">
         <v>812</v>
-      </c>
-      <c r="F45" s="139" t="s">
-        <v>813</v>
       </c>
       <c r="G45" s="145">
         <v>12.88</v>
@@ -12285,7 +12368,7 @@
         <v>0.9</v>
       </c>
       <c r="J45" s="140" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="K45" s="143">
         <v>0</v>
@@ -12294,7 +12377,7 @@
         <v>54</v>
       </c>
       <c r="M45" s="138" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="N45" s="141">
         <v>1.6199999999999999E-2</v>
@@ -12305,16 +12388,16 @@
         <v>1170</v>
       </c>
       <c r="B46" s="138" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C46" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D46" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E46" s="140" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F46" s="140" t="e" cm="1" vm="2">
         <f t="array" ref="F46">-_FV(HKD$43,"37")</f>
@@ -12330,7 +12413,7 @@
         <v>0.36</v>
       </c>
       <c r="J46" s="140" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K46" s="143">
         <v>7.1999999999999995E-2</v>
@@ -12339,7 +12422,7 @@
         <v>44894</v>
       </c>
       <c r="M46" s="138" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="N46" s="141">
         <v>0</v>
@@ -12350,19 +12433,19 @@
         <v>1023</v>
       </c>
       <c r="B47" s="138" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C47" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D47" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E47" s="140" t="s">
+        <v>820</v>
+      </c>
+      <c r="F47" s="139" t="s">
         <v>821</v>
-      </c>
-      <c r="F47" s="139" t="s">
-        <v>822</v>
       </c>
       <c r="G47" s="139">
         <v>3.69</v>
@@ -12374,7 +12457,7 @@
         <v>0.26</v>
       </c>
       <c r="J47" s="145" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K47" s="143">
         <v>6.9699999999999998E-2</v>
@@ -12383,7 +12466,7 @@
         <v>54</v>
       </c>
       <c r="M47" s="138" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="N47" s="141">
         <v>1.6899999999999998E-2</v>
@@ -12391,22 +12474,22 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="150" t="s">
+        <v>824</v>
+      </c>
+      <c r="B48" s="138" t="s">
         <v>825</v>
       </c>
-      <c r="B48" s="138" t="s">
-        <v>826</v>
-      </c>
       <c r="C48" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D48" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E48" s="140" t="s">
+        <v>826</v>
+      </c>
+      <c r="F48" s="139" t="s">
         <v>827</v>
-      </c>
-      <c r="F48" s="139" t="s">
-        <v>828</v>
       </c>
       <c r="G48" s="138" t="s">
         <v>54</v>
@@ -12418,7 +12501,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="J48" s="140" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="K48" s="143">
         <v>0</v>
@@ -12427,7 +12510,7 @@
         <v>54</v>
       </c>
       <c r="M48" s="138" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="N48" s="141">
         <v>2.8E-3</v>
@@ -12438,19 +12521,19 @@
         <v>676</v>
       </c>
       <c r="B49" s="138" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C49" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D49" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E49" s="140" t="s">
+        <v>831</v>
+      </c>
+      <c r="F49" s="140" t="s">
         <v>832</v>
-      </c>
-      <c r="F49" s="140" t="s">
-        <v>833</v>
       </c>
       <c r="G49" s="140">
         <v>49.46</v>
@@ -12462,7 +12545,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J49" s="140" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="K49" s="143">
         <v>2.0000000000000001E-4</v>
@@ -12471,7 +12554,7 @@
         <v>54</v>
       </c>
       <c r="M49" s="138" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="N49" s="141">
         <v>1.4500000000000001E-2</v>
@@ -12479,22 +12562,22 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="150" t="s">
+        <v>835</v>
+      </c>
+      <c r="B50" s="138" t="s">
         <v>836</v>
       </c>
-      <c r="B50" s="138" t="s">
-        <v>837</v>
-      </c>
       <c r="C50" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D50" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E50" s="140" t="s">
+        <v>837</v>
+      </c>
+      <c r="F50" s="139" t="s">
         <v>838</v>
-      </c>
-      <c r="F50" s="139" t="s">
-        <v>839</v>
       </c>
       <c r="G50" s="145">
         <v>23.01</v>
@@ -12506,7 +12589,7 @@
         <v>0.05</v>
       </c>
       <c r="J50" s="140" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K50" s="143">
         <v>4.8099999999999997E-2</v>
@@ -12515,7 +12598,7 @@
         <v>44970</v>
       </c>
       <c r="M50" s="138" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="N50" s="141">
         <v>1.9E-3</v>
@@ -12523,22 +12606,22 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="150" t="s">
+        <v>824</v>
+      </c>
+      <c r="B51" s="138" t="s">
         <v>825</v>
       </c>
-      <c r="B51" s="138" t="s">
-        <v>826</v>
-      </c>
       <c r="C51" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D51" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E51" s="140" t="s">
+        <v>841</v>
+      </c>
+      <c r="F51" s="139" t="s">
         <v>842</v>
-      </c>
-      <c r="F51" s="139" t="s">
-        <v>843</v>
       </c>
       <c r="G51" s="140">
         <v>30.81</v>
@@ -12550,7 +12633,7 @@
         <v>1.28</v>
       </c>
       <c r="J51" s="145" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="K51" s="143">
         <v>0</v>
@@ -12559,7 +12642,7 @@
         <v>54</v>
       </c>
       <c r="M51" s="138" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="N51" s="143">
         <v>-2E-3</v>
@@ -12567,22 +12650,22 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="152" t="s">
+        <v>845</v>
+      </c>
+      <c r="B52" s="138" t="s">
         <v>846</v>
       </c>
-      <c r="B52" s="138" t="s">
-        <v>847</v>
-      </c>
       <c r="C52" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D52" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E52" s="140" t="s">
+        <v>847</v>
+      </c>
+      <c r="F52" s="139" t="s">
         <v>848</v>
-      </c>
-      <c r="F52" s="139" t="s">
-        <v>849</v>
       </c>
       <c r="G52" s="138" t="s">
         <v>54</v>
@@ -12594,7 +12677,7 @@
         <v>2.14</v>
       </c>
       <c r="J52" s="140" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="K52" s="143">
         <v>8.6599999999999996E-2</v>
@@ -12603,7 +12686,7 @@
         <v>44970</v>
       </c>
       <c r="M52" s="138" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="N52" s="141">
         <v>9.4999999999999998E-3</v>
@@ -12611,22 +12694,22 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="152" t="s">
+        <v>845</v>
+      </c>
+      <c r="B53" s="138" t="s">
         <v>846</v>
       </c>
-      <c r="B53" s="138" t="s">
-        <v>847</v>
-      </c>
       <c r="C53" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D53" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E53" s="140" t="s">
+        <v>851</v>
+      </c>
+      <c r="F53" s="140" t="s">
         <v>852</v>
-      </c>
-      <c r="F53" s="140" t="s">
-        <v>853</v>
       </c>
       <c r="G53" s="138" t="s">
         <v>54</v>
@@ -12638,7 +12721,7 @@
         <v>1.99</v>
       </c>
       <c r="J53" s="140" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="K53" s="146">
         <v>0.25640000000000002</v>
@@ -12647,7 +12730,7 @@
         <v>54</v>
       </c>
       <c r="M53" s="138" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="N53" s="141">
         <v>5.8999999999999999E-3</v>
@@ -12655,22 +12738,22 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="152" t="s">
+        <v>855</v>
+      </c>
+      <c r="B54" s="138" t="s">
         <v>856</v>
       </c>
-      <c r="B54" s="138" t="s">
-        <v>857</v>
-      </c>
       <c r="C54" s="148" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D54" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E54" s="140" t="s">
+        <v>857</v>
+      </c>
+      <c r="F54" s="140" t="s">
         <v>858</v>
-      </c>
-      <c r="F54" s="140" t="s">
-        <v>859</v>
       </c>
       <c r="G54" s="138" t="s">
         <v>54</v>
@@ -12702,19 +12785,19 @@
         <v>1028</v>
       </c>
       <c r="B55" s="138" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C55" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D55" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E55" s="140" t="s">
+        <v>860</v>
+      </c>
+      <c r="F55" s="140" t="s">
         <v>861</v>
-      </c>
-      <c r="F55" s="140" t="s">
-        <v>862</v>
       </c>
       <c r="G55" s="138" t="s">
         <v>54</v>
@@ -12726,7 +12809,7 @@
         <v>0.3</v>
       </c>
       <c r="J55" s="140" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="K55" s="143">
         <v>5.96E-2</v>
@@ -12735,7 +12818,7 @@
         <v>54</v>
       </c>
       <c r="M55" s="138" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="N55" s="141">
         <v>1.2699999999999999E-2</v>
@@ -12746,16 +12829,16 @@
         <v>1386</v>
       </c>
       <c r="B56" s="138" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C56" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D56" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E56" s="140" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F56" s="140" t="e" cm="1" vm="3">
         <f t="array" ref="F56">-_FV(HKD$10,"34")</f>
@@ -12780,7 +12863,7 @@
         <v>54</v>
       </c>
       <c r="M56" s="138" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="N56" s="143">
         <v>-1.09E-2</v>
@@ -12791,19 +12874,19 @@
         <v>1842</v>
       </c>
       <c r="B57" s="138" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C57" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D57" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E57" s="140" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F57" s="140" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G57" s="138" t="s">
         <v>54</v>
@@ -12815,7 +12898,7 @@
         <v>1.19</v>
       </c>
       <c r="J57" s="139" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K57" s="143">
         <v>0</v>
@@ -12824,7 +12907,7 @@
         <v>54</v>
       </c>
       <c r="M57" s="138" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N57" s="143">
         <v>-6.9400000000000003E-2</v>
@@ -12832,10 +12915,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="152" t="s">
+        <v>870</v>
+      </c>
+      <c r="B58" s="138" t="s">
         <v>871</v>
-      </c>
-      <c r="B58" s="138" t="s">
-        <v>872</v>
       </c>
       <c r="C58" s="148" t="s">
         <v>39</v>
@@ -12844,7 +12927,7 @@
         <v>567</v>
       </c>
       <c r="E58" s="140" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F58" s="138" t="s">
         <v>54</v>
@@ -12868,7 +12951,7 @@
         <v>54</v>
       </c>
       <c r="M58" s="138" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="N58" s="143">
         <v>-1.5699999999999999E-2</v>
@@ -12879,19 +12962,19 @@
         <v>738</v>
       </c>
       <c r="B59" s="138" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C59" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D59" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E59" s="140" t="s">
+        <v>875</v>
+      </c>
+      <c r="F59" s="140" t="s">
         <v>876</v>
-      </c>
-      <c r="F59" s="140" t="s">
-        <v>877</v>
       </c>
       <c r="G59" s="138" t="s">
         <v>54</v>
@@ -12903,7 +12986,7 @@
         <v>0.26</v>
       </c>
       <c r="J59" s="140" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K59" s="143">
         <v>0</v>
@@ -12912,7 +12995,7 @@
         <v>44858</v>
       </c>
       <c r="M59" s="138" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="N59" s="143">
         <v>-3.4099999999999998E-2</v>
@@ -12923,16 +13006,16 @@
         <v>264</v>
       </c>
       <c r="B60" s="138" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C60" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D60" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E60" s="140" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="F60" s="140" t="e" cm="1" vm="4">
         <f t="array" ref="F60">-_FV(HKD$20,"94")</f>
@@ -12948,7 +13031,7 @@
         <v>-2.35</v>
       </c>
       <c r="J60" s="140" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="K60" s="143">
         <v>0</v>
@@ -12957,7 +13040,7 @@
         <v>54</v>
       </c>
       <c r="M60" s="138" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="N60" s="141">
         <v>0</v>
@@ -12965,22 +13048,22 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="152" t="s">
+        <v>883</v>
+      </c>
+      <c r="B61" s="138" t="s">
         <v>884</v>
       </c>
-      <c r="B61" s="138" t="s">
-        <v>885</v>
-      </c>
       <c r="C61" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D61" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E61" s="140" t="s">
+        <v>885</v>
+      </c>
+      <c r="F61" s="139" t="s">
         <v>886</v>
-      </c>
-      <c r="F61" s="139" t="s">
-        <v>887</v>
       </c>
       <c r="G61" s="138" t="s">
         <v>54</v>
@@ -12992,7 +13075,7 @@
         <v>1.98</v>
       </c>
       <c r="J61" s="140" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K61" s="143">
         <v>0</v>
@@ -13001,7 +13084,7 @@
         <v>54</v>
       </c>
       <c r="M61" s="138" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="N61" s="143">
         <v>-2.76E-2</v>
@@ -13009,22 +13092,22 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="152" t="s">
+        <v>889</v>
+      </c>
+      <c r="B62" s="138" t="s">
         <v>890</v>
       </c>
-      <c r="B62" s="138" t="s">
-        <v>891</v>
-      </c>
       <c r="C62" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D62" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E62" s="140" t="s">
+        <v>891</v>
+      </c>
+      <c r="F62" s="139" t="s">
         <v>892</v>
-      </c>
-      <c r="F62" s="139" t="s">
-        <v>893</v>
       </c>
       <c r="G62" s="139">
         <v>10.11</v>
@@ -13036,7 +13119,7 @@
         <v>0.94</v>
       </c>
       <c r="J62" s="140" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K62" s="143">
         <v>0</v>
@@ -13045,7 +13128,7 @@
         <v>54</v>
       </c>
       <c r="M62" s="138" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="N62" s="141">
         <v>1.6999999999999999E-3</v>
@@ -13053,22 +13136,22 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="152" t="s">
+        <v>889</v>
+      </c>
+      <c r="B63" s="138" t="s">
         <v>890</v>
       </c>
-      <c r="B63" s="138" t="s">
-        <v>891</v>
-      </c>
       <c r="C63" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D63" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E63" s="140" t="s">
+        <v>895</v>
+      </c>
+      <c r="F63" s="139" t="s">
         <v>896</v>
-      </c>
-      <c r="F63" s="139" t="s">
-        <v>897</v>
       </c>
       <c r="G63" s="139">
         <v>7.01</v>
@@ -13080,7 +13163,7 @@
         <v>0.88</v>
       </c>
       <c r="J63" s="140" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="K63" s="143">
         <v>0</v>
@@ -13089,7 +13172,7 @@
         <v>54</v>
       </c>
       <c r="M63" s="138" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="N63" s="143">
         <v>-1.01E-2</v>
@@ -13097,22 +13180,22 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="152" t="s">
+        <v>899</v>
+      </c>
+      <c r="B64" s="138" t="s">
         <v>900</v>
       </c>
-      <c r="B64" s="138" t="s">
-        <v>901</v>
-      </c>
       <c r="C64" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D64" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E64" s="140" t="s">
+        <v>901</v>
+      </c>
+      <c r="F64" s="145" t="s">
         <v>902</v>
-      </c>
-      <c r="F64" s="145" t="s">
-        <v>903</v>
       </c>
       <c r="G64" s="140">
         <v>54.03</v>
@@ -13124,7 +13207,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="J64" s="140" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K64" s="143">
         <v>0</v>
@@ -13133,7 +13216,7 @@
         <v>54</v>
       </c>
       <c r="M64" s="138" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="N64" s="143">
         <v>-1.4500000000000001E-2</v>
@@ -13144,16 +13227,16 @@
         <v>1255</v>
       </c>
       <c r="B65" s="138" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C65" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D65" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E65" s="140" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F65" s="140" t="e" cm="1" vm="5">
         <f t="array" ref="F65">-_FV(HKD$43,"21")</f>
@@ -13169,7 +13252,7 @@
         <v>6.69</v>
       </c>
       <c r="J65" s="140" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K65" s="143">
         <v>0</v>
@@ -13178,7 +13261,7 @@
         <v>54</v>
       </c>
       <c r="M65" s="138" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="N65" s="141">
         <v>0</v>
@@ -13189,19 +13272,19 @@
         <v>1027</v>
       </c>
       <c r="B66" s="138" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C66" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D66" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E66" s="140" t="s">
+        <v>910</v>
+      </c>
+      <c r="F66" s="140" t="s">
         <v>911</v>
-      </c>
-      <c r="F66" s="140" t="s">
-        <v>912</v>
       </c>
       <c r="G66" s="140">
         <v>454.12</v>
@@ -13213,7 +13296,7 @@
         <v>0.42</v>
       </c>
       <c r="J66" s="140" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="K66" s="143">
         <v>0</v>
@@ -13222,7 +13305,7 @@
         <v>54</v>
       </c>
       <c r="M66" s="138" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="N66" s="141">
         <v>0.125</v>
@@ -13233,19 +13316,19 @@
         <v>2683</v>
       </c>
       <c r="B67" s="138" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C67" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D67" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E67" s="140" t="s">
+        <v>915</v>
+      </c>
+      <c r="F67" s="145" t="s">
         <v>916</v>
-      </c>
-      <c r="F67" s="145" t="s">
-        <v>917</v>
       </c>
       <c r="G67" s="139">
         <v>4.93</v>
@@ -13257,7 +13340,7 @@
         <v>0.61</v>
       </c>
       <c r="J67" s="145" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K67" s="143">
         <v>0</v>
@@ -13266,7 +13349,7 @@
         <v>44886</v>
       </c>
       <c r="M67" s="138" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="N67" s="141">
         <v>1.4500000000000001E-2</v>
@@ -13274,22 +13357,22 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="152" t="s">
+        <v>919</v>
+      </c>
+      <c r="B68" s="138" t="s">
         <v>920</v>
       </c>
-      <c r="B68" s="138" t="s">
-        <v>921</v>
-      </c>
       <c r="C68" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D68" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E68" s="140" t="s">
+        <v>921</v>
+      </c>
+      <c r="F68" s="145" t="s">
         <v>922</v>
-      </c>
-      <c r="F68" s="145" t="s">
-        <v>923</v>
       </c>
       <c r="G68" s="138" t="s">
         <v>54</v>
@@ -13301,7 +13384,7 @@
         <v>1.46</v>
       </c>
       <c r="J68" s="140" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K68" s="143">
         <v>0</v>
@@ -13310,7 +13393,7 @@
         <v>54</v>
       </c>
       <c r="M68" s="138" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="N68" s="141">
         <v>2.2000000000000001E-3</v>
@@ -13318,22 +13401,22 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="152" t="s">
+        <v>925</v>
+      </c>
+      <c r="B69" s="138" t="s">
         <v>926</v>
       </c>
-      <c r="B69" s="138" t="s">
-        <v>927</v>
-      </c>
       <c r="C69" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D69" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E69" s="140" t="s">
+        <v>927</v>
+      </c>
+      <c r="F69" s="145" t="s">
         <v>928</v>
-      </c>
-      <c r="F69" s="145" t="s">
-        <v>929</v>
       </c>
       <c r="G69" s="140">
         <v>41.12</v>
@@ -13345,7 +13428,7 @@
         <v>0.34</v>
       </c>
       <c r="J69" s="140" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="K69" s="143">
         <v>0</v>
@@ -13354,7 +13437,7 @@
         <v>54</v>
       </c>
       <c r="M69" s="138" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="N69" s="141">
         <v>1.8E-3</v>
@@ -13362,10 +13445,10 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="152" t="s">
+        <v>931</v>
+      </c>
+      <c r="B70" s="138" t="s">
         <v>932</v>
-      </c>
-      <c r="B70" s="138" t="s">
-        <v>933</v>
       </c>
       <c r="C70" s="148" t="s">
         <v>39</v>
@@ -13374,7 +13457,7 @@
         <v>567</v>
       </c>
       <c r="E70" s="140" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F70" s="138" t="s">
         <v>54</v>
@@ -13389,7 +13472,7 @@
         <v>2.34</v>
       </c>
       <c r="J70" s="140" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K70" s="146">
         <v>0.14030000000000001</v>
@@ -13398,7 +13481,7 @@
         <v>54</v>
       </c>
       <c r="M70" s="138" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="N70" s="141">
         <v>3.5700000000000003E-2</v>
@@ -13406,22 +13489,22 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="152" t="s">
+        <v>936</v>
+      </c>
+      <c r="B71" s="138" t="s">
         <v>937</v>
       </c>
-      <c r="B71" s="138" t="s">
-        <v>938</v>
-      </c>
       <c r="C71" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D71" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E71" s="140" t="s">
+        <v>938</v>
+      </c>
+      <c r="F71" s="145" t="s">
         <v>939</v>
-      </c>
-      <c r="F71" s="145" t="s">
-        <v>940</v>
       </c>
       <c r="G71" s="140">
         <v>27.17</v>
@@ -13433,7 +13516,7 @@
         <v>1.76</v>
       </c>
       <c r="J71" s="140" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="K71" s="143">
         <v>0</v>
@@ -13442,7 +13525,7 @@
         <v>54</v>
       </c>
       <c r="M71" s="138" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="N71" s="143">
         <v>-1.12E-2</v>
@@ -13450,10 +13533,10 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="152" t="s">
+        <v>942</v>
+      </c>
+      <c r="B72" s="138" t="s">
         <v>943</v>
-      </c>
-      <c r="B72" s="138" t="s">
-        <v>944</v>
       </c>
       <c r="C72" s="148" t="s">
         <v>13</v>
@@ -13462,10 +13545,10 @@
         <v>567</v>
       </c>
       <c r="E72" s="140" t="s">
+        <v>944</v>
+      </c>
+      <c r="F72" s="140" t="s">
         <v>945</v>
-      </c>
-      <c r="F72" s="140" t="s">
-        <v>946</v>
       </c>
       <c r="G72" s="138" t="s">
         <v>54</v>
@@ -13477,7 +13560,7 @@
         <v>1.18</v>
       </c>
       <c r="J72" s="140" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K72" s="146">
         <v>0.34989999999999999</v>
@@ -13486,7 +13569,7 @@
         <v>54</v>
       </c>
       <c r="M72" s="138" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="N72" s="141">
         <v>1.2999999999999999E-2</v>
@@ -13494,22 +13577,22 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="152" t="s">
+        <v>948</v>
+      </c>
+      <c r="B73" s="138" t="s">
         <v>949</v>
       </c>
-      <c r="B73" s="138" t="s">
-        <v>950</v>
-      </c>
       <c r="C73" s="148" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D73" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E73" s="140" t="s">
+        <v>950</v>
+      </c>
+      <c r="F73" s="145" t="s">
         <v>951</v>
-      </c>
-      <c r="F73" s="145" t="s">
-        <v>952</v>
       </c>
       <c r="G73" s="145">
         <v>19.47</v>
@@ -13521,7 +13604,7 @@
         <v>0.16</v>
       </c>
       <c r="J73" s="140" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K73" s="143">
         <v>0</v>
@@ -13530,7 +13613,7 @@
         <v>54</v>
       </c>
       <c r="M73" s="138" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="N73" s="143">
         <v>-4.3E-3</v>
@@ -13538,22 +13621,22 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="152" t="s">
+        <v>948</v>
+      </c>
+      <c r="B74" s="138" t="s">
         <v>949</v>
       </c>
-      <c r="B74" s="138" t="s">
-        <v>950</v>
-      </c>
       <c r="C74" s="148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D74" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E74" s="140" t="s">
+        <v>954</v>
+      </c>
+      <c r="F74" s="145" t="s">
         <v>955</v>
-      </c>
-      <c r="F74" s="145" t="s">
-        <v>956</v>
       </c>
       <c r="G74" s="145">
         <v>21.33</v>
@@ -13565,7 +13648,7 @@
         <v>0.05</v>
       </c>
       <c r="J74" s="140" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="K74" s="143">
         <v>0</v>
@@ -13574,7 +13657,7 @@
         <v>54</v>
       </c>
       <c r="M74" s="138" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="N74" s="143">
         <v>-1.04E-2</v>
@@ -13585,19 +13668,19 @@
         <v>1096</v>
       </c>
       <c r="B75" s="138" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C75" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D75" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E75" s="140" t="s">
+        <v>959</v>
+      </c>
+      <c r="F75" s="140" t="s">
         <v>960</v>
-      </c>
-      <c r="F75" s="140" t="s">
-        <v>961</v>
       </c>
       <c r="G75" s="138" t="s">
         <v>54</v>
@@ -13618,7 +13701,7 @@
         <v>54</v>
       </c>
       <c r="M75" s="138" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="N75" s="141">
         <v>0</v>
@@ -13629,19 +13712,19 @@
         <v>8285</v>
       </c>
       <c r="B76" s="138" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C76" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D76" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E76" s="140" t="s">
+        <v>963</v>
+      </c>
+      <c r="F76" s="140" t="s">
         <v>964</v>
-      </c>
-      <c r="F76" s="140" t="s">
-        <v>965</v>
       </c>
       <c r="G76" s="138" t="s">
         <v>54</v>
@@ -13653,7 +13736,7 @@
         <v>2.08</v>
       </c>
       <c r="J76" s="140" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="K76" s="143">
         <v>0</v>
@@ -13662,7 +13745,7 @@
         <v>44875</v>
       </c>
       <c r="M76" s="138" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="N76" s="141">
         <v>5.8799999999999998E-2</v>
@@ -13670,22 +13753,22 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="152" t="s">
+        <v>967</v>
+      </c>
+      <c r="B77" s="138" t="s">
         <v>968</v>
       </c>
-      <c r="B77" s="138" t="s">
-        <v>969</v>
-      </c>
       <c r="C77" s="148" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D77" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E77" s="140" t="s">
+        <v>969</v>
+      </c>
+      <c r="F77" s="140" t="s">
         <v>970</v>
-      </c>
-      <c r="F77" s="140" t="s">
-        <v>971</v>
       </c>
       <c r="G77" s="138" t="s">
         <v>54</v>
@@ -13717,16 +13800,16 @@
         <v>8187</v>
       </c>
       <c r="B78" s="138" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C78" s="148" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D78" s="138" t="s">
         <v>567</v>
       </c>
       <c r="E78" s="140" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F78" s="140" t="e" cm="1" vm="6">
         <f t="array" ref="F78">-_FV(HKD$9,"39")</f>
@@ -13742,7 +13825,7 @@
         <v>-4.46</v>
       </c>
       <c r="J78" s="139" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="K78" s="143">
         <v>0</v>
@@ -13751,7 +13834,7 @@
         <v>54</v>
       </c>
       <c r="M78" s="138" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="N78" s="141">
         <v>9.0899999999999995E-2</v>
@@ -13856,13 +13939,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AM55"/>
+  <dimension ref="A1:AO56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13884,25 +13967,27 @@
     <col min="37" max="37" width="9.1640625" style="1"/>
     <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.1640625" style="1"/>
+    <col min="40" max="40" width="38.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="51.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="155" t="s">
+      <c r="F1" s="156" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-      <c r="O1" s="155"/>
-      <c r="P1" s="155"/>
-      <c r="Q1" s="155"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
+      <c r="Q1" s="156"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
         <v>14.953293230057294</v>
@@ -13974,7 +14059,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14085,10 +14170,16 @@
         <v>522</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
+        <v>1011</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14102,19 +14193,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$49</f>
+        <f>[1]Main!$C$6*$E$50</f>
         <v>95.947999999999993</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$49</f>
+        <f>[1]Main!$C$8*$E$50</f>
         <v>149582.932</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$49</f>
+        <f>[1]Main!$C$11*$E$50</f>
         <v>987.69999999999993</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$49</f>
+        <f>[1]Main!$C$12*$E$50</f>
         <v>148595.23199999999</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -14130,15 +14221,15 @@
         <v>29.611379424412871</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AF$21*1000*E49</f>
+        <f>'[1]Financial Model'!$AF$21*1000*E50</f>
         <v>5018.1799999999939</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AE$21*1000*E49</f>
+        <f>'[1]Financial Model'!$AE$21*1000*E50</f>
         <v>4753.409999999998</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E49</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E50</f>
         <v>2107.37</v>
       </c>
       <c r="R3" s="51">
@@ -14184,7 +14275,7 @@
         <v>0.19333333333333316</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E49</f>
+        <f>[1]Main!$C$26*E50</f>
         <v>8019.46</v>
       </c>
       <c r="AF3" s="53">
@@ -14210,8 +14301,11 @@
       <c r="AM3" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN3" s="4" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14225,19 +14319,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$49</f>
+        <f>[2]Main!$C$6*$E$50</f>
         <v>27.572599999999998</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$49</f>
+        <f>[2]Main!$C$8*$E$50</f>
         <v>10689.566148799999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$49</f>
+        <f>[2]Main!$C$11*$E$50</f>
         <v>-3872.8090499999998</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$49</f>
+        <f>[2]Main!$C$12*$E$50</f>
         <v>14562.375198799997</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -14253,15 +14347,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E49</f>
+        <f>'[2]Financial Model'!$AA$22*E50</f>
         <v>1151.127829999999</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$49</f>
+        <f>'[2]Financial Model'!$Z$22*$E$50</f>
         <v>338.51467000000116</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$49</f>
+        <f>'[2]Financial Model'!$Y$22*$E$50</f>
         <v>563.94267000000013</v>
       </c>
       <c r="R4" s="51">
@@ -14296,7 +14390,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E49</f>
+        <f>[2]Main!$C$26*E50</f>
         <v>1943.3578499999999</v>
       </c>
       <c r="AF4" s="53">
@@ -14317,10 +14411,13 @@
         <v>Denver, US</v>
       </c>
       <c r="AM4" s="4" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.15">
+        <v>984</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14439,8 +14536,11 @@
       <c r="AM5" s="4" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN5" s="4" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14566,8 +14666,11 @@
       <c r="AM6" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN6" s="4" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14693,8 +14796,11 @@
       <c r="AM7" s="4" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN7" s="4" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -14708,19 +14814,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E49</f>
+        <f>[6]Main!$C$6*E50</f>
         <v>6.8806999999999992</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E49</f>
+        <f>[6]Main!$C$8*E50</f>
         <v>3126.0533853999996</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$49</f>
+        <f>[6]Main!$C$11*$E$50</f>
         <v>149.62410000000008</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$49</f>
+        <f>[6]Main!$C$12*$E$50</f>
         <v>2976.4292853999996</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -14736,15 +14842,15 @@
         <v>24.790599499495396</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$49</f>
+        <f>'[6]Financial Model'!$AA$20*$E$50</f>
         <v>-455.81691000000001</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$49</f>
+        <f>'[6]Financial Model'!$Z$20*$E$50</f>
         <v>76.477859999999353</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$49</f>
+        <f>'[6]Financial Model'!$Y$20*$E$50</f>
         <v>-38.43066000000033</v>
       </c>
       <c r="R8" s="52">
@@ -14793,7 +14899,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E49</f>
+        <f>[6]Main!$C$27*E50</f>
         <v>896.74860000000001</v>
       </c>
       <c r="AF8" s="53">
@@ -14824,8 +14930,11 @@
       <c r="AM8" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN8" s="4" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -14839,19 +14948,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E49</f>
+        <f>[7]Main!$C$6*E50</f>
         <v>21.189900000000002</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$49</f>
+        <f>[7]Main!$C$8*$E$50</f>
         <v>1953.161232984</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E49</f>
+        <f>[7]Main!$C$11*E50</f>
         <v>322.90402999999998</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E49</f>
+        <f>[7]Main!$C$12*E50</f>
         <v>1630.2572029840001</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -14888,7 +14997,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E49</f>
+        <f>[7]Main!$C$26*E50</f>
         <v>617.17056999999988</v>
       </c>
       <c r="AF9" s="53">
@@ -14908,10 +15017,13 @@
         <v>Philadelphia, PA</v>
       </c>
       <c r="AM9" s="4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.15">
+        <v>982</v>
+      </c>
+      <c r="AN9" s="4" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -14925,19 +15037,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E49</f>
+        <f>[8]Main!$C$6*E50</f>
         <v>10.723599999999999</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E49</f>
+        <f>[8]Main!$C$8*E50</f>
         <v>1932.2747603999996</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$49</f>
+        <f>[8]Main!$C$11*$E$50</f>
         <v>-230.99563999999998</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$49</f>
+        <f>[8]Main!$C$12*$E$50</f>
         <v>2163.2704003999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -14957,11 +15069,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E49</f>
+        <f>'[8]Financial Model'!$Z$17*E50</f>
         <v>348.28957999999989</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F49</f>
+        <f>'[8]Financial Model'!$Y$17*F50</f>
         <v>-252.21325301204848</v>
       </c>
       <c r="Q10" s="4"/>
@@ -15004,7 +15116,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E49</f>
+        <f>[8]Main!$C$26*E50</f>
         <v>570.24818000000005</v>
       </c>
       <c r="AF10" s="53">
@@ -15033,10 +15145,13 @@
         <v>Pittsburgh, US</v>
       </c>
       <c r="AM10" s="4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.15">
+        <v>982</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15172,8 +15287,11 @@
       <c r="AM11" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN11" s="4" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15187,19 +15305,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E49</f>
+        <f>[10]Main!$C$6*E50</f>
         <v>18.7746</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E49</f>
+        <f>[10]Main!$C$8*E50</f>
         <v>929.07985559999986</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E49</f>
+        <f>[10]Main!$C$11*E50</f>
         <v>123.55711999999997</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E49</f>
+        <f>[10]Main!$C$12*E50</f>
         <v>805.52273559999992</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -15220,15 +15338,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E49</f>
+        <f>'[10]Financial Model'!$X$18*E50</f>
         <v>218.29829999999976</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$49</f>
+        <f>'[10]Financial Model'!$W$18*$E$50</f>
         <v>-94.637430000000123</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$49</f>
+        <f>'[10]Financial Model'!$V$18*$E$50</f>
         <v>32.667140000000508</v>
       </c>
       <c r="R12" s="52">
@@ -15277,7 +15395,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E49</f>
+        <f>'[10]Financial Model'!$Q$41*E50</f>
         <v>615.8292899999999</v>
       </c>
       <c r="AF12" s="53">
@@ -15306,10 +15424,13 @@
         <v>Ohio, US</v>
       </c>
       <c r="AM12" s="4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.15">
+        <v>982</v>
+      </c>
+      <c r="AN12" s="4" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15430,8 +15551,11 @@
       <c r="AM13" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" s="103" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AN13" s="4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15534,8 +15658,14 @@
       <c r="AM14" s="105" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AN14" s="105" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AO14" s="103" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15673,10 +15803,13 @@
         <v>Cheltenham, UK</v>
       </c>
       <c r="AM15" s="4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" s="91" customFormat="1" x14ac:dyDescent="0.15">
+        <v>982</v>
+      </c>
+      <c r="AN15" s="4" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -15792,8 +15925,14 @@
       <c r="AM16" s="93" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AN16" s="93" t="s">
+        <v>1004</v>
+      </c>
+      <c r="AO16" s="91" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -15892,7 +16031,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -15918,12 +16057,12 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B19" s="136" t="s">
+        <v>582</v>
+      </c>
+      <c r="C19" s="133" t="s">
         <v>583</v>
-      </c>
-      <c r="C19" s="133" t="s">
-        <v>584</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="56"/>
@@ -15949,12 +16088,12 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B20" s="135" t="s">
+        <v>975</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>976</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>977</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>31</v>
@@ -15969,10 +16108,13 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.15">
+        <v>977</v>
+      </c>
+      <c r="AN20" s="4" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -15996,7 +16138,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16019,10 +16161,10 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
       <c r="AM22" s="4" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16044,10 +16186,10 @@
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
       <c r="AM23" s="4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16061,19 +16203,19 @@
         <v>505</v>
       </c>
       <c r="F24" s="54">
-        <f>[16]Main!$C$6*E49</f>
+        <f>[16]Main!$C$6*E50</f>
         <v>275.07030000000003</v>
       </c>
       <c r="G24" s="56">
-        <f>[16]Main!$C$8*E49</f>
+        <f>[16]Main!$C$8*E50</f>
         <v>33641.097689999995</v>
       </c>
       <c r="H24" s="56">
-        <f>[16]Main!$C$11*E49</f>
+        <f>[16]Main!$C$11*E50</f>
         <v>0</v>
       </c>
       <c r="I24" s="56">
-        <f>[16]Main!$C$12*E49</f>
+        <f>[16]Main!$C$12*E50</f>
         <v>33641.097689999995</v>
       </c>
       <c r="AK24" s="4">
@@ -16088,7 +16230,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16102,7 +16244,7 @@
         <v>565</v>
       </c>
       <c r="F25" s="54">
-        <f>81600*E51</f>
+        <f>81600*E52</f>
         <v>489.6</v>
       </c>
       <c r="G25" s="56"/>
@@ -16117,19 +16259,22 @@
       <c r="AM25" s="4" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AN25" s="4" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>578</v>
+        <v>1009</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>573</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F26" s="54"/>
       <c r="G26" s="56"/>
@@ -16140,8 +16285,11 @@
       <c r="AM26" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AN26" s="4" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16152,7 +16300,7 @@
         <v>573</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F27" s="54"/>
       <c r="G27" s="56"/>
@@ -16163,8 +16311,11 @@
       <c r="AM27" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AN27" s="4" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="1"/>
@@ -16174,9 +16325,9 @@
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B29" s="136" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C29" s="133" t="s">
         <v>554</v>
@@ -16190,7 +16341,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>511</v>
       </c>
@@ -16204,7 +16355,7 @@
         <v>505</v>
       </c>
       <c r="F30" s="7">
-        <f>18.22*E49</f>
+        <f>18.22*E50</f>
         <v>15.122599999999998</v>
       </c>
       <c r="G30" s="56"/>
@@ -16223,7 +16374,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B31" s="3" t="s">
         <v>540</v>
       </c>
@@ -16287,7 +16438,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>541</v>
       </c>
@@ -16314,7 +16465,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>575</v>
       </c>
@@ -16325,7 +16476,7 @@
         <v>573</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="56"/>
@@ -16339,9 +16490,9 @@
         <v>553</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>266</v>
@@ -16350,7 +16501,7 @@
         <v>31</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="56"/>
@@ -16364,9 +16515,9 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>272</v>
@@ -16375,7 +16526,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="56"/>
@@ -16389,7 +16540,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
       <c r="H36" s="1"/>
@@ -16399,9 +16550,9 @@
       <c r="M36" s="56"/>
       <c r="N36" s="56"/>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B37" s="136" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C37" s="133" t="s">
         <v>567</v>
@@ -16414,12 +16565,18 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
-        <v>580</v>
+        <v>985</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>585</v>
+        <v>986</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>505</v>
       </c>
       <c r="G38" s="56"/>
       <c r="H38" s="1"/>
@@ -16429,15 +16586,18 @@
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
       <c r="AM38" s="4" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.15">
+        <v>987</v>
+      </c>
+      <c r="AN38" s="4" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G39" s="56"/>
       <c r="H39" s="1"/>
@@ -16447,18 +16607,15 @@
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
       <c r="AM39" s="4" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.15">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>31</v>
+        <v>585</v>
       </c>
       <c r="G40" s="56"/>
       <c r="H40" s="1"/>
@@ -16468,21 +16625,18 @@
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
       <c r="AM40" s="4" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.15">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
-        <v>568</v>
+        <v>581</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>571</v>
+        <v>586</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G41" s="56"/>
       <c r="H41" s="1"/>
@@ -16492,138 +16646,153 @@
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
       <c r="AM41" s="4" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="B42" s="3" t="s">
-        <v>569</v>
+        <v>978</v>
+      </c>
+    </row>
+    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B42" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>489</v>
+        <v>13</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="54">
+      <c r="G42" s="56"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="AM42" s="4" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B43" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="54">
         <f>[18]Main!$C$6</f>
         <v>2.4049999999999998</v>
       </c>
-      <c r="G42" s="56">
+      <c r="G43" s="56">
         <f>[18]Main!$C$8</f>
         <v>120.24999999999999</v>
       </c>
-      <c r="H42" s="56">
+      <c r="H43" s="56">
         <f>[18]Main!$C$11</f>
         <v>13.872</v>
       </c>
-      <c r="I42" s="56">
+      <c r="I43" s="56">
         <f>[18]Main!$C$12</f>
         <v>106.37799999999999</v>
       </c>
-      <c r="J42" s="4" t="str">
+      <c r="J43" s="4" t="str">
         <f>[18]Main!$C$29</f>
         <v>H122</v>
       </c>
-      <c r="K42" s="85">
+      <c r="K43" s="85">
         <f>[18]Main!$D$29</f>
         <v>45063</v>
       </c>
-      <c r="L42" s="50">
+      <c r="L43" s="50">
         <f>[18]Main!$C$38</f>
         <v>8.8692679673169916</v>
       </c>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="O42" s="56">
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56">
         <f>'[18]Financial Model'!$T$16</f>
         <v>7.0139999999999958</v>
       </c>
-      <c r="P42" s="56">
+      <c r="P43" s="56">
         <f>'[18]Financial Model'!$S$16</f>
         <v>-11.902999999999997</v>
       </c>
-      <c r="Q42" s="56">
+      <c r="Q43" s="56">
         <f>'[18]Financial Model'!$R$17</f>
         <v>0</v>
       </c>
-      <c r="R42" s="51">
+      <c r="R43" s="51">
         <f>[18]Main!$C$37</f>
         <v>10.025846256461564</v>
       </c>
-      <c r="S42" s="156">
+      <c r="S43" s="153">
         <f>'[18]Financial Model'!$T$83</f>
         <v>4.5587396635300852</v>
       </c>
-      <c r="T42" s="51">
+      <c r="T43" s="51">
         <f>[18]Main!$C$34</f>
         <v>4.0893015030946032</v>
       </c>
-      <c r="W42" s="53">
+      <c r="W43" s="53">
         <f>'[18]Financial Model'!$T$21</f>
         <v>-2.7951830820442503E-2</v>
       </c>
-      <c r="Z42" s="53">
+      <c r="Z43" s="53">
         <f>'[18]Financial Model'!$K$26</f>
         <v>0.19490724836825837</v>
       </c>
-      <c r="AA42" s="53">
+      <c r="AA43" s="53">
         <f>'[18]Financial Model'!$K$27</f>
         <v>5.2401809229359962E-2</v>
       </c>
-      <c r="AB42" s="53">
+      <c r="AB43" s="53">
         <f>'[18]Financial Model'!$K$28</f>
         <v>4.1008244589488214E-2</v>
       </c>
-      <c r="AC42" s="53">
+      <c r="AC43" s="53">
         <f>'[18]Financial Model'!$K$29</f>
         <v>6.4337034617896707E-2</v>
       </c>
-      <c r="AE42" s="56">
+      <c r="AE43" s="56">
         <f>[18]Main!$C$27</f>
         <v>31.096</v>
       </c>
-      <c r="AF42" s="53">
+      <c r="AF43" s="53">
         <f>'[18]Financial Model'!$K$72</f>
         <v>9.3658776773467567E-2</v>
       </c>
-      <c r="AG42" s="53">
+      <c r="AG43" s="53">
         <f>'[18]Financial Model'!$K$73</f>
         <v>0.23735625323305887</v>
       </c>
-      <c r="AH42" s="53">
+      <c r="AH43" s="53">
         <f>'[18]Financial Model'!$K$74</f>
         <v>0.20930060375174159</v>
       </c>
-      <c r="AI42" s="4">
+      <c r="AI43" s="4">
         <f>[18]Main!$C$25</f>
         <v>388</v>
       </c>
-      <c r="AK42" s="4">
+      <c r="AK43" s="4">
         <f>[18]Main!$C$24</f>
         <v>1917</v>
       </c>
-      <c r="AL42" s="4" t="str">
+      <c r="AL43" s="4" t="str">
         <f>[18]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
-      <c r="AM42" s="4" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="G43" s="56"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
-    </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AM43" s="4" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G44" s="56"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -16632,7 +16801,7 @@
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -16641,15 +16810,16 @@
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="G46" s="49"/>
-      <c r="I46" s="4"/>
+    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="G46" s="56"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G47" s="49"/>
       <c r="I47" s="4"/>
       <c r="J47" s="1"/>
@@ -16657,29 +16827,21 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.15">
-      <c r="D48" s="153" t="s">
-        <v>495</v>
-      </c>
-      <c r="E48" s="154"/>
-      <c r="F48" s="42" t="s">
-        <v>496</v>
-      </c>
+    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D49" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E49" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="F49" s="45">
-        <f>1/E49</f>
-        <v>1.2048192771084338</v>
+      <c r="D49" s="154" t="s">
+        <v>495</v>
+      </c>
+      <c r="E49" s="155"/>
+      <c r="F49" s="42" t="s">
+        <v>496</v>
       </c>
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
@@ -16688,14 +16850,14 @@
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D50" s="43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E50" s="44">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="F50" s="45">
         <f>1/E50</f>
-        <v>1.1494252873563218</v>
+        <v>1.2048192771084338</v>
       </c>
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
@@ -16703,19 +16865,32 @@
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E51" s="44">
+        <v>0.87</v>
+      </c>
+      <c r="F51" s="45">
+        <f>1/E51</f>
+        <v>1.1494252873563218</v>
+      </c>
+      <c r="G51" s="49"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
+      <c r="D52" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="E51" s="48">
+      <c r="E52" s="48">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F51" s="47">
-        <f>1/E51</f>
+      <c r="F52" s="47">
+        <f>1/E52</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="G51" s="49"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G52" s="49"/>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.15">
@@ -16727,9 +16902,12 @@
     <row r="55" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G55" s="49"/>
     </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.15">
+      <c r="G56" s="49"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -16753,7 +16931,7 @@
     <hyperlink ref="B37" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
     <hyperlink ref="B29" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
     <hyperlink ref="B19" r:id="rId20" xr:uid="{8B27DD55-F39A-E042-A7A2-82BE3E8447D7}"/>
-    <hyperlink ref="B42" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
+    <hyperlink ref="B43" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId22"/>

</xml_diff>

<commit_message>
Start $FL model, latest Q3 results
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D58741-CDE4-184E-AAAD-343C696DFB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CE399A-BA5F-4F38-AD0C-202043C1DB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -38,28 +38,19 @@
     <externalReference r:id="rId21"/>
     <externalReference r:id="rId22"/>
     <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -67,7 +58,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -76,42 +67,42 @@
   <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
@@ -146,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="1013">
   <si>
     <t>Ticker</t>
   </si>
@@ -3192,14 +3183,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3642,7 +3633,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3651,13 +3642,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3686,16 +3677,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3704,12 +3695,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3746,7 +3737,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3764,7 +3755,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3785,7 +3776,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3812,15 +3803,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3829,7 +3820,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3840,16 +3831,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3884,7 +3875,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3896,7 +3887,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3931,7 +3922,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3950,7 +3941,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5150,6 +5141,93 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>39.19</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>3657.2275341299996</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-103</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>3760.2275341299996</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>NYC, NY</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1879</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2794</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>1685</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>1.1231500460263886</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="26">
+          <cell r="U26">
+            <v>0.32029452369995398</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="U27">
+            <v>7.2250345144960884E-2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="U28">
+            <v>4.4178554993097099E-2</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="U29">
+            <v>0.32867132867132864</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="U71">
+            <v>0.29515757109915453</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6613,25 +6691,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6673,7 +6751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6717,7 +6795,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6761,7 +6839,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6805,7 +6883,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -6849,7 +6927,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -6893,7 +6971,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -6937,7 +7015,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -6981,7 +7059,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -7025,7 +7103,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -7069,7 +7147,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -7113,7 +7191,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -7157,7 +7235,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -7201,7 +7279,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7245,7 +7323,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7289,7 +7367,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7333,7 +7411,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7377,7 +7455,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7421,7 +7499,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7465,7 +7543,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7509,7 +7587,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7553,7 +7631,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7597,7 +7675,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7641,7 +7719,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7685,7 +7763,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7729,7 +7807,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7773,7 +7851,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -7817,7 +7895,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -7861,7 +7939,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -7905,7 +7983,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -7949,7 +8027,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -7993,7 +8071,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -8037,7 +8115,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -8081,7 +8159,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -8125,7 +8203,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -8169,7 +8247,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8213,7 +8291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8257,7 +8335,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8301,7 +8379,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8345,7 +8423,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8389,7 +8467,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8433,7 +8511,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8477,7 +8555,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8521,7 +8599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8639,25 +8717,25 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8699,7 +8777,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8743,7 +8821,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8787,7 +8865,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -8831,7 +8909,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -8875,7 +8953,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -8919,7 +8997,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -8963,7 +9041,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -9007,7 +9085,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -9051,7 +9129,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -9095,7 +9173,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -9139,7 +9217,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -9183,7 +9261,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9227,7 +9305,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9271,7 +9349,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9315,7 +9393,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9359,7 +9437,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9403,7 +9481,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9447,7 +9525,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9491,7 +9569,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9535,7 +9613,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9579,7 +9657,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9623,7 +9701,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9667,7 +9745,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9711,7 +9789,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9755,7 +9833,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9799,7 +9877,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -9843,7 +9921,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -9887,7 +9965,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -9931,7 +10009,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -9975,7 +10053,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -10019,7 +10097,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -10063,7 +10141,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -10107,7 +10185,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -10151,7 +10229,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -10195,7 +10273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10239,7 +10317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10283,7 +10361,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10395,16 +10473,16 @@
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10446,7 +10524,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="150" t="s">
         <v>589</v>
       </c>
@@ -10490,7 +10568,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="150" t="s">
         <v>589</v>
       </c>
@@ -10534,7 +10612,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="150" t="s">
         <v>597</v>
       </c>
@@ -10578,7 +10656,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="150" t="s">
         <v>604</v>
       </c>
@@ -10622,7 +10700,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="150" t="s">
         <v>608</v>
       </c>
@@ -10666,7 +10744,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="150" t="s">
         <v>614</v>
       </c>
@@ -10710,7 +10788,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
         <v>619</v>
       </c>
@@ -10754,7 +10832,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
         <v>622</v>
       </c>
@@ -10798,7 +10876,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="150" t="s">
         <v>627</v>
       </c>
@@ -10842,7 +10920,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="150" t="s">
         <v>632</v>
       </c>
@@ -10886,7 +10964,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="150" t="s">
         <v>635</v>
       </c>
@@ -10930,7 +11008,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="150" t="s">
         <v>641</v>
       </c>
@@ -10974,7 +11052,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="150" t="s">
         <v>646</v>
       </c>
@@ -11018,7 +11096,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="150" t="s">
         <v>652</v>
       </c>
@@ -11062,7 +11140,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -11106,7 +11184,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="150" t="s">
         <v>661</v>
       </c>
@@ -11150,7 +11228,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="150" t="s">
         <v>666</v>
       </c>
@@ -11194,7 +11272,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="150" t="s">
         <v>666</v>
       </c>
@@ -11238,7 +11316,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="150" t="s">
         <v>678</v>
       </c>
@@ -11282,7 +11360,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="150" t="s">
         <v>684</v>
       </c>
@@ -11326,7 +11404,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="150" t="s">
         <v>690</v>
       </c>
@@ -11370,7 +11448,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="150" t="s">
         <v>696</v>
       </c>
@@ -11414,7 +11492,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="150" t="s">
         <v>699</v>
       </c>
@@ -11458,7 +11536,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11502,7 +11580,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11546,7 +11624,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="150" t="s">
         <v>714</v>
       </c>
@@ -11590,7 +11668,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="150" t="s">
         <v>720</v>
       </c>
@@ -11634,7 +11712,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11678,7 +11756,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="150" t="s">
         <v>731</v>
       </c>
@@ -11722,7 +11800,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11766,7 +11844,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="150" t="s">
         <v>741</v>
       </c>
@@ -11810,7 +11888,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="150" t="s">
         <v>747</v>
       </c>
@@ -11854,7 +11932,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="150" t="s">
         <v>752</v>
       </c>
@@ -11898,7 +11976,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -11943,7 +12021,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="150" t="s">
         <v>762</v>
       </c>
@@ -11987,7 +12065,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -12031,7 +12109,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="150" t="s">
         <v>773</v>
       </c>
@@ -12075,7 +12153,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="150" t="s">
         <v>779</v>
       </c>
@@ -12119,7 +12197,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="150" t="s">
         <v>785</v>
       </c>
@@ -12163,7 +12241,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="150" t="s">
         <v>790</v>
       </c>
@@ -12207,7 +12285,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12251,7 +12329,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="150" t="s">
         <v>800</v>
       </c>
@@ -12295,7 +12373,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12339,7 +12417,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12383,7 +12461,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12428,7 +12506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12472,7 +12550,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="150" t="s">
         <v>824</v>
       </c>
@@ -12516,7 +12594,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12560,7 +12638,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="150" t="s">
         <v>835</v>
       </c>
@@ -12604,7 +12682,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="150" t="s">
         <v>824</v>
       </c>
@@ -12648,7 +12726,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="152" t="s">
         <v>845</v>
       </c>
@@ -12692,7 +12770,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="152" t="s">
         <v>845</v>
       </c>
@@ -12736,7 +12814,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="152" t="s">
         <v>855</v>
       </c>
@@ -12780,7 +12858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -12824,7 +12902,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -12869,7 +12947,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -12913,7 +12991,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="152" t="s">
         <v>870</v>
       </c>
@@ -12957,7 +13035,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -13001,7 +13079,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -13046,7 +13124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="152" t="s">
         <v>883</v>
       </c>
@@ -13090,7 +13168,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="152" t="s">
         <v>889</v>
       </c>
@@ -13134,7 +13212,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="152" t="s">
         <v>889</v>
       </c>
@@ -13178,7 +13256,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="152" t="s">
         <v>899</v>
       </c>
@@ -13222,7 +13300,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13267,7 +13345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13311,7 +13389,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13355,7 +13433,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="152" t="s">
         <v>919</v>
       </c>
@@ -13399,7 +13477,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="152" t="s">
         <v>925</v>
       </c>
@@ -13443,7 +13521,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="152" t="s">
         <v>931</v>
       </c>
@@ -13487,7 +13565,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="152" t="s">
         <v>936</v>
       </c>
@@ -13531,7 +13609,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="152" t="s">
         <v>942</v>
       </c>
@@ -13575,7 +13653,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="152" t="s">
         <v>948</v>
       </c>
@@ -13619,7 +13697,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="152" t="s">
         <v>948</v>
       </c>
@@ -13663,7 +13741,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13707,7 +13785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13751,7 +13829,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="152" t="s">
         <v>967</v>
       </c>
@@ -13795,7 +13873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -13942,37 +14020,37 @@
   <dimension ref="A1:AO56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AO3" sqref="AO3"/>
+      <selection pane="bottomRight" activeCell="AI41" sqref="AI41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="24" width="9.1640625" style="4"/>
-    <col min="25" max="30" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="24" width="9.140625" style="4"/>
+    <col min="25" max="30" width="9.140625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.1640625" style="4"/>
-    <col min="35" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="1"/>
-    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="38.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="51.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.1640625" style="1"/>
+    <col min="32" max="34" width="9.140625" style="4"/>
+    <col min="35" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="1"/>
+    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="156" t="s">
         <v>499</v>
@@ -14059,7 +14137,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14175,11 +14253,11 @@
       <c r="AN2" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AO2" s="5" t="s">
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14194,19 +14272,19 @@
       </c>
       <c r="F3" s="7">
         <f>[1]Main!$C$6*$E$50</f>
-        <v>95.947999999999993</v>
+        <v>94.791999999999987</v>
       </c>
       <c r="G3" s="49">
         <f>[1]Main!$C$8*$E$50</f>
-        <v>149582.932</v>
+        <v>147780.72799999997</v>
       </c>
       <c r="H3" s="49">
         <f>[1]Main!$C$11*$E$50</f>
-        <v>987.69999999999993</v>
+        <v>975.8</v>
       </c>
       <c r="I3" s="49">
         <f>[1]Main!$C$12*$E$50</f>
-        <v>148595.23199999999</v>
+        <v>146804.92799999999</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>[1]Main!$C$28</f>
@@ -14222,15 +14300,15 @@
       </c>
       <c r="O3" s="56">
         <f>'[1]Financial Model'!$AF$21*1000*E50</f>
-        <v>5018.1799999999939</v>
+        <v>4957.7199999999939</v>
       </c>
       <c r="P3" s="56">
         <f>'[1]Financial Model'!$AE$21*1000*E50</f>
-        <v>4753.409999999998</v>
+        <v>4696.1399999999985</v>
       </c>
       <c r="Q3" s="56">
         <f>'[1]Financial Model'!$AD$21*1000*E50</f>
-        <v>2107.37</v>
+        <v>2081.98</v>
       </c>
       <c r="R3" s="51">
         <f>[1]Main!$C$34</f>
@@ -14276,7 +14354,7 @@
       </c>
       <c r="AE3" s="56">
         <f>[1]Main!$C$26*E50</f>
-        <v>8019.46</v>
+        <v>7922.8399999999992</v>
       </c>
       <c r="AF3" s="53">
         <f>'[1]Financial Model'!$X$72</f>
@@ -14305,7 +14383,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14320,19 +14398,19 @@
       </c>
       <c r="F4" s="7">
         <f>[2]Main!$C$6*$E$50</f>
-        <v>27.572599999999998</v>
+        <v>27.240399999999998</v>
       </c>
       <c r="G4" s="49">
         <f>[2]Main!$C$8*$E$50</f>
-        <v>10689.566148799999</v>
+        <v>10560.776195199998</v>
       </c>
       <c r="H4" s="49">
         <f>[2]Main!$C$11*$E$50</f>
-        <v>-3872.8090499999998</v>
+        <v>-3826.1486999999997</v>
       </c>
       <c r="I4" s="49">
         <f>[2]Main!$C$12*$E$50</f>
-        <v>14562.375198799997</v>
+        <v>14386.924895199996</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>[2]Main!$C$28</f>
@@ -14348,15 +14426,15 @@
       </c>
       <c r="O4" s="56">
         <f>'[2]Financial Model'!$AA$22*E50</f>
-        <v>1151.127829999999</v>
+        <v>1137.2588199999991</v>
       </c>
       <c r="P4" s="56">
         <f>'[2]Financial Model'!$Z$22*$E$50</f>
-        <v>338.51467000000116</v>
+        <v>334.43618000000112</v>
       </c>
       <c r="Q4" s="56">
         <f>'[2]Financial Model'!$Y$22*$E$50</f>
-        <v>563.94267000000013</v>
+        <v>557.14818000000014</v>
       </c>
       <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
@@ -14391,7 +14469,7 @@
       </c>
       <c r="AE4" s="56">
         <f>[2]Main!$C$26*E50</f>
-        <v>1943.3578499999999</v>
+        <v>1919.9438999999998</v>
       </c>
       <c r="AF4" s="53">
         <f>'[2]Financial Model'!$T$76</f>
@@ -14417,7 +14495,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14540,7 +14618,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14670,7 +14748,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14800,7 +14878,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -14815,19 +14893,19 @@
       </c>
       <c r="F8" s="7">
         <f>[6]Main!$C$6*E50</f>
-        <v>6.8806999999999992</v>
+        <v>6.7977999999999987</v>
       </c>
       <c r="G8" s="49">
         <f>[6]Main!$C$8*E50</f>
-        <v>3126.0533853999996</v>
+        <v>3088.3900915999993</v>
       </c>
       <c r="H8" s="49">
         <f>[6]Main!$C$11*$E$50</f>
-        <v>149.62410000000008</v>
+        <v>147.82140000000007</v>
       </c>
       <c r="I8" s="49">
         <f>[6]Main!$C$12*$E$50</f>
-        <v>2976.4292853999996</v>
+        <v>2940.5686915999995</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
@@ -14843,15 +14921,15 @@
       </c>
       <c r="O8" s="56">
         <f>'[6]Financial Model'!$AA$20*$E$50</f>
-        <v>-455.81691000000001</v>
+        <v>-450.32513999999998</v>
       </c>
       <c r="P8" s="56">
         <f>'[6]Financial Model'!$Z$20*$E$50</f>
-        <v>76.477859999999353</v>
+        <v>75.55643999999937</v>
       </c>
       <c r="Q8" s="56">
         <f>'[6]Financial Model'!$Y$20*$E$50</f>
-        <v>-38.43066000000033</v>
+        <v>-37.967640000000323</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
@@ -14900,7 +14978,7 @@
       </c>
       <c r="AE8" s="56">
         <f>[6]Main!$C$27*E50</f>
-        <v>896.74860000000001</v>
+        <v>885.94439999999997</v>
       </c>
       <c r="AF8" s="53">
         <f>'[6]Financial Model'!$R$79</f>
@@ -14934,7 +15012,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -14949,19 +15027,19 @@
       </c>
       <c r="F9" s="7">
         <f>[7]Main!$C$6*E50</f>
-        <v>21.189900000000002</v>
+        <v>20.9346</v>
       </c>
       <c r="G9" s="49">
         <f>[7]Main!$C$8*$E$50</f>
-        <v>1953.161232984</v>
+        <v>1929.6291699359999</v>
       </c>
       <c r="H9" s="49">
         <f>[7]Main!$C$11*E50</f>
-        <v>322.90402999999998</v>
+        <v>319.01362</v>
       </c>
       <c r="I9" s="49">
         <f>[7]Main!$C$12*E50</f>
-        <v>1630.2572029840001</v>
+        <v>1610.615549936</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>[7]Main!$C$29</f>
@@ -14998,7 +15076,7 @@
       </c>
       <c r="AE9" s="56">
         <f>[7]Main!$C$26*E50</f>
-        <v>617.17056999999988</v>
+        <v>609.73477999999989</v>
       </c>
       <c r="AF9" s="53">
         <f>'[7]Financial Model'!$M$63</f>
@@ -15023,7 +15101,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -15038,19 +15116,19 @@
       </c>
       <c r="F10" s="7">
         <f>[8]Main!$C$6*E50</f>
-        <v>10.723599999999999</v>
+        <v>10.594399999999998</v>
       </c>
       <c r="G10" s="49">
         <f>[8]Main!$C$8*E50</f>
-        <v>1932.2747603999996</v>
+        <v>1908.9943415999996</v>
       </c>
       <c r="H10" s="49">
         <f>[8]Main!$C$11*$E$50</f>
-        <v>-230.99563999999998</v>
+        <v>-228.21255999999997</v>
       </c>
       <c r="I10" s="49">
         <f>[8]Main!$C$12*$E$50</f>
-        <v>2163.2704003999997</v>
+        <v>2137.2069015999996</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>[8]Main!$C$28</f>
@@ -15070,11 +15148,11 @@
       </c>
       <c r="O10" s="56">
         <f>'[8]Financial Model'!$Z$17*E50</f>
-        <v>348.28957999999989</v>
+        <v>344.09331999999989</v>
       </c>
       <c r="P10" s="56">
         <f>'[8]Financial Model'!$Y$17*F50</f>
-        <v>-252.21325301204848</v>
+        <v>-255.28902439024415</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="52">
@@ -15117,7 +15195,7 @@
       </c>
       <c r="AE10" s="56">
         <f>[8]Main!$C$26*E50</f>
-        <v>570.24818000000005</v>
+        <v>563.37771999999995</v>
       </c>
       <c r="AF10" s="53">
         <f>'[8]Financial Model'!$P$72</f>
@@ -15151,7 +15229,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15291,7 +15369,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15306,19 +15384,19 @@
       </c>
       <c r="F12" s="54">
         <f>[10]Main!$C$6*E50</f>
-        <v>18.7746</v>
+        <v>18.548400000000001</v>
       </c>
       <c r="G12" s="49">
         <f>[10]Main!$C$8*E50</f>
-        <v>929.07985559999986</v>
+        <v>917.88612239999986</v>
       </c>
       <c r="H12" s="49">
         <f>[10]Main!$C$11*E50</f>
-        <v>123.55711999999997</v>
+        <v>122.06847999999998</v>
       </c>
       <c r="I12" s="49">
         <f>[10]Main!$C$12*E50</f>
-        <v>805.52273559999992</v>
+        <v>795.81764239999984</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>[10]Main!$C$27</f>
@@ -15339,15 +15417,15 @@
       <c r="N12" s="50"/>
       <c r="O12" s="56">
         <f>'[10]Financial Model'!$X$18*E50</f>
-        <v>218.29829999999976</v>
+        <v>215.66819999999976</v>
       </c>
       <c r="P12" s="56">
         <f>'[10]Financial Model'!$W$18*$E$50</f>
-        <v>-94.637430000000123</v>
+        <v>-93.497220000000127</v>
       </c>
       <c r="Q12" s="56">
         <f>'[10]Financial Model'!$V$18*$E$50</f>
-        <v>32.667140000000508</v>
+        <v>32.273560000000501</v>
       </c>
       <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
@@ -15396,7 +15474,7 @@
       </c>
       <c r="AE12" s="56">
         <f>'[10]Financial Model'!$Q$41*E50</f>
-        <v>615.8292899999999</v>
+        <v>608.40965999999992</v>
       </c>
       <c r="AF12" s="53">
         <f>'[10]Financial Model'!$X$74</f>
@@ -15430,7 +15508,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15555,7 +15633,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15661,11 +15739,11 @@
       <c r="AN14" s="105" t="s">
         <v>1002</v>
       </c>
-      <c r="AO14" s="103" t="s">
+      <c r="AO14" s="105" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15809,7 +15887,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -15928,11 +16006,11 @@
       <c r="AN16" s="93" t="s">
         <v>1004</v>
       </c>
-      <c r="AO16" s="91" t="s">
+      <c r="AO16" s="93" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -16031,7 +16109,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -16057,7 +16135,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B19" s="136" t="s">
         <v>582</v>
       </c>
@@ -16088,7 +16166,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B20" s="135" t="s">
         <v>975</v>
       </c>
@@ -16114,7 +16192,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -16138,7 +16216,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16164,7 +16242,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16189,7 +16267,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16204,11 +16282,11 @@
       </c>
       <c r="F24" s="54">
         <f>[16]Main!$C$6*E50</f>
-        <v>275.07030000000003</v>
+        <v>271.75619999999998</v>
       </c>
       <c r="G24" s="56">
         <f>[16]Main!$C$8*E50</f>
-        <v>33641.097689999995</v>
+        <v>33235.783259999997</v>
       </c>
       <c r="H24" s="56">
         <f>[16]Main!$C$11*E50</f>
@@ -16216,7 +16294,7 @@
       </c>
       <c r="I24" s="56">
         <f>[16]Main!$C$12*E50</f>
-        <v>33641.097689999995</v>
+        <v>33235.783259999997</v>
       </c>
       <c r="AK24" s="4">
         <f>[16]Main!$C$24</f>
@@ -16230,7 +16308,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16263,7 +16341,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
@@ -16289,7 +16367,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16315,7 +16393,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="1"/>
@@ -16325,7 +16403,7 @@
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B29" s="136" t="s">
         <v>582</v>
       </c>
@@ -16341,7 +16419,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>511</v>
       </c>
@@ -16356,7 +16434,7 @@
       </c>
       <c r="F30" s="7">
         <f>18.22*E50</f>
-        <v>15.122599999999998</v>
+        <v>14.940399999999999</v>
       </c>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
@@ -16374,7 +16452,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>540</v>
       </c>
@@ -16438,7 +16516,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>541</v>
       </c>
@@ -16465,7 +16543,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>575</v>
       </c>
@@ -16490,7 +16568,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>587</v>
       </c>
@@ -16515,7 +16593,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>588</v>
       </c>
@@ -16540,7 +16618,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
       <c r="H36" s="1"/>
@@ -16550,7 +16628,7 @@
       <c r="M36" s="56"/>
       <c r="N36" s="56"/>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B37" s="136" t="s">
         <v>582</v>
       </c>
@@ -16565,7 +16643,7 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>985</v>
       </c>
@@ -16592,7 +16670,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>579</v>
       </c>
@@ -16610,7 +16688,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>580</v>
       </c>
@@ -16628,8 +16706,8 @@
         <v>981</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
         <v>581</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -16638,18 +16716,74 @@
       <c r="D41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G41" s="56"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="E41" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F41" s="54">
+        <f>[19]Main!$C$6*$E$50</f>
+        <v>32.135799999999996</v>
+      </c>
+      <c r="G41" s="49">
+        <f>[19]Main!$C$8*$E$50</f>
+        <v>2998.9265779865996</v>
+      </c>
+      <c r="H41" s="1">
+        <f>[19]Main!$C$11*E50</f>
+        <v>-84.46</v>
+      </c>
+      <c r="I41" s="56">
+        <f>[19]Main!$C$12*E50</f>
+        <v>3083.3865779865996</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
+      <c r="T41" s="51">
+        <f>[19]Main!$C$35</f>
+        <v>1.1231500460263886</v>
+      </c>
+      <c r="Z41" s="53">
+        <f>'[19]Financial Model'!$U$26</f>
+        <v>0.32029452369995398</v>
+      </c>
+      <c r="AA41" s="53">
+        <f>'[19]Financial Model'!$U$27</f>
+        <v>7.2250345144960884E-2</v>
+      </c>
+      <c r="AB41" s="53">
+        <f>'[19]Financial Model'!$U$28</f>
+        <v>4.4178554993097099E-2</v>
+      </c>
+      <c r="AC41" s="53">
+        <f>'[19]Financial Model'!$U$29</f>
+        <v>0.32867132867132864</v>
+      </c>
+      <c r="AE41" s="56">
+        <f>[19]Main!$C$28*E50</f>
+        <v>1381.6999999999998</v>
+      </c>
+      <c r="AF41" s="53">
+        <f>'[19]Financial Model'!$U$71</f>
+        <v>0.29515757109915453</v>
+      </c>
+      <c r="AI41" s="57">
+        <f>[19]Main!$C$25</f>
+        <v>2794</v>
+      </c>
+      <c r="AK41" s="4">
+        <f>[19]Main!$C$24</f>
+        <v>1879</v>
+      </c>
+      <c r="AL41" s="4" t="str">
+        <f>[19]Main!$C$23</f>
+        <v>NYC, NY</v>
+      </c>
       <c r="AM41" s="4" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>568</v>
       </c>
@@ -16673,7 +16807,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>569</v>
       </c>
@@ -16792,7 +16926,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G44" s="56"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -16801,7 +16935,7 @@
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -16810,7 +16944,7 @@
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G46" s="56"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -16819,7 +16953,7 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G47" s="49"/>
       <c r="I47" s="4"/>
       <c r="J47" s="1"/>
@@ -16827,7 +16961,7 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
@@ -16835,7 +16969,7 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D49" s="154" t="s">
         <v>495</v>
       </c>
@@ -16848,23 +16982,23 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D50" s="43" t="s">
         <v>497</v>
       </c>
       <c r="E50" s="44">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="F50" s="45">
         <f>1/E50</f>
-        <v>1.2048192771084338</v>
+        <v>1.2195121951219512</v>
       </c>
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D51" s="43" t="s">
         <v>498</v>
       </c>
@@ -16880,7 +17014,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D52" s="46" t="s">
         <v>564</v>
       </c>
@@ -16893,16 +17027,16 @@
       </c>
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G56" s="49"/>
     </row>
   </sheetData>
@@ -16932,9 +17066,10 @@
     <hyperlink ref="B29" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
     <hyperlink ref="B19" r:id="rId20" xr:uid="{8B27DD55-F39A-E042-A7A2-82BE3E8447D7}"/>
     <hyperlink ref="B43" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
+    <hyperlink ref="B41" r:id="rId22" xr:uid="{FD9CE6D1-58BD-4F93-B596-F3E2DED3874C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId22"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId23"/>
   <ignoredErrors>
     <ignoredError sqref="AI12 G12 Z1 T1" formula="1"/>
   </ignoredErrors>
@@ -16952,21 +17087,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -16977,7 +17112,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -17004,98 +17139,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
Q1-4 and FY21 $FL
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CE399A-BA5F-4F38-AD0C-202043C1DB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71877A9D-8F78-4B6B-B2A4-5D086CF2AB88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="1016">
   <si>
     <t>Ticker</t>
   </si>
@@ -3176,6 +3176,15 @@
   </si>
   <si>
     <t>Key Notes</t>
+  </si>
+  <si>
+    <t>Foot Locker, Champs Sports &amp; more</t>
+  </si>
+  <si>
+    <t>Crocs</t>
+  </si>
+  <si>
+    <t>Skechers, Mark Nason</t>
   </si>
 </sst>
 </file>
@@ -3541,7 +3550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3942,6 +3951,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5017,130 +5029,110 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
-      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>2.4049999999999998</v>
+            <v>39.19</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>120.24999999999999</v>
+            <v>3657.2275341299996</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>13.872</v>
+            <v>-103</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>106.37799999999999</v>
+            <v>3760.2275341299996</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Leicester, UK</v>
+            <v>NYC, NY</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1917</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>388</v>
+            <v>1879</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>31.096</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29" t="str">
-            <v>H122</v>
-          </cell>
-          <cell r="D29">
-            <v>45063</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>4.0893015030946032</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>10.025846256461564</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>8.8692679673169916</v>
+            <v>2794</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>1685</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Q322</v>
+          </cell>
+          <cell r="D30">
+            <v>43405</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>1.1231500460263886</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39">
+            <v>8.8684611654009426</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="16">
-          <cell r="S16">
-            <v>-11.902999999999997</v>
-          </cell>
-          <cell r="T16">
-            <v>7.0139999999999958</v>
-          </cell>
-        </row>
         <row r="21">
-          <cell r="T21">
-            <v>-2.7951830820442503E-2</v>
+          <cell r="AH21">
+            <v>0.18680445151033376</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="K26">
-            <v>0.19490724836825837</v>
+          <cell r="U26">
+            <v>0.32029452369995398</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="K27">
-            <v>5.2401809229359962E-2</v>
+          <cell r="U27">
+            <v>7.2250345144960884E-2</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="K28">
-            <v>4.1008244589488214E-2</v>
+          <cell r="U28">
+            <v>4.4178554993097099E-2</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="K29">
-            <v>6.4337034617896707E-2</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="K72">
-            <v>9.3658776773467567E-2</v>
+          <cell r="U29">
+            <v>0.32867132867132864</v>
           </cell>
         </row>
         <row r="73">
-          <cell r="K73">
-            <v>0.23735625323305887</v>
+          <cell r="U73">
+            <v>0.29515757109915453</v>
           </cell>
         </row>
         <row r="74">
-          <cell r="K74">
-            <v>0.20930060375174159</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="T83">
-            <v>4.5587396635300852</v>
+          <cell r="U74">
+            <v>2.4939172749391725E-2</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="U75">
+            <v>0.19248343614347727</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5152,82 +5144,130 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>39.19</v>
+            <v>2.4049999999999998</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>3657.2275341299996</v>
+            <v>120.24999999999999</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-103</v>
+            <v>13.872</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>3760.2275341299996</v>
+            <v>106.37799999999999</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>NYC, NY</v>
+            <v>Leicester, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1879</v>
+            <v>1917</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>2794</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>1685</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>1.1231500460263886</v>
+            <v>388</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>31.096</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D29">
+            <v>45063</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>4.0893015030946032</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>10.025846256461564</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>8.8692679673169916</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="16">
+          <cell r="S16">
+            <v>-11.902999999999997</v>
+          </cell>
+          <cell r="T16">
+            <v>7.0139999999999958</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="T21">
+            <v>-2.7951830820442503E-2</v>
+          </cell>
+        </row>
         <row r="26">
-          <cell r="U26">
-            <v>0.32029452369995398</v>
+          <cell r="K26">
+            <v>0.19490724836825837</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="U27">
-            <v>7.2250345144960884E-2</v>
+          <cell r="K27">
+            <v>5.2401809229359962E-2</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="U28">
-            <v>4.4178554993097099E-2</v>
+          <cell r="K28">
+            <v>4.1008244589488214E-2</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="U29">
-            <v>0.32867132867132864</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="U71">
-            <v>0.29515757109915453</v>
+          <cell r="K29">
+            <v>6.4337034617896707E-2</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="K72">
+            <v>9.3658776773467567E-2</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="K73">
+            <v>0.23735625323305887</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="K74">
+            <v>0.20930060375174159</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="T83">
+            <v>4.5587396635300852</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14020,10 +14060,10 @@
   <dimension ref="A1:AO56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="X15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI41" sqref="AI41"/>
+      <selection pane="bottomRight" activeCell="AN41" sqref="AN41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14052,20 +14092,20 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="156" t="s">
+      <c r="F1" s="157" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156"/>
-      <c r="M1" s="156"/>
-      <c r="N1" s="156"/>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
         <v>14.953293230057294</v>
@@ -14651,7 +14691,7 @@
         <f>[4]Main!$C$28</f>
         <v>H123</v>
       </c>
-      <c r="K6" s="85">
+      <c r="K6" s="130">
         <f>[4]Main!$D$28</f>
         <v>44826</v>
       </c>
@@ -14781,7 +14821,7 @@
         <f>[5]Main!$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="K7" s="85">
+      <c r="K7" s="130">
         <f>[5]Main!$D$29</f>
         <v>44765</v>
       </c>
@@ -16687,6 +16727,9 @@
       <c r="AM39" s="4" t="s">
         <v>980</v>
       </c>
+      <c r="AN39" s="4" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
@@ -16705,6 +16748,9 @@
       <c r="AM40" s="4" t="s">
         <v>981</v>
       </c>
+      <c r="AN40" s="4" t="s">
+        <v>1015</v>
+      </c>
     </row>
     <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
@@ -16720,67 +16766,92 @@
         <v>505</v>
       </c>
       <c r="F41" s="54">
-        <f>[19]Main!$C$6*$E$50</f>
+        <f>[18]Main!$C$6*$E$50</f>
         <v>32.135799999999996</v>
       </c>
       <c r="G41" s="49">
-        <f>[19]Main!$C$8*$E$50</f>
+        <f>[18]Main!$C$8*$E$50</f>
         <v>2998.9265779865996</v>
       </c>
       <c r="H41" s="1">
-        <f>[19]Main!$C$11*E50</f>
+        <f>[18]Main!$C$11*E50</f>
         <v>-84.46</v>
       </c>
       <c r="I41" s="56">
-        <f>[19]Main!$C$12*E50</f>
+        <f>[18]Main!$C$12*E50</f>
         <v>3083.3865779865996</v>
       </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="J41" s="4" t="str">
+        <f>[18]Main!$C$30</f>
+        <v>Q322</v>
+      </c>
+      <c r="K41" s="154">
+        <f>[18]Main!$D$30</f>
+        <v>43405</v>
+      </c>
+      <c r="L41" s="50">
+        <f>[18]Main!$C$39</f>
+        <v>8.8684611654009426</v>
+      </c>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
       <c r="T41" s="51">
-        <f>[19]Main!$C$35</f>
+        <f>[18]Main!$C$35</f>
         <v>1.1231500460263886</v>
       </c>
+      <c r="W41" s="53">
+        <f>'[18]Financial Model'!$AH$21</f>
+        <v>0.18680445151033376</v>
+      </c>
       <c r="Z41" s="53">
-        <f>'[19]Financial Model'!$U$26</f>
+        <f>'[18]Financial Model'!$U$26</f>
         <v>0.32029452369995398</v>
       </c>
       <c r="AA41" s="53">
-        <f>'[19]Financial Model'!$U$27</f>
+        <f>'[18]Financial Model'!$U$27</f>
         <v>7.2250345144960884E-2</v>
       </c>
       <c r="AB41" s="53">
-        <f>'[19]Financial Model'!$U$28</f>
+        <f>'[18]Financial Model'!$U$28</f>
         <v>4.4178554993097099E-2</v>
       </c>
       <c r="AC41" s="53">
-        <f>'[19]Financial Model'!$U$29</f>
+        <f>'[18]Financial Model'!$U$29</f>
         <v>0.32867132867132864</v>
       </c>
       <c r="AE41" s="56">
-        <f>[19]Main!$C$28*E50</f>
+        <f>[18]Main!$C$28*E50</f>
         <v>1381.6999999999998</v>
       </c>
       <c r="AF41" s="53">
-        <f>'[19]Financial Model'!$U$71</f>
+        <f>'[18]Financial Model'!$U$73</f>
         <v>0.29515757109915453</v>
       </c>
+      <c r="AG41" s="53">
+        <f>'[18]Financial Model'!$U$74</f>
+        <v>2.4939172749391725E-2</v>
+      </c>
+      <c r="AH41" s="53">
+        <f>'[18]Financial Model'!$U$75</f>
+        <v>0.19248343614347727</v>
+      </c>
       <c r="AI41" s="57">
-        <f>[19]Main!$C$25</f>
+        <f>[18]Main!$C$27</f>
         <v>2794</v>
       </c>
       <c r="AK41" s="4">
-        <f>[19]Main!$C$24</f>
+        <f>[18]Main!$C$24</f>
         <v>1879</v>
       </c>
       <c r="AL41" s="4" t="str">
-        <f>[19]Main!$C$23</f>
+        <f>[18]Main!$C$23</f>
         <v>NYC, NY</v>
       </c>
       <c r="AM41" s="4" t="s">
         <v>978</v>
+      </c>
+      <c r="AN41" s="4" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="42" spans="2:40" x14ac:dyDescent="0.2">
@@ -16821,105 +16892,105 @@
         <v>15</v>
       </c>
       <c r="F43" s="54">
-        <f>[18]Main!$C$6</f>
+        <f>[19]Main!$C$6</f>
         <v>2.4049999999999998</v>
       </c>
       <c r="G43" s="56">
-        <f>[18]Main!$C$8</f>
+        <f>[19]Main!$C$8</f>
         <v>120.24999999999999</v>
       </c>
       <c r="H43" s="56">
-        <f>[18]Main!$C$11</f>
+        <f>[19]Main!$C$11</f>
         <v>13.872</v>
       </c>
       <c r="I43" s="56">
-        <f>[18]Main!$C$12</f>
+        <f>[19]Main!$C$12</f>
         <v>106.37799999999999</v>
       </c>
       <c r="J43" s="4" t="str">
-        <f>[18]Main!$C$29</f>
+        <f>[19]Main!$C$29</f>
         <v>H122</v>
       </c>
       <c r="K43" s="85">
-        <f>[18]Main!$D$29</f>
+        <f>[19]Main!$D$29</f>
         <v>45063</v>
       </c>
       <c r="L43" s="50">
-        <f>[18]Main!$C$38</f>
+        <f>[19]Main!$C$38</f>
         <v>8.8692679673169916</v>
       </c>
       <c r="M43" s="56"/>
       <c r="N43" s="56"/>
       <c r="O43" s="56">
-        <f>'[18]Financial Model'!$T$16</f>
+        <f>'[19]Financial Model'!$T$16</f>
         <v>7.0139999999999958</v>
       </c>
       <c r="P43" s="56">
-        <f>'[18]Financial Model'!$S$16</f>
+        <f>'[19]Financial Model'!$S$16</f>
         <v>-11.902999999999997</v>
       </c>
       <c r="Q43" s="56">
-        <f>'[18]Financial Model'!$R$17</f>
+        <f>'[19]Financial Model'!$R$17</f>
         <v>0</v>
       </c>
       <c r="R43" s="51">
-        <f>[18]Main!$C$37</f>
+        <f>[19]Main!$C$37</f>
         <v>10.025846256461564</v>
       </c>
       <c r="S43" s="153">
-        <f>'[18]Financial Model'!$T$83</f>
+        <f>'[19]Financial Model'!$T$83</f>
         <v>4.5587396635300852</v>
       </c>
       <c r="T43" s="51">
-        <f>[18]Main!$C$34</f>
+        <f>[19]Main!$C$34</f>
         <v>4.0893015030946032</v>
       </c>
       <c r="W43" s="53">
-        <f>'[18]Financial Model'!$T$21</f>
+        <f>'[19]Financial Model'!$T$21</f>
         <v>-2.7951830820442503E-2</v>
       </c>
       <c r="Z43" s="53">
-        <f>'[18]Financial Model'!$K$26</f>
+        <f>'[19]Financial Model'!$K$26</f>
         <v>0.19490724836825837</v>
       </c>
       <c r="AA43" s="53">
-        <f>'[18]Financial Model'!$K$27</f>
+        <f>'[19]Financial Model'!$K$27</f>
         <v>5.2401809229359962E-2</v>
       </c>
       <c r="AB43" s="53">
-        <f>'[18]Financial Model'!$K$28</f>
+        <f>'[19]Financial Model'!$K$28</f>
         <v>4.1008244589488214E-2</v>
       </c>
       <c r="AC43" s="53">
-        <f>'[18]Financial Model'!$K$29</f>
+        <f>'[19]Financial Model'!$K$29</f>
         <v>6.4337034617896707E-2</v>
       </c>
       <c r="AE43" s="56">
-        <f>[18]Main!$C$27</f>
+        <f>[19]Main!$C$27</f>
         <v>31.096</v>
       </c>
       <c r="AF43" s="53">
-        <f>'[18]Financial Model'!$K$72</f>
+        <f>'[19]Financial Model'!$K$72</f>
         <v>9.3658776773467567E-2</v>
       </c>
       <c r="AG43" s="53">
-        <f>'[18]Financial Model'!$K$73</f>
+        <f>'[19]Financial Model'!$K$73</f>
         <v>0.23735625323305887</v>
       </c>
       <c r="AH43" s="53">
-        <f>'[18]Financial Model'!$K$74</f>
+        <f>'[19]Financial Model'!$K$74</f>
         <v>0.20930060375174159</v>
       </c>
       <c r="AI43" s="4">
-        <f>[18]Main!$C$25</f>
+        <f>[19]Main!$C$25</f>
         <v>388</v>
       </c>
       <c r="AK43" s="4">
-        <f>[18]Main!$C$24</f>
+        <f>[19]Main!$C$24</f>
         <v>1917</v>
       </c>
       <c r="AL43" s="4" t="str">
-        <f>[18]Main!$C$23</f>
+        <f>[19]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
       <c r="AM43" s="4" t="s">
@@ -16970,10 +17041,10 @@
       <c r="N48" s="56"/>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D49" s="154" t="s">
+      <c r="D49" s="155" t="s">
         <v>495</v>
       </c>
-      <c r="E49" s="155"/>
+      <c r="E49" s="156"/>
       <c r="F49" s="42" t="s">
         <v>496</v>
       </c>

</xml_diff>

<commit_message>
Update currency pairs, update $UA price
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055080C4-A843-4C14-816F-D6608EC2713B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519E78A-CA2D-8C46-B521-ADAD8900ED75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -45,12 +45,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -58,7 +68,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -67,42 +77,42 @@
   <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
@@ -3195,14 +3205,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3645,7 +3655,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3654,13 +3664,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3689,16 +3699,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3707,12 +3717,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3749,7 +3759,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3767,7 +3777,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3788,7 +3798,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3815,15 +3825,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3832,7 +3842,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3843,16 +3853,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3887,7 +3897,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3899,7 +3909,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3934,7 +3944,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5966,7 +5976,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6751,25 +6761,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6811,7 +6821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6855,7 +6865,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6899,7 +6909,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6943,7 +6953,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -6987,7 +6997,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -7031,7 +7041,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -7075,7 +7085,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -7119,7 +7129,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -7163,7 +7173,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -7207,7 +7217,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -7251,7 +7261,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -7295,7 +7305,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -7339,7 +7349,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7383,7 +7393,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7427,7 +7437,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7471,7 +7481,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7515,7 +7525,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7559,7 +7569,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7603,7 +7613,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7647,7 +7657,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7691,7 +7701,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7735,7 +7745,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7779,7 +7789,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7823,7 +7833,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7867,7 +7877,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7911,7 +7921,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -7955,7 +7965,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -7999,7 +8009,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -8043,7 +8053,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -8087,7 +8097,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -8131,7 +8141,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -8175,7 +8185,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -8219,7 +8229,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -8263,7 +8273,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -8307,7 +8317,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8351,7 +8361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8395,7 +8405,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8439,7 +8449,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8483,7 +8493,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8527,7 +8537,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8571,7 +8581,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8615,7 +8625,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8659,7 +8669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8777,25 +8787,25 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8837,7 +8847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8881,7 +8891,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8925,7 +8935,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -8969,7 +8979,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -9013,7 +9023,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -9057,7 +9067,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -9101,7 +9111,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -9145,7 +9155,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -9189,7 +9199,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -9233,7 +9243,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -9277,7 +9287,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -9321,7 +9331,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9365,7 +9375,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9409,7 +9419,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9453,7 +9463,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9497,7 +9507,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9541,7 +9551,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9585,7 +9595,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9629,7 +9639,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9673,7 +9683,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9717,7 +9727,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9761,7 +9771,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9805,7 +9815,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9849,7 +9859,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9893,7 +9903,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9937,7 +9947,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -9981,7 +9991,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -10025,7 +10035,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -10069,7 +10079,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -10113,7 +10123,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -10157,7 +10167,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -10201,7 +10211,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -10245,7 +10255,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -10289,7 +10299,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -10333,7 +10343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10377,7 +10387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10421,7 +10431,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10533,16 +10543,16 @@
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10584,7 +10594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="150" t="s">
         <v>589</v>
       </c>
@@ -10628,7 +10638,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="150" t="s">
         <v>589</v>
       </c>
@@ -10672,7 +10682,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="150" t="s">
         <v>597</v>
       </c>
@@ -10716,7 +10726,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="150" t="s">
         <v>604</v>
       </c>
@@ -10760,7 +10770,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="150" t="s">
         <v>608</v>
       </c>
@@ -10804,7 +10814,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="150" t="s">
         <v>614</v>
       </c>
@@ -10848,7 +10858,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="150" t="s">
         <v>619</v>
       </c>
@@ -10892,7 +10902,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="150" t="s">
         <v>622</v>
       </c>
@@ -10936,7 +10946,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="150" t="s">
         <v>627</v>
       </c>
@@ -10980,7 +10990,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="150" t="s">
         <v>632</v>
       </c>
@@ -11024,7 +11034,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="150" t="s">
         <v>635</v>
       </c>
@@ -11068,7 +11078,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="150" t="s">
         <v>641</v>
       </c>
@@ -11112,7 +11122,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="150" t="s">
         <v>646</v>
       </c>
@@ -11156,7 +11166,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="150" t="s">
         <v>652</v>
       </c>
@@ -11200,7 +11210,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -11244,7 +11254,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="150" t="s">
         <v>661</v>
       </c>
@@ -11288,7 +11298,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="150" t="s">
         <v>666</v>
       </c>
@@ -11332,7 +11342,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="150" t="s">
         <v>666</v>
       </c>
@@ -11376,7 +11386,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="150" t="s">
         <v>678</v>
       </c>
@@ -11420,7 +11430,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="150" t="s">
         <v>684</v>
       </c>
@@ -11464,7 +11474,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="150" t="s">
         <v>690</v>
       </c>
@@ -11508,7 +11518,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
         <v>696</v>
       </c>
@@ -11552,7 +11562,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="150" t="s">
         <v>699</v>
       </c>
@@ -11596,7 +11606,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11640,7 +11650,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11684,7 +11694,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="150" t="s">
         <v>714</v>
       </c>
@@ -11728,7 +11738,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="150" t="s">
         <v>720</v>
       </c>
@@ -11772,7 +11782,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11816,7 +11826,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="150" t="s">
         <v>731</v>
       </c>
@@ -11860,7 +11870,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11904,7 +11914,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="150" t="s">
         <v>741</v>
       </c>
@@ -11948,7 +11958,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="150" t="s">
         <v>747</v>
       </c>
@@ -11992,7 +12002,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="150" t="s">
         <v>752</v>
       </c>
@@ -12036,7 +12046,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -12081,7 +12091,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="150" t="s">
         <v>762</v>
       </c>
@@ -12125,7 +12135,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -12169,7 +12179,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="150" t="s">
         <v>773</v>
       </c>
@@ -12213,7 +12223,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="150" t="s">
         <v>779</v>
       </c>
@@ -12257,7 +12267,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="150" t="s">
         <v>785</v>
       </c>
@@ -12301,7 +12311,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="150" t="s">
         <v>790</v>
       </c>
@@ -12345,7 +12355,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12389,7 +12399,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="150" t="s">
         <v>800</v>
       </c>
@@ -12433,7 +12443,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12477,7 +12487,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12521,7 +12531,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12566,7 +12576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12610,7 +12620,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="150" t="s">
         <v>824</v>
       </c>
@@ -12654,7 +12664,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12698,7 +12708,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="150" t="s">
         <v>835</v>
       </c>
@@ -12742,7 +12752,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="150" t="s">
         <v>824</v>
       </c>
@@ -12786,7 +12796,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="152" t="s">
         <v>845</v>
       </c>
@@ -12830,7 +12840,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="152" t="s">
         <v>845</v>
       </c>
@@ -12874,7 +12884,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="152" t="s">
         <v>855</v>
       </c>
@@ -12918,7 +12928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -12962,7 +12972,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -13007,7 +13017,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -13051,7 +13061,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="152" t="s">
         <v>870</v>
       </c>
@@ -13095,7 +13105,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -13139,7 +13149,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -13184,7 +13194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="152" t="s">
         <v>883</v>
       </c>
@@ -13228,7 +13238,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="152" t="s">
         <v>889</v>
       </c>
@@ -13272,7 +13282,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="152" t="s">
         <v>889</v>
       </c>
@@ -13316,7 +13326,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="152" t="s">
         <v>899</v>
       </c>
@@ -13360,7 +13370,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13405,7 +13415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13449,7 +13459,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13493,7 +13503,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="152" t="s">
         <v>919</v>
       </c>
@@ -13537,7 +13547,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="152" t="s">
         <v>925</v>
       </c>
@@ -13581,7 +13591,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="152" t="s">
         <v>931</v>
       </c>
@@ -13625,7 +13635,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="152" t="s">
         <v>936</v>
       </c>
@@ -13669,7 +13679,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="152" t="s">
         <v>942</v>
       </c>
@@ -13713,7 +13723,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="152" t="s">
         <v>948</v>
       </c>
@@ -13757,7 +13767,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="152" t="s">
         <v>948</v>
       </c>
@@ -13801,7 +13811,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13845,7 +13855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13889,7 +13899,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="152" t="s">
         <v>967</v>
       </c>
@@ -13933,7 +13943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -14083,34 +14093,34 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="24" width="9.140625" style="4"/>
-    <col min="25" max="30" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="24" width="9.1640625" style="4"/>
+    <col min="25" max="30" width="9.1640625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.140625" style="4"/>
-    <col min="35" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="41.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="32" max="34" width="9.1640625" style="4"/>
+    <col min="35" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="156" t="s">
         <v>499</v>
@@ -14197,7 +14207,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14317,7 +14327,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14332,19 +14342,19 @@
       </c>
       <c r="F3" s="7">
         <f>[1]Main!$C$6*$E$50</f>
-        <v>94.791999999999987</v>
+        <v>92.48</v>
       </c>
       <c r="G3" s="49">
         <f>[1]Main!$C$8*$E$50</f>
-        <v>147780.72799999997</v>
+        <v>144176.32000000001</v>
       </c>
       <c r="H3" s="49">
         <f>[1]Main!$C$11*$E$50</f>
-        <v>975.8</v>
+        <v>952</v>
       </c>
       <c r="I3" s="49">
         <f>[1]Main!$C$12*$E$50</f>
-        <v>146804.92799999999</v>
+        <v>143224.32000000001</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>[1]Main!$C$28</f>
@@ -14360,15 +14370,15 @@
       </c>
       <c r="O3" s="56">
         <f>'[1]Financial Model'!$AF$21*1000*E50</f>
-        <v>4957.7199999999939</v>
+        <v>4836.7999999999947</v>
       </c>
       <c r="P3" s="56">
         <f>'[1]Financial Model'!$AE$21*1000*E50</f>
-        <v>4696.1399999999985</v>
+        <v>4581.5999999999985</v>
       </c>
       <c r="Q3" s="56">
         <f>'[1]Financial Model'!$AD$21*1000*E50</f>
-        <v>2081.98</v>
+        <v>2031.2</v>
       </c>
       <c r="R3" s="51">
         <f>[1]Main!$C$34</f>
@@ -14414,7 +14424,7 @@
       </c>
       <c r="AE3" s="56">
         <f>[1]Main!$C$26*E50</f>
-        <v>7922.8399999999992</v>
+        <v>7729.6</v>
       </c>
       <c r="AF3" s="53">
         <f>'[1]Financial Model'!$X$72</f>
@@ -14443,7 +14453,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14458,19 +14468,19 @@
       </c>
       <c r="F4" s="7">
         <f>[2]Main!$C$6*$E$50</f>
-        <v>27.240399999999998</v>
+        <v>26.576000000000001</v>
       </c>
       <c r="G4" s="49">
         <f>[2]Main!$C$8*$E$50</f>
-        <v>10560.776195199998</v>
+        <v>10303.196287999999</v>
       </c>
       <c r="H4" s="49">
         <f>[2]Main!$C$11*$E$50</f>
-        <v>-3826.1486999999997</v>
+        <v>-3732.828</v>
       </c>
       <c r="I4" s="49">
         <f>[2]Main!$C$12*$E$50</f>
-        <v>14386.924895199996</v>
+        <v>14036.024287999999</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>[2]Main!$C$28</f>
@@ -14486,15 +14496,15 @@
       </c>
       <c r="O4" s="56">
         <f>'[2]Financial Model'!$AA$22*E50</f>
-        <v>1137.2588199999991</v>
+        <v>1109.5207999999991</v>
       </c>
       <c r="P4" s="56">
         <f>'[2]Financial Model'!$Z$22*$E$50</f>
-        <v>334.43618000000112</v>
+        <v>326.27920000000114</v>
       </c>
       <c r="Q4" s="56">
         <f>'[2]Financial Model'!$Y$22*$E$50</f>
-        <v>557.14818000000014</v>
+        <v>543.55920000000015</v>
       </c>
       <c r="R4" s="51">
         <f>[2]Main!$C$34</f>
@@ -14529,7 +14539,7 @@
       </c>
       <c r="AE4" s="56">
         <f>[2]Main!$C$26*E50</f>
-        <v>1919.9438999999998</v>
+        <v>1873.116</v>
       </c>
       <c r="AF4" s="53">
         <f>'[2]Financial Model'!$T$76</f>
@@ -14555,7 +14565,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14678,7 +14688,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14808,7 +14818,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14938,7 +14948,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -14953,19 +14963,19 @@
       </c>
       <c r="F8" s="7">
         <f>[6]Main!$C$6*E50</f>
-        <v>6.7977999999999987</v>
+        <v>6.6319999999999997</v>
       </c>
       <c r="G8" s="49">
         <f>[6]Main!$C$8*E50</f>
-        <v>3088.3900915999993</v>
+        <v>3013.0635039999997</v>
       </c>
       <c r="H8" s="49">
         <f>[6]Main!$C$11*$E$50</f>
-        <v>147.82140000000007</v>
+        <v>144.21600000000009</v>
       </c>
       <c r="I8" s="49">
         <f>[6]Main!$C$12*$E$50</f>
-        <v>2940.5686915999995</v>
+        <v>2868.8475039999998</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
@@ -14981,15 +14991,15 @@
       </c>
       <c r="O8" s="56">
         <f>'[6]Financial Model'!$AA$20*$E$50</f>
-        <v>-450.32513999999998</v>
+        <v>-439.34160000000003</v>
       </c>
       <c r="P8" s="56">
         <f>'[6]Financial Model'!$Z$20*$E$50</f>
-        <v>75.55643999999937</v>
+        <v>73.713599999999389</v>
       </c>
       <c r="Q8" s="56">
         <f>'[6]Financial Model'!$Y$20*$E$50</f>
-        <v>-37.967640000000323</v>
+        <v>-37.041600000000322</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
@@ -15038,7 +15048,7 @@
       </c>
       <c r="AE8" s="56">
         <f>[6]Main!$C$27*E50</f>
-        <v>885.94439999999997</v>
+        <v>864.33600000000013</v>
       </c>
       <c r="AF8" s="53">
         <f>'[6]Financial Model'!$R$79</f>
@@ -15072,7 +15082,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -15087,19 +15097,19 @@
       </c>
       <c r="F9" s="7">
         <f>[7]Main!$C$6*E50</f>
-        <v>20.9346</v>
+        <v>20.424000000000003</v>
       </c>
       <c r="G9" s="49">
         <f>[7]Main!$C$8*$E$50</f>
-        <v>1929.6291699359999</v>
+        <v>1882.56504384</v>
       </c>
       <c r="H9" s="49">
         <f>[7]Main!$C$11*E50</f>
-        <v>319.01362</v>
+        <v>311.2328</v>
       </c>
       <c r="I9" s="49">
         <f>[7]Main!$C$12*E50</f>
-        <v>1610.615549936</v>
+        <v>1571.33224384</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>[7]Main!$C$29</f>
@@ -15136,7 +15146,7 @@
       </c>
       <c r="AE9" s="56">
         <f>[7]Main!$C$26*E50</f>
-        <v>609.73477999999989</v>
+        <v>594.86320000000001</v>
       </c>
       <c r="AF9" s="53">
         <f>'[7]Financial Model'!$M$63</f>
@@ -15161,7 +15171,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -15176,19 +15186,19 @@
       </c>
       <c r="F10" s="7">
         <f>[8]Main!$C$6*E50</f>
-        <v>10.594399999999998</v>
+        <v>10.336</v>
       </c>
       <c r="G10" s="49">
         <f>[8]Main!$C$8*E50</f>
-        <v>1908.9943415999996</v>
+        <v>1862.4335039999999</v>
       </c>
       <c r="H10" s="49">
         <f>[8]Main!$C$11*$E$50</f>
-        <v>-228.21255999999997</v>
+        <v>-222.6464</v>
       </c>
       <c r="I10" s="49">
         <f>[8]Main!$C$12*$E$50</f>
-        <v>2137.2069015999996</v>
+        <v>2085.0799039999997</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>[8]Main!$C$28</f>
@@ -15208,11 +15218,11 @@
       </c>
       <c r="O10" s="56">
         <f>'[8]Financial Model'!$Z$17*E50</f>
-        <v>344.09331999999989</v>
+        <v>335.7007999999999</v>
       </c>
       <c r="P10" s="56">
         <f>'[8]Financial Model'!$Y$17*F50</f>
-        <v>-255.28902439024415</v>
+        <v>-261.67125000000027</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="52">
@@ -15255,7 +15265,7 @@
       </c>
       <c r="AE10" s="56">
         <f>[8]Main!$C$26*E50</f>
-        <v>563.37771999999995</v>
+        <v>549.63680000000011</v>
       </c>
       <c r="AF10" s="53">
         <f>'[8]Financial Model'!$P$72</f>
@@ -15289,7 +15299,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15429,7 +15439,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15444,19 +15454,19 @@
       </c>
       <c r="F12" s="54">
         <f>[10]Main!$C$6*E50</f>
-        <v>18.548400000000001</v>
+        <v>18.096</v>
       </c>
       <c r="G12" s="49">
         <f>[10]Main!$C$8*E50</f>
-        <v>917.88612239999986</v>
+        <v>895.49865599999998</v>
       </c>
       <c r="H12" s="49">
         <f>[10]Main!$C$11*E50</f>
-        <v>122.06847999999998</v>
+        <v>119.09119999999999</v>
       </c>
       <c r="I12" s="49">
         <f>[10]Main!$C$12*E50</f>
-        <v>795.81764239999984</v>
+        <v>776.40745599999991</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>[10]Main!$C$27</f>
@@ -15477,15 +15487,15 @@
       <c r="N12" s="50"/>
       <c r="O12" s="56">
         <f>'[10]Financial Model'!$X$18*E50</f>
-        <v>215.66819999999976</v>
+        <v>210.40799999999979</v>
       </c>
       <c r="P12" s="56">
         <f>'[10]Financial Model'!$W$18*$E$50</f>
-        <v>-93.497220000000127</v>
+        <v>-91.216800000000134</v>
       </c>
       <c r="Q12" s="56">
         <f>'[10]Financial Model'!$V$18*$E$50</f>
-        <v>32.273560000000501</v>
+        <v>31.486400000000494</v>
       </c>
       <c r="R12" s="52">
         <f>[10]Main!$C$33</f>
@@ -15534,7 +15544,7 @@
       </c>
       <c r="AE12" s="56">
         <f>'[10]Financial Model'!$Q$41*E50</f>
-        <v>608.40965999999992</v>
+        <v>593.57039999999995</v>
       </c>
       <c r="AF12" s="53">
         <f>'[10]Financial Model'!$X$74</f>
@@ -15568,7 +15578,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15693,7 +15703,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15803,7 +15813,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15947,7 +15957,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -16070,7 +16080,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -16169,7 +16179,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -16195,7 +16205,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B19" s="136" t="s">
         <v>582</v>
       </c>
@@ -16226,7 +16236,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B20" s="135" t="s">
         <v>975</v>
       </c>
@@ -16252,7 +16262,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -16276,7 +16286,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16302,7 +16312,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16327,7 +16337,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16342,11 +16352,11 @@
       </c>
       <c r="F24" s="54">
         <f>[16]Main!$C$6*E50</f>
-        <v>271.75619999999998</v>
+        <v>265.12800000000004</v>
       </c>
       <c r="G24" s="56">
         <f>[16]Main!$C$8*E50</f>
-        <v>33235.783259999997</v>
+        <v>32425.154399999999</v>
       </c>
       <c r="H24" s="56">
         <f>[16]Main!$C$11*E50</f>
@@ -16354,7 +16364,7 @@
       </c>
       <c r="I24" s="56">
         <f>[16]Main!$C$12*E50</f>
-        <v>33235.783259999997</v>
+        <v>32425.154399999999</v>
       </c>
       <c r="AK24" s="4">
         <f>[16]Main!$C$24</f>
@@ -16368,7 +16378,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16383,7 +16393,7 @@
       </c>
       <c r="F25" s="54">
         <f>81600*E52</f>
-        <v>489.6</v>
+        <v>505.91999999999996</v>
       </c>
       <c r="G25" s="56"/>
       <c r="H25" s="56"/>
@@ -16401,7 +16411,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
@@ -16427,7 +16437,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16453,7 +16463,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="1"/>
@@ -16463,7 +16473,7 @@
       <c r="M28" s="56"/>
       <c r="N28" s="56"/>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B29" s="136" t="s">
         <v>582</v>
       </c>
@@ -16479,7 +16489,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>511</v>
       </c>
@@ -16494,7 +16504,7 @@
       </c>
       <c r="F30" s="7">
         <f>18.22*E50</f>
-        <v>14.940399999999999</v>
+        <v>14.576000000000001</v>
       </c>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
@@ -16512,7 +16522,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B31" s="3" t="s">
         <v>540</v>
       </c>
@@ -16576,7 +16586,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>541</v>
       </c>
@@ -16603,7 +16613,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>575</v>
       </c>
@@ -16628,7 +16638,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>587</v>
       </c>
@@ -16653,7 +16663,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>588</v>
       </c>
@@ -16678,7 +16688,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
       <c r="H36" s="1"/>
@@ -16688,7 +16698,7 @@
       <c r="M36" s="56"/>
       <c r="N36" s="56"/>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B37" s="136" t="s">
         <v>582</v>
       </c>
@@ -16703,7 +16713,7 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>985</v>
       </c>
@@ -16730,7 +16740,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>579</v>
       </c>
@@ -16751,7 +16761,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>580</v>
       </c>
@@ -16772,7 +16782,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
         <v>581</v>
       </c>
@@ -16787,19 +16797,19 @@
       </c>
       <c r="F41" s="54">
         <f>[18]Main!$C$6*$E$50</f>
-        <v>32.135799999999996</v>
+        <v>31.352</v>
       </c>
       <c r="G41" s="49">
         <f>[18]Main!$C$8*$E$50</f>
-        <v>2998.9265779865996</v>
+        <v>2925.7820273039997</v>
       </c>
       <c r="H41" s="1">
         <f>[18]Main!$C$11*E50</f>
-        <v>-84.46</v>
+        <v>-82.4</v>
       </c>
       <c r="I41" s="56">
         <f>[18]Main!$C$12*E50</f>
-        <v>3083.3865779865996</v>
+        <v>3008.1820273039998</v>
       </c>
       <c r="J41" s="4" t="str">
         <f>[18]Main!$C$30</f>
@@ -16857,7 +16867,7 @@
       </c>
       <c r="AE41" s="56">
         <f>[18]Main!$C$28*E50</f>
-        <v>1381.6999999999998</v>
+        <v>1348</v>
       </c>
       <c r="AF41" s="53">
         <f>'[18]Financial Model'!$U$73</f>
@@ -16890,7 +16900,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>568</v>
       </c>
@@ -16917,7 +16927,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B43" s="3" t="s">
         <v>569</v>
       </c>
@@ -17036,7 +17046,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G44" s="56"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -17045,7 +17055,7 @@
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -17054,7 +17064,7 @@
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G46" s="56"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -17063,7 +17073,7 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G47" s="49"/>
       <c r="I47" s="4"/>
       <c r="J47" s="1"/>
@@ -17071,7 +17081,7 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
@@ -17079,7 +17089,7 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D49" s="154" t="s">
         <v>495</v>
       </c>
@@ -17092,61 +17102,61 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D50" s="43" t="s">
         <v>497</v>
       </c>
       <c r="E50" s="44">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="F50" s="45">
         <f>1/E50</f>
-        <v>1.2195121951219512</v>
+        <v>1.25</v>
       </c>
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D51" s="43" t="s">
         <v>498</v>
       </c>
       <c r="E51" s="44">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="F51" s="45">
         <f>1/E51</f>
-        <v>1.1494252873563218</v>
+        <v>1.1363636363636365</v>
       </c>
       <c r="G51" s="49"/>
       <c r="I51" s="4"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
       <c r="D52" s="46" t="s">
         <v>564</v>
       </c>
       <c r="E52" s="48">
-        <v>6.0000000000000001E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="F52" s="47">
         <f>1/E52</f>
-        <v>166.66666666666666</v>
+        <v>161.29032258064515</v>
       </c>
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G56" s="49"/>
     </row>
   </sheetData>
@@ -17197,21 +17207,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -17222,7 +17232,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -17249,98 +17259,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
Add 8022 Mizuno Corporation to Fashion backlog
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519E78A-CA2D-8C46-B521-ADAD8900ED75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4687553-CE2C-8A4A-A197-EE17C8AFE9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="1019">
   <si>
     <t>Ticker</t>
   </si>
@@ -3198,6 +3198,12 @@
   </si>
   <si>
     <t>Dr. Martens, Griggs</t>
+  </si>
+  <si>
+    <t>Mizuno Corporation</t>
+  </si>
+  <si>
+    <t>Osaka, Japan</t>
   </si>
 </sst>
 </file>
@@ -3563,7 +3569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3963,9 +3969,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5089,7 +5092,7 @@
             <v>Q322</v>
           </cell>
           <cell r="D30">
-            <v>43405</v>
+            <v>45248</v>
           </cell>
         </row>
         <row r="35">
@@ -5845,12 +5848,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>8.2899999999999991</v>
+            <v>10.33</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>3766.3293799999997</v>
+            <v>4693.1462600000004</v>
           </cell>
         </row>
         <row r="11">
@@ -5860,7 +5863,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>3586.0593799999997</v>
+            <v>4512.87626</v>
           </cell>
         </row>
         <row r="23">
@@ -5893,12 +5896,12 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>24.790599499495396</v>
+            <v>31.197728787313238</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>26.576806095253207</v>
+            <v>33.116816280333616</v>
           </cell>
         </row>
         <row r="36">
@@ -5908,12 +5911,12 @@
         </row>
         <row r="37">
           <cell r="C37">
-            <v>2.1978320161703082</v>
+            <v>2.7386736703304329</v>
           </cell>
         </row>
         <row r="41">
           <cell r="C41">
-            <v>10.717736377270443</v>
+            <v>13.355152807865343</v>
           </cell>
         </row>
       </sheetData>
@@ -14087,13 +14090,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AO56"/>
+  <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14122,31 +14125,31 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="156" t="s">
+      <c r="F1" s="155" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156"/>
-      <c r="M1" s="156"/>
-      <c r="N1" s="156"/>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
+      <c r="L1" s="155"/>
+      <c r="M1" s="155"/>
+      <c r="N1" s="155"/>
+      <c r="O1" s="155"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="155"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
-        <v>14.953293230057294</v>
+        <v>15.54783961051915</v>
       </c>
       <c r="S1" s="98">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.123110370046593</v>
+        <v>13.386852013106079</v>
       </c>
       <c r="T1" s="98">
         <f>AVERAGE(T3:T17)</f>
-        <v>2.7642101449543128</v>
+        <v>2.8002662552316551</v>
       </c>
       <c r="U1" s="111">
         <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
@@ -14341,19 +14344,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$50</f>
+        <f>[1]Main!$C$6*$E$51</f>
         <v>92.48</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$50</f>
+        <f>[1]Main!$C$8*$E$51</f>
         <v>144176.32000000001</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$50</f>
+        <f>[1]Main!$C$11*$E$51</f>
         <v>952</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$50</f>
+        <f>[1]Main!$C$12*$E$51</f>
         <v>143224.32000000001</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -14369,15 +14372,15 @@
         <v>29.611379424412871</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AF$21*1000*E50</f>
+        <f>'[1]Financial Model'!$AF$21*1000*E51</f>
         <v>4836.7999999999947</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AE$21*1000*E50</f>
+        <f>'[1]Financial Model'!$AE$21*1000*E51</f>
         <v>4581.5999999999985</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E50</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E51</f>
         <v>2031.2</v>
       </c>
       <c r="R3" s="51">
@@ -14423,7 +14426,7 @@
         <v>0.19333333333333316</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E50</f>
+        <f>[1]Main!$C$26*E51</f>
         <v>7729.6</v>
       </c>
       <c r="AF3" s="53">
@@ -14467,19 +14470,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$50</f>
+        <f>[2]Main!$C$6*$E$51</f>
         <v>26.576000000000001</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$50</f>
+        <f>[2]Main!$C$8*$E$51</f>
         <v>10303.196287999999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$50</f>
+        <f>[2]Main!$C$11*$E$51</f>
         <v>-3732.828</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$50</f>
+        <f>[2]Main!$C$12*$E$51</f>
         <v>14036.024287999999</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -14495,15 +14498,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E50</f>
+        <f>'[2]Financial Model'!$AA$22*E51</f>
         <v>1109.5207999999991</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$50</f>
+        <f>'[2]Financial Model'!$Z$22*$E$51</f>
         <v>326.27920000000114</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$50</f>
+        <f>'[2]Financial Model'!$Y$22*$E$51</f>
         <v>543.55920000000015</v>
       </c>
       <c r="R4" s="51">
@@ -14538,7 +14541,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E50</f>
+        <f>[2]Main!$C$26*E51</f>
         <v>1873.116</v>
       </c>
       <c r="AF4" s="53">
@@ -14962,20 +14965,20 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E50</f>
-        <v>6.6319999999999997</v>
+        <f>[6]Main!$C$6*E51</f>
+        <v>8.2640000000000011</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E50</f>
-        <v>3013.0635039999997</v>
+        <f>[6]Main!$C$8*E51</f>
+        <v>3754.5170080000007</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$50</f>
+        <f>[6]Main!$C$11*$E$51</f>
         <v>144.21600000000009</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$50</f>
-        <v>2868.8475039999998</v>
+        <f>[6]Main!$C$12*$E$51</f>
+        <v>3610.3010080000004</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>[6]Main!$C$29</f>
@@ -14987,31 +14990,31 @@
       </c>
       <c r="L8" s="50">
         <f>[6]Main!$C$34</f>
-        <v>24.790599499495396</v>
+        <v>31.197728787313238</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$50</f>
+        <f>'[6]Financial Model'!$AA$20*$E$51</f>
         <v>-439.34160000000003</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$50</f>
+        <f>'[6]Financial Model'!$Z$20*$E$51</f>
         <v>73.713599999999389</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$50</f>
+        <f>'[6]Financial Model'!$Y$20*$E$51</f>
         <v>-37.041600000000322</v>
       </c>
       <c r="R8" s="52">
         <f>[6]Main!$C$35</f>
-        <v>26.576806095253207</v>
+        <v>33.116816280333616</v>
       </c>
       <c r="S8" s="52">
         <f>[6]Main!$C$41</f>
-        <v>10.717736377270443</v>
+        <v>13.355152807865343</v>
       </c>
       <c r="T8" s="52">
         <f>[6]Main!$C$37</f>
-        <v>2.1978320161703082</v>
+        <v>2.7386736703304329</v>
       </c>
       <c r="U8" s="131">
         <f>[6]Main!$C$36</f>
@@ -15047,7 +15050,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E50</f>
+        <f>[6]Main!$C$27*E51</f>
         <v>864.33600000000013</v>
       </c>
       <c r="AF8" s="53">
@@ -15096,19 +15099,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E50</f>
+        <f>[7]Main!$C$6*E51</f>
         <v>20.424000000000003</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$50</f>
+        <f>[7]Main!$C$8*$E$51</f>
         <v>1882.56504384</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E50</f>
+        <f>[7]Main!$C$11*E51</f>
         <v>311.2328</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E50</f>
+        <f>[7]Main!$C$12*E51</f>
         <v>1571.33224384</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -15145,7 +15148,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E50</f>
+        <f>[7]Main!$C$26*E51</f>
         <v>594.86320000000001</v>
       </c>
       <c r="AF9" s="53">
@@ -15185,19 +15188,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E50</f>
+        <f>[8]Main!$C$6*E51</f>
         <v>10.336</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E50</f>
+        <f>[8]Main!$C$8*E51</f>
         <v>1862.4335039999999</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$50</f>
+        <f>[8]Main!$C$11*$E$51</f>
         <v>-222.6464</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$50</f>
+        <f>[8]Main!$C$12*$E$51</f>
         <v>2085.0799039999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -15217,11 +15220,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E50</f>
+        <f>'[8]Financial Model'!$Z$17*E51</f>
         <v>335.7007999999999</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F50</f>
+        <f>'[8]Financial Model'!$Y$17*F51</f>
         <v>-261.67125000000027</v>
       </c>
       <c r="Q10" s="4"/>
@@ -15264,7 +15267,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E50</f>
+        <f>[8]Main!$C$26*E51</f>
         <v>549.63680000000011</v>
       </c>
       <c r="AF10" s="53">
@@ -15453,19 +15456,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E50</f>
+        <f>[10]Main!$C$6*E51</f>
         <v>18.096</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E50</f>
+        <f>[10]Main!$C$8*E51</f>
         <v>895.49865599999998</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E50</f>
+        <f>[10]Main!$C$11*E51</f>
         <v>119.09119999999999</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E50</f>
+        <f>[10]Main!$C$12*E51</f>
         <v>776.40745599999991</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -15486,15 +15489,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E50</f>
+        <f>'[10]Financial Model'!$X$18*E51</f>
         <v>210.40799999999979</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$50</f>
+        <f>'[10]Financial Model'!$W$18*$E$51</f>
         <v>-91.216800000000134</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$50</f>
+        <f>'[10]Financial Model'!$V$18*$E$51</f>
         <v>31.486400000000494</v>
       </c>
       <c r="R12" s="52">
@@ -15543,7 +15546,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E50</f>
+        <f>'[10]Financial Model'!$Q$41*E51</f>
         <v>593.57039999999995</v>
       </c>
       <c r="AF12" s="53">
@@ -16351,19 +16354,19 @@
         <v>505</v>
       </c>
       <c r="F24" s="54">
-        <f>[16]Main!$C$6*E50</f>
+        <f>[16]Main!$C$6*E51</f>
         <v>265.12800000000004</v>
       </c>
       <c r="G24" s="56">
-        <f>[16]Main!$C$8*E50</f>
+        <f>[16]Main!$C$8*E51</f>
         <v>32425.154399999999</v>
       </c>
       <c r="H24" s="56">
-        <f>[16]Main!$C$11*E50</f>
+        <f>[16]Main!$C$11*E51</f>
         <v>0</v>
       </c>
       <c r="I24" s="56">
-        <f>[16]Main!$C$12*E50</f>
+        <f>[16]Main!$C$12*E51</f>
         <v>32425.154399999999</v>
       </c>
       <c r="AK24" s="4">
@@ -16392,7 +16395,7 @@
         <v>565</v>
       </c>
       <c r="F25" s="54">
-        <f>81600*E52</f>
+        <f>81600*E53</f>
         <v>505.91999999999996</v>
       </c>
       <c r="G25" s="56"/>
@@ -16464,22 +16467,43 @@
       </c>
     </row>
     <row r="28" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
+      <c r="B28" s="135">
+        <v>8022</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F28" s="54">
+        <f>2769*E53</f>
+        <v>17.1678</v>
+      </c>
+      <c r="G28" s="56">
+        <v>25.55</v>
+      </c>
+      <c r="H28" s="56">
+        <v>0</v>
+      </c>
+      <c r="I28" s="56">
+        <f>F28*G28</f>
+        <v>438.63729000000001</v>
+      </c>
+      <c r="AK28" s="4">
+        <v>1906</v>
+      </c>
+      <c r="AL28" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="AM28" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="29" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B29" s="136" t="s">
-        <v>582</v>
-      </c>
-      <c r="C29" s="133" t="s">
-        <v>554</v>
-      </c>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="1"/>
@@ -16490,143 +16514,134 @@
       <c r="N29" s="56"/>
     </row>
     <row r="30" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B30" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="F30" s="7">
-        <f>18.22*E50</f>
-        <v>14.576000000000001</v>
+      <c r="B30" s="136" t="s">
+        <v>582</v>
+      </c>
+      <c r="C30" s="133" t="s">
+        <v>554</v>
       </c>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
-      <c r="I30" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>490</v>
-      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="56"/>
       <c r="M30" s="56"/>
       <c r="N30" s="56"/>
-      <c r="AM30" s="4" t="s">
+    </row>
+    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B31" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F31" s="7">
+        <f>18.22*E51</f>
+        <v>14.576000000000001</v>
+      </c>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="AM31" s="4" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B31" s="3" t="s">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B32" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="54">
+      <c r="F32" s="54">
         <f>[17]Main!$C$6</f>
         <v>20.806000000000001</v>
       </c>
-      <c r="G31" s="56">
+      <c r="G32" s="56">
         <f>[17]Main!$C$8</f>
         <v>8041.1028800000004</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="56">
+      <c r="H32" s="1"/>
+      <c r="I32" s="56">
         <f>[17]Main!$C$12</f>
         <v>8041.1028800000004</v>
       </c>
-      <c r="J31" s="4" t="str">
+      <c r="J32" s="4" t="str">
         <f>[17]Main!$C$29</f>
         <v>H122</v>
       </c>
-      <c r="K31" s="85">
+      <c r="K32" s="85">
         <f>[17]Main!$D$29</f>
         <v>44882</v>
       </c>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="Z31" s="53">
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="Z32" s="53">
         <f>'[17]Financial Model'!$K$28</f>
         <v>0.70111524163568772</v>
       </c>
-      <c r="AA31" s="53">
+      <c r="AA32" s="53">
         <f>'[17]Financial Model'!$K$29</f>
         <v>0.19553903345724907</v>
       </c>
-      <c r="AB31" s="53">
+      <c r="AB32" s="53">
         <f>'[17]Financial Model'!$K$30</f>
         <v>0.14423791821561338</v>
       </c>
-      <c r="AC31" s="53">
+      <c r="AC32" s="53">
         <f>'[17]Financial Model'!$K$31</f>
         <v>0.22709163346613545</v>
       </c>
-      <c r="AK31" s="4">
+      <c r="AK32" s="4">
         <f>[17]Main!$C$24</f>
         <v>1856</v>
       </c>
-      <c r="AL31" s="4" t="str">
+      <c r="AL32" s="4" t="str">
         <f>[17]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AM31" s="4" t="s">
+      <c r="AM32" s="4" t="s">
         <v>552</v>
-      </c>
-    </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B32" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="7">
-        <v>2.9</v>
-      </c>
-      <c r="G32" s="56"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="AM32" s="4" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="33" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>575</v>
+        <v>541</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>574</v>
+        <v>542</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>573</v>
+        <v>489</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2.9</v>
+      </c>
       <c r="G33" s="56"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -16635,18 +16650,18 @@
       <c r="M33" s="56"/>
       <c r="N33" s="56"/>
       <c r="AM33" s="4" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="34" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>266</v>
+        <v>574</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>31</v>
+        <v>573</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>578</v>
@@ -16665,10 +16680,10 @@
     </row>
     <row r="35" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>31</v>
@@ -16689,6 +16704,18 @@
       </c>
     </row>
     <row r="36" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>578</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
       <c r="H36" s="1"/>
@@ -16697,14 +16724,12 @@
       <c r="K36" s="1"/>
       <c r="M36" s="56"/>
       <c r="N36" s="56"/>
+      <c r="AM36" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="37" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B37" s="136" t="s">
-        <v>582</v>
-      </c>
-      <c r="C37" s="133" t="s">
-        <v>567</v>
-      </c>
+      <c r="F37" s="7"/>
       <c r="G37" s="56"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -16714,17 +16739,11 @@
       <c r="N37" s="56"/>
     </row>
     <row r="38" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B38" s="1" t="s">
-        <v>985</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>505</v>
+      <c r="B38" s="136" t="s">
+        <v>582</v>
+      </c>
+      <c r="C38" s="133" t="s">
+        <v>567</v>
       </c>
       <c r="G38" s="56"/>
       <c r="H38" s="1"/>
@@ -16733,19 +16752,19 @@
       <c r="K38" s="1"/>
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
-      <c r="AM38" s="4" t="s">
-        <v>987</v>
-      </c>
-      <c r="AN38" s="4" t="s">
-        <v>988</v>
-      </c>
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>579</v>
+        <v>985</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>584</v>
+        <v>986</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>505</v>
       </c>
       <c r="G39" s="56"/>
       <c r="H39" s="1"/>
@@ -16755,18 +16774,18 @@
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
       <c r="AM39" s="4" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
       <c r="AN39" s="4" t="s">
-        <v>1014</v>
+        <v>988</v>
       </c>
     </row>
     <row r="40" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G40" s="56"/>
       <c r="H40" s="1"/>
@@ -16776,284 +16795,296 @@
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
       <c r="AM40" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="AN40" s="4" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B41" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="G41" s="56"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+      <c r="AM41" s="4" t="s">
         <v>981</v>
       </c>
-      <c r="AN40" s="4" t="s">
+      <c r="AN41" s="4" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="F41" s="54">
-        <f>[18]Main!$C$6*$E$50</f>
+      <c r="F42" s="54">
+        <f>[18]Main!$C$6*$E$51</f>
         <v>31.352</v>
       </c>
-      <c r="G41" s="49">
-        <f>[18]Main!$C$8*$E$50</f>
+      <c r="G42" s="49">
+        <f>[18]Main!$C$8*$E$51</f>
         <v>2925.7820273039997</v>
       </c>
-      <c r="H41" s="1">
-        <f>[18]Main!$C$11*E50</f>
+      <c r="H42" s="1">
+        <f>[18]Main!$C$11*E51</f>
         <v>-82.4</v>
       </c>
-      <c r="I41" s="56">
-        <f>[18]Main!$C$12*E50</f>
+      <c r="I42" s="56">
+        <f>[18]Main!$C$12*E51</f>
         <v>3008.1820273039998</v>
       </c>
-      <c r="J41" s="4" t="str">
+      <c r="J42" s="4" t="str">
         <f>[18]Main!$C$30</f>
         <v>Q322</v>
       </c>
-      <c r="K41" s="153">
+      <c r="K42" s="85">
         <f>[18]Main!$D$30</f>
-        <v>43405</v>
-      </c>
-      <c r="L41" s="50">
+        <v>45248</v>
+      </c>
+      <c r="L42" s="50">
         <f>[18]Main!$C$39</f>
         <v>8.8684611654009426</v>
       </c>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-      <c r="O41" s="56">
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56">
         <f>'[18]Financial Model'!$AH$17</f>
         <v>892</v>
       </c>
-      <c r="P41" s="56">
+      <c r="P42" s="56">
         <f>'[18]Financial Model'!$AG$17</f>
         <v>323</v>
       </c>
-      <c r="R41" s="51">
+      <c r="R42" s="51">
         <f>[18]Main!$C$38</f>
         <v>8.9160063090667094</v>
       </c>
-      <c r="S41" s="51">
+      <c r="S42" s="51">
         <f>'[18]Financial Model'!$AH$84</f>
         <v>4.844618834080717</v>
       </c>
-      <c r="T41" s="51">
+      <c r="T42" s="51">
         <f>[18]Main!$C$35</f>
         <v>1.1231500460263886</v>
       </c>
-      <c r="W41" s="53">
+      <c r="W42" s="53">
         <f>'[18]Financial Model'!$AH$21</f>
         <v>0.18680445151033376</v>
       </c>
-      <c r="Z41" s="53">
+      <c r="Z42" s="53">
         <f>'[18]Financial Model'!$U$26</f>
         <v>0.32029452369995398</v>
       </c>
-      <c r="AA41" s="53">
+      <c r="AA42" s="53">
         <f>'[18]Financial Model'!$U$27</f>
         <v>7.2250345144960884E-2</v>
       </c>
-      <c r="AB41" s="53">
+      <c r="AB42" s="53">
         <f>'[18]Financial Model'!$U$28</f>
         <v>4.4178554993097099E-2</v>
       </c>
-      <c r="AC41" s="53">
+      <c r="AC42" s="53">
         <f>'[18]Financial Model'!$U$29</f>
         <v>0.32867132867132864</v>
       </c>
-      <c r="AE41" s="56">
-        <f>[18]Main!$C$28*E50</f>
+      <c r="AE42" s="56">
+        <f>[18]Main!$C$28*E51</f>
         <v>1348</v>
       </c>
-      <c r="AF41" s="53">
+      <c r="AF42" s="53">
         <f>'[18]Financial Model'!$U$73</f>
         <v>0.29515757109915453</v>
       </c>
-      <c r="AG41" s="53">
+      <c r="AG42" s="53">
         <f>'[18]Financial Model'!$U$74</f>
         <v>2.4939172749391725E-2</v>
       </c>
-      <c r="AH41" s="53">
+      <c r="AH42" s="53">
         <f>'[18]Financial Model'!$U$75</f>
         <v>0.19248343614347727</v>
       </c>
-      <c r="AI41" s="57">
+      <c r="AI42" s="57">
         <f>[18]Main!$C$27</f>
         <v>2794</v>
       </c>
-      <c r="AK41" s="4">
+      <c r="AK42" s="4">
         <f>[18]Main!$C$24</f>
         <v>1879</v>
       </c>
-      <c r="AL41" s="4" t="str">
+      <c r="AL42" s="4" t="str">
         <f>[18]Main!$C$23</f>
         <v>NYC, NY</v>
       </c>
-      <c r="AM41" s="4" t="s">
+      <c r="AM42" s="4" t="s">
         <v>978</v>
       </c>
-      <c r="AN41" s="4" t="s">
+      <c r="AN42" s="4" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B42" s="1" t="s">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B43" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="56"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="AM42" s="4" t="s">
-        <v>980</v>
-      </c>
-      <c r="AN42" s="4" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="B43" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>489</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="54">
+      <c r="G43" s="56"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="AM43" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="AN43" s="4" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
+      <c r="B44" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="54">
         <f>[19]Main!$C$6</f>
         <v>2.4049999999999998</v>
       </c>
-      <c r="G43" s="56">
+      <c r="G44" s="56">
         <f>[19]Main!$C$8</f>
         <v>120.24999999999999</v>
       </c>
-      <c r="H43" s="56">
+      <c r="H44" s="56">
         <f>[19]Main!$C$11</f>
         <v>13.872</v>
       </c>
-      <c r="I43" s="56">
+      <c r="I44" s="56">
         <f>[19]Main!$C$12</f>
         <v>106.37799999999999</v>
       </c>
-      <c r="J43" s="4" t="str">
+      <c r="J44" s="4" t="str">
         <f>[19]Main!$C$29</f>
         <v>H122</v>
       </c>
-      <c r="K43" s="85">
+      <c r="K44" s="85">
         <f>[19]Main!$D$29</f>
         <v>45063</v>
       </c>
-      <c r="L43" s="50">
+      <c r="L44" s="50">
         <f>[19]Main!$C$38</f>
         <v>8.8692679673169916</v>
       </c>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
-      <c r="O43" s="56">
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56">
         <f>'[19]Financial Model'!$T$16</f>
         <v>7.0139999999999958</v>
       </c>
-      <c r="P43" s="56">
+      <c r="P44" s="56">
         <f>'[19]Financial Model'!$S$16</f>
         <v>-11.902999999999997</v>
       </c>
-      <c r="Q43" s="56">
+      <c r="Q44" s="56">
         <f>'[19]Financial Model'!$R$17</f>
         <v>0</v>
       </c>
-      <c r="R43" s="51">
+      <c r="R44" s="51">
         <f>[19]Main!$C$37</f>
         <v>10.025846256461564</v>
       </c>
-      <c r="S43" s="51">
+      <c r="S44" s="51">
         <f>'[19]Financial Model'!$T$83</f>
         <v>4.5587396635300852</v>
       </c>
-      <c r="T43" s="51">
+      <c r="T44" s="51">
         <f>[19]Main!$C$34</f>
         <v>4.0893015030946032</v>
       </c>
-      <c r="W43" s="53">
+      <c r="W44" s="53">
         <f>'[19]Financial Model'!$T$21</f>
         <v>-2.7951830820442503E-2</v>
       </c>
-      <c r="Z43" s="53">
+      <c r="Z44" s="53">
         <f>'[19]Financial Model'!$K$26</f>
         <v>0.19490724836825837</v>
       </c>
-      <c r="AA43" s="53">
+      <c r="AA44" s="53">
         <f>'[19]Financial Model'!$K$27</f>
         <v>5.2401809229359962E-2</v>
       </c>
-      <c r="AB43" s="53">
+      <c r="AB44" s="53">
         <f>'[19]Financial Model'!$K$28</f>
         <v>4.1008244589488214E-2</v>
       </c>
-      <c r="AC43" s="53">
+      <c r="AC44" s="53">
         <f>'[19]Financial Model'!$K$29</f>
         <v>6.4337034617896707E-2</v>
       </c>
-      <c r="AE43" s="56">
+      <c r="AE44" s="56">
         <f>[19]Main!$C$27</f>
         <v>31.096</v>
       </c>
-      <c r="AF43" s="53">
+      <c r="AF44" s="53">
         <f>'[19]Financial Model'!$K$72</f>
         <v>9.3658776773467567E-2</v>
       </c>
-      <c r="AG43" s="53">
+      <c r="AG44" s="53">
         <f>'[19]Financial Model'!$K$73</f>
         <v>0.23735625323305887</v>
       </c>
-      <c r="AH43" s="53">
+      <c r="AH44" s="53">
         <f>'[19]Financial Model'!$K$74</f>
         <v>0.20930060375174159</v>
       </c>
-      <c r="AI43" s="4">
+      <c r="AI44" s="4">
         <f>[19]Main!$C$25</f>
         <v>388</v>
       </c>
-      <c r="AK43" s="4">
+      <c r="AK44" s="4">
         <f>[19]Main!$C$24</f>
         <v>1917</v>
       </c>
-      <c r="AL43" s="4" t="str">
+      <c r="AL44" s="4" t="str">
         <f>[19]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
-      <c r="AM43" s="4" t="s">
+      <c r="AM44" s="4" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="G44" s="56"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G45" s="56"/>
@@ -17074,8 +17105,9 @@
       <c r="N46" s="56"/>
     </row>
     <row r="47" spans="2:40" x14ac:dyDescent="0.15">
-      <c r="G47" s="49"/>
-      <c r="I47" s="4"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="M47" s="56"/>
@@ -17089,79 +17121,87 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D49" s="154" t="s">
-        <v>495</v>
-      </c>
-      <c r="E49" s="155"/>
-      <c r="F49" s="42" t="s">
-        <v>496</v>
-      </c>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D50" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E50" s="44">
-        <v>0.8</v>
-      </c>
-      <c r="F50" s="45">
-        <f>1/E50</f>
-        <v>1.25</v>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D50" s="153" t="s">
+        <v>495</v>
+      </c>
+      <c r="E50" s="154"/>
+      <c r="F50" s="42" t="s">
+        <v>496</v>
       </c>
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D51" s="43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E51" s="44">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="F51" s="45">
         <f>1/E51</f>
-        <v>1.1363636363636365</v>
+        <v>1.25</v>
       </c>
       <c r="G51" s="49"/>
       <c r="I51" s="4"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D52" s="46" t="s">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D52" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E52" s="44">
+        <v>0.88</v>
+      </c>
+      <c r="F52" s="45">
+        <f>1/E52</f>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="G52" s="49"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D53" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="E52" s="48">
+      <c r="E53" s="48">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="F52" s="47">
-        <f>1/E52</f>
+      <c r="F53" s="47">
+        <f>1/E53</f>
         <v>161.29032258064515</v>
       </c>
-      <c r="G52" s="49"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.15">
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G56" s="49"/>
+    </row>
+    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="G57" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>
@@ -17179,14 +17219,14 @@
     <hyperlink ref="B11" r:id="rId12" xr:uid="{C5D52FC8-A5DA-4E8D-95C5-8F2FEDCE57A7}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{F6AD6AD9-5D37-406B-868D-B0E7E41FA1D2}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{BAC6CF45-03B1-5841-BFC0-D0179DCFA24C}"/>
-    <hyperlink ref="B31" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
+    <hyperlink ref="B32" r:id="rId15" xr:uid="{CA134008-3168-4DEA-918C-4560BFF458AB}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{183ACAEF-5A70-4D85-94EE-2D4C25FF95CC}"/>
     <hyperlink ref="B24" r:id="rId17" xr:uid="{226F06AA-680C-4ED4-9C60-0E27D3777D9C}"/>
-    <hyperlink ref="B37" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
-    <hyperlink ref="B29" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
+    <hyperlink ref="B38" r:id="rId18" xr:uid="{4EB45FA7-C446-BB41-AE63-80350FA95328}"/>
+    <hyperlink ref="B30" r:id="rId19" xr:uid="{985B34CB-3468-8842-8DCE-6868BEDADF1C}"/>
     <hyperlink ref="B19" r:id="rId20" xr:uid="{8B27DD55-F39A-E042-A7A2-82BE3E8447D7}"/>
-    <hyperlink ref="B43" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
-    <hyperlink ref="B41" r:id="rId22" xr:uid="{FD9CE6D1-58BD-4F93-B596-F3E2DED3874C}"/>
+    <hyperlink ref="B44" r:id="rId21" xr:uid="{DA29334E-4505-4032-AE0E-2DE4183961E1}"/>
+    <hyperlink ref="B42" r:id="rId22" xr:uid="{FD9CE6D1-58BD-4F93-B596-F3E2DED3874C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId23"/>

</xml_diff>

<commit_message>
£SHOE NPV and first forecast
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4687553-CE2C-8A4A-A197-EE17C8AFE9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8921BD7-F1BD-4C23-A7DC-27C8235E2E08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -45,22 +45,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -68,7 +58,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -77,42 +67,42 @@
   <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
@@ -3211,14 +3201,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3569,7 +3559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3661,7 +3651,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3670,13 +3660,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3705,16 +3695,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3723,12 +3713,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3765,7 +3755,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3783,7 +3773,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3804,7 +3794,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3831,15 +3821,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3848,7 +3838,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3859,16 +3849,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3903,7 +3893,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3915,7 +3905,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3950,7 +3940,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3976,6 +3966,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4674,8 +4667,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5183,12 +5176,17 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>2.4049999999999998</v>
+            <v>2.2280000000000002</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="W7">
+            <v>4.433098591549296</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>120.24999999999999</v>
+            <v>111.4</v>
           </cell>
         </row>
         <row r="11">
@@ -5198,7 +5196,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>106.37799999999999</v>
+            <v>97.528000000000006</v>
           </cell>
         </row>
         <row r="23">
@@ -5231,22 +5229,25 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>4.0893015030946032</v>
+            <v>3.7883425151329635</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>10.025846256461564</v>
+            <v>9.2879773219943313</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>8.8692679673169916</v>
+            <v>8.1313990328497585</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="16">
+          <cell r="R16">
+            <v>5.7139999999999933</v>
+          </cell>
           <cell r="S16">
             <v>-11.902999999999997</v>
           </cell>
@@ -5255,6 +5256,12 @@
           </cell>
         </row>
         <row r="21">
+          <cell r="R21">
+            <v>8.9157301621889395E-3</v>
+          </cell>
+          <cell r="S21">
+            <v>-0.24362684900059861</v>
+          </cell>
           <cell r="T21">
             <v>-2.7951830820442503E-2</v>
           </cell>
@@ -5279,28 +5286,28 @@
             <v>6.4337034617896707E-2</v>
           </cell>
         </row>
-        <row r="72">
-          <cell r="K72">
-            <v>9.3658776773467567E-2</v>
-          </cell>
-        </row>
         <row r="73">
           <cell r="K73">
-            <v>0.23735625323305887</v>
+            <v>9.3658776773467567E-2</v>
           </cell>
         </row>
         <row r="74">
           <cell r="K74">
+            <v>0.23735625323305887</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="K75">
             <v>0.20930060375174159</v>
           </cell>
         </row>
-        <row r="83">
-          <cell r="T83">
+        <row r="84">
+          <cell r="T84">
             <v>4.5587396635300852</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6764,25 +6771,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6824,7 +6831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6868,7 +6875,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6912,7 +6919,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6956,7 +6963,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -7000,7 +7007,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -7044,7 +7051,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -7088,7 +7095,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -7132,7 +7139,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -7176,7 +7183,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -7220,7 +7227,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -7264,7 +7271,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -7308,7 +7315,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -7352,7 +7359,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7396,7 +7403,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7440,7 +7447,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7484,7 +7491,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7528,7 +7535,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7572,7 +7579,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7616,7 +7623,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7660,7 +7667,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7704,7 +7711,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7748,7 +7755,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7792,7 +7799,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7836,7 +7843,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7880,7 +7887,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7924,7 +7931,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -7968,7 +7975,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -8012,7 +8019,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -8056,7 +8063,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -8100,7 +8107,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -8144,7 +8151,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -8188,7 +8195,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -8232,7 +8239,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -8276,7 +8283,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -8320,7 +8327,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8364,7 +8371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8408,7 +8415,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8452,7 +8459,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8496,7 +8503,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8540,7 +8547,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8584,7 +8591,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8628,7 +8635,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8672,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8790,25 +8797,25 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8850,7 +8857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8894,7 +8901,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8938,7 +8945,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -8982,7 +8989,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -9026,7 +9033,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -9070,7 +9077,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -9114,7 +9121,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -9158,7 +9165,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -9202,7 +9209,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -9246,7 +9253,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -9290,7 +9297,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -9334,7 +9341,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9378,7 +9385,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9422,7 +9429,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9466,7 +9473,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9510,7 +9517,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9554,7 +9561,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9598,7 +9605,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9642,7 +9649,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9686,7 +9693,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9730,7 +9737,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9774,7 +9781,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9818,7 +9825,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9862,7 +9869,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9906,7 +9913,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9950,7 +9957,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -9994,7 +10001,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -10038,7 +10045,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -10082,7 +10089,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -10126,7 +10133,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -10170,7 +10177,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -10214,7 +10221,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -10258,7 +10265,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -10302,7 +10309,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -10346,7 +10353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10390,7 +10397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10434,7 +10441,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10546,16 +10553,16 @@
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10597,7 +10604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="150" t="s">
         <v>589</v>
       </c>
@@ -10641,7 +10648,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="150" t="s">
         <v>589</v>
       </c>
@@ -10685,7 +10692,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="150" t="s">
         <v>597</v>
       </c>
@@ -10729,7 +10736,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="150" t="s">
         <v>604</v>
       </c>
@@ -10773,7 +10780,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="150" t="s">
         <v>608</v>
       </c>
@@ -10817,7 +10824,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="150" t="s">
         <v>614</v>
       </c>
@@ -10861,7 +10868,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
         <v>619</v>
       </c>
@@ -10905,7 +10912,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
         <v>622</v>
       </c>
@@ -10949,7 +10956,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="150" t="s">
         <v>627</v>
       </c>
@@ -10993,7 +11000,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="150" t="s">
         <v>632</v>
       </c>
@@ -11037,7 +11044,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="150" t="s">
         <v>635</v>
       </c>
@@ -11081,7 +11088,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="150" t="s">
         <v>641</v>
       </c>
@@ -11125,7 +11132,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="150" t="s">
         <v>646</v>
       </c>
@@ -11169,7 +11176,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="150" t="s">
         <v>652</v>
       </c>
@@ -11213,7 +11220,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -11257,7 +11264,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="150" t="s">
         <v>661</v>
       </c>
@@ -11301,7 +11308,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="150" t="s">
         <v>666</v>
       </c>
@@ -11345,7 +11352,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="150" t="s">
         <v>666</v>
       </c>
@@ -11389,7 +11396,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="150" t="s">
         <v>678</v>
       </c>
@@ -11433,7 +11440,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="150" t="s">
         <v>684</v>
       </c>
@@ -11477,7 +11484,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="150" t="s">
         <v>690</v>
       </c>
@@ -11521,7 +11528,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="150" t="s">
         <v>696</v>
       </c>
@@ -11565,7 +11572,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="150" t="s">
         <v>699</v>
       </c>
@@ -11609,7 +11616,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11653,7 +11660,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11697,7 +11704,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="150" t="s">
         <v>714</v>
       </c>
@@ -11741,7 +11748,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="150" t="s">
         <v>720</v>
       </c>
@@ -11785,7 +11792,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11829,7 +11836,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="150" t="s">
         <v>731</v>
       </c>
@@ -11873,7 +11880,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11917,7 +11924,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="150" t="s">
         <v>741</v>
       </c>
@@ -11961,7 +11968,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="150" t="s">
         <v>747</v>
       </c>
@@ -12005,7 +12012,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="150" t="s">
         <v>752</v>
       </c>
@@ -12049,7 +12056,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -12094,7 +12101,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="150" t="s">
         <v>762</v>
       </c>
@@ -12138,7 +12145,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -12182,7 +12189,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="150" t="s">
         <v>773</v>
       </c>
@@ -12226,7 +12233,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="150" t="s">
         <v>779</v>
       </c>
@@ -12270,7 +12277,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="150" t="s">
         <v>785</v>
       </c>
@@ -12314,7 +12321,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="150" t="s">
         <v>790</v>
       </c>
@@ -12358,7 +12365,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12402,7 +12409,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="150" t="s">
         <v>800</v>
       </c>
@@ -12446,7 +12453,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12490,7 +12497,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12534,7 +12541,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12579,7 +12586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12623,7 +12630,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="150" t="s">
         <v>824</v>
       </c>
@@ -12667,7 +12674,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12711,7 +12718,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="150" t="s">
         <v>835</v>
       </c>
@@ -12755,7 +12762,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="150" t="s">
         <v>824</v>
       </c>
@@ -12799,7 +12806,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="152" t="s">
         <v>845</v>
       </c>
@@ -12843,7 +12850,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="152" t="s">
         <v>845</v>
       </c>
@@ -12887,7 +12894,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="152" t="s">
         <v>855</v>
       </c>
@@ -12931,7 +12938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -12975,7 +12982,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -13020,7 +13027,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -13064,7 +13071,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="152" t="s">
         <v>870</v>
       </c>
@@ -13108,7 +13115,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -13152,7 +13159,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -13197,7 +13204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="152" t="s">
         <v>883</v>
       </c>
@@ -13241,7 +13248,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="152" t="s">
         <v>889</v>
       </c>
@@ -13285,7 +13292,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="152" t="s">
         <v>889</v>
       </c>
@@ -13329,7 +13336,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="152" t="s">
         <v>899</v>
       </c>
@@ -13373,7 +13380,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13418,7 +13425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13462,7 +13469,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13506,7 +13513,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="152" t="s">
         <v>919</v>
       </c>
@@ -13550,7 +13557,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="152" t="s">
         <v>925</v>
       </c>
@@ -13594,7 +13601,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="152" t="s">
         <v>931</v>
       </c>
@@ -13638,7 +13645,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="152" t="s">
         <v>936</v>
       </c>
@@ -13682,7 +13689,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="152" t="s">
         <v>942</v>
       </c>
@@ -13726,7 +13733,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="152" t="s">
         <v>948</v>
       </c>
@@ -13770,7 +13777,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="152" t="s">
         <v>948</v>
       </c>
@@ -13814,7 +13821,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13858,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13902,7 +13909,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="152" t="s">
         <v>967</v>
       </c>
@@ -13946,7 +13953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -14093,37 +14100,37 @@
   <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
+      <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="24" width="9.1640625" style="4"/>
-    <col min="25" max="30" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="24" width="9.140625" style="4"/>
+    <col min="25" max="30" width="9.140625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.1640625" style="4"/>
-    <col min="35" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="1"/>
-    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="56.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.1640625" style="1"/>
+    <col min="32" max="34" width="9.140625" style="4"/>
+    <col min="35" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="1"/>
+    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="155" t="s">
         <v>499</v>
@@ -14210,7 +14217,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14330,7 +14337,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14456,7 +14463,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14568,7 +14575,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14691,7 +14698,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14821,7 +14828,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14951,7 +14958,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -15085,7 +15092,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -15174,7 +15181,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -15302,7 +15309,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15442,7 +15449,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15581,7 +15588,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15706,7 +15713,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15816,7 +15823,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15960,7 +15967,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -16083,7 +16090,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -16182,7 +16189,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -16208,7 +16215,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B19" s="136" t="s">
         <v>582</v>
       </c>
@@ -16239,7 +16246,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B20" s="135" t="s">
         <v>975</v>
       </c>
@@ -16265,7 +16272,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -16289,7 +16296,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16315,7 +16322,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16340,7 +16347,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16381,7 +16388,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16414,7 +16421,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
@@ -16440,7 +16447,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16466,7 +16473,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B28" s="135">
         <v>8022</v>
       </c>
@@ -16503,7 +16510,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="1"/>
@@ -16513,7 +16520,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B30" s="136" t="s">
         <v>582</v>
       </c>
@@ -16529,7 +16536,7 @@
       <c r="M30" s="56"/>
       <c r="N30" s="56"/>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>511</v>
       </c>
@@ -16562,7 +16569,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>540</v>
       </c>
@@ -16626,7 +16633,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>541</v>
       </c>
@@ -16653,7 +16660,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>575</v>
       </c>
@@ -16678,7 +16685,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>587</v>
       </c>
@@ -16703,7 +16710,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>588</v>
       </c>
@@ -16728,7 +16735,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F37" s="7"/>
       <c r="G37" s="56"/>
       <c r="H37" s="1"/>
@@ -16738,7 +16745,7 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="136" t="s">
         <v>582</v>
       </c>
@@ -16753,7 +16760,7 @@
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>985</v>
       </c>
@@ -16780,7 +16787,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>579</v>
       </c>
@@ -16801,7 +16808,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>580</v>
       </c>
@@ -16822,7 +16829,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>581</v>
       </c>
@@ -16940,7 +16947,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>568</v>
       </c>
@@ -16960,6 +16967,7 @@
       <c r="K43" s="1"/>
       <c r="M43" s="56"/>
       <c r="N43" s="56"/>
+      <c r="Y43" s="4"/>
       <c r="AM43" s="4" t="s">
         <v>980</v>
       </c>
@@ -16967,7 +16975,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>569</v>
       </c>
@@ -16982,11 +16990,11 @@
       </c>
       <c r="F44" s="54">
         <f>[19]Main!$C$6</f>
-        <v>2.4049999999999998</v>
+        <v>2.2280000000000002</v>
       </c>
       <c r="G44" s="56">
         <f>[19]Main!$C$8</f>
-        <v>120.24999999999999</v>
+        <v>111.4</v>
       </c>
       <c r="H44" s="56">
         <f>[19]Main!$C$11</f>
@@ -16994,19 +17002,19 @@
       </c>
       <c r="I44" s="56">
         <f>[19]Main!$C$12</f>
-        <v>106.37799999999999</v>
+        <v>97.528000000000006</v>
       </c>
       <c r="J44" s="4" t="str">
         <f>[19]Main!$C$29</f>
         <v>H122</v>
       </c>
-      <c r="K44" s="85">
+      <c r="K44" s="130">
         <f>[19]Main!$D$29</f>
         <v>45063</v>
       </c>
       <c r="L44" s="50">
         <f>[19]Main!$C$38</f>
-        <v>8.8692679673169916</v>
+        <v>8.1313990328497585</v>
       </c>
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
@@ -17019,25 +17027,33 @@
         <v>-11.902999999999997</v>
       </c>
       <c r="Q44" s="56">
-        <f>'[19]Financial Model'!$R$17</f>
-        <v>0</v>
+        <f>'[19]Financial Model'!$R$16</f>
+        <v>5.7139999999999933</v>
       </c>
       <c r="R44" s="51">
         <f>[19]Main!$C$37</f>
-        <v>10.025846256461564</v>
+        <v>9.2879773219943313</v>
       </c>
       <c r="S44" s="51">
-        <f>'[19]Financial Model'!$T$83</f>
+        <f>'[19]Financial Model'!$T$84</f>
         <v>4.5587396635300852</v>
       </c>
       <c r="T44" s="51">
         <f>[19]Main!$C$34</f>
-        <v>4.0893015030946032</v>
+        <v>3.7883425151329635</v>
       </c>
       <c r="W44" s="53">
         <f>'[19]Financial Model'!$T$21</f>
         <v>-2.7951830820442503E-2</v>
       </c>
+      <c r="X44" s="53">
+        <f>'[19]Financial Model'!$S$21</f>
+        <v>-0.24362684900059861</v>
+      </c>
+      <c r="Y44" s="53">
+        <f>'[19]Financial Model'!$R$21</f>
+        <v>8.9157301621889395E-3</v>
+      </c>
       <c r="Z44" s="53">
         <f>'[19]Financial Model'!$K$26</f>
         <v>0.19490724836825837</v>
@@ -17059,21 +17075,25 @@
         <v>31.096</v>
       </c>
       <c r="AF44" s="53">
-        <f>'[19]Financial Model'!$K$72</f>
+        <f>'[19]Financial Model'!$K$73</f>
         <v>9.3658776773467567E-2</v>
       </c>
       <c r="AG44" s="53">
-        <f>'[19]Financial Model'!$K$73</f>
+        <f>'[19]Financial Model'!$K$74</f>
         <v>0.23735625323305887</v>
       </c>
       <c r="AH44" s="53">
-        <f>'[19]Financial Model'!$K$74</f>
+        <f>'[19]Financial Model'!$K$75</f>
         <v>0.20930060375174159</v>
       </c>
       <c r="AI44" s="4">
         <f>[19]Main!$C$25</f>
         <v>388</v>
       </c>
+      <c r="AJ44" s="156">
+        <f>[19]Main!$W$7</f>
+        <v>4.433098591549296</v>
+      </c>
       <c r="AK44" s="4">
         <f>[19]Main!$C$24</f>
         <v>1917</v>
@@ -17086,7 +17106,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -17095,7 +17115,7 @@
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G46" s="56"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -17104,7 +17124,7 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G47" s="56"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -17113,7 +17133,7 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
@@ -17121,7 +17141,7 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
@@ -17129,7 +17149,7 @@
       <c r="M49" s="56"/>
       <c r="N49" s="56"/>
     </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D50" s="153" t="s">
         <v>495</v>
       </c>
@@ -17142,7 +17162,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D51" s="43" t="s">
         <v>497</v>
       </c>
@@ -17158,7 +17178,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D52" s="43" t="s">
         <v>498</v>
       </c>
@@ -17174,7 +17194,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D53" s="46" t="s">
         <v>564</v>
       </c>
@@ -17187,16 +17207,16 @@
       </c>
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G56" s="49"/>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G57" s="49"/>
     </row>
   </sheetData>
@@ -17247,21 +17267,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -17272,7 +17292,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -17299,98 +17319,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
$FL FY17,18,19 & first forecast
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF0846B-9D5F-0446-8A77-4A7A9CF6B299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC96B49-83ED-4879-B6E3-BB85047D3D24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="540" windowWidth="30280" windowHeight="18860" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -45,22 +45,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -68,7 +58,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -77,42 +67,42 @@
   <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="4"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="5"/>
         </ext>
       </extLst>
@@ -3211,14 +3201,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0\x"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="169" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.#\x"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3661,7 +3651,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3670,13 +3660,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3705,16 +3695,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3723,12 +3713,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3765,7 +3755,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3783,7 +3773,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3804,7 +3794,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3831,15 +3821,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3848,7 +3838,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3859,16 +3849,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3903,7 +3893,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3915,7 +3905,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3950,7 +3940,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3972,6 +3962,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3979,9 +3972,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5119,6 +5109,9 @@
       </sheetData>
       <sheetData sheetId="1">
         <row r="17">
+          <cell r="AF17">
+            <v>491</v>
+          </cell>
           <cell r="AG17">
             <v>323</v>
           </cell>
@@ -6784,25 +6777,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6844,7 +6837,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6888,7 +6881,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6932,7 +6925,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6976,7 +6969,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -7020,7 +7013,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -7064,7 +7057,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -7108,7 +7101,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -7152,7 +7145,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -7196,7 +7189,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -7240,7 +7233,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -7284,7 +7277,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -7328,7 +7321,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -7372,7 +7365,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7416,7 +7409,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7460,7 +7453,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7504,7 +7497,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7548,7 +7541,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7592,7 +7585,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7636,7 +7629,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7680,7 +7673,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7724,7 +7717,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7768,7 +7761,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7812,7 +7805,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7856,7 +7849,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7900,7 +7893,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7944,7 +7937,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -7988,7 +7981,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -8032,7 +8025,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -8076,7 +8069,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -8120,7 +8113,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -8164,7 +8157,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -8208,7 +8201,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -8252,7 +8245,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -8296,7 +8289,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -8340,7 +8333,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8384,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8428,7 +8421,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8472,7 +8465,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8516,7 +8509,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8560,7 +8553,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8604,7 +8597,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8648,7 +8641,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8692,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8810,25 +8803,25 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8870,7 +8863,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8914,7 +8907,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8958,7 +8951,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -9002,7 +8995,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -9046,7 +9039,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -9090,7 +9083,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -9134,7 +9127,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -9178,7 +9171,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -9222,7 +9215,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -9266,7 +9259,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -9310,7 +9303,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -9354,7 +9347,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9398,7 +9391,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9442,7 +9435,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9486,7 +9479,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9530,7 +9523,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9574,7 +9567,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9618,7 +9611,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9662,7 +9655,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9706,7 +9699,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9750,7 +9743,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9794,7 +9787,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9838,7 +9831,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9882,7 +9875,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9926,7 +9919,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9970,7 +9963,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -10014,7 +10007,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -10058,7 +10051,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -10102,7 +10095,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -10146,7 +10139,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -10190,7 +10183,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -10234,7 +10227,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -10278,7 +10271,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -10322,7 +10315,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -10366,7 +10359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10410,7 +10403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10454,7 +10447,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10566,16 +10559,16 @@
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10617,7 +10610,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="150" t="s">
         <v>589</v>
       </c>
@@ -10661,7 +10654,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="150" t="s">
         <v>589</v>
       </c>
@@ -10705,7 +10698,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="150" t="s">
         <v>597</v>
       </c>
@@ -10749,7 +10742,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="150" t="s">
         <v>604</v>
       </c>
@@ -10793,7 +10786,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="150" t="s">
         <v>608</v>
       </c>
@@ -10837,7 +10830,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="150" t="s">
         <v>614</v>
       </c>
@@ -10881,7 +10874,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
         <v>619</v>
       </c>
@@ -10925,7 +10918,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
         <v>622</v>
       </c>
@@ -10969,7 +10962,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="150" t="s">
         <v>627</v>
       </c>
@@ -11013,7 +11006,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="150" t="s">
         <v>632</v>
       </c>
@@ -11057,7 +11050,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="150" t="s">
         <v>635</v>
       </c>
@@ -11101,7 +11094,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="150" t="s">
         <v>641</v>
       </c>
@@ -11145,7 +11138,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="150" t="s">
         <v>646</v>
       </c>
@@ -11189,7 +11182,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="150" t="s">
         <v>652</v>
       </c>
@@ -11233,7 +11226,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -11277,7 +11270,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="150" t="s">
         <v>661</v>
       </c>
@@ -11321,7 +11314,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="150" t="s">
         <v>666</v>
       </c>
@@ -11365,7 +11358,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="150" t="s">
         <v>666</v>
       </c>
@@ -11409,7 +11402,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="150" t="s">
         <v>678</v>
       </c>
@@ -11453,7 +11446,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="150" t="s">
         <v>684</v>
       </c>
@@ -11497,7 +11490,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="150" t="s">
         <v>690</v>
       </c>
@@ -11541,7 +11534,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="150" t="s">
         <v>696</v>
       </c>
@@ -11585,7 +11578,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="150" t="s">
         <v>699</v>
       </c>
@@ -11629,7 +11622,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11673,7 +11666,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11717,7 +11710,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="150" t="s">
         <v>714</v>
       </c>
@@ -11761,7 +11754,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="150" t="s">
         <v>720</v>
       </c>
@@ -11805,7 +11798,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11849,7 +11842,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="150" t="s">
         <v>731</v>
       </c>
@@ -11893,7 +11886,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11937,7 +11930,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="150" t="s">
         <v>741</v>
       </c>
@@ -11981,7 +11974,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="150" t="s">
         <v>747</v>
       </c>
@@ -12025,7 +12018,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="150" t="s">
         <v>752</v>
       </c>
@@ -12069,7 +12062,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -12114,7 +12107,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="150" t="s">
         <v>762</v>
       </c>
@@ -12158,7 +12151,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -12202,7 +12195,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="150" t="s">
         <v>773</v>
       </c>
@@ -12246,7 +12239,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="150" t="s">
         <v>779</v>
       </c>
@@ -12290,7 +12283,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="150" t="s">
         <v>785</v>
       </c>
@@ -12334,7 +12327,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="150" t="s">
         <v>790</v>
       </c>
@@ -12378,7 +12371,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12422,7 +12415,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="150" t="s">
         <v>800</v>
       </c>
@@ -12466,7 +12459,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12510,7 +12503,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12554,7 +12547,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12599,7 +12592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12643,7 +12636,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="150" t="s">
         <v>824</v>
       </c>
@@ -12687,7 +12680,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12731,7 +12724,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="150" t="s">
         <v>835</v>
       </c>
@@ -12775,7 +12768,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="150" t="s">
         <v>824</v>
       </c>
@@ -12819,7 +12812,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="152" t="s">
         <v>845</v>
       </c>
@@ -12863,7 +12856,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="152" t="s">
         <v>845</v>
       </c>
@@ -12907,7 +12900,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="152" t="s">
         <v>855</v>
       </c>
@@ -12951,7 +12944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -12995,7 +12988,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -13040,7 +13033,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -13084,7 +13077,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="152" t="s">
         <v>870</v>
       </c>
@@ -13128,7 +13121,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -13172,7 +13165,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -13217,7 +13210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="152" t="s">
         <v>883</v>
       </c>
@@ -13261,7 +13254,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="152" t="s">
         <v>889</v>
       </c>
@@ -13305,7 +13298,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="152" t="s">
         <v>889</v>
       </c>
@@ -13349,7 +13342,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="152" t="s">
         <v>899</v>
       </c>
@@ -13393,7 +13386,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13438,7 +13431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13482,7 +13475,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13526,7 +13519,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="152" t="s">
         <v>919</v>
       </c>
@@ -13570,7 +13563,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="152" t="s">
         <v>925</v>
       </c>
@@ -13614,7 +13607,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="152" t="s">
         <v>931</v>
       </c>
@@ -13658,7 +13651,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="152" t="s">
         <v>936</v>
       </c>
@@ -13702,7 +13695,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="152" t="s">
         <v>942</v>
       </c>
@@ -13746,7 +13739,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="152" t="s">
         <v>948</v>
       </c>
@@ -13790,7 +13783,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="152" t="s">
         <v>948</v>
       </c>
@@ -13834,7 +13827,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13878,7 +13871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13922,7 +13915,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="152" t="s">
         <v>967</v>
       </c>
@@ -13966,7 +13959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -14113,52 +14106,52 @@
   <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1640625" style="6"/>
-    <col min="10" max="11" width="9.1640625" style="4"/>
-    <col min="12" max="19" width="9.1640625" style="1"/>
-    <col min="20" max="24" width="9.1640625" style="4"/>
-    <col min="25" max="30" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="19" width="9.140625" style="1"/>
+    <col min="20" max="24" width="9.140625" style="4"/>
+    <col min="25" max="30" width="9.140625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.1640625" style="4"/>
-    <col min="35" max="35" width="9.1640625" style="1"/>
-    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="1"/>
-    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="56.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.1640625" style="1"/>
+    <col min="32" max="34" width="9.140625" style="4"/>
+    <col min="35" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="1"/>
+    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="156" t="s">
+      <c r="F1" s="157" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156"/>
-      <c r="M1" s="156"/>
-      <c r="N1" s="156"/>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
         <v>15.54783961051915</v>
@@ -14230,7 +14223,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14350,7 +14343,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14476,7 +14469,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14588,7 +14581,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14621,7 +14614,7 @@
         <f>[3]Main!$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="K5" s="157"/>
+      <c r="K5" s="154"/>
       <c r="L5" s="50">
         <f>[3]Main!$C$33</f>
         <v>12.142042391143919</v>
@@ -14712,7 +14705,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14842,7 +14835,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14972,7 +14965,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -15106,7 +15099,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -15195,7 +15188,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -15323,7 +15316,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>481</v>
       </c>
@@ -15463,7 +15456,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15602,7 +15595,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15727,7 +15720,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15837,7 +15830,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -15981,7 +15974,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -16104,7 +16097,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -16203,7 +16196,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -16229,7 +16222,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B19" s="136" t="s">
         <v>582</v>
       </c>
@@ -16260,7 +16253,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B20" s="135" t="s">
         <v>975</v>
       </c>
@@ -16286,7 +16279,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -16310,7 +16303,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16336,7 +16329,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16361,7 +16354,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16402,7 +16395,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16435,7 +16428,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
@@ -16461,7 +16454,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16487,7 +16480,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B28" s="135">
         <v>8022</v>
       </c>
@@ -16524,7 +16517,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="1"/>
@@ -16534,7 +16527,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B30" s="136" t="s">
         <v>582</v>
       </c>
@@ -16550,7 +16543,7 @@
       <c r="M30" s="56"/>
       <c r="N30" s="56"/>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>511</v>
       </c>
@@ -16583,7 +16576,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>540</v>
       </c>
@@ -16647,7 +16640,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>541</v>
       </c>
@@ -16674,7 +16667,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>575</v>
       </c>
@@ -16699,7 +16692,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>587</v>
       </c>
@@ -16724,7 +16717,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>588</v>
       </c>
@@ -16749,7 +16742,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F37" s="7"/>
       <c r="G37" s="56"/>
       <c r="H37" s="1"/>
@@ -16759,7 +16752,7 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="136" t="s">
         <v>582</v>
       </c>
@@ -16774,7 +16767,7 @@
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>985</v>
       </c>
@@ -16801,7 +16794,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>579</v>
       </c>
@@ -16822,7 +16815,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>580</v>
       </c>
@@ -16843,7 +16836,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>581</v>
       </c>
@@ -16887,12 +16880,16 @@
       <c r="M42" s="56"/>
       <c r="N42" s="56"/>
       <c r="O42" s="56">
-        <f>'[18]Financial Model'!$AH$17</f>
-        <v>892</v>
+        <f>'[18]Financial Model'!$AH$17*E51</f>
+        <v>713.6</v>
       </c>
       <c r="P42" s="56">
-        <f>'[18]Financial Model'!$AG$17</f>
-        <v>323</v>
+        <f>'[18]Financial Model'!$AG$17*E51</f>
+        <v>258.40000000000003</v>
+      </c>
+      <c r="Q42" s="56">
+        <f>'[18]Financial Model'!$AF$17*E51</f>
+        <v>392.8</v>
       </c>
       <c r="R42" s="51">
         <f>[18]Main!$C$38</f>
@@ -16961,7 +16958,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>568</v>
       </c>
@@ -16989,7 +16986,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>569</v>
       </c>
@@ -17120,7 +17117,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -17129,7 +17126,7 @@
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G46" s="56"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -17138,7 +17135,7 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G47" s="56"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -17147,7 +17144,7 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G48" s="49"/>
       <c r="I48" s="4"/>
       <c r="J48" s="1"/>
@@ -17155,7 +17152,7 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
@@ -17163,11 +17160,11 @@
       <c r="M49" s="56"/>
       <c r="N49" s="56"/>
     </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
-      <c r="D50" s="154" t="s">
+    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D50" s="155" t="s">
         <v>495</v>
       </c>
-      <c r="E50" s="155"/>
+      <c r="E50" s="156"/>
       <c r="F50" s="42" t="s">
         <v>496</v>
       </c>
@@ -17176,7 +17173,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D51" s="43" t="s">
         <v>497</v>
       </c>
@@ -17192,7 +17189,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D52" s="43" t="s">
         <v>498</v>
       </c>
@@ -17208,7 +17205,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D53" s="46" t="s">
         <v>564</v>
       </c>
@@ -17221,16 +17218,16 @@
       </c>
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G56" s="49"/>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G57" s="49"/>
     </row>
   </sheetData>
@@ -17281,21 +17278,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -17306,7 +17303,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -17333,98 +17330,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
£SDRY H123 results & model updates
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEFFF95-2ADB-4185-A384-5A38986C7901}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41059176-36E6-4518-B673-8D06E1AE4F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -4534,22 +4534,22 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>1.5638000000000001</v>
+            <v>1.206</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>128.04249279359999</v>
+            <v>98.746160831999987</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>8.3000000000000007</v>
+            <v>-32.79999999999999</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>119.74249279359999</v>
+            <v>131.54616083199997</v>
           </cell>
         </row>
         <row r="24">
@@ -4564,45 +4564,45 @@
         </row>
         <row r="26">
           <cell r="C26">
-            <v>220</v>
+            <v>219</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>132.69999999999999</v>
+            <v>172.6</v>
           </cell>
         </row>
         <row r="29">
           <cell r="C29" t="str">
-            <v>FY22</v>
+            <v>H123</v>
           </cell>
           <cell r="D29">
-            <v>44841</v>
+            <v>44953</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>5.2749996825374366</v>
+            <v>16.4432701039999</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>5.6406384490572599</v>
+            <v>0.15074999999999913</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1.2323627795341676</v>
+            <v>1.1385687625057996</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>9.7478359051562061E-2</v>
+            <v>1.4467338886453514E-2</v>
           </cell>
         </row>
         <row r="39">
           <cell r="C39">
-            <v>-3.5533429472132991</v>
+            <v>-2.7403322639335199</v>
           </cell>
         </row>
         <row r="42">
@@ -4636,38 +4636,43 @@
           <cell r="S21">
             <v>-0.19192382700470356</v>
           </cell>
-          <cell r="T21">
-            <v>-0.21053378762066999</v>
+          <cell r="U21">
+            <v>9.6205718395971918E-2</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="J33">
-            <v>0.5523088023088023</v>
+          <cell r="L33">
+            <v>0.5205431754874652</v>
           </cell>
         </row>
         <row r="34">
-          <cell r="T34">
-            <v>-5.3048012947311589E-2</v>
+          <cell r="L34">
+            <v>-5.2576601671309189E-2</v>
           </cell>
         </row>
         <row r="35">
-          <cell r="T35">
-            <v>-6.4916381945693172E-2</v>
+          <cell r="L35">
+            <v>-4.247910863509749E-2</v>
           </cell>
         </row>
         <row r="36">
-          <cell r="T36">
-            <v>1.6348773841961865E-2</v>
+          <cell r="L36">
+            <v>0.31073446327683618</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="L79">
+            <v>8.2810539523211935E-2</v>
           </cell>
         </row>
         <row r="80">
-          <cell r="K80">
-            <v>-0.16750313676286088</v>
+          <cell r="L80">
+            <v>0.30067822155237378</v>
           </cell>
         </row>
         <row r="82">
-          <cell r="T82">
-            <v>0.26667865491818021</v>
+          <cell r="L82">
+            <v>0.2785668173014848</v>
           </cell>
         </row>
       </sheetData>
@@ -5177,144 +5182,31 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
-      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="W7">
-            <v>4.433098591549296</v>
+            <v>48.38</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>114.99999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>13.872</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>101.12799999999999</v>
+            <v>610.07180000000005</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Leicester, UK</v>
+            <v>Nashville, TN</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1917</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>388</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>31.096</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29" t="str">
-            <v>H122</v>
-          </cell>
-          <cell r="D29">
-            <v>45063</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>3.910766510236003</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>9.5881273970318492</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>8.4315491078872764</v>
+            <v>1924</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="16">
-          <cell r="R16">
-            <v>5.7139999999999933</v>
-          </cell>
-          <cell r="S16">
-            <v>-11.902999999999997</v>
-          </cell>
-          <cell r="T16">
-            <v>7.0139999999999958</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="R21">
-            <v>8.9157301621889395E-3</v>
-          </cell>
-          <cell r="S21">
-            <v>-0.24362684900059861</v>
-          </cell>
-          <cell r="T21">
-            <v>-2.7951830820442503E-2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="K26">
-            <v>0.19490724836825837</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="K27">
-            <v>5.2401809229359962E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="K28">
-            <v>4.1008244589488214E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="K29">
-            <v>6.4337034617896707E-2</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="K73">
-            <v>9.3658776773467567E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="K74">
-            <v>0.23735625323305887</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="K75">
-            <v>0.20930060375174159</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="T84">
-            <v>4.5587396635300852</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5449,21 +5341,144 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>48.38</v>
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="W7">
+            <v>4.433098591549296</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>610.07180000000005</v>
+            <v>114.99999999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>13.872</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>101.12799999999999</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Leicester, UK</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1917</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>388</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>31.096</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>H122</v>
+          </cell>
+          <cell r="D29">
+            <v>45063</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>3.910766510236003</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>9.5881273970318492</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>8.4315491078872764</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="16">
+          <cell r="R16">
+            <v>5.7139999999999933</v>
+          </cell>
+          <cell r="S16">
+            <v>-11.902999999999997</v>
+          </cell>
+          <cell r="T16">
+            <v>7.0139999999999958</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="R21">
+            <v>8.9157301621889395E-3</v>
+          </cell>
+          <cell r="S21">
+            <v>-0.24362684900059861</v>
+          </cell>
+          <cell r="T21">
+            <v>-2.7951830820442503E-2</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="K26">
+            <v>0.19490724836825837</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="K27">
+            <v>5.2401809229359962E-2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="K28">
+            <v>4.1008244589488214E-2</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="K29">
+            <v>6.4337034617896707E-2</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="K73">
+            <v>9.3658776773467567E-2</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="K74">
+            <v>0.23735625323305887</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="K75">
+            <v>0.20930060375174159</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="T84">
+            <v>4.5587396635300852</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14130,13 +14145,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A458185-0254-419D-98B2-758EDFAF7DB7}">
-  <dimension ref="A1:AO57"/>
+  <dimension ref="A1:AO58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14181,19 +14196,19 @@
       <c r="Q1" s="157"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
-        <v>15.54783961051915</v>
+        <v>15.048758842423034</v>
       </c>
       <c r="S1" s="98">
         <f>AVERAGE(S3:S16)</f>
-        <v>13.386852013106079</v>
+        <v>13.468153081434059</v>
       </c>
       <c r="T1" s="98">
         <f>AVERAGE(T3:T17)</f>
-        <v>2.8002662552316551</v>
+        <v>2.7940133207630971</v>
       </c>
       <c r="U1" s="111">
         <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
-        <v>4.375835462356302E-2</v>
+        <v>3.5457252607052167E-2</v>
       </c>
       <c r="V1" s="87"/>
       <c r="W1" s="111">
@@ -14210,19 +14225,19 @@
       </c>
       <c r="Z1" s="88">
         <f>AVERAGE(Z3:Z17)</f>
-        <v>0.46898934901498002</v>
+        <v>0.46687164056022418</v>
       </c>
       <c r="AA1" s="88">
         <f t="shared" si="0"/>
-        <v>4.4975127375012261E-2</v>
+        <v>4.5008799609012433E-2</v>
       </c>
       <c r="AB1" s="88">
         <f t="shared" si="0"/>
-        <v>2.5743424183751244E-2</v>
+        <v>2.7346086563079509E-2</v>
       </c>
       <c r="AC1" s="88">
         <f>AVERAGE(AC3:AC17)</f>
-        <v>0.218339323956832</v>
+        <v>0.23796503658582363</v>
       </c>
       <c r="AD1" s="87"/>
       <c r="AE1" s="89" t="s">
@@ -14230,19 +14245,19 @@
       </c>
       <c r="AF1" s="88">
         <f>AVERAGE(AF3:AF17)</f>
-        <v>0.32071271966059578</v>
+        <v>0.32623342229547664</v>
       </c>
       <c r="AG1" s="88">
         <f>AVERAGE(AG3:AG16)</f>
-        <v>4.8531130468231862E-2</v>
+        <v>0.10055128139214682</v>
       </c>
       <c r="AH1" s="88">
         <f>AVERAGE(AH3:AH16)</f>
-        <v>0.241472515171548</v>
+        <v>0.2424631953701567</v>
       </c>
       <c r="AI1" s="90">
         <f>AVERAGE(AI3:AI16)</f>
-        <v>668.36363636363637</v>
+        <v>668.27272727272725</v>
       </c>
       <c r="AJ1" s="126">
         <f>AVERAGE(AJ3:AJ16)</f>
@@ -14384,19 +14399,19 @@
         <v>505</v>
       </c>
       <c r="F3" s="7">
-        <f>[1]Main!$C$6*$E$51</f>
+        <f>[1]Main!$C$6*$E$52</f>
         <v>92.48</v>
       </c>
       <c r="G3" s="49">
-        <f>[1]Main!$C$8*$E$51</f>
+        <f>[1]Main!$C$8*$E$52</f>
         <v>144176.32000000001</v>
       </c>
       <c r="H3" s="49">
-        <f>[1]Main!$C$11*$E$51</f>
+        <f>[1]Main!$C$11*$E$52</f>
         <v>952</v>
       </c>
       <c r="I3" s="49">
-        <f>[1]Main!$C$12*$E$51</f>
+        <f>[1]Main!$C$12*$E$52</f>
         <v>143224.32000000001</v>
       </c>
       <c r="J3" s="4" t="str">
@@ -14412,15 +14427,15 @@
         <v>29.611379424412871</v>
       </c>
       <c r="O3" s="56">
-        <f>'[1]Financial Model'!$AF$21*1000*E51</f>
+        <f>'[1]Financial Model'!$AF$21*1000*E52</f>
         <v>4836.7999999999947</v>
       </c>
       <c r="P3" s="56">
-        <f>'[1]Financial Model'!$AE$21*1000*E51</f>
+        <f>'[1]Financial Model'!$AE$21*1000*E52</f>
         <v>4581.5999999999985</v>
       </c>
       <c r="Q3" s="56">
-        <f>'[1]Financial Model'!$AD$21*1000*E51</f>
+        <f>'[1]Financial Model'!$AD$21*1000*E52</f>
         <v>2031.2</v>
       </c>
       <c r="R3" s="51">
@@ -14466,7 +14481,7 @@
         <v>0.19333333333333316</v>
       </c>
       <c r="AE3" s="56">
-        <f>[1]Main!$C$26*E51</f>
+        <f>[1]Main!$C$26*E52</f>
         <v>7729.6</v>
       </c>
       <c r="AF3" s="53">
@@ -14510,19 +14525,19 @@
         <v>505</v>
       </c>
       <c r="F4" s="7">
-        <f>[2]Main!$C$6*$E$51</f>
+        <f>[2]Main!$C$6*$E$52</f>
         <v>26.576000000000001</v>
       </c>
       <c r="G4" s="49">
-        <f>[2]Main!$C$8*$E$51</f>
+        <f>[2]Main!$C$8*$E$52</f>
         <v>10303.196287999999</v>
       </c>
       <c r="H4" s="49">
-        <f>[2]Main!$C$11*$E$51</f>
+        <f>[2]Main!$C$11*$E$52</f>
         <v>-3732.828</v>
       </c>
       <c r="I4" s="49">
-        <f>[2]Main!$C$12*$E$51</f>
+        <f>[2]Main!$C$12*$E$52</f>
         <v>14036.024287999999</v>
       </c>
       <c r="J4" s="4" t="str">
@@ -14538,15 +14553,15 @@
         <v>12.65052830735576</v>
       </c>
       <c r="O4" s="56">
-        <f>'[2]Financial Model'!$AA$22*E51</f>
+        <f>'[2]Financial Model'!$AA$22*E52</f>
         <v>1109.5207999999991</v>
       </c>
       <c r="P4" s="56">
-        <f>'[2]Financial Model'!$Z$22*$E$51</f>
+        <f>'[2]Financial Model'!$Z$22*$E$52</f>
         <v>326.27920000000114</v>
       </c>
       <c r="Q4" s="56">
-        <f>'[2]Financial Model'!$Y$22*$E$51</f>
+        <f>'[2]Financial Model'!$Y$22*$E$52</f>
         <v>543.55920000000015</v>
       </c>
       <c r="R4" s="51">
@@ -14581,7 +14596,7 @@
         <v>0.20153557290196375</v>
       </c>
       <c r="AE4" s="56">
-        <f>[2]Main!$C$26*E51</f>
+        <f>[2]Main!$C$26*E52</f>
         <v>1873.116</v>
       </c>
       <c r="AF4" s="53">
@@ -15006,19 +15021,19 @@
         <v>505</v>
       </c>
       <c r="F8" s="7">
-        <f>[6]Main!$C$6*E51</f>
+        <f>[6]Main!$C$6*E52</f>
         <v>8.2640000000000011</v>
       </c>
       <c r="G8" s="49">
-        <f>[6]Main!$C$8*E51</f>
+        <f>[6]Main!$C$8*E52</f>
         <v>3754.5170080000007</v>
       </c>
       <c r="H8" s="49">
-        <f>[6]Main!$C$11*$E$51</f>
+        <f>[6]Main!$C$11*$E$52</f>
         <v>144.21600000000009</v>
       </c>
       <c r="I8" s="49">
-        <f>[6]Main!$C$12*$E$51</f>
+        <f>[6]Main!$C$12*$E$52</f>
         <v>3610.3010080000004</v>
       </c>
       <c r="J8" s="4" t="str">
@@ -15034,15 +15049,15 @@
         <v>31.197728787313238</v>
       </c>
       <c r="O8" s="56">
-        <f>'[6]Financial Model'!$AA$20*$E$51</f>
+        <f>'[6]Financial Model'!$AA$20*$E$52</f>
         <v>-439.34160000000003</v>
       </c>
       <c r="P8" s="56">
-        <f>'[6]Financial Model'!$Z$20*$E$51</f>
+        <f>'[6]Financial Model'!$Z$20*$E$52</f>
         <v>73.713599999999389</v>
       </c>
       <c r="Q8" s="56">
-        <f>'[6]Financial Model'!$Y$20*$E$51</f>
+        <f>'[6]Financial Model'!$Y$20*$E$52</f>
         <v>-37.041600000000322</v>
       </c>
       <c r="R8" s="52">
@@ -15091,7 +15106,7 @@
         <v>0.20212746629846307</v>
       </c>
       <c r="AE8" s="56">
-        <f>[6]Main!$C$27*E51</f>
+        <f>[6]Main!$C$27*E52</f>
         <v>864.33600000000013</v>
       </c>
       <c r="AF8" s="53">
@@ -15140,19 +15155,19 @@
         <v>505</v>
       </c>
       <c r="F9" s="7">
-        <f>[7]Main!$C$6*E51</f>
+        <f>[7]Main!$C$6*E52</f>
         <v>20.424000000000003</v>
       </c>
       <c r="G9" s="49">
-        <f>[7]Main!$C$8*$E$51</f>
+        <f>[7]Main!$C$8*$E$52</f>
         <v>1882.56504384</v>
       </c>
       <c r="H9" s="49">
-        <f>[7]Main!$C$11*E51</f>
+        <f>[7]Main!$C$11*E52</f>
         <v>311.2328</v>
       </c>
       <c r="I9" s="49">
-        <f>[7]Main!$C$12*E51</f>
+        <f>[7]Main!$C$12*E52</f>
         <v>1571.33224384</v>
       </c>
       <c r="J9" s="4" t="str">
@@ -15189,7 +15204,7 @@
         <v>0.28811258341459722</v>
       </c>
       <c r="AE9" s="56">
-        <f>[7]Main!$C$26*E51</f>
+        <f>[7]Main!$C$26*E52</f>
         <v>594.86320000000001</v>
       </c>
       <c r="AF9" s="53">
@@ -15229,19 +15244,19 @@
         <v>505</v>
       </c>
       <c r="F10" s="7">
-        <f>[8]Main!$C$6*E51</f>
+        <f>[8]Main!$C$6*E52</f>
         <v>10.336</v>
       </c>
       <c r="G10" s="49">
-        <f>[8]Main!$C$8*E51</f>
+        <f>[8]Main!$C$8*E52</f>
         <v>1862.4335039999999</v>
       </c>
       <c r="H10" s="49">
-        <f>[8]Main!$C$11*$E$51</f>
+        <f>[8]Main!$C$11*$E$52</f>
         <v>-222.6464</v>
       </c>
       <c r="I10" s="49">
-        <f>[8]Main!$C$12*$E$51</f>
+        <f>[8]Main!$C$12*$E$52</f>
         <v>2085.0799039999997</v>
       </c>
       <c r="J10" s="4" t="str">
@@ -15261,11 +15276,11 @@
         <v>8.663850071253929</v>
       </c>
       <c r="O10" s="56">
-        <f>'[8]Financial Model'!$Z$17*E51</f>
+        <f>'[8]Financial Model'!$Z$17*E52</f>
         <v>335.7007999999999</v>
       </c>
       <c r="P10" s="56">
-        <f>'[8]Financial Model'!$Y$17*F51</f>
+        <f>'[8]Financial Model'!$Y$17*F52</f>
         <v>-261.67125000000027</v>
       </c>
       <c r="Q10" s="4"/>
@@ -15308,7 +15323,7 @@
         <v>0.10849393290506794</v>
       </c>
       <c r="AE10" s="56">
-        <f>[8]Main!$C$26*E51</f>
+        <f>[8]Main!$C$26*E52</f>
         <v>549.63680000000011</v>
       </c>
       <c r="AF10" s="53">
@@ -15497,19 +15512,19 @@
         <v>505</v>
       </c>
       <c r="F12" s="54">
-        <f>[10]Main!$C$6*E51</f>
+        <f>[10]Main!$C$6*E52</f>
         <v>18.096</v>
       </c>
       <c r="G12" s="49">
-        <f>[10]Main!$C$8*E51</f>
+        <f>[10]Main!$C$8*E52</f>
         <v>895.49865599999998</v>
       </c>
       <c r="H12" s="49">
-        <f>[10]Main!$C$11*E51</f>
+        <f>[10]Main!$C$11*E52</f>
         <v>119.09119999999999</v>
       </c>
       <c r="I12" s="49">
-        <f>[10]Main!$C$12*E51</f>
+        <f>[10]Main!$C$12*E52</f>
         <v>776.40745599999991</v>
       </c>
       <c r="J12" s="4" t="str">
@@ -15530,15 +15545,15 @@
       </c>
       <c r="N12" s="50"/>
       <c r="O12" s="56">
-        <f>'[10]Financial Model'!$X$18*E51</f>
+        <f>'[10]Financial Model'!$X$18*E52</f>
         <v>210.40799999999979</v>
       </c>
       <c r="P12" s="56">
-        <f>'[10]Financial Model'!$W$18*$E$51</f>
+        <f>'[10]Financial Model'!$W$18*$E$52</f>
         <v>-91.216800000000134</v>
       </c>
       <c r="Q12" s="56">
-        <f>'[10]Financial Model'!$V$18*$E$51</f>
+        <f>'[10]Financial Model'!$V$18*$E$52</f>
         <v>31.486400000000494</v>
       </c>
       <c r="R12" s="52">
@@ -15587,7 +15602,7 @@
         <v>1.070062451209991</v>
       </c>
       <c r="AE12" s="56">
-        <f>'[10]Financial Model'!$Q$41*E51</f>
+        <f>'[10]Financial Model'!$Q$41*E52</f>
         <v>593.57039999999995</v>
       </c>
       <c r="AF12" s="53">
@@ -15872,31 +15887,31 @@
       </c>
       <c r="F15" s="7">
         <f>[13]Main!$C$6</f>
-        <v>1.5638000000000001</v>
+        <v>1.206</v>
       </c>
       <c r="G15" s="49">
         <f>[13]Main!$C$8</f>
-        <v>128.04249279359999</v>
+        <v>98.746160831999987</v>
       </c>
       <c r="H15" s="49">
         <f>[13]Main!$C$11</f>
-        <v>8.3000000000000007</v>
+        <v>-32.79999999999999</v>
       </c>
       <c r="I15" s="49">
         <f>[13]Main!$C$12</f>
-        <v>119.74249279359999</v>
+        <v>131.54616083199997</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>[13]Main!$C$29</f>
-        <v>FY22</v>
+        <v>H123</v>
       </c>
       <c r="K15" s="85">
         <f>[13]Main!$D$29</f>
-        <v>44841</v>
+        <v>44953</v>
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>5.2749996825374366</v>
+        <v>16.4432701039999</v>
       </c>
       <c r="N15" s="1">
         <f xml:space="preserve"> '[13]Financial Model'!$T$17</f>
@@ -15916,23 +15931,23 @@
       </c>
       <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>5.6406384490572599</v>
+        <v>0.15074999999999913</v>
       </c>
       <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
-        <v>-3.5533429472132991</v>
+        <v>-2.7403322639335199</v>
       </c>
       <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>1.2323627795341676</v>
+        <v>1.1385687625057996</v>
       </c>
       <c r="U15" s="131">
         <f>[13]Main!$C$38</f>
-        <v>9.7478359051562061E-2</v>
+        <v>1.4467338886453514E-2</v>
       </c>
       <c r="V15" s="53">
-        <f xml:space="preserve"> '[13]Financial Model'!$T$21</f>
-        <v>-0.21053378762066999</v>
+        <f>'[13]Financial Model'!$U$21</f>
+        <v>9.6205718395971918E-2</v>
       </c>
       <c r="W15" s="53">
         <f>'[13]Financial Model'!$S$21</f>
@@ -15947,40 +15962,40 @@
         <v>0.15957446808510634</v>
       </c>
       <c r="Z15" s="53">
-        <f>'[13]Financial Model'!$J$33</f>
-        <v>0.5523088023088023</v>
+        <f>'[13]Financial Model'!$L$33</f>
+        <v>0.5205431754874652</v>
       </c>
       <c r="AA15" s="53">
-        <f>'[13]Financial Model'!T34</f>
-        <v>-5.3048012947311589E-2</v>
+        <f>'[13]Financial Model'!L34</f>
+        <v>-5.2576601671309189E-2</v>
       </c>
       <c r="AB15" s="53">
-        <f>'[13]Financial Model'!T35</f>
-        <v>-6.4916381945693172E-2</v>
+        <f>'[13]Financial Model'!L35</f>
+        <v>-4.247910863509749E-2</v>
       </c>
       <c r="AC15" s="53">
-        <f>'[13]Financial Model'!T36</f>
-        <v>1.6348773841961865E-2</v>
+        <f>'[13]Financial Model'!L36</f>
+        <v>0.31073446327683618</v>
       </c>
       <c r="AE15" s="56">
         <f>[13]Main!$C$27</f>
-        <v>132.69999999999999</v>
+        <v>172.6</v>
       </c>
       <c r="AF15" s="53">
-        <f>'[13]Financial Model'!T79</f>
-        <v>0</v>
+        <f>'[13]Financial Model'!L79</f>
+        <v>8.2810539523211935E-2</v>
       </c>
       <c r="AG15" s="53">
-        <f>'[13]Financial Model'!$K$80</f>
-        <v>-0.16750313676286088</v>
+        <f>'[13]Financial Model'!$L$80</f>
+        <v>0.30067822155237378</v>
       </c>
       <c r="AH15" s="53">
-        <f>'[13]Financial Model'!$T$82</f>
-        <v>0.26667865491818021</v>
+        <f>'[13]Financial Model'!$L$82</f>
+        <v>0.2785668173014848</v>
       </c>
       <c r="AI15" s="57">
         <f>[13]Main!$C$26</f>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AJ15" s="125">
         <f>[13]Main!$C$42</f>
@@ -16395,19 +16410,19 @@
         <v>505</v>
       </c>
       <c r="F24" s="54">
-        <f>[16]Main!$C$6*E51</f>
+        <f>[16]Main!$C$6*E52</f>
         <v>265.12800000000004</v>
       </c>
       <c r="G24" s="56">
-        <f>[16]Main!$C$8*E51</f>
+        <f>[16]Main!$C$8*E52</f>
         <v>32425.154399999999</v>
       </c>
       <c r="H24" s="56">
-        <f>[16]Main!$C$11*E51</f>
+        <f>[16]Main!$C$11*E52</f>
         <v>0</v>
       </c>
       <c r="I24" s="56">
-        <f>[16]Main!$C$12*E51</f>
+        <f>[16]Main!$C$12*E52</f>
         <v>32425.154399999999</v>
       </c>
       <c r="AK24" s="4">
@@ -16436,7 +16451,7 @@
         <v>565</v>
       </c>
       <c r="F25" s="54">
-        <f>81600*E53</f>
+        <f>81600*E54</f>
         <v>505.91999999999996</v>
       </c>
       <c r="G25" s="56"/>
@@ -16521,7 +16536,7 @@
         <v>565</v>
       </c>
       <c r="F28" s="54">
-        <f>2769*E53</f>
+        <f>2769*E54</f>
         <v>17.1678</v>
       </c>
       <c r="G28" s="56">
@@ -16584,7 +16599,7 @@
         <v>505</v>
       </c>
       <c r="F31" s="7">
-        <f>18.22*E51</f>
+        <f>18.22*E52</f>
         <v>14.576000000000001</v>
       </c>
       <c r="G31" s="56"/>
@@ -16808,19 +16823,19 @@
         <v>505</v>
       </c>
       <c r="F39" s="54">
-        <f>[18]Main!$C$6*$E$51</f>
+        <f>[18]Main!$C$6*$E$52</f>
         <v>31.104000000000003</v>
       </c>
       <c r="G39" s="49">
-        <f>[18]Main!$C$8*$E$51</f>
+        <f>[18]Main!$C$8*$E$52</f>
         <v>2902.6385614080004</v>
       </c>
       <c r="H39" s="1">
-        <f>[18]Main!$C$11*E51</f>
+        <f>[18]Main!$C$11*E52</f>
         <v>-82.4</v>
       </c>
       <c r="I39" s="56">
-        <f>[18]Main!$C$12*E51</f>
+        <f>[18]Main!$C$12*E52</f>
         <v>2985.0385614080005</v>
       </c>
       <c r="J39" s="4" t="str">
@@ -16838,15 +16853,15 @@
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
       <c r="O39" s="56">
-        <f>'[18]Financial Model'!$AH$17*E51</f>
+        <f>'[18]Financial Model'!$AH$17*E52</f>
         <v>713.6</v>
       </c>
       <c r="P39" s="56">
-        <f>'[18]Financial Model'!$AG$17*E51</f>
+        <f>'[18]Financial Model'!$AG$17*E52</f>
         <v>258.40000000000003</v>
       </c>
       <c r="Q39" s="56">
-        <f>'[18]Financial Model'!$AF$17*E51</f>
+        <f>'[18]Financial Model'!$AF$17*E52</f>
         <v>392.8</v>
       </c>
       <c r="R39" s="51">
@@ -16882,7 +16897,7 @@
         <v>0.32867132867132864</v>
       </c>
       <c r="AE39" s="56">
-        <f>[18]Main!$C$28*E51</f>
+        <f>[18]Main!$C$28*E52</f>
         <v>1348</v>
       </c>
       <c r="AF39" s="53">
@@ -16930,11 +16945,11 @@
         <v>505</v>
       </c>
       <c r="F40" s="54">
-        <f>[20]Main!$C$6*E51</f>
+        <f>[19]Main!$C$6*E52</f>
         <v>38.704000000000008</v>
       </c>
       <c r="G40" s="56">
-        <f>[20]Main!$C$8*E51</f>
+        <f>[19]Main!$C$8*E52</f>
         <v>488.05744000000004</v>
       </c>
       <c r="H40" s="1"/>
@@ -16943,6 +16958,14 @@
       <c r="K40" s="1"/>
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
+      <c r="AK40" s="4">
+        <f>[19]Main!$C$24</f>
+        <v>1924</v>
+      </c>
+      <c r="AL40" s="4" t="str">
+        <f>[19]Main!$C$23</f>
+        <v>Nashville, TN</v>
+      </c>
       <c r="AM40" s="4" t="s">
         <v>987</v>
       </c>
@@ -16964,117 +16987,117 @@
         <v>15</v>
       </c>
       <c r="F41" s="54">
-        <f>[19]Main!$C$6</f>
+        <f>[20]Main!$C$6</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="G41" s="56">
-        <f>[19]Main!$C$8</f>
+        <f>[20]Main!$C$8</f>
         <v>114.99999999999999</v>
       </c>
       <c r="H41" s="56">
-        <f>[19]Main!$C$11</f>
+        <f>[20]Main!$C$11</f>
         <v>13.872</v>
       </c>
       <c r="I41" s="56">
-        <f>[19]Main!$C$12</f>
+        <f>[20]Main!$C$12</f>
         <v>101.12799999999999</v>
       </c>
       <c r="J41" s="4" t="str">
-        <f>[19]Main!$C$29</f>
+        <f>[20]Main!$C$29</f>
         <v>H122</v>
       </c>
       <c r="K41" s="130">
-        <f>[19]Main!$D$29</f>
+        <f>[20]Main!$D$29</f>
         <v>45063</v>
       </c>
       <c r="L41" s="50">
-        <f>[19]Main!$C$38</f>
+        <f>[20]Main!$C$38</f>
         <v>8.4315491078872764</v>
       </c>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
       <c r="O41" s="56">
-        <f>'[19]Financial Model'!$T$16</f>
+        <f>'[20]Financial Model'!$T$16</f>
         <v>7.0139999999999958</v>
       </c>
       <c r="P41" s="56">
-        <f>'[19]Financial Model'!$S$16</f>
+        <f>'[20]Financial Model'!$S$16</f>
         <v>-11.902999999999997</v>
       </c>
       <c r="Q41" s="56">
-        <f>'[19]Financial Model'!$R$16</f>
+        <f>'[20]Financial Model'!$R$16</f>
         <v>5.7139999999999933</v>
       </c>
       <c r="R41" s="51">
-        <f>[19]Main!$C$37</f>
+        <f>[20]Main!$C$37</f>
         <v>9.5881273970318492</v>
       </c>
       <c r="S41" s="51">
-        <f>'[19]Financial Model'!$T$84</f>
+        <f>'[20]Financial Model'!$T$84</f>
         <v>4.5587396635300852</v>
       </c>
       <c r="T41" s="51">
-        <f>[19]Main!$C$34</f>
+        <f>[20]Main!$C$34</f>
         <v>3.910766510236003</v>
       </c>
       <c r="W41" s="53">
-        <f>'[19]Financial Model'!$T$21</f>
+        <f>'[20]Financial Model'!$T$21</f>
         <v>-2.7951830820442503E-2</v>
       </c>
       <c r="X41" s="53">
-        <f>'[19]Financial Model'!$S$21</f>
+        <f>'[20]Financial Model'!$S$21</f>
         <v>-0.24362684900059861</v>
       </c>
       <c r="Y41" s="53">
-        <f>'[19]Financial Model'!$R$21</f>
+        <f>'[20]Financial Model'!$R$21</f>
         <v>8.9157301621889395E-3</v>
       </c>
       <c r="Z41" s="53">
-        <f>'[19]Financial Model'!$K$26</f>
+        <f>'[20]Financial Model'!$K$26</f>
         <v>0.19490724836825837</v>
       </c>
       <c r="AA41" s="53">
-        <f>'[19]Financial Model'!$K$27</f>
+        <f>'[20]Financial Model'!$K$27</f>
         <v>5.2401809229359962E-2</v>
       </c>
       <c r="AB41" s="53">
-        <f>'[19]Financial Model'!$K$28</f>
+        <f>'[20]Financial Model'!$K$28</f>
         <v>4.1008244589488214E-2</v>
       </c>
       <c r="AC41" s="53">
-        <f>'[19]Financial Model'!$K$29</f>
+        <f>'[20]Financial Model'!$K$29</f>
         <v>6.4337034617896707E-2</v>
       </c>
       <c r="AE41" s="56">
-        <f>[19]Main!$C$27</f>
+        <f>[20]Main!$C$27</f>
         <v>31.096</v>
       </c>
       <c r="AF41" s="53">
-        <f>'[19]Financial Model'!$K$73</f>
+        <f>'[20]Financial Model'!$K$73</f>
         <v>9.3658776773467567E-2</v>
       </c>
       <c r="AG41" s="53">
-        <f>'[19]Financial Model'!$K$74</f>
+        <f>'[20]Financial Model'!$K$74</f>
         <v>0.23735625323305887</v>
       </c>
       <c r="AH41" s="53">
-        <f>'[19]Financial Model'!$K$75</f>
+        <f>'[20]Financial Model'!$K$75</f>
         <v>0.20930060375174159</v>
       </c>
       <c r="AI41" s="4">
-        <f>[19]Main!$C$25</f>
+        <f>[20]Main!$C$25</f>
         <v>388</v>
       </c>
       <c r="AJ41" s="153">
-        <f>[19]Main!$W$7</f>
+        <f>[20]Main!$W$7</f>
         <v>4.433098591549296</v>
       </c>
       <c r="AK41" s="4">
-        <f>[19]Main!$C$24</f>
+        <f>[20]Main!$C$24</f>
         <v>1917</v>
       </c>
       <c r="AL41" s="4" t="str">
-        <f>[19]Main!$C$23</f>
+        <f>[20]Main!$C$23</f>
         <v>Leicester, UK</v>
       </c>
       <c r="AM41" s="4" t="s">
@@ -17082,41 +17105,46 @@
       </c>
     </row>
     <row r="42" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>505</v>
-      </c>
+      <c r="B42" s="3"/>
+      <c r="F42" s="54"/>
       <c r="G42" s="56"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="50"/>
       <c r="M42" s="56"/>
       <c r="N42" s="56"/>
-      <c r="AM42" s="4" t="s">
-        <v>980</v>
-      </c>
-      <c r="AN42" s="4" t="s">
-        <v>1014</v>
-      </c>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="53"/>
+      <c r="Y42" s="53"/>
+      <c r="Z42" s="53"/>
+      <c r="AA42" s="53"/>
+      <c r="AB42" s="53"/>
+      <c r="AC42" s="53"/>
+      <c r="AE42" s="56"/>
+      <c r="AF42" s="53"/>
+      <c r="AG42" s="53"/>
+      <c r="AH42" s="53"/>
+      <c r="AI42" s="4"/>
+      <c r="AJ42" s="153"/>
+      <c r="AK42" s="4"/>
+      <c r="AL42" s="4"/>
     </row>
     <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>505</v>
@@ -17129,24 +17157,24 @@
       <c r="M43" s="56"/>
       <c r="N43" s="56"/>
       <c r="AM43" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="AN43" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>15</v>
+        <v>505</v>
       </c>
       <c r="G44" s="56"/>
       <c r="H44" s="1"/>
@@ -17155,15 +17183,26 @@
       <c r="K44" s="1"/>
       <c r="M44" s="56"/>
       <c r="N44" s="56"/>
-      <c r="Y44" s="4"/>
       <c r="AM44" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="AN44" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G45" s="56"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -17171,6 +17210,13 @@
       <c r="K45" s="1"/>
       <c r="M45" s="56"/>
       <c r="N45" s="56"/>
+      <c r="Y45" s="4"/>
+      <c r="AM45" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="AN45" s="4" t="s">
+        <v>1016</v>
+      </c>
     </row>
     <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="G46" s="56"/>
@@ -17191,8 +17237,9 @@
       <c r="N47" s="56"/>
     </row>
     <row r="48" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="G48" s="49"/>
-      <c r="I48" s="4"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="M48" s="56"/>
@@ -17207,28 +17254,20 @@
       <c r="N49" s="56"/>
     </row>
     <row r="50" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D50" s="155" t="s">
-        <v>495</v>
-      </c>
-      <c r="E50" s="156"/>
-      <c r="F50" s="42" t="s">
-        <v>496</v>
-      </c>
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
     </row>
     <row r="51" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D51" s="43" t="s">
-        <v>497</v>
-      </c>
-      <c r="E51" s="44">
-        <v>0.8</v>
-      </c>
-      <c r="F51" s="45">
-        <f>1/E51</f>
-        <v>1.25</v>
+      <c r="D51" s="155" t="s">
+        <v>495</v>
+      </c>
+      <c r="E51" s="156"/>
+      <c r="F51" s="42" t="s">
+        <v>496</v>
       </c>
       <c r="G51" s="49"/>
       <c r="I51" s="4"/>
@@ -17237,14 +17276,14 @@
     </row>
     <row r="52" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D52" s="43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E52" s="44">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="F52" s="45">
         <f>1/E52</f>
-        <v>1.1363636363636365</v>
+        <v>1.25</v>
       </c>
       <c r="G52" s="49"/>
       <c r="I52" s="4"/>
@@ -17252,19 +17291,32 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D53" s="46" t="s">
+      <c r="D53" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="E53" s="44">
+        <v>0.88</v>
+      </c>
+      <c r="F53" s="45">
+        <f>1/E53</f>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="G53" s="49"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D54" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="E53" s="48">
+      <c r="E54" s="48">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="F53" s="47">
-        <f>1/E53</f>
+      <c r="F54" s="47">
+        <f>1/E54</f>
         <v>161.29032258064515</v>
       </c>
-      <c r="G53" s="49"/>
-    </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G54" s="49"/>
     </row>
     <row r="55" spans="4:14" x14ac:dyDescent="0.2">
@@ -17276,9 +17328,12 @@
     <row r="57" spans="4:14" x14ac:dyDescent="0.2">
       <c r="G57" s="49"/>
     </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G58" s="49"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="F1:Q1"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
$GCO initial look at latest results
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41059176-36E6-4518-B673-8D06E1AE4F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056CF5C0-03C2-43A9-91EF-6318FCDACBB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -3560,7 +3560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3975,6 +3975,9 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4676,8 +4679,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5051,12 +5054,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>38.880000000000003</v>
+            <v>43.98</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>3628.2982017600002</v>
+            <v>4104.2323794599997</v>
           </cell>
         </row>
         <row r="11">
@@ -5066,7 +5069,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>3731.2982017600002</v>
+            <v>4207.2323794599997</v>
           </cell>
         </row>
         <row r="23">
@@ -5099,17 +5102,17 @@
         </row>
         <row r="35">
           <cell r="C35">
-            <v>1.1142657256827251</v>
+            <v>1.2604271248849341</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>8.8454790838610293</v>
+            <v>10.005765692083539</v>
           </cell>
         </row>
         <row r="39">
           <cell r="C39">
-            <v>8.8002316079245286</v>
+            <v>9.9227178760849046</v>
           </cell>
         </row>
       </sheetData>
@@ -5192,7 +5195,17 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>610.07180000000005</v>
+            <v>587.23644000000002</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-57.274999999999991</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>644.51143999999999</v>
           </cell>
         </row>
         <row r="23">
@@ -5205,8 +5218,57 @@
             <v>1924</v>
           </cell>
         </row>
+        <row r="26">
+          <cell r="C26">
+            <v>1404</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>563.49</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>FQ323</v>
+          </cell>
+          <cell r="D29">
+            <v>37591</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>1.0498682203942842</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="31">
+          <cell r="U31">
+            <v>0.48660622602635362</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="U32">
+            <v>4.3182375270790468E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="U33">
+            <v>3.3746944291705099E-2</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="U34">
+            <v>0.18684556276625364</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="U81">
+            <v>0.66124210638034442</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14148,10 +14210,10 @@
   <dimension ref="A1:AO58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomRight" activeCell="Z40" sqref="Z40:AC40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16824,11 +16886,11 @@
       </c>
       <c r="F39" s="54">
         <f>[18]Main!$C$6*$E$52</f>
-        <v>31.104000000000003</v>
+        <v>35.183999999999997</v>
       </c>
       <c r="G39" s="49">
         <f>[18]Main!$C$8*$E$52</f>
-        <v>2902.6385614080004</v>
+        <v>3283.3859035679998</v>
       </c>
       <c r="H39" s="1">
         <f>[18]Main!$C$11*E52</f>
@@ -16836,7 +16898,7 @@
       </c>
       <c r="I39" s="56">
         <f>[18]Main!$C$12*E52</f>
-        <v>2985.0385614080005</v>
+        <v>3365.7859035679999</v>
       </c>
       <c r="J39" s="4" t="str">
         <f>[18]Main!$C$30</f>
@@ -16848,7 +16910,7 @@
       </c>
       <c r="L39" s="50">
         <f>[18]Main!$C$39</f>
-        <v>8.8002316079245286</v>
+        <v>9.9227178760849046</v>
       </c>
       <c r="M39" s="56"/>
       <c r="N39" s="56"/>
@@ -16866,7 +16928,7 @@
       </c>
       <c r="R39" s="51">
         <f>[18]Main!$C$38</f>
-        <v>8.8454790838610293</v>
+        <v>10.005765692083539</v>
       </c>
       <c r="S39" s="51">
         <f>'[18]Financial Model'!$AH$84</f>
@@ -16874,7 +16936,7 @@
       </c>
       <c r="T39" s="51">
         <f>[18]Main!$C$35</f>
-        <v>1.1142657256827251</v>
+        <v>1.2604271248849341</v>
       </c>
       <c r="W39" s="53">
         <f>'[18]Financial Model'!$AH$21</f>
@@ -16950,14 +17012,58 @@
       </c>
       <c r="G40" s="56">
         <f>[19]Main!$C$8*E52</f>
-        <v>488.05744000000004</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+        <v>469.78915200000006</v>
+      </c>
+      <c r="H40" s="1">
+        <f>[19]Main!$C$11*$E$52</f>
+        <v>-45.819999999999993</v>
+      </c>
+      <c r="I40" s="56">
+        <f>[19]Main!$C$12*$E$52</f>
+        <v>515.60915199999999</v>
+      </c>
+      <c r="J40" s="4" t="str">
+        <f>[19]Main!$C$29</f>
+        <v>FQ323</v>
+      </c>
+      <c r="K40" s="158">
+        <f>[19]Main!$D$29</f>
+        <v>37591</v>
+      </c>
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
+      <c r="T40" s="51">
+        <f>[19]Main!$C$34</f>
+        <v>1.0498682203942842</v>
+      </c>
+      <c r="Z40" s="53">
+        <f>'[19]Financial Model'!$U$31</f>
+        <v>0.48660622602635362</v>
+      </c>
+      <c r="AA40" s="53">
+        <f>'[19]Financial Model'!$U$32</f>
+        <v>4.3182375270790468E-2</v>
+      </c>
+      <c r="AB40" s="53">
+        <f>'[19]Financial Model'!$U$33</f>
+        <v>3.3746944291705099E-2</v>
+      </c>
+      <c r="AC40" s="53">
+        <f>'[19]Financial Model'!$U$34</f>
+        <v>0.18684556276625364</v>
+      </c>
+      <c r="AE40" s="56">
+        <f>[19]Main!$C$27*$E$52</f>
+        <v>450.79200000000003</v>
+      </c>
+      <c r="AF40" s="53">
+        <f>'[19]Financial Model'!$U$81</f>
+        <v>0.66124210638034442</v>
+      </c>
+      <c r="AI40" s="57">
+        <f>[19]Main!$C$26</f>
+        <v>1404</v>
+      </c>
       <c r="AK40" s="4">
         <f>[19]Main!$C$24</f>
         <v>1924</v>
@@ -17110,7 +17216,7 @@
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
-      <c r="K42" s="130"/>
+      <c r="K42" s="50"/>
       <c r="L42" s="50"/>
       <c r="M42" s="56"/>
       <c r="N42" s="56"/>

</xml_diff>

<commit_message>
$GCO Full 21 results
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9355B502-5937-42C3-A4D2-BB803CC705E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750204D2-F1A3-4895-914C-50814EEC5CFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -3966,6 +3966,9 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3973,9 +3976,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4679,8 +4679,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5190,12 +5190,12 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>48.38</v>
+            <v>47.76</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>587.23644000000002</v>
+            <v>579.71087999999997</v>
           </cell>
         </row>
         <row r="11">
@@ -5205,7 +5205,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>644.51143999999999</v>
+            <v>636.98587999999995</v>
           </cell>
         </row>
         <row r="23">
@@ -5238,34 +5238,59 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>1.0498682203942842</v>
+            <v>1.0364139356352007</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.6517157789899475</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>6.6976413685782017</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="20">
+          <cell r="AE20">
+            <v>114.88199999999999</v>
+          </cell>
+        </row>
         <row r="31">
-          <cell r="U31">
+          <cell r="V31">
             <v>0.48660622602635362</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="U32">
+          <cell r="V32">
             <v>4.3182375270790468E-2</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="U33">
+          <cell r="V33">
             <v>3.3746944291705099E-2</v>
           </cell>
         </row>
         <row r="34">
-          <cell r="U34">
+          <cell r="V34">
             <v>0.18684556276625364</v>
           </cell>
         </row>
         <row r="81">
-          <cell r="U81">
+          <cell r="V81">
             <v>0.66124210638034442</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="V82">
+            <v>0.11090301161589489</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="V83">
+            <v>0.23601398601398599</v>
           </cell>
         </row>
       </sheetData>
@@ -5409,7 +5434,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>2.2999999999999998</v>
+            <v>2.4491000000000001</v>
           </cell>
         </row>
         <row r="7">
@@ -5419,7 +5444,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>114.99999999999999</v>
+            <v>122.455</v>
           </cell>
         </row>
         <row r="11">
@@ -5429,7 +5454,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>101.12799999999999</v>
+            <v>108.583</v>
           </cell>
         </row>
         <row r="23">
@@ -5462,17 +5487,17 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>3.910766510236003</v>
+            <v>4.1642862000952157</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>9.5881273970318492</v>
+            <v>10.209688177422045</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>8.4315491078872764</v>
+            <v>9.0531098882774721</v>
           </cell>
         </row>
       </sheetData>
@@ -14210,10 +14235,10 @@
   <dimension ref="A1:AO58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomRight" activeCell="AH40" sqref="AH40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14242,20 +14267,20 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="157" t="s">
+      <c r="F1" s="158" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
-      <c r="J1" s="157"/>
-      <c r="K1" s="157"/>
-      <c r="L1" s="157"/>
-      <c r="M1" s="157"/>
-      <c r="N1" s="157"/>
-      <c r="O1" s="157"/>
-      <c r="P1" s="157"/>
-      <c r="Q1" s="157"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="158"/>
+      <c r="O1" s="158"/>
+      <c r="P1" s="158"/>
+      <c r="Q1" s="158"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
         <v>15.048758842423034</v>
@@ -17008,11 +17033,11 @@
       </c>
       <c r="F40" s="54">
         <f>[19]Main!$C$6*$E$52</f>
-        <v>38.704000000000008</v>
+        <v>38.207999999999998</v>
       </c>
       <c r="G40" s="56">
         <f>[19]Main!$C$8*$E$52</f>
-        <v>469.78915200000006</v>
+        <v>463.76870400000001</v>
       </c>
       <c r="H40" s="1">
         <f>[19]Main!$C$11*$E$52</f>
@@ -17020,36 +17045,48 @@
       </c>
       <c r="I40" s="56">
         <f>[19]Main!$C$12*$E$52</f>
-        <v>515.60915199999999</v>
+        <v>509.58870400000001</v>
       </c>
       <c r="J40" s="4" t="str">
         <f>[19]Main!$C$29</f>
         <v>FQ323</v>
       </c>
-      <c r="K40" s="158">
+      <c r="K40" s="155">
         <f>[19]Main!$D$29</f>
         <v>37591</v>
       </c>
+      <c r="L40" s="50">
+        <f>[19]Main!$C$38</f>
+        <v>6.6976413685782017</v>
+      </c>
       <c r="M40" s="56"/>
       <c r="N40" s="56"/>
+      <c r="O40" s="56">
+        <f>'[19]Financial Model'!$AE$20*E52</f>
+        <v>91.905599999999993</v>
+      </c>
+      <c r="R40" s="51">
+        <f>[19]Main!$C$37</f>
+        <v>6.6517157789899475</v>
+      </c>
       <c r="T40" s="51">
         <f>[19]Main!$C$34</f>
-        <v>1.0498682203942842</v>
+        <v>1.0364139356352007</v>
       </c>
       <c r="Z40" s="53">
-        <f>'[19]Financial Model'!$U$31</f>
+        <f>'[19]Financial Model'!$V$31</f>
         <v>0.48660622602635362</v>
       </c>
       <c r="AA40" s="53">
-        <f>'[19]Financial Model'!$U$32</f>
+        <f>'[19]Financial Model'!$V$32</f>
         <v>4.3182375270790468E-2</v>
       </c>
       <c r="AB40" s="53">
-        <f>'[19]Financial Model'!$U$33</f>
+        <f>'[19]Financial Model'!$V$33</f>
         <v>3.3746944291705099E-2</v>
       </c>
       <c r="AC40" s="53">
-        <f>'[19]Financial Model'!$U$34</f>
+        <f>'[19]Financial Model'!$V$34</f>
         <v>0.18684556276625364</v>
       </c>
       <c r="AE40" s="56">
@@ -17057,8 +17094,16 @@
         <v>450.79200000000003</v>
       </c>
       <c r="AF40" s="53">
-        <f>'[19]Financial Model'!$U$81</f>
+        <f>'[19]Financial Model'!$V$81</f>
         <v>0.66124210638034442</v>
+      </c>
+      <c r="AG40" s="53">
+        <f>'[19]Financial Model'!$V$82</f>
+        <v>0.11090301161589489</v>
+      </c>
+      <c r="AH40" s="53">
+        <f>'[19]Financial Model'!$V$83</f>
+        <v>0.23601398601398599</v>
       </c>
       <c r="AI40" s="57">
         <f>[19]Main!$C$26</f>
@@ -17094,11 +17139,11 @@
       </c>
       <c r="F41" s="54">
         <f>[20]Main!$C$6</f>
-        <v>2.2999999999999998</v>
+        <v>2.4491000000000001</v>
       </c>
       <c r="G41" s="56">
         <f>[20]Main!$C$8</f>
-        <v>114.99999999999999</v>
+        <v>122.455</v>
       </c>
       <c r="H41" s="56">
         <f>[20]Main!$C$11</f>
@@ -17106,7 +17151,7 @@
       </c>
       <c r="I41" s="56">
         <f>[20]Main!$C$12</f>
-        <v>101.12799999999999</v>
+        <v>108.583</v>
       </c>
       <c r="J41" s="4" t="str">
         <f>[20]Main!$C$29</f>
@@ -17118,7 +17163,7 @@
       </c>
       <c r="L41" s="50">
         <f>[20]Main!$C$38</f>
-        <v>8.4315491078872764</v>
+        <v>9.0531098882774721</v>
       </c>
       <c r="M41" s="56"/>
       <c r="N41" s="56"/>
@@ -17136,7 +17181,7 @@
       </c>
       <c r="R41" s="51">
         <f>[20]Main!$C$37</f>
-        <v>9.5881273970318492</v>
+        <v>10.209688177422045</v>
       </c>
       <c r="S41" s="51">
         <f>'[20]Financial Model'!$T$84</f>
@@ -17144,7 +17189,7 @@
       </c>
       <c r="T41" s="51">
         <f>[20]Main!$C$34</f>
-        <v>3.910766510236003</v>
+        <v>4.1642862000952157</v>
       </c>
       <c r="W41" s="53">
         <f>'[20]Financial Model'!$T$21</f>
@@ -17368,10 +17413,10 @@
       <c r="N50" s="56"/>
     </row>
     <row r="51" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D51" s="155" t="s">
+      <c r="D51" s="156" t="s">
         <v>495</v>
       </c>
-      <c r="E51" s="156"/>
+      <c r="E51" s="157"/>
       <c r="F51" s="42" t="s">
         <v>496</v>
       </c>

</xml_diff>

<commit_message>
£SDRY January Trustpilot update
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA2482B-3C0A-4249-8A6A-938EEA68020C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E151B838-D9D6-4BDB-93F7-22CCFDA7EED7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -4613,7 +4613,7 @@
         </row>
         <row r="42">
           <cell r="C42">
-            <v>4.0934845655588719</v>
+            <v>3.7508794583966352</v>
           </cell>
         </row>
       </sheetData>
@@ -14238,10 +14238,10 @@
   <dimension ref="A1:AO58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14351,7 +14351,7 @@
       </c>
       <c r="AJ1" s="126">
         <f>AVERAGE(AJ3:AJ16)</f>
-        <v>3.8389198675346181</v>
+        <v>3.6676173139534995</v>
       </c>
       <c r="AK1" s="90"/>
     </row>
@@ -16092,7 +16092,7 @@
       </c>
       <c r="AJ15" s="125">
         <f>[13]Main!$C$42</f>
-        <v>4.0934845655588719</v>
+        <v>3.7508794583966352</v>
       </c>
       <c r="AK15" s="4">
         <f>[13]Main!$C$25</f>

</xml_diff>

<commit_message>
£ITS Trustpilot analysis & minor update
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EDDAB4-DF32-4104-A1C7-3523004DDEA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AE4F8C-7072-44F1-BF37-B445E8D1325B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="540" windowWidth="30285" windowHeight="18855" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -4828,27 +4828,52 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Trustpilot Reviews"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>0.13569999999999999</v>
+            <v>7.0000000000000007E-2</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>7.1242497285999988</v>
+            <v>3.6749998600000002</v>
+          </cell>
+          <cell r="Y8">
+            <v>4.2661870503597124</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="Y9">
+            <v>2.8633093525179856</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="Y10">
+            <v>3.1970802919708028</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
             <v>4.2919999999999998</v>
           </cell>
+          <cell r="Y11">
+            <v>3.6590909090909092</v>
+          </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>2.832249728599999</v>
+            <v>-0.61700013999999959</v>
+          </cell>
+          <cell r="Y12">
+            <v>4.2666666666666666</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="Y13">
+            <v>3.9398496240601504</v>
           </cell>
         </row>
         <row r="23">
@@ -4876,11 +4901,22 @@
         </row>
         <row r="36">
           <cell r="C36">
-            <v>0.92751591311027226</v>
+            <v>0.4784533081629998</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="20">
+          <cell r="Q20">
+            <v>-2.1569999999999996</v>
+          </cell>
+          <cell r="R20">
+            <v>0.62499999999999734</v>
+          </cell>
+          <cell r="S20">
+            <v>-1.329000000000002</v>
+          </cell>
+        </row>
         <row r="25">
           <cell r="R25">
             <v>1.3159612495467026</v>
@@ -4925,6 +4961,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10687,7 +10724,7 @@
   </sheetPr>
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
@@ -14241,7 +14278,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14294,7 +14331,7 @@
       </c>
       <c r="T1" s="98">
         <f>AVERAGE(T3:T17)</f>
-        <v>2.7940133207630971</v>
+        <v>2.7640758137666119</v>
       </c>
       <c r="U1" s="111">
         <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
@@ -16247,11 +16284,11 @@
       </c>
       <c r="F17" s="7">
         <f>[15]Main!$C$6</f>
-        <v>0.13569999999999999</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G17" s="49">
         <f>[15]Main!$C$8</f>
-        <v>7.1242497285999988</v>
+        <v>3.6749998600000002</v>
       </c>
       <c r="H17" s="49">
         <f>[15]Main!$C$11</f>
@@ -16259,7 +16296,7 @@
       </c>
       <c r="I17" s="49">
         <f>[15]Main!$C$12</f>
-        <v>2.832249728599999</v>
+        <v>-0.61700013999999959</v>
       </c>
       <c r="J17" s="4" t="str">
         <f>[15]Main!$C$28</f>
@@ -16272,15 +16309,28 @@
       <c r="L17" s="56"/>
       <c r="M17" s="56"/>
       <c r="N17" s="56"/>
+      <c r="O17" s="56">
+        <f>'[15]Financial Model'!$S$20</f>
+        <v>-1.329000000000002</v>
+      </c>
+      <c r="P17" s="56">
+        <f>'[15]Financial Model'!$R$20</f>
+        <v>0.62499999999999734</v>
+      </c>
+      <c r="Q17" s="56">
+        <f>'[15]Financial Model'!$Q$20</f>
+        <v>-2.1569999999999996</v>
+      </c>
       <c r="T17" s="51">
         <f>[15]Main!$C$36</f>
-        <v>0.92751591311027226</v>
-      </c>
-      <c r="V17" s="53">
+        <v>0.4784533081629998</v>
+      </c>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53">
         <f>'[15]Financial Model'!$S$25</f>
         <v>0.2821160943965999</v>
       </c>
-      <c r="W17" s="53">
+      <c r="X17" s="53">
         <f>'[15]Financial Model'!$R$25</f>
         <v>1.3159612495467026</v>
       </c>
@@ -16318,6 +16368,10 @@
       </c>
       <c r="AI17" s="4">
         <v>0</v>
+      </c>
+      <c r="AJ17" s="153">
+        <f>AVERAGE([15]Main!$Y$8:$Y$13)</f>
+        <v>3.698697315777705</v>
       </c>
       <c r="AK17" s="4">
         <f>[15]Main!$C$24</f>

</xml_diff>

<commit_message>
$UA UK expansion news
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie Hill\Desktop\Work\Misc\Financial-Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3BAF91-7F05-46C3-BE20-A9742C801F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC913B98-4F7E-AF40-BFBA-D8CFAB59841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener - Apparel, Accessories" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +49,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -59,15 +61,60 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="6">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
         </ext>
       </extLst>
     </bk>
@@ -77,6 +124,26 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="6">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
+    <bk>
+      <rc t="2" v="3"/>
+    </bk>
+    <bk>
+      <rc t="2" v="4"/>
+    </bk>
+    <bk>
+      <rc t="2" v="5"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
@@ -3148,14 +3215,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.#\x"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="169" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -3598,7 +3665,7 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3607,13 +3674,13 @@
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3642,16 +3709,16 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3660,12 +3727,12 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3702,7 +3769,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -3720,7 +3787,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3741,7 +3808,7 @@
     <xf numFmtId="15" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3768,15 +3835,15 @@
     <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3785,7 +3852,7 @@
     <xf numFmtId="16" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3796,16 +3863,16 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="11" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3840,7 +3907,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3852,7 +3919,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3887,7 +3954,7 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -6102,8 +6169,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6495,6 +6562,91 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+  <rv s="0">
+    <v>12</v>
+    <v>22</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>37</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>34</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>94</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>21</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>39</v>
+    <v>0</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="field" t="s"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6803,25 +6955,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -6863,7 +7015,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>241</v>
       </c>
@@ -6907,7 +7059,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>248</v>
       </c>
@@ -6951,7 +7103,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>253</v>
       </c>
@@ -6995,7 +7147,7 @@
         <v>3.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>259</v>
       </c>
@@ -7039,7 +7191,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>265</v>
       </c>
@@ -7083,7 +7235,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>271</v>
       </c>
@@ -7127,7 +7279,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>277</v>
       </c>
@@ -7171,7 +7323,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>283</v>
       </c>
@@ -7215,7 +7367,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>289</v>
       </c>
@@ -7259,7 +7411,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -7303,7 +7455,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>301</v>
       </c>
@@ -7347,7 +7499,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>306</v>
       </c>
@@ -7391,7 +7543,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="122" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="122" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="113" t="s">
         <v>312</v>
       </c>
@@ -7435,7 +7587,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>317</v>
       </c>
@@ -7479,7 +7631,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>323</v>
       </c>
@@ -7523,7 +7675,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>329</v>
       </c>
@@ -7567,7 +7719,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>335</v>
       </c>
@@ -7611,7 +7763,7 @@
         <v>-4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>341</v>
       </c>
@@ -7655,7 +7807,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>347</v>
       </c>
@@ -7699,7 +7851,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>353</v>
       </c>
@@ -7743,7 +7895,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>357</v>
       </c>
@@ -7787,7 +7939,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>363</v>
       </c>
@@ -7831,7 +7983,7 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>369</v>
       </c>
@@ -7875,7 +8027,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>375</v>
       </c>
@@ -7919,7 +8071,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>380</v>
       </c>
@@ -7963,7 +8115,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>386</v>
       </c>
@@ -8007,7 +8159,7 @@
         <v>-1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>391</v>
       </c>
@@ -8051,7 +8203,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>396</v>
       </c>
@@ -8095,7 +8247,7 @@
         <v>-0.14979999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>402</v>
       </c>
@@ -8139,7 +8291,7 @@
         <v>-1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>10</v>
       </c>
@@ -8183,7 +8335,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>413</v>
       </c>
@@ -8227,7 +8379,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>418</v>
       </c>
@@ -8271,7 +8423,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>423</v>
       </c>
@@ -8315,7 +8467,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>428</v>
       </c>
@@ -8359,7 +8511,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>434</v>
       </c>
@@ -8403,7 +8555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>439</v>
       </c>
@@ -8447,7 +8599,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
         <v>445</v>
       </c>
@@ -8491,7 +8643,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>451</v>
       </c>
@@ -8535,7 +8687,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>456</v>
       </c>
@@ -8579,7 +8731,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>462</v>
       </c>
@@ -8623,7 +8775,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>467</v>
       </c>
@@ -8667,7 +8819,7 @@
         <v>-0.16239999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>472</v>
       </c>
@@ -8711,7 +8863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>476</v>
       </c>
@@ -8829,25 +8981,25 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>16</v>
@@ -8889,7 +9041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
@@ -8933,7 +9085,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>37</v>
       </c>
@@ -8977,7 +9129,7 @@
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -9021,7 +9173,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>50</v>
       </c>
@@ -9065,7 +9217,7 @@
         <v>-2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>56</v>
       </c>
@@ -9109,7 +9261,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -9153,7 +9305,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -9197,7 +9349,7 @@
         <v>5.7299999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
@@ -9241,7 +9393,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>80</v>
       </c>
@@ -9285,7 +9437,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>86</v>
       </c>
@@ -9329,7 +9481,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>92</v>
       </c>
@@ -9373,7 +9525,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
@@ -9417,7 +9569,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>104</v>
       </c>
@@ -9461,7 +9613,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>110</v>
       </c>
@@ -9505,7 +9657,7 @@
         <v>4.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>116</v>
       </c>
@@ -9549,7 +9701,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>121</v>
       </c>
@@ -9593,7 +9745,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>127</v>
       </c>
@@ -9637,7 +9789,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>133</v>
       </c>
@@ -9681,7 +9833,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>139</v>
       </c>
@@ -9725,7 +9877,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>145</v>
       </c>
@@ -9769,7 +9921,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>151</v>
       </c>
@@ -9813,7 +9965,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -9857,7 +10009,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>163</v>
       </c>
@@ -9901,7 +10053,7 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>169</v>
       </c>
@@ -9945,7 +10097,7 @@
         <v>3.56E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>175</v>
       </c>
@@ -9989,7 +10141,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>181</v>
       </c>
@@ -10033,7 +10185,7 @@
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
@@ -10077,7 +10229,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>193</v>
       </c>
@@ -10121,7 +10273,7 @@
         <v>8.5699999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>199</v>
       </c>
@@ -10165,7 +10317,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>204</v>
       </c>
@@ -10209,7 +10361,7 @@
         <v>-1.37E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
@@ -10253,7 +10405,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>214</v>
       </c>
@@ -10297,7 +10449,7 @@
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>219</v>
       </c>
@@ -10341,7 +10493,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>223</v>
       </c>
@@ -10385,7 +10537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>227</v>
       </c>
@@ -10429,7 +10581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>232</v>
       </c>
@@ -10473,7 +10625,7 @@
         <v>-0.21229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>236</v>
       </c>
@@ -10585,16 +10737,16 @@
       <selection activeCell="C66" sqref="C66:L76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="149"/>
       <c r="B1" s="137" t="s">
         <v>16</v>
@@ -10636,7 +10788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="150" t="s">
         <v>589</v>
       </c>
@@ -10680,7 +10832,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="150" t="s">
         <v>589</v>
       </c>
@@ -10724,7 +10876,7 @@
         <v>-8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="150" t="s">
         <v>597</v>
       </c>
@@ -10768,7 +10920,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="150" t="s">
         <v>604</v>
       </c>
@@ -10812,7 +10964,7 @@
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="150" t="s">
         <v>608</v>
       </c>
@@ -10856,7 +11008,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="150" t="s">
         <v>614</v>
       </c>
@@ -10900,7 +11052,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="150" t="s">
         <v>619</v>
       </c>
@@ -10944,7 +11096,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="150" t="s">
         <v>622</v>
       </c>
@@ -10988,7 +11140,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="150" t="s">
         <v>627</v>
       </c>
@@ -11032,7 +11184,7 @@
         <v>-1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="150" t="s">
         <v>632</v>
       </c>
@@ -11076,7 +11228,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="150" t="s">
         <v>635</v>
       </c>
@@ -11120,7 +11272,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="150" t="s">
         <v>641</v>
       </c>
@@ -11164,7 +11316,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="150" t="s">
         <v>646</v>
       </c>
@@ -11208,7 +11360,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="150" t="s">
         <v>652</v>
       </c>
@@ -11252,7 +11404,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="150">
         <v>1910</v>
       </c>
@@ -11296,7 +11448,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="150" t="s">
         <v>661</v>
       </c>
@@ -11340,7 +11492,7 @@
         <v>-2.8E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="150" t="s">
         <v>666</v>
       </c>
@@ -11384,7 +11536,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="150" t="s">
         <v>666</v>
       </c>
@@ -11428,7 +11580,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="150" t="s">
         <v>678</v>
       </c>
@@ -11472,7 +11624,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="150" t="s">
         <v>684</v>
       </c>
@@ -11516,7 +11668,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="150" t="s">
         <v>690</v>
       </c>
@@ -11560,7 +11712,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
         <v>696</v>
       </c>
@@ -11604,7 +11756,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="150" t="s">
         <v>699</v>
       </c>
@@ -11648,7 +11800,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="150">
         <v>551</v>
       </c>
@@ -11692,7 +11844,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="150">
         <v>1121</v>
       </c>
@@ -11736,7 +11888,7 @@
         <v>1.67E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="150" t="s">
         <v>714</v>
       </c>
@@ -11780,7 +11932,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="150" t="s">
         <v>720</v>
       </c>
@@ -11824,7 +11976,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="150">
         <v>1836</v>
       </c>
@@ -11868,7 +12020,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="150" t="s">
         <v>731</v>
       </c>
@@ -11912,7 +12064,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="150">
         <v>3813</v>
       </c>
@@ -11956,7 +12108,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="150" t="s">
         <v>741</v>
       </c>
@@ -12000,7 +12152,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="150" t="s">
         <v>747</v>
       </c>
@@ -12044,7 +12196,7 @@
         <v>-2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="150" t="s">
         <v>752</v>
       </c>
@@ -12088,7 +12240,7 @@
         <v>7.51E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="150">
         <v>1058</v>
       </c>
@@ -12104,9 +12256,9 @@
       <c r="E35" s="140" t="s">
         <v>759</v>
       </c>
-      <c r="F35" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F35" ca="1">-_FV(HKD$31,"22")</f>
-        <v>#NAME?</v>
+      <c r="F35" s="140" t="e" cm="1" vm="1">
+        <f t="array" ref="F35">-_FV(HKD$31,"22")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G35" s="138" t="s">
         <v>54</v>
@@ -12133,7 +12285,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="150" t="s">
         <v>762</v>
       </c>
@@ -12177,7 +12329,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="150">
         <v>210</v>
       </c>
@@ -12221,7 +12373,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="150" t="s">
         <v>773</v>
       </c>
@@ -12265,7 +12417,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="150" t="s">
         <v>779</v>
       </c>
@@ -12309,7 +12461,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="150" t="s">
         <v>785</v>
       </c>
@@ -12353,7 +12505,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="150" t="s">
         <v>790</v>
       </c>
@@ -12397,7 +12549,7 @@
         <v>-7.4200000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="150">
         <v>1488</v>
       </c>
@@ -12441,7 +12593,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="150" t="s">
         <v>800</v>
       </c>
@@ -12485,7 +12637,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="150" t="s">
         <v>569</v>
       </c>
@@ -12529,7 +12681,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="150">
         <v>1100</v>
       </c>
@@ -12573,7 +12725,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="150">
         <v>1170</v>
       </c>
@@ -12589,9 +12741,9 @@
       <c r="E46" s="140" t="s">
         <v>816</v>
       </c>
-      <c r="F46" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F46" ca="1">-_FV(HKD$43,"37")</f>
-        <v>#NAME?</v>
+      <c r="F46" s="140" t="e" cm="1" vm="2">
+        <f t="array" ref="F46">-_FV(HKD$43,"37")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G46" s="138" t="s">
         <v>54</v>
@@ -12618,7 +12770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="150">
         <v>1023</v>
       </c>
@@ -12662,7 +12814,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="150" t="s">
         <v>824</v>
       </c>
@@ -12706,7 +12858,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="150">
         <v>676</v>
       </c>
@@ -12750,7 +12902,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="150" t="s">
         <v>835</v>
       </c>
@@ -12794,7 +12946,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="150" t="s">
         <v>824</v>
       </c>
@@ -12838,7 +12990,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="152" t="s">
         <v>845</v>
       </c>
@@ -12882,7 +13034,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="152" t="s">
         <v>845</v>
       </c>
@@ -12926,7 +13078,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="152" t="s">
         <v>855</v>
       </c>
@@ -12970,7 +13122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="152">
         <v>1028</v>
       </c>
@@ -13014,7 +13166,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="152">
         <v>1386</v>
       </c>
@@ -13030,9 +13182,9 @@
       <c r="E56" s="140" t="s">
         <v>865</v>
       </c>
-      <c r="F56" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F56" ca="1">-_FV(HKD$10,"34")</f>
-        <v>#NAME?</v>
+      <c r="F56" s="140" t="e" cm="1" vm="3">
+        <f t="array" ref="F56">-_FV(HKD$10,"34")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G56" s="138" t="s">
         <v>54</v>
@@ -13059,7 +13211,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="152">
         <v>1842</v>
       </c>
@@ -13103,7 +13255,7 @@
         <v>-6.9400000000000003E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="152" t="s">
         <v>870</v>
       </c>
@@ -13147,7 +13299,7 @@
         <v>-1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="152">
         <v>738</v>
       </c>
@@ -13191,7 +13343,7 @@
         <v>-3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="152">
         <v>264</v>
       </c>
@@ -13207,9 +13359,9 @@
       <c r="E60" s="140" t="s">
         <v>880</v>
       </c>
-      <c r="F60" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F60" ca="1">-_FV(HKD$20,"94")</f>
-        <v>#NAME?</v>
+      <c r="F60" s="140" t="e" cm="1" vm="4">
+        <f t="array" ref="F60">-_FV(HKD$20,"94")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G60" s="138" t="s">
         <v>54</v>
@@ -13236,7 +13388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="152" t="s">
         <v>883</v>
       </c>
@@ -13280,7 +13432,7 @@
         <v>-2.76E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="152" t="s">
         <v>889</v>
       </c>
@@ -13324,7 +13476,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="152" t="s">
         <v>889</v>
       </c>
@@ -13368,7 +13520,7 @@
         <v>-1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="152" t="s">
         <v>899</v>
       </c>
@@ -13412,7 +13564,7 @@
         <v>-1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="152">
         <v>1255</v>
       </c>
@@ -13428,9 +13580,9 @@
       <c r="E65" s="140" t="s">
         <v>906</v>
       </c>
-      <c r="F65" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F65" ca="1">-_FV(HKD$43,"21")</f>
-        <v>#NAME?</v>
+      <c r="F65" s="140" t="e" cm="1" vm="5">
+        <f t="array" ref="F65">-_FV(HKD$43,"21")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G65" s="138" t="s">
         <v>54</v>
@@ -13457,7 +13609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="152">
         <v>1027</v>
       </c>
@@ -13501,7 +13653,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="152">
         <v>2683</v>
       </c>
@@ -13545,7 +13697,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="152" t="s">
         <v>919</v>
       </c>
@@ -13589,7 +13741,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="152" t="s">
         <v>925</v>
       </c>
@@ -13633,7 +13785,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="152" t="s">
         <v>931</v>
       </c>
@@ -13677,7 +13829,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="152" t="s">
         <v>936</v>
       </c>
@@ -13721,7 +13873,7 @@
         <v>-1.12E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="152" t="s">
         <v>942</v>
       </c>
@@ -13765,7 +13917,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="152" t="s">
         <v>948</v>
       </c>
@@ -13809,7 +13961,7 @@
         <v>-4.3E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="152" t="s">
         <v>948</v>
       </c>
@@ -13853,7 +14005,7 @@
         <v>-1.04E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="152">
         <v>1096</v>
       </c>
@@ -13897,7 +14049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="152">
         <v>8285</v>
       </c>
@@ -13941,7 +14093,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="152" t="s">
         <v>967</v>
       </c>
@@ -13985,7 +14137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="152">
         <v>8187</v>
       </c>
@@ -14001,9 +14153,9 @@
       <c r="E78" s="140" t="s">
         <v>972</v>
       </c>
-      <c r="F78" s="140" t="e" cm="1">
-        <f t="array" aca="1" ref="F78" ca="1">-_FV(HKD$9,"39")</f>
-        <v>#NAME?</v>
+      <c r="F78" s="140" t="e" cm="1" vm="6">
+        <f t="array" ref="F78">-_FV(HKD$9,"39")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G78" s="138" t="s">
         <v>54</v>
@@ -14135,34 +14287,34 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="19" width="9.140625" style="1"/>
-    <col min="20" max="24" width="9.140625" style="4"/>
-    <col min="25" max="30" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="4"/>
+    <col min="6" max="6" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1640625" style="6"/>
+    <col min="10" max="11" width="9.1640625" style="4"/>
+    <col min="12" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="24" width="9.1640625" style="4"/>
+    <col min="25" max="30" width="9.1640625" style="1"/>
     <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.140625" style="4"/>
-    <col min="35" max="35" width="9.140625" style="1"/>
-    <col min="36" max="36" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="41.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="56.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="32" max="34" width="9.1640625" style="4"/>
+    <col min="35" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
       <c r="F1" s="158" t="s">
         <v>499</v>
@@ -14249,7 +14401,7 @@
       </c>
       <c r="AK1" s="90"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -14369,7 +14521,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>529</v>
       </c>
@@ -14495,7 +14647,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>523</v>
       </c>
@@ -14607,7 +14759,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>56</v>
       </c>
@@ -14731,7 +14883,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -14861,7 +15013,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B7" s="96" t="s">
         <v>526</v>
       </c>
@@ -14991,7 +15143,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>485</v>
       </c>
@@ -15125,7 +15277,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>486</v>
       </c>
@@ -15214,7 +15366,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>491</v>
       </c>
@@ -15342,7 +15494,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>1019</v>
       </c>
@@ -15485,7 +15637,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>500</v>
       </c>
@@ -15624,7 +15776,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
@@ -15749,7 +15901,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" s="103" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="104" t="s">
         <v>391</v>
       </c>
@@ -15859,7 +16011,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -16003,7 +16155,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" s="91" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="92" t="s">
         <v>445</v>
       </c>
@@ -16126,7 +16278,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>503</v>
       </c>
@@ -16242,7 +16394,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="F18" s="7"/>
       <c r="G18" s="49"/>
@@ -16268,7 +16420,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B19" s="136" t="s">
         <v>582</v>
       </c>
@@ -16299,7 +16451,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B20" s="135" t="s">
         <v>975</v>
       </c>
@@ -16325,7 +16477,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -16349,7 +16501,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>214</v>
       </c>
@@ -16375,7 +16527,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>492</v>
       </c>
@@ -16400,7 +16552,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
         <v>556</v>
       </c>
@@ -16441,7 +16593,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B25" s="135">
         <v>9983</v>
       </c>
@@ -16474,7 +16626,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B26" s="135" t="s">
         <v>577</v>
       </c>
@@ -16500,7 +16652,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B27" s="135" t="s">
         <v>576</v>
       </c>
@@ -16526,7 +16678,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B28" s="135">
         <v>8022</v>
       </c>
@@ -16563,7 +16715,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="1"/>
@@ -16573,7 +16725,7 @@
       <c r="M29" s="56"/>
       <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B30" s="136" t="s">
         <v>582</v>
       </c>
@@ -16589,7 +16741,7 @@
       <c r="M30" s="56"/>
       <c r="N30" s="56"/>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>511</v>
       </c>
@@ -16622,7 +16774,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B32" s="3" t="s">
         <v>540</v>
       </c>
@@ -16686,7 +16838,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>541</v>
       </c>
@@ -16713,7 +16865,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>575</v>
       </c>
@@ -16738,7 +16890,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>587</v>
       </c>
@@ -16763,7 +16915,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>588</v>
       </c>
@@ -16788,7 +16940,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.15">
       <c r="F37" s="7"/>
       <c r="G37" s="56"/>
       <c r="H37" s="1"/>
@@ -16798,7 +16950,7 @@
       <c r="M37" s="56"/>
       <c r="N37" s="56"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B38" s="136" t="s">
         <v>582</v>
       </c>
@@ -16813,7 +16965,7 @@
       <c r="M38" s="56"/>
       <c r="N38" s="56"/>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
         <v>581</v>
       </c>
@@ -16935,7 +17087,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B40" s="3" t="s">
         <v>985</v>
       </c>
@@ -17041,7 +17193,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
         <v>569</v>
       </c>
@@ -17172,7 +17324,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B42" s="3"/>
       <c r="F42" s="54"/>
       <c r="G42" s="56"/>
@@ -17204,7 +17356,7 @@
       <c r="AK42" s="4"/>
       <c r="AL42" s="4"/>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>579</v>
       </c>
@@ -17231,7 +17383,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>580</v>
       </c>
@@ -17258,7 +17410,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>568</v>
       </c>
@@ -17286,7 +17438,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G46" s="56"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -17295,7 +17447,7 @@
       <c r="M46" s="56"/>
       <c r="N46" s="56"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G47" s="56"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -17304,7 +17456,7 @@
       <c r="M47" s="56"/>
       <c r="N47" s="56"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.15">
       <c r="G48" s="56"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -17313,7 +17465,7 @@
       <c r="M48" s="56"/>
       <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G49" s="49"/>
       <c r="I49" s="4"/>
       <c r="J49" s="1"/>
@@ -17321,7 +17473,7 @@
       <c r="M49" s="56"/>
       <c r="N49" s="56"/>
     </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G50" s="49"/>
       <c r="I50" s="4"/>
       <c r="J50" s="1"/>
@@ -17329,7 +17481,7 @@
       <c r="M50" s="56"/>
       <c r="N50" s="56"/>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D51" s="156" t="s">
         <v>495</v>
       </c>
@@ -17342,7 +17494,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D52" s="43" t="s">
         <v>497</v>
       </c>
@@ -17358,7 +17510,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D53" s="43" t="s">
         <v>498</v>
       </c>
@@ -17374,7 +17526,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D54" s="46" t="s">
         <v>564</v>
       </c>
@@ -17387,16 +17539,16 @@
       </c>
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G56" s="49"/>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G57" s="49"/>
     </row>
-    <row r="58" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:14" x14ac:dyDescent="0.15">
       <c r="G58" s="49"/>
     </row>
   </sheetData>
@@ -17448,21 +17600,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E1" s="90" t="e">
         <f>AVERAGE(E3:E16)</f>
         <v>#DIV/0!</v>
@@ -17473,7 +17625,7 @@
       </c>
       <c r="G1" s="90"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>558</v>
@@ -17500,98 +17652,98 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="133" t="s">
         <v>554</v>
       </c>
       <c r="D24" s="133"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>

</xml_diff>

<commit_message>
£SDRY updated Trustpilot stats
</commit_message>
<xml_diff>
--- a/Overview - Fashion Retailers.xlsx
+++ b/Overview - Fashion Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E051162F-60CF-417D-B97A-2B2C2DFD2E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CD7761-89A4-41A4-BB3E-A2B969C70DCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{791689F3-ED44-47EC-8DFE-D53B17FD85F9}"/>
   </bookViews>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="1021">
   <si>
     <t>Ticker</t>
   </si>
@@ -4600,22 +4600,22 @@
         </row>
         <row r="34">
           <cell r="C34">
-            <v>10.095356069249942</v>
+            <v>-0.54532645883862241</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>5.7959434715237013</v>
+            <v>-0.30936040067521942</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>0.52963273280742429</v>
+            <v>-0.86283004406779817</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38">
-            <v>1.4467338886453514E-2</v>
+            <v>-0.81606519208381867</v>
           </cell>
         </row>
         <row r="39">
@@ -4694,8 +4694,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14290,7 +14290,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14335,7 +14335,7 @@
       <c r="Q1" s="161"/>
       <c r="R1" s="98">
         <f>AVERAGE(R3:R16)</f>
-        <v>14.711850714269159</v>
+        <v>14.156823089523801</v>
       </c>
       <c r="S1" s="98">
         <f>AVERAGE(S3:S16)</f>
@@ -14343,11 +14343,11 @@
       </c>
       <c r="T1" s="98">
         <f>AVERAGE(T3:T17)</f>
-        <v>2.6065048414499694</v>
+        <v>2.513673989658288</v>
       </c>
       <c r="U1" s="111">
         <f t="shared" ref="U1:AB1" si="0">AVERAGE(U3:U16)</f>
-        <v>4.973206324375111E-2</v>
+        <v>-3.3321189853276104E-2</v>
       </c>
       <c r="V1" s="87"/>
       <c r="W1" s="111">
@@ -16063,7 +16063,7 @@
       </c>
       <c r="L15" s="50">
         <f>[13]Main!$C$34</f>
-        <v>10.095356069249942</v>
+        <v>-0.54532645883862241</v>
       </c>
       <c r="N15" s="1">
         <f xml:space="preserve"> '[13]Financial Model'!$U$17</f>
@@ -16083,7 +16083,7 @@
       </c>
       <c r="R15" s="51">
         <f>[13]Main!$C$35</f>
-        <v>5.7959434715237013</v>
+        <v>-0.30936040067521942</v>
       </c>
       <c r="S15" s="51">
         <f>[13]Main!$C$39</f>
@@ -16091,11 +16091,11 @@
       </c>
       <c r="T15" s="51">
         <f>[13]Main!$C$37</f>
-        <v>0.52963273280742429</v>
+        <v>-0.86283004406779817</v>
       </c>
       <c r="U15" s="131">
         <f>[13]Main!$C$38</f>
-        <v>1.4467338886453514E-2</v>
+        <v>-0.81606519208381867</v>
       </c>
       <c r="V15" s="53">
         <f>'[13]Financial Model'!$V$21</f>

</xml_diff>